<commit_message>
Se añaden ajusten en la generación de los R08
</commit_message>
<xml_diff>
--- a/Oficial/Patron_FL.xlsx
+++ b/Oficial/Patron_FL.xlsx
@@ -9,13 +9,14 @@
   </bookViews>
   <sheets>
     <sheet name="BASE_SSE" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Labs" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="158">
   <si>
     <t>SOLICITUD  DE SERVICIO EXTERNO A LABORATORIO</t>
   </si>
@@ -343,6 +344,162 @@
   </si>
   <si>
     <t>si</t>
+  </si>
+  <si>
+    <t>LABORATORIO</t>
+  </si>
+  <si>
+    <t>DIRECCIÓN</t>
+  </si>
+  <si>
+    <t>HORARIO</t>
+  </si>
+  <si>
+    <t>Teléfono</t>
+  </si>
+  <si>
+    <t>A nombre</t>
+  </si>
+  <si>
+    <t>AVENIDA CENTRAL N°681, QUILICURA SANTIAGO</t>
+  </si>
+  <si>
+    <t>L-V 9:30 a 18:00
+S 9:30 a 12:00 (previo aviso)</t>
+  </si>
+  <si>
+    <t>LABORATORIO HIDROLAB</t>
+  </si>
+  <si>
+    <t>U DE CONCEPCIÓN</t>
+  </si>
+  <si>
+    <t>CABINA 5, BARRIO UNIVERSITARIO S/N, CONCEPCIÓN</t>
+  </si>
+  <si>
+    <t>ANDREA CONTRERAS (Administración)
+GABRIELA FRANYOLA (muestras)</t>
+  </si>
+  <si>
+    <t>SGS-SANTIAGO</t>
+  </si>
+  <si>
+    <t>PUERTO MADERO 130. PUDAHUEL</t>
+  </si>
+  <si>
+    <t>L-V 8:00 a 20:00h y Sáb. 9:00 a 13:00h (previo aviso)</t>
+  </si>
+  <si>
+    <t>LEYDI CORTÉS</t>
+  </si>
+  <si>
+    <t>SGS-ANTOFA</t>
+  </si>
+  <si>
+    <t>PEDRO AGUIRRE CERDA N°7367. ANTOFAGASTA</t>
+  </si>
+  <si>
+    <t>L-V 8:30 a 18:00h y Sáb. 9:00 a 13:00h (previo aviso)</t>
+  </si>
+  <si>
+    <t>CECILIA TAPIA</t>
+  </si>
+  <si>
+    <t>ALS-ANTOFA</t>
+  </si>
+  <si>
+    <t>JUAN GUTEMBERG N°438, GALPÓN 9 Y 10. ANTOFAGASTA</t>
+  </si>
+  <si>
+    <t>L-V 8:30 a 17:30h (Holding cortos antes de las 15:00 hrs)</t>
+  </si>
+  <si>
+    <t>55 2899201</t>
+  </si>
+  <si>
+    <t>JOHANNA GONZALEZ</t>
+  </si>
+  <si>
+    <t>ALS-SANTIAGO</t>
+  </si>
+  <si>
+    <t>HERMANOS CARRERA PINTO 159, PAQUE INDUSTRIAL LOS LIBERTADOSRES COLINA</t>
+  </si>
+  <si>
+    <t>L-V 8:00 a 17:00h
+(Holding cortos antes de las 15:00 hrs)</t>
+  </si>
+  <si>
+    <t>PAULETTE BENAVIDEZ</t>
+  </si>
+  <si>
+    <t>LUIS LOPEZ</t>
+  </si>
+  <si>
+    <t>PRIMERA DEL SUR #    871 PLACILLA, VALPARAISO.</t>
+  </si>
+  <si>
+    <t>2298803 | 8-5955842</t>
+  </si>
+  <si>
+    <t>CENMA</t>
+  </si>
+  <si>
+    <t>AVENIDA LARRAÍN 9975. LA REINA</t>
+  </si>
+  <si>
+    <t>SYLVIA PARRA</t>
+  </si>
+  <si>
+    <t>DICTUC</t>
+  </si>
+  <si>
+    <t>AV. VICUÑA MACKENNA #4860 - EDIFICIO HERNÁN BRIONES - PISO 1 - MACUL -</t>
+  </si>
+  <si>
+    <t>L-V 8:30 a 18:00</t>
+  </si>
+  <si>
+    <t>MARÍA ALEJANDRA  ESPINOZA (Negocio)
+BELEN PAREDES (muestras)</t>
+  </si>
+  <si>
+    <t>ANAM</t>
+  </si>
+  <si>
+    <t>AVENIDA AMÉRICO VESPUCIO N° 451. QUILICURA</t>
+  </si>
+  <si>
+    <t>LUNES A VIERNES 9-17:50</t>
+  </si>
+  <si>
+    <t>VERÓNICA RIVAS (Administración)
+ARTURO GIVOVICH
+(muestras)</t>
+  </si>
+  <si>
+    <t>ARRAÚ MÉNDEZ S/N PEDRO DE VALDIVIA. CONCEPCIÖN</t>
+  </si>
+  <si>
+    <t>LUNES A VIERNES  DE 9 A 18:30 Y SABADO DE 9 A 12:00</t>
+  </si>
+  <si>
+    <t>MAURICIO GATICA (Administración)
+MANUEL ARAVENA (muestras)</t>
+  </si>
+  <si>
+    <t>CORTHON S.A</t>
+  </si>
+  <si>
+    <t>PALACIO RIESCO 4549
+HUECHURABA
+SANTIAGO</t>
+  </si>
+  <si>
+    <t>LUNES A VIERNES  DE 9 A 17:30</t>
+  </si>
+  <si>
+    <t>JUAN MANDUCHER (Administración)</t>
   </si>
 </sst>
 </file>
@@ -353,11 +510,12 @@
     <numFmt numFmtId="164" formatCode="GENERAL"/>
     <numFmt numFmtId="165" formatCode="0.00"/>
   </numFmts>
-  <fonts count="14">
+  <fonts count="16">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -379,6 +537,7 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -386,24 +545,28 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="12"/>
       <name val="arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -411,6 +574,7 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -418,6 +582,7 @@
       <color rgb="FF800000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -425,18 +590,36 @@
       <color rgb="FF800000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="14"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="12"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="11"/>
+      <color rgb="FF1F497D"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF17365D"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="7">
@@ -477,7 +660,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="13">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -562,6 +745,21 @@
       <bottom style="thin"/>
       <diagonal/>
     </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair">
+        <color rgb="FF00000A"/>
+      </left>
+      <right style="hair">
+        <color rgb="FF00000A"/>
+      </right>
+      <top style="hair">
+        <color rgb="FF00000A"/>
+      </top>
+      <bottom style="hair">
+        <color rgb="FF00000A"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -588,7 +786,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="62">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -823,6 +1021,18 @@
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -846,7 +1056,7 @@
       <rgbColor rgb="FF00FFFF"/>
       <rgbColor rgb="FF800000"/>
       <rgbColor rgb="FF008000"/>
-      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF00000A"/>
       <rgbColor rgb="FF808000"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
@@ -884,13 +1094,13 @@
       <rgbColor rgb="FFFF6600"/>
       <rgbColor rgb="FF666699"/>
       <rgbColor rgb="FF969696"/>
-      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF17365D"/>
       <rgbColor rgb="FF339966"/>
       <rgbColor rgb="FF003300"/>
       <rgbColor rgb="FF333300"/>
       <rgbColor rgb="FF993300"/>
       <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF1F497D"/>
       <rgbColor rgb="FF333333"/>
     </indexedColors>
   </colors>
@@ -902,15 +1112,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>334440</xdr:colOff>
+      <xdr:colOff>415440</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>7560</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>897840</xdr:colOff>
+      <xdr:colOff>977760</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>778680</xdr:rowOff>
+      <xdr:rowOff>777600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -923,8 +1133,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="334440" y="7560"/>
-          <a:ext cx="563400" cy="771120"/>
+          <a:off x="415440" y="7560"/>
+          <a:ext cx="562320" cy="770040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -946,8 +1156,8 @@
   </sheetPr>
   <dimension ref="A1:S53"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J5" activeCellId="0" sqref="J5"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G22" activeCellId="1" sqref="B4:F9 G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -2163,4 +2373,230 @@
   </headerFooter>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:E13"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E1" activeCellId="1" sqref="B4:F9 E1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.2040816326531"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="76.0561224489796"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="50.8010204081633"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="36.6989795918367"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="59" t="s">
+        <v>109</v>
+      </c>
+      <c r="B1" s="59" t="s">
+        <v>110</v>
+      </c>
+      <c r="C1" s="59" t="s">
+        <v>111</v>
+      </c>
+      <c r="D1" s="59" t="s">
+        <v>112</v>
+      </c>
+      <c r="E1" s="59" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="60" t="s">
+        <v>77</v>
+      </c>
+      <c r="B2" s="60" t="s">
+        <v>114</v>
+      </c>
+      <c r="C2" s="61" t="s">
+        <v>115</v>
+      </c>
+      <c r="D2" s="61"/>
+      <c r="E2" s="60" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="60" t="s">
+        <v>117</v>
+      </c>
+      <c r="B3" s="60" t="s">
+        <v>118</v>
+      </c>
+      <c r="C3" s="60"/>
+      <c r="D3" s="60"/>
+      <c r="E3" s="61" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="60" t="s">
+        <v>120</v>
+      </c>
+      <c r="B4" s="60" t="s">
+        <v>121</v>
+      </c>
+      <c r="C4" s="60" t="s">
+        <v>122</v>
+      </c>
+      <c r="D4" s="60"/>
+      <c r="E4" s="60" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="60" t="s">
+        <v>124</v>
+      </c>
+      <c r="B5" s="60" t="s">
+        <v>125</v>
+      </c>
+      <c r="C5" s="60" t="s">
+        <v>126</v>
+      </c>
+      <c r="D5" s="60"/>
+      <c r="E5" s="60" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="60" t="s">
+        <v>128</v>
+      </c>
+      <c r="B6" s="60" t="s">
+        <v>129</v>
+      </c>
+      <c r="C6" s="60" t="s">
+        <v>130</v>
+      </c>
+      <c r="D6" s="60" t="s">
+        <v>131</v>
+      </c>
+      <c r="E6" s="61" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="60" t="s">
+        <v>133</v>
+      </c>
+      <c r="B7" s="60" t="s">
+        <v>134</v>
+      </c>
+      <c r="C7" s="61" t="s">
+        <v>135</v>
+      </c>
+      <c r="D7" s="61"/>
+      <c r="E7" s="60" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="60" t="s">
+        <v>137</v>
+      </c>
+      <c r="B8" s="60" t="s">
+        <v>138</v>
+      </c>
+      <c r="C8" s="61"/>
+      <c r="D8" s="61" t="s">
+        <v>139</v>
+      </c>
+      <c r="E8" s="60" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="60" t="s">
+        <v>140</v>
+      </c>
+      <c r="B9" s="60" t="s">
+        <v>141</v>
+      </c>
+      <c r="C9" s="60"/>
+      <c r="D9" s="60"/>
+      <c r="E9" s="60" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="60" t="s">
+        <v>143</v>
+      </c>
+      <c r="B10" s="60" t="s">
+        <v>144</v>
+      </c>
+      <c r="C10" s="60" t="s">
+        <v>145</v>
+      </c>
+      <c r="D10" s="60"/>
+      <c r="E10" s="61" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="60" t="s">
+        <v>147</v>
+      </c>
+      <c r="B11" s="60" t="s">
+        <v>148</v>
+      </c>
+      <c r="C11" s="60" t="s">
+        <v>149</v>
+      </c>
+      <c r="D11" s="60"/>
+      <c r="E11" s="61" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="60" t="s">
+        <v>68</v>
+      </c>
+      <c r="B12" s="60" t="s">
+        <v>151</v>
+      </c>
+      <c r="C12" s="60" t="s">
+        <v>152</v>
+      </c>
+      <c r="D12" s="60"/>
+      <c r="E12" s="61" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="60" t="s">
+        <v>154</v>
+      </c>
+      <c r="B13" s="61" t="s">
+        <v>155</v>
+      </c>
+      <c r="C13" s="60" t="s">
+        <v>156</v>
+      </c>
+      <c r="D13" s="60"/>
+      <c r="E13" s="61" t="s">
+        <v>157</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Nuevos ajustes a plantilla patron, transponiendo observaciones
</commit_message>
<xml_diff>
--- a/Oficial/Patron_FL.xlsx
+++ b/Oficial/Patron_FL.xlsx
@@ -261,6 +261,24 @@
     <t>Matriz\Estaciones</t>
   </si>
   <si>
+    <t>Agua Salar</t>
+  </si>
+  <si>
+    <t>Agua Salar Dulce</t>
+  </si>
+  <si>
+    <t>Agua Dulce</t>
+  </si>
+  <si>
+    <t>Sedimento Salar</t>
+  </si>
+  <si>
+    <t>Sedimento Salar Dulce</t>
+  </si>
+  <si>
+    <t>Sedimento Dulce</t>
+  </si>
+  <si>
     <t>RCA-01</t>
   </si>
   <si>
@@ -289,24 +307,6 @@
   </si>
   <si>
     <t>RCA-10</t>
-  </si>
-  <si>
-    <t>Agua Salar</t>
-  </si>
-  <si>
-    <t>Agua Salar Dulce</t>
-  </si>
-  <si>
-    <t>Agua Dulce</t>
-  </si>
-  <si>
-    <t>Sedimento Salar</t>
-  </si>
-  <si>
-    <t>Sedimento Salar Dulce</t>
-  </si>
-  <si>
-    <t>Sedimento Dulce</t>
   </si>
   <si>
     <t>Equipos-Materiales</t>
@@ -510,7 +510,7 @@
     <numFmt numFmtId="164" formatCode="GENERAL"/>
     <numFmt numFmtId="165" formatCode="0.00"/>
   </numFmts>
-  <fonts count="16">
+  <fonts count="13">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -571,30 +571,6 @@
     <font>
       <b val="true"/>
       <sz val="14"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="14"/>
-      <color rgb="FF800000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="14"/>
-      <color rgb="FF800000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="14"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -638,7 +614,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC6D9F1"/>
-        <bgColor rgb="FFCCCCFF"/>
+        <bgColor rgb="FFD9D9D9"/>
       </patternFill>
     </fill>
     <fill>
@@ -655,8 +631,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFCCCCFF"/>
-        <bgColor rgb="FFC6D9F1"/>
+        <fgColor rgb="FF66FFFF"/>
+        <bgColor rgb="FF00FFFF"/>
       </patternFill>
     </fill>
   </fills>
@@ -786,7 +762,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="60">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -975,23 +951,15 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="9" fillId="2" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="10" fillId="6" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="6" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="6" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1003,7 +971,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1023,15 +991,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1069,7 +1037,7 @@
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
       <rgbColor rgb="FF0066CC"/>
-      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FFC6D9F1"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FFFFFF00"/>
@@ -1079,7 +1047,7 @@
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FF00CCFF"/>
-      <rgbColor rgb="FFC6D9F1"/>
+      <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FFCCFFCC"/>
       <rgbColor rgb="FFFFFF99"/>
       <rgbColor rgb="FF8EB4E3"/>
@@ -1087,7 +1055,7 @@
       <rgbColor rgb="FFCC99FF"/>
       <rgbColor rgb="FFFFCC99"/>
       <rgbColor rgb="FF3366FF"/>
-      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF66FFFF"/>
       <rgbColor rgb="FF99CC00"/>
       <rgbColor rgb="FFFFCC00"/>
       <rgbColor rgb="FFFF9900"/>
@@ -1112,15 +1080,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>415440</xdr:colOff>
+      <xdr:colOff>469440</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>7560</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>977760</xdr:colOff>
+      <xdr:colOff>1031040</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>777600</xdr:rowOff>
+      <xdr:rowOff>776880</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1133,8 +1101,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="415440" y="7560"/>
-          <a:ext cx="562320" cy="770040"/>
+          <a:off x="469440" y="7560"/>
+          <a:ext cx="561600" cy="769320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1154,10 +1122,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:S53"/>
+  <dimension ref="A1:S55"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G22" activeCellId="1" sqref="B4:F9 G22"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A14" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E35" activeCellId="0" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1168,9 +1136,12 @@
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.6275510204082"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.8775510204082"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="19.7448979591837"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="16.1071428571429"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="15.9642857142857"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.8979591836735"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="22.4540816326531"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="17.0918367346939"/>
+    <col collapsed="false" hidden="false" max="18" min="10" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="32.3010204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="20" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="82.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1934,73 +1905,43 @@
       <c r="R23" s="44"/>
       <c r="S23" s="44"/>
     </row>
-    <row r="25" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="47" t="s">
         <v>80</v>
       </c>
-      <c r="B25" s="48" t="s">
+      <c r="B25" s="47" t="s">
+        <v>41</v>
+      </c>
+      <c r="C25" s="47" t="s">
         <v>81</v>
       </c>
-      <c r="C25" s="49" t="s">
+      <c r="D25" s="47" t="s">
         <v>82</v>
       </c>
-      <c r="D25" s="49" t="s">
+      <c r="E25" s="47" t="s">
         <v>83</v>
       </c>
-      <c r="E25" s="49" t="s">
+      <c r="F25" s="47" t="s">
+        <v>60</v>
+      </c>
+      <c r="G25" s="47" t="s">
         <v>84</v>
       </c>
-      <c r="F25" s="49" t="s">
+      <c r="H25" s="47" t="s">
         <v>85</v>
       </c>
-      <c r="G25" s="49" t="s">
+      <c r="I25" s="47" t="s">
         <v>86</v>
       </c>
-      <c r="H25" s="49" t="s">
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
         <v>87</v>
       </c>
-      <c r="I25" s="49" t="s">
-        <v>88</v>
-      </c>
-      <c r="J25" s="49" t="s">
-        <v>89</v>
-      </c>
-      <c r="K25" s="49" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="45" t="s">
-        <v>41</v>
-      </c>
-      <c r="B26" s="45" t="n">
-        <v>1</v>
-      </c>
-      <c r="C26" s="45" t="n">
-        <v>1</v>
-      </c>
-      <c r="D26" s="45" t="n">
-        <v>1</v>
-      </c>
-      <c r="E26" s="45" t="n">
-        <v>1</v>
-      </c>
-      <c r="F26" s="45" t="n">
-        <v>1</v>
-      </c>
-      <c r="G26" s="45" t="n">
-        <v>1</v>
-      </c>
-      <c r="H26" s="45" t="n">
-        <v>1</v>
-      </c>
-      <c r="I26" s="45" t="n">
-        <v>1</v>
-      </c>
-      <c r="J26" s="45" t="n">
-        <v>1</v>
-      </c>
-      <c r="K26" s="45" t="n">
+      <c r="B26" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F26" s="0" t="n">
         <v>1</v>
       </c>
       <c r="L26" s="9"/>
@@ -2013,19 +1954,15 @@
       <c r="S26" s="9"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="45" t="s">
-        <v>91</v>
-      </c>
-      <c r="B27" s="45"/>
-      <c r="C27" s="45"/>
-      <c r="D27" s="45"/>
-      <c r="E27" s="45"/>
-      <c r="F27" s="45"/>
-      <c r="G27" s="45"/>
-      <c r="H27" s="45"/>
-      <c r="I27" s="45"/>
-      <c r="J27" s="45"/>
-      <c r="K27" s="45"/>
+      <c r="A27" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="B27" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F27" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="L27" s="9"/>
       <c r="M27" s="9"/>
       <c r="N27" s="9"/>
@@ -2036,19 +1973,12 @@
       <c r="S27" s="9"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="45" t="s">
-        <v>92</v>
-      </c>
-      <c r="B28" s="45"/>
-      <c r="C28" s="45"/>
-      <c r="D28" s="45"/>
-      <c r="E28" s="45"/>
-      <c r="F28" s="45"/>
-      <c r="G28" s="45"/>
-      <c r="H28" s="45"/>
-      <c r="I28" s="45"/>
-      <c r="J28" s="45"/>
-      <c r="K28" s="45"/>
+      <c r="A28" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="B28" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="L28" s="9"/>
       <c r="M28" s="9"/>
       <c r="N28" s="9"/>
@@ -2059,19 +1989,12 @@
       <c r="S28" s="9"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="45" t="s">
-        <v>93</v>
-      </c>
-      <c r="B29" s="45"/>
-      <c r="C29" s="45"/>
-      <c r="D29" s="45"/>
-      <c r="E29" s="45"/>
-      <c r="F29" s="45"/>
-      <c r="G29" s="45"/>
-      <c r="H29" s="45"/>
-      <c r="I29" s="45"/>
-      <c r="J29" s="45"/>
-      <c r="K29" s="45"/>
+      <c r="A29" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="B29" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="L29" s="9"/>
       <c r="M29" s="9"/>
       <c r="N29" s="9"/>
@@ -2082,27 +2005,13 @@
       <c r="S29" s="9"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="45" t="s">
-        <v>60</v>
-      </c>
-      <c r="B30" s="45" t="n">
-        <v>1</v>
-      </c>
-      <c r="C30" s="45" t="n">
-        <v>1</v>
-      </c>
-      <c r="D30" s="45"/>
-      <c r="E30" s="45"/>
-      <c r="F30" s="45" t="n">
-        <v>1</v>
-      </c>
-      <c r="G30" s="45"/>
-      <c r="H30" s="45"/>
-      <c r="I30" s="45" t="n">
-        <v>1</v>
-      </c>
-      <c r="J30" s="45"/>
-      <c r="K30" s="45" t="n">
+      <c r="A30" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="B30" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F30" s="0" t="n">
         <v>1</v>
       </c>
       <c r="L30" s="9"/>
@@ -2115,19 +2024,12 @@
       <c r="S30" s="9"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="45" t="s">
-        <v>94</v>
-      </c>
-      <c r="B31" s="45"/>
-      <c r="C31" s="45"/>
-      <c r="D31" s="45"/>
-      <c r="E31" s="45"/>
-      <c r="F31" s="45"/>
-      <c r="G31" s="45"/>
-      <c r="H31" s="45"/>
-      <c r="I31" s="45"/>
-      <c r="J31" s="45"/>
-      <c r="K31" s="45"/>
+      <c r="A31" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="B31" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="L31" s="9"/>
       <c r="M31" s="9"/>
       <c r="N31" s="9"/>
@@ -2138,19 +2040,12 @@
       <c r="S31" s="9"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="45" t="s">
-        <v>95</v>
-      </c>
-      <c r="B32" s="45"/>
-      <c r="C32" s="45"/>
-      <c r="D32" s="45"/>
-      <c r="E32" s="45"/>
-      <c r="F32" s="45"/>
-      <c r="G32" s="45"/>
-      <c r="H32" s="45"/>
-      <c r="I32" s="45"/>
-      <c r="J32" s="45"/>
-      <c r="K32" s="45"/>
+      <c r="A32" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="B32" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="L32" s="9"/>
       <c r="M32" s="9"/>
       <c r="N32" s="9"/>
@@ -2161,19 +2056,15 @@
       <c r="S32" s="9"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="45" t="s">
-        <v>96</v>
-      </c>
-      <c r="B33" s="45"/>
-      <c r="C33" s="45"/>
-      <c r="D33" s="45"/>
-      <c r="E33" s="45"/>
-      <c r="F33" s="45"/>
-      <c r="G33" s="45"/>
-      <c r="H33" s="45"/>
-      <c r="I33" s="45"/>
-      <c r="J33" s="45"/>
-      <c r="K33" s="45"/>
+      <c r="A33" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="B33" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F33" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="L33" s="9"/>
       <c r="M33" s="9"/>
       <c r="N33" s="9"/>
@@ -2183,174 +2074,219 @@
       <c r="R33" s="9"/>
       <c r="S33" s="9"/>
     </row>
-    <row r="35" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="50" t="s">
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="B34" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="L34" s="9"/>
+      <c r="M34" s="9"/>
+      <c r="N34" s="9"/>
+      <c r="O34" s="9"/>
+      <c r="P34" s="9"/>
+      <c r="Q34" s="9"/>
+      <c r="R34" s="9"/>
+      <c r="S34" s="9"/>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="B35" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F35" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="L35" s="9"/>
+      <c r="M35" s="9"/>
+      <c r="N35" s="9"/>
+      <c r="O35" s="9"/>
+      <c r="P35" s="9"/>
+      <c r="Q35" s="9"/>
+      <c r="R35" s="9"/>
+      <c r="S35" s="9"/>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L36" s="9"/>
+      <c r="M36" s="9"/>
+      <c r="N36" s="9"/>
+      <c r="O36" s="9"/>
+      <c r="P36" s="9"/>
+      <c r="Q36" s="9"/>
+      <c r="R36" s="9"/>
+      <c r="S36" s="9"/>
+    </row>
+    <row r="37" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="48" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="51" t="s">
+    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="49" t="s">
         <v>98</v>
       </c>
-      <c r="B36" s="51" t="s">
+      <c r="B38" s="49" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="52" t="n">
-        <v>1</v>
-      </c>
-      <c r="B37" s="53" t="s">
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="50" t="n">
+        <v>1</v>
+      </c>
+      <c r="B39" s="51" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="52" t="n">
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="50" t="n">
         <v>3</v>
       </c>
-      <c r="B38" s="53" t="s">
+      <c r="B40" s="51" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="52" t="n">
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="50" t="n">
         <v>2</v>
       </c>
-      <c r="B39" s="53" t="s">
+      <c r="B41" s="51" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="52" t="n">
-        <v>1</v>
-      </c>
-      <c r="B40" s="53" t="s">
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="50" t="n">
+        <v>1</v>
+      </c>
+      <c r="B42" s="51" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="54" t="s">
+    <row r="45" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="52" t="s">
         <v>104</v>
       </c>
-      <c r="B43" s="51" t="s">
+      <c r="B45" s="49" t="s">
         <v>43</v>
       </c>
-      <c r="C43" s="51" t="s">
+      <c r="C45" s="49" t="s">
         <v>56</v>
       </c>
-      <c r="D43" s="51" t="s">
+      <c r="D45" s="49" t="s">
         <v>50</v>
       </c>
-      <c r="E43" s="51" t="s">
+      <c r="E45" s="49" t="s">
         <v>68</v>
       </c>
-      <c r="F43" s="51" t="s">
+      <c r="F45" s="49" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="23.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A44" s="45" t="s">
+    <row r="46" customFormat="false" ht="23.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A46" s="45" t="s">
         <v>41</v>
       </c>
-      <c r="B44" s="55"/>
-      <c r="C44" s="56" t="s">
+      <c r="B46" s="53"/>
+      <c r="C46" s="54" t="s">
         <v>105</v>
       </c>
-      <c r="D44" s="56" t="s">
+      <c r="D46" s="54" t="s">
         <v>105</v>
       </c>
-      <c r="E44" s="56" t="s">
+      <c r="E46" s="54" t="s">
         <v>105</v>
       </c>
-      <c r="F44" s="56" t="s">
+      <c r="F46" s="54" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="23.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A45" s="45" t="s">
-        <v>91</v>
-      </c>
-      <c r="B45" s="55"/>
-      <c r="C45" s="56"/>
-      <c r="D45" s="56"/>
-      <c r="E45" s="56"/>
-      <c r="F45" s="56"/>
-    </row>
-    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="45" t="s">
-        <v>92</v>
-      </c>
-      <c r="B46" s="55"/>
-      <c r="C46" s="55"/>
-      <c r="D46" s="55"/>
-      <c r="E46" s="55"/>
-      <c r="F46" s="55"/>
-    </row>
-    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="23.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="45" t="s">
-        <v>93</v>
-      </c>
-      <c r="B47" s="55"/>
-      <c r="C47" s="55"/>
-      <c r="D47" s="55"/>
-      <c r="E47" s="55"/>
-      <c r="F47" s="55"/>
-    </row>
-    <row r="48" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="57" t="s">
-        <v>60</v>
-      </c>
-      <c r="B48" s="56" t="s">
-        <v>106</v>
-      </c>
-      <c r="C48" s="55"/>
-      <c r="D48" s="55"/>
-      <c r="E48" s="55"/>
-      <c r="F48" s="55"/>
+        <v>81</v>
+      </c>
+      <c r="B47" s="53"/>
+      <c r="C47" s="54"/>
+      <c r="D47" s="54"/>
+      <c r="E47" s="54"/>
+      <c r="F47" s="54"/>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="45" t="s">
+        <v>82</v>
+      </c>
+      <c r="B48" s="53"/>
+      <c r="C48" s="53"/>
+      <c r="D48" s="53"/>
+      <c r="E48" s="53"/>
+      <c r="F48" s="53"/>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="45" t="s">
-        <v>94</v>
-      </c>
-      <c r="B49" s="56"/>
-      <c r="C49" s="55"/>
-      <c r="D49" s="55"/>
-      <c r="E49" s="55"/>
-      <c r="F49" s="55"/>
-    </row>
-    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="45" t="s">
-        <v>95</v>
-      </c>
-      <c r="B50" s="55"/>
-      <c r="C50" s="55"/>
-      <c r="D50" s="55"/>
-      <c r="E50" s="55"/>
-      <c r="F50" s="55"/>
+        <v>83</v>
+      </c>
+      <c r="B49" s="53"/>
+      <c r="C49" s="53"/>
+      <c r="D49" s="53"/>
+      <c r="E49" s="53"/>
+      <c r="F49" s="53"/>
+    </row>
+    <row r="50" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="55" t="s">
+        <v>60</v>
+      </c>
+      <c r="B50" s="54" t="s">
+        <v>106</v>
+      </c>
+      <c r="C50" s="53"/>
+      <c r="D50" s="53"/>
+      <c r="E50" s="53"/>
+      <c r="F50" s="53"/>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="45" t="s">
-        <v>96</v>
-      </c>
-      <c r="B51" s="55"/>
-      <c r="C51" s="55"/>
-      <c r="D51" s="55"/>
-      <c r="E51" s="55"/>
-      <c r="F51" s="55"/>
+        <v>84</v>
+      </c>
+      <c r="B51" s="54"/>
+      <c r="C51" s="53"/>
+      <c r="D51" s="53"/>
+      <c r="E51" s="53"/>
+      <c r="F51" s="53"/>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="45" t="s">
+        <v>85</v>
+      </c>
+      <c r="B52" s="53"/>
+      <c r="C52" s="53"/>
+      <c r="D52" s="53"/>
+      <c r="E52" s="53"/>
+      <c r="F52" s="53"/>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="58" t="s">
+      <c r="A53" s="45" t="s">
+        <v>86</v>
+      </c>
+      <c r="B53" s="53"/>
+      <c r="C53" s="53"/>
+      <c r="D53" s="53"/>
+      <c r="E53" s="53"/>
+      <c r="F53" s="53"/>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="56" t="s">
         <v>107</v>
       </c>
-      <c r="B53" s="55" t="s">
+      <c r="B55" s="53" t="s">
         <v>108</v>
       </c>
-      <c r="C53" s="55"/>
-      <c r="D53" s="55"/>
-      <c r="E53" s="55" t="s">
+      <c r="C55" s="53"/>
+      <c r="D55" s="53"/>
+      <c r="E55" s="53" t="s">
         <v>108</v>
       </c>
-      <c r="F53" s="55"/>
+      <c r="F55" s="53"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -2383,7 +2319,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="1" sqref="B4:F9 E1"/>
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -2396,197 +2332,197 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="59" t="s">
+      <c r="A1" s="57" t="s">
         <v>109</v>
       </c>
-      <c r="B1" s="59" t="s">
+      <c r="B1" s="57" t="s">
         <v>110</v>
       </c>
-      <c r="C1" s="59" t="s">
+      <c r="C1" s="57" t="s">
         <v>111</v>
       </c>
-      <c r="D1" s="59" t="s">
+      <c r="D1" s="57" t="s">
         <v>112</v>
       </c>
-      <c r="E1" s="59" t="s">
+      <c r="E1" s="57" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="60" t="s">
+      <c r="A2" s="58" t="s">
         <v>77</v>
       </c>
-      <c r="B2" s="60" t="s">
+      <c r="B2" s="58" t="s">
         <v>114</v>
       </c>
-      <c r="C2" s="61" t="s">
+      <c r="C2" s="59" t="s">
         <v>115</v>
       </c>
-      <c r="D2" s="61"/>
-      <c r="E2" s="60" t="s">
+      <c r="D2" s="59"/>
+      <c r="E2" s="58" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="60" t="s">
+      <c r="A3" s="58" t="s">
         <v>117</v>
       </c>
-      <c r="B3" s="60" t="s">
+      <c r="B3" s="58" t="s">
         <v>118</v>
       </c>
-      <c r="C3" s="60"/>
-      <c r="D3" s="60"/>
-      <c r="E3" s="61" t="s">
+      <c r="C3" s="58"/>
+      <c r="D3" s="58"/>
+      <c r="E3" s="59" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="60" t="s">
+      <c r="A4" s="58" t="s">
         <v>120</v>
       </c>
-      <c r="B4" s="60" t="s">
+      <c r="B4" s="58" t="s">
         <v>121</v>
       </c>
-      <c r="C4" s="60" t="s">
+      <c r="C4" s="58" t="s">
         <v>122</v>
       </c>
-      <c r="D4" s="60"/>
-      <c r="E4" s="60" t="s">
+      <c r="D4" s="58"/>
+      <c r="E4" s="58" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="60" t="s">
+      <c r="A5" s="58" t="s">
         <v>124</v>
       </c>
-      <c r="B5" s="60" t="s">
+      <c r="B5" s="58" t="s">
         <v>125</v>
       </c>
-      <c r="C5" s="60" t="s">
+      <c r="C5" s="58" t="s">
         <v>126</v>
       </c>
-      <c r="D5" s="60"/>
-      <c r="E5" s="60" t="s">
+      <c r="D5" s="58"/>
+      <c r="E5" s="58" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="60" t="s">
+      <c r="A6" s="58" t="s">
         <v>128</v>
       </c>
-      <c r="B6" s="60" t="s">
+      <c r="B6" s="58" t="s">
         <v>129</v>
       </c>
-      <c r="C6" s="60" t="s">
+      <c r="C6" s="58" t="s">
         <v>130</v>
       </c>
-      <c r="D6" s="60" t="s">
+      <c r="D6" s="58" t="s">
         <v>131</v>
       </c>
-      <c r="E6" s="61" t="s">
+      <c r="E6" s="59" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="60" t="s">
+      <c r="A7" s="58" t="s">
         <v>133</v>
       </c>
-      <c r="B7" s="60" t="s">
+      <c r="B7" s="58" t="s">
         <v>134</v>
       </c>
-      <c r="C7" s="61" t="s">
+      <c r="C7" s="59" t="s">
         <v>135</v>
       </c>
-      <c r="D7" s="61"/>
-      <c r="E7" s="60" t="s">
+      <c r="D7" s="59"/>
+      <c r="E7" s="58" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="60" t="s">
+      <c r="A8" s="58" t="s">
         <v>137</v>
       </c>
-      <c r="B8" s="60" t="s">
+      <c r="B8" s="58" t="s">
         <v>138</v>
       </c>
-      <c r="C8" s="61"/>
-      <c r="D8" s="61" t="s">
+      <c r="C8" s="59"/>
+      <c r="D8" s="59" t="s">
         <v>139</v>
       </c>
-      <c r="E8" s="60" t="s">
+      <c r="E8" s="58" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="60" t="s">
+      <c r="A9" s="58" t="s">
         <v>140</v>
       </c>
-      <c r="B9" s="60" t="s">
+      <c r="B9" s="58" t="s">
         <v>141</v>
       </c>
-      <c r="C9" s="60"/>
-      <c r="D9" s="60"/>
-      <c r="E9" s="60" t="s">
+      <c r="C9" s="58"/>
+      <c r="D9" s="58"/>
+      <c r="E9" s="58" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="60" t="s">
+      <c r="A10" s="58" t="s">
         <v>143</v>
       </c>
-      <c r="B10" s="60" t="s">
+      <c r="B10" s="58" t="s">
         <v>144</v>
       </c>
-      <c r="C10" s="60" t="s">
+      <c r="C10" s="58" t="s">
         <v>145</v>
       </c>
-      <c r="D10" s="60"/>
-      <c r="E10" s="61" t="s">
+      <c r="D10" s="58"/>
+      <c r="E10" s="59" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="60" t="s">
+      <c r="A11" s="58" t="s">
         <v>147</v>
       </c>
-      <c r="B11" s="60" t="s">
+      <c r="B11" s="58" t="s">
         <v>148</v>
       </c>
-      <c r="C11" s="60" t="s">
+      <c r="C11" s="58" t="s">
         <v>149</v>
       </c>
-      <c r="D11" s="60"/>
-      <c r="E11" s="61" t="s">
+      <c r="D11" s="58"/>
+      <c r="E11" s="59" t="s">
         <v>150</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="60" t="s">
+      <c r="A12" s="58" t="s">
         <v>68</v>
       </c>
-      <c r="B12" s="60" t="s">
+      <c r="B12" s="58" t="s">
         <v>151</v>
       </c>
-      <c r="C12" s="60" t="s">
+      <c r="C12" s="58" t="s">
         <v>152</v>
       </c>
-      <c r="D12" s="60"/>
-      <c r="E12" s="61" t="s">
+      <c r="D12" s="58"/>
+      <c r="E12" s="59" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="60" t="s">
+      <c r="A13" s="58" t="s">
         <v>154</v>
       </c>
-      <c r="B13" s="61" t="s">
+      <c r="B13" s="59" t="s">
         <v>155</v>
       </c>
-      <c r="C13" s="60" t="s">
+      <c r="C13" s="58" t="s">
         <v>156</v>
       </c>
-      <c r="D13" s="60"/>
-      <c r="E13" s="61" t="s">
+      <c r="D13" s="58"/>
+      <c r="E13" s="59" t="s">
         <v>157</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Se ajusta planilla para generar intervalos entre cuadros sin vacio
</commit_message>
<xml_diff>
--- a/Oficial/Patron_FL.xlsx
+++ b/Oficial/Patron_FL.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="628" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="430" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="BASE_SSE" sheetId="1" state="visible" r:id="rId2"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="170">
   <si>
     <t>SOLICITUD  DE SERVICIO EXTERNO A LABORATORIO</t>
   </si>
@@ -367,10 +367,13 @@
     <t>Se solicita debido a que entrega es mas rapida</t>
   </si>
   <si>
-    <t>Agregar laboratorios y escribir en cada celda, si o no, si adjunta algún documento en particular</t>
-  </si>
-  <si>
-    <t>ADJUNTA </t>
+    <t>Cuadro 5</t>
+  </si>
+  <si>
+    <t>Agregar todos los laboratorios involucrados y escribir en cada celda, solo 'si', si adjunta algún documento en particular</t>
+  </si>
+  <si>
+    <t>ADJUNTA</t>
   </si>
   <si>
     <t>(si/no)</t>
@@ -544,7 +547,7 @@
     <numFmt numFmtId="165" formatCode="DD/MM/YYYY"/>
     <numFmt numFmtId="166" formatCode="0.00"/>
   </numFmts>
-  <fonts count="16">
+  <fonts count="17">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -600,6 +603,13 @@
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="1"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="16"/>
+      <name val="Arial"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
@@ -827,7 +837,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="63">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -896,20 +906,16 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="9" fillId="2" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="2" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="10" fillId="2" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="2" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="2" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -1028,11 +1034,11 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="7" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="7" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="7" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="7" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1040,15 +1046,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="2" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="2" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1072,15 +1078,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="15" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1161,15 +1167,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>496440</xdr:colOff>
+      <xdr:colOff>523440</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>7560</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1057680</xdr:colOff>
+      <xdr:colOff>1084320</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>776520</xdr:rowOff>
+      <xdr:rowOff>776160</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1182,8 +1188,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="496440" y="7560"/>
-          <a:ext cx="561240" cy="768960"/>
+          <a:off x="523440" y="7560"/>
+          <a:ext cx="560880" cy="768600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1203,10 +1209,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:S72"/>
+  <dimension ref="A1:S71"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A43" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B65" activeCellId="0" sqref="B65"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A52" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B64" activeCellId="0" sqref="B64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1417,27 +1423,6 @@
       <c r="R9" s="9"/>
       <c r="S9" s="9"/>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="15"/>
-      <c r="B10" s="13"/>
-      <c r="C10" s="16"/>
-      <c r="D10" s="16"/>
-      <c r="E10" s="16"/>
-      <c r="F10" s="16"/>
-      <c r="G10" s="16"/>
-      <c r="H10" s="16"/>
-      <c r="I10" s="16"/>
-      <c r="J10" s="16"/>
-      <c r="K10" s="16"/>
-      <c r="L10" s="9"/>
-      <c r="M10" s="9"/>
-      <c r="N10" s="9"/>
-      <c r="O10" s="9"/>
-      <c r="P10" s="9"/>
-      <c r="Q10" s="9"/>
-      <c r="R10" s="9"/>
-      <c r="S10" s="9"/>
-    </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="17" t="s">
         <v>15</v>
@@ -1486,623 +1471,603 @@
       <c r="R12" s="9"/>
       <c r="S12" s="9"/>
     </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="20"/>
-      <c r="C13" s="16"/>
-      <c r="D13" s="16"/>
-      <c r="E13" s="16"/>
-      <c r="F13" s="16"/>
-      <c r="G13" s="16"/>
-      <c r="H13" s="16"/>
-      <c r="I13" s="16"/>
-      <c r="J13" s="16"/>
-      <c r="K13" s="16"/>
-      <c r="L13" s="9"/>
-      <c r="M13" s="9"/>
-      <c r="N13" s="9"/>
-      <c r="O13" s="9"/>
-      <c r="P13" s="9"/>
-      <c r="Q13" s="9"/>
-      <c r="R13" s="9"/>
-      <c r="S13" s="9"/>
-    </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="21" t="s">
+      <c r="A14" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="B14" s="21"/>
-      <c r="C14" s="21"/>
-      <c r="D14" s="21"/>
-      <c r="E14" s="21"/>
-      <c r="F14" s="21"/>
-      <c r="G14" s="22" t="s">
+      <c r="B14" s="20"/>
+      <c r="C14" s="20"/>
+      <c r="D14" s="20"/>
+      <c r="E14" s="20"/>
+      <c r="F14" s="20"/>
+      <c r="G14" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="H14" s="22"/>
-      <c r="I14" s="22"/>
-      <c r="J14" s="22"/>
-      <c r="K14" s="22"/>
-      <c r="L14" s="23"/>
-      <c r="M14" s="24" t="s">
+      <c r="H14" s="21"/>
+      <c r="I14" s="21"/>
+      <c r="J14" s="21"/>
+      <c r="K14" s="21"/>
+      <c r="L14" s="22"/>
+      <c r="M14" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="N14" s="24"/>
-      <c r="O14" s="24"/>
-      <c r="P14" s="24"/>
-      <c r="Q14" s="24"/>
-      <c r="R14" s="25" t="s">
+      <c r="N14" s="23"/>
+      <c r="O14" s="23"/>
+      <c r="P14" s="23"/>
+      <c r="Q14" s="23"/>
+      <c r="R14" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="S14" s="25"/>
+      <c r="S14" s="24"/>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="26" t="s">
+      <c r="A15" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="B15" s="21"/>
-      <c r="C15" s="27"/>
-      <c r="D15" s="27"/>
-      <c r="E15" s="27"/>
-      <c r="F15" s="27"/>
-      <c r="G15" s="28" t="s">
+      <c r="B15" s="20"/>
+      <c r="C15" s="26"/>
+      <c r="D15" s="26"/>
+      <c r="E15" s="26"/>
+      <c r="F15" s="26"/>
+      <c r="G15" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="H15" s="28"/>
-      <c r="I15" s="28"/>
-      <c r="J15" s="29"/>
-      <c r="K15" s="30"/>
-      <c r="L15" s="30"/>
-      <c r="M15" s="31" t="s">
+      <c r="H15" s="27"/>
+      <c r="I15" s="27"/>
+      <c r="J15" s="28"/>
+      <c r="K15" s="29"/>
+      <c r="L15" s="29"/>
+      <c r="M15" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="N15" s="32"/>
-      <c r="O15" s="33"/>
-      <c r="P15" s="33"/>
-      <c r="Q15" s="34"/>
-      <c r="R15" s="35" t="s">
+      <c r="N15" s="31"/>
+      <c r="O15" s="32"/>
+      <c r="P15" s="32"/>
+      <c r="Q15" s="33"/>
+      <c r="R15" s="34" t="s">
         <v>22</v>
       </c>
-      <c r="S15" s="36"/>
+      <c r="S15" s="35"/>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="26" t="s">
+      <c r="A16" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="21"/>
-      <c r="C16" s="27"/>
-      <c r="D16" s="27"/>
-      <c r="E16" s="27"/>
-      <c r="F16" s="27"/>
-      <c r="G16" s="28" t="s">
+      <c r="B16" s="20"/>
+      <c r="C16" s="26"/>
+      <c r="D16" s="26"/>
+      <c r="E16" s="26"/>
+      <c r="F16" s="26"/>
+      <c r="G16" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="H16" s="28"/>
-      <c r="I16" s="28"/>
-      <c r="J16" s="29"/>
-      <c r="K16" s="30"/>
-      <c r="L16" s="30"/>
-      <c r="M16" s="31" t="s">
+      <c r="H16" s="27"/>
+      <c r="I16" s="27"/>
+      <c r="J16" s="28"/>
+      <c r="K16" s="29"/>
+      <c r="L16" s="29"/>
+      <c r="M16" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="N16" s="32"/>
-      <c r="O16" s="37"/>
-      <c r="P16" s="37"/>
-      <c r="Q16" s="38"/>
-      <c r="R16" s="35" t="s">
+      <c r="N16" s="31"/>
+      <c r="O16" s="36"/>
+      <c r="P16" s="36"/>
+      <c r="Q16" s="37"/>
+      <c r="R16" s="34" t="s">
         <v>23</v>
       </c>
-      <c r="S16" s="25"/>
+      <c r="S16" s="24"/>
     </row>
     <row r="17" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="39" t="s">
+      <c r="A17" s="38" t="s">
         <v>24</v>
       </c>
-      <c r="B17" s="39" t="s">
+      <c r="B17" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="C17" s="39" t="s">
+      <c r="C17" s="38" t="s">
         <v>26</v>
       </c>
-      <c r="D17" s="39" t="s">
+      <c r="D17" s="38" t="s">
         <v>27</v>
       </c>
-      <c r="E17" s="39" t="s">
+      <c r="E17" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="F17" s="39" t="s">
+      <c r="F17" s="38" t="s">
         <v>29</v>
       </c>
-      <c r="G17" s="40" t="s">
+      <c r="G17" s="39" t="s">
         <v>30</v>
       </c>
-      <c r="H17" s="40" t="s">
+      <c r="H17" s="39" t="s">
         <v>31</v>
       </c>
-      <c r="I17" s="40" t="s">
+      <c r="I17" s="39" t="s">
         <v>32</v>
       </c>
-      <c r="J17" s="40" t="s">
+      <c r="J17" s="39" t="s">
         <v>33</v>
       </c>
-      <c r="K17" s="40" t="s">
+      <c r="K17" s="39" t="s">
         <v>34</v>
       </c>
-      <c r="L17" s="41" t="s">
+      <c r="L17" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="M17" s="42" t="s">
+      <c r="M17" s="41" t="s">
         <v>36</v>
       </c>
-      <c r="N17" s="42" t="s">
+      <c r="N17" s="41" t="s">
         <v>37</v>
       </c>
-      <c r="O17" s="43" t="s">
+      <c r="O17" s="42" t="s">
         <v>38</v>
       </c>
-      <c r="P17" s="43" t="s">
+      <c r="P17" s="42" t="s">
         <v>39</v>
       </c>
-      <c r="Q17" s="43" t="s">
+      <c r="Q17" s="42" t="s">
         <v>40</v>
       </c>
-      <c r="R17" s="44" t="s">
+      <c r="R17" s="43" t="s">
         <v>41</v>
       </c>
-      <c r="S17" s="45" t="s">
+      <c r="S17" s="44" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="46" t="n">
+      <c r="A18" s="45" t="n">
         <v>10</v>
       </c>
-      <c r="B18" s="47" t="s">
+      <c r="B18" s="46" t="s">
         <v>43</v>
       </c>
-      <c r="C18" s="46" t="n">
+      <c r="C18" s="45" t="n">
         <v>1</v>
       </c>
-      <c r="D18" s="48" t="s">
+      <c r="D18" s="47" t="s">
         <v>44</v>
       </c>
-      <c r="E18" s="46" t="s">
+      <c r="E18" s="45" t="s">
         <v>45</v>
       </c>
-      <c r="F18" s="46" t="n">
+      <c r="F18" s="45" t="n">
         <v>0</v>
       </c>
-      <c r="G18" s="46" t="s">
+      <c r="G18" s="45" t="s">
         <v>46</v>
       </c>
-      <c r="H18" s="46" t="s">
+      <c r="H18" s="45" t="s">
         <v>47</v>
       </c>
-      <c r="I18" s="46" t="s">
+      <c r="I18" s="45" t="s">
         <v>48</v>
       </c>
-      <c r="J18" s="46" t="s">
+      <c r="J18" s="45" t="s">
         <v>49</v>
       </c>
-      <c r="K18" s="46" t="n">
+      <c r="K18" s="45" t="n">
         <v>0.35</v>
       </c>
-      <c r="L18" s="46" t="s">
+      <c r="L18" s="45" t="s">
         <v>50</v>
       </c>
-      <c r="M18" s="47"/>
-      <c r="N18" s="47"/>
-      <c r="O18" s="47"/>
-      <c r="P18" s="47"/>
-      <c r="Q18" s="47"/>
-      <c r="R18" s="47"/>
-      <c r="S18" s="47"/>
+      <c r="M18" s="46"/>
+      <c r="N18" s="46"/>
+      <c r="O18" s="46"/>
+      <c r="P18" s="46"/>
+      <c r="Q18" s="46"/>
+      <c r="R18" s="46"/>
+      <c r="S18" s="46"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="46" t="n">
+      <c r="A19" s="45" t="n">
         <v>10</v>
       </c>
-      <c r="B19" s="47" t="s">
+      <c r="B19" s="46" t="s">
         <v>51</v>
       </c>
-      <c r="C19" s="46" t="n">
+      <c r="C19" s="45" t="n">
         <v>1</v>
       </c>
-      <c r="D19" s="48" t="s">
+      <c r="D19" s="47" t="s">
         <v>44</v>
       </c>
-      <c r="E19" s="46" t="s">
+      <c r="E19" s="45" t="s">
         <v>45</v>
       </c>
-      <c r="F19" s="46" t="s">
+      <c r="F19" s="45" t="s">
         <v>52</v>
       </c>
-      <c r="G19" s="46" t="s">
+      <c r="G19" s="45" t="s">
         <v>53</v>
       </c>
-      <c r="H19" s="46" t="s">
+      <c r="H19" s="45" t="s">
         <v>47</v>
       </c>
-      <c r="I19" s="46" t="s">
+      <c r="I19" s="45" t="s">
         <v>48</v>
       </c>
-      <c r="J19" s="46" t="n">
+      <c r="J19" s="45" t="n">
         <v>600</v>
       </c>
-      <c r="K19" s="46" t="n">
+      <c r="K19" s="45" t="n">
         <v>20</v>
       </c>
-      <c r="L19" s="46" t="s">
+      <c r="L19" s="45" t="s">
         <v>54</v>
       </c>
-      <c r="M19" s="47"/>
-      <c r="N19" s="47"/>
-      <c r="O19" s="47"/>
-      <c r="P19" s="47"/>
-      <c r="Q19" s="47"/>
-      <c r="R19" s="47"/>
-      <c r="S19" s="47"/>
+      <c r="M19" s="46"/>
+      <c r="N19" s="46"/>
+      <c r="O19" s="46"/>
+      <c r="P19" s="46"/>
+      <c r="Q19" s="46"/>
+      <c r="R19" s="46"/>
+      <c r="S19" s="46"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="46" t="n">
+      <c r="A20" s="45" t="n">
         <v>10</v>
       </c>
-      <c r="B20" s="47" t="s">
+      <c r="B20" s="46" t="s">
         <v>55</v>
       </c>
-      <c r="C20" s="46" t="n">
+      <c r="C20" s="45" t="n">
         <v>1</v>
       </c>
-      <c r="D20" s="48" t="s">
+      <c r="D20" s="47" t="s">
         <v>44</v>
       </c>
-      <c r="E20" s="46" t="s">
+      <c r="E20" s="45" t="s">
         <v>45</v>
       </c>
-      <c r="F20" s="46" t="s">
+      <c r="F20" s="45" t="s">
         <v>56</v>
       </c>
-      <c r="G20" s="46" t="s">
+      <c r="G20" s="45" t="s">
         <v>46</v>
       </c>
-      <c r="H20" s="46" t="s">
+      <c r="H20" s="45" t="s">
         <v>47</v>
       </c>
-      <c r="I20" s="46" t="s">
+      <c r="I20" s="45" t="s">
         <v>48</v>
       </c>
-      <c r="J20" s="46" t="s">
+      <c r="J20" s="45" t="s">
         <v>49</v>
       </c>
-      <c r="K20" s="46" t="n">
+      <c r="K20" s="45" t="n">
         <v>0.15</v>
       </c>
-      <c r="L20" s="46" t="s">
+      <c r="L20" s="45" t="s">
         <v>50</v>
       </c>
-      <c r="M20" s="47"/>
-      <c r="N20" s="47"/>
-      <c r="O20" s="47"/>
-      <c r="P20" s="47"/>
-      <c r="Q20" s="47"/>
-      <c r="R20" s="47"/>
-      <c r="S20" s="47"/>
+      <c r="M20" s="46"/>
+      <c r="N20" s="46"/>
+      <c r="O20" s="46"/>
+      <c r="P20" s="46"/>
+      <c r="Q20" s="46"/>
+      <c r="R20" s="46"/>
+      <c r="S20" s="46"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="46" t="n">
+      <c r="A21" s="45" t="n">
         <v>10</v>
       </c>
-      <c r="B21" s="47" t="s">
+      <c r="B21" s="46" t="s">
         <v>57</v>
       </c>
-      <c r="C21" s="46" t="n">
+      <c r="C21" s="45" t="n">
         <v>1</v>
       </c>
-      <c r="D21" s="48" t="s">
+      <c r="D21" s="47" t="s">
         <v>44</v>
       </c>
-      <c r="E21" s="46" t="s">
+      <c r="E21" s="45" t="s">
         <v>45</v>
       </c>
-      <c r="F21" s="46" t="s">
+      <c r="F21" s="45" t="s">
         <v>58</v>
       </c>
-      <c r="G21" s="46" t="s">
+      <c r="G21" s="45" t="s">
         <v>59</v>
       </c>
-      <c r="H21" s="46" t="s">
+      <c r="H21" s="45" t="s">
         <v>60</v>
       </c>
-      <c r="I21" s="46" t="s">
+      <c r="I21" s="45" t="s">
         <v>61</v>
       </c>
-      <c r="J21" s="46" t="n">
+      <c r="J21" s="45" t="n">
         <v>42</v>
       </c>
-      <c r="K21" s="46" t="n">
+      <c r="K21" s="45" t="n">
         <v>0.42</v>
       </c>
-      <c r="L21" s="46" t="s">
+      <c r="L21" s="45" t="s">
         <v>50</v>
       </c>
-      <c r="M21" s="47"/>
-      <c r="N21" s="47"/>
-      <c r="O21" s="47"/>
-      <c r="P21" s="47"/>
-      <c r="Q21" s="47"/>
-      <c r="R21" s="47"/>
-      <c r="S21" s="47"/>
+      <c r="M21" s="46"/>
+      <c r="N21" s="46"/>
+      <c r="O21" s="46"/>
+      <c r="P21" s="46"/>
+      <c r="Q21" s="46"/>
+      <c r="R21" s="46"/>
+      <c r="S21" s="46"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="46" t="n">
+      <c r="A22" s="45" t="n">
         <v>3</v>
       </c>
-      <c r="B22" s="47" t="s">
+      <c r="B22" s="46" t="s">
         <v>62</v>
       </c>
-      <c r="C22" s="46" t="n">
+      <c r="C22" s="45" t="n">
         <v>1</v>
       </c>
-      <c r="D22" s="48" t="s">
+      <c r="D22" s="47" t="s">
         <v>63</v>
       </c>
-      <c r="E22" s="46" t="s">
+      <c r="E22" s="45" t="s">
         <v>45</v>
       </c>
-      <c r="F22" s="46" t="s">
+      <c r="F22" s="45" t="s">
         <v>64</v>
       </c>
-      <c r="G22" s="46" t="s">
+      <c r="G22" s="45" t="s">
         <v>46</v>
       </c>
-      <c r="H22" s="46" t="s">
+      <c r="H22" s="45" t="s">
         <v>65</v>
       </c>
-      <c r="I22" s="46" t="s">
+      <c r="I22" s="45" t="s">
         <v>66</v>
       </c>
-      <c r="J22" s="46" t="n">
+      <c r="J22" s="45" t="n">
         <v>42</v>
       </c>
-      <c r="K22" s="46" t="n">
+      <c r="K22" s="45" t="n">
         <v>0.2</v>
       </c>
-      <c r="L22" s="46" t="s">
+      <c r="L22" s="45" t="s">
         <v>50</v>
       </c>
-      <c r="M22" s="47"/>
-      <c r="N22" s="47"/>
-      <c r="O22" s="47"/>
-      <c r="P22" s="47"/>
-      <c r="Q22" s="47"/>
-      <c r="R22" s="47"/>
-      <c r="S22" s="47"/>
+      <c r="M22" s="46"/>
+      <c r="N22" s="46"/>
+      <c r="O22" s="46"/>
+      <c r="P22" s="46"/>
+      <c r="Q22" s="46"/>
+      <c r="R22" s="46"/>
+      <c r="S22" s="46"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="46" t="n">
+      <c r="A23" s="45" t="n">
         <v>3</v>
       </c>
-      <c r="B23" s="47" t="s">
+      <c r="B23" s="46" t="s">
         <v>67</v>
       </c>
-      <c r="C23" s="46" t="n">
+      <c r="C23" s="45" t="n">
         <v>1</v>
       </c>
-      <c r="D23" s="48" t="s">
+      <c r="D23" s="47" t="s">
         <v>63</v>
       </c>
-      <c r="E23" s="46" t="s">
+      <c r="E23" s="45" t="s">
         <v>45</v>
       </c>
-      <c r="F23" s="46" t="s">
+      <c r="F23" s="45" t="s">
         <v>68</v>
       </c>
-      <c r="G23" s="46" t="s">
+      <c r="G23" s="45" t="s">
         <v>46</v>
       </c>
-      <c r="H23" s="46" t="s">
+      <c r="H23" s="45" t="s">
         <v>65</v>
       </c>
-      <c r="I23" s="46" t="s">
+      <c r="I23" s="45" t="s">
         <v>66</v>
       </c>
-      <c r="J23" s="46" t="n">
+      <c r="J23" s="45" t="n">
         <v>42</v>
       </c>
-      <c r="K23" s="46" t="n">
+      <c r="K23" s="45" t="n">
         <v>0.43</v>
       </c>
-      <c r="L23" s="46" t="s">
+      <c r="L23" s="45" t="s">
         <v>50</v>
       </c>
-      <c r="M23" s="47"/>
-      <c r="N23" s="47"/>
-      <c r="O23" s="47"/>
-      <c r="P23" s="47"/>
-      <c r="Q23" s="47"/>
-      <c r="R23" s="47"/>
-      <c r="S23" s="47"/>
+      <c r="M23" s="46"/>
+      <c r="N23" s="46"/>
+      <c r="O23" s="46"/>
+      <c r="P23" s="46"/>
+      <c r="Q23" s="46"/>
+      <c r="R23" s="46"/>
+      <c r="S23" s="46"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="46" t="n">
+      <c r="A24" s="45" t="n">
         <v>10</v>
       </c>
-      <c r="B24" s="47" t="s">
+      <c r="B24" s="46" t="s">
         <v>69</v>
       </c>
-      <c r="C24" s="46" t="n">
+      <c r="C24" s="45" t="n">
         <v>1</v>
       </c>
-      <c r="D24" s="48" t="s">
+      <c r="D24" s="47" t="s">
         <v>44</v>
       </c>
-      <c r="E24" s="46" t="s">
+      <c r="E24" s="45" t="s">
         <v>45</v>
       </c>
-      <c r="F24" s="46" t="s">
+      <c r="F24" s="45" t="s">
         <v>70</v>
       </c>
-      <c r="G24" s="46" t="s">
+      <c r="G24" s="45" t="s">
         <v>71</v>
       </c>
-      <c r="H24" s="46" t="s">
+      <c r="H24" s="45" t="s">
         <v>72</v>
       </c>
-      <c r="I24" s="46" t="s">
+      <c r="I24" s="45" t="s">
         <v>73</v>
       </c>
-      <c r="J24" s="46" t="n">
+      <c r="J24" s="45" t="n">
         <v>8962</v>
       </c>
-      <c r="K24" s="46" t="n">
+      <c r="K24" s="45" t="n">
         <v>21580</v>
       </c>
-      <c r="L24" s="46" t="s">
+      <c r="L24" s="45" t="s">
         <v>74</v>
       </c>
-      <c r="M24" s="47"/>
-      <c r="N24" s="47"/>
-      <c r="O24" s="47"/>
-      <c r="P24" s="47"/>
-      <c r="Q24" s="47"/>
-      <c r="R24" s="47"/>
-      <c r="S24" s="47"/>
+      <c r="M24" s="46"/>
+      <c r="N24" s="46"/>
+      <c r="O24" s="46"/>
+      <c r="P24" s="46"/>
+      <c r="Q24" s="46"/>
+      <c r="R24" s="46"/>
+      <c r="S24" s="46"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="46" t="n">
+      <c r="A25" s="45" t="n">
         <v>10</v>
       </c>
-      <c r="B25" s="49" t="s">
+      <c r="B25" s="48" t="s">
         <v>75</v>
       </c>
-      <c r="C25" s="46" t="n">
+      <c r="C25" s="45" t="n">
         <v>1</v>
       </c>
-      <c r="D25" s="48" t="s">
+      <c r="D25" s="47" t="s">
         <v>44</v>
       </c>
-      <c r="E25" s="46" t="s">
+      <c r="E25" s="45" t="s">
         <v>45</v>
       </c>
-      <c r="F25" s="46" t="s">
+      <c r="F25" s="45" t="s">
         <v>76</v>
       </c>
-      <c r="G25" s="46" t="s">
+      <c r="G25" s="45" t="s">
         <v>46</v>
       </c>
-      <c r="H25" s="47" t="s">
+      <c r="H25" s="46" t="s">
         <v>77</v>
       </c>
-      <c r="I25" s="46" t="s">
+      <c r="I25" s="45" t="s">
         <v>78</v>
       </c>
-      <c r="J25" s="46" t="s">
+      <c r="J25" s="45" t="s">
         <v>49</v>
       </c>
-      <c r="K25" s="46" t="n">
+      <c r="K25" s="45" t="n">
         <v>0.43</v>
       </c>
-      <c r="L25" s="46" t="s">
+      <c r="L25" s="45" t="s">
         <v>50</v>
       </c>
-      <c r="M25" s="47"/>
-      <c r="N25" s="47"/>
-      <c r="O25" s="47"/>
-      <c r="P25" s="47"/>
-      <c r="Q25" s="47"/>
-      <c r="R25" s="47"/>
-      <c r="S25" s="47"/>
+      <c r="M25" s="46"/>
+      <c r="N25" s="46"/>
+      <c r="O25" s="46"/>
+      <c r="P25" s="46"/>
+      <c r="Q25" s="46"/>
+      <c r="R25" s="46"/>
+      <c r="S25" s="46"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="46" t="n">
+      <c r="A26" s="45" t="n">
         <v>10</v>
       </c>
-      <c r="B26" s="49" t="s">
+      <c r="B26" s="48" t="s">
         <v>79</v>
       </c>
-      <c r="C26" s="46" t="n">
+      <c r="C26" s="45" t="n">
         <v>1</v>
       </c>
-      <c r="D26" s="48" t="s">
+      <c r="D26" s="47" t="s">
         <v>44</v>
       </c>
-      <c r="E26" s="46" t="s">
+      <c r="E26" s="45" t="s">
         <v>45</v>
       </c>
-      <c r="F26" s="47"/>
-      <c r="G26" s="46" t="s">
+      <c r="F26" s="46"/>
+      <c r="G26" s="45" t="s">
         <v>80</v>
       </c>
-      <c r="H26" s="46" t="s">
+      <c r="H26" s="45" t="s">
         <v>81</v>
       </c>
-      <c r="I26" s="46" t="s">
+      <c r="I26" s="45" t="s">
         <v>82</v>
       </c>
-      <c r="J26" s="46" t="n">
+      <c r="J26" s="45" t="n">
         <v>5632</v>
       </c>
-      <c r="K26" s="46" t="n">
+      <c r="K26" s="45" t="n">
         <v>9123</v>
       </c>
-      <c r="L26" s="46" t="s">
+      <c r="L26" s="45" t="s">
         <v>74</v>
       </c>
-      <c r="M26" s="47"/>
-      <c r="N26" s="47"/>
-      <c r="O26" s="47"/>
-      <c r="P26" s="47"/>
-      <c r="Q26" s="47"/>
-      <c r="R26" s="47"/>
-      <c r="S26" s="47"/>
+      <c r="M26" s="46"/>
+      <c r="N26" s="46"/>
+      <c r="O26" s="46"/>
+      <c r="P26" s="46"/>
+      <c r="Q26" s="46"/>
+      <c r="R26" s="46"/>
+      <c r="S26" s="46"/>
     </row>
     <row r="28" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="50" t="s">
+      <c r="A28" s="49" t="s">
         <v>83</v>
       </c>
-      <c r="B28" s="51" t="s">
+      <c r="B28" s="50" t="s">
         <v>84</v>
       </c>
-      <c r="C28" s="51"/>
-      <c r="D28" s="51"/>
-      <c r="E28" s="51"/>
-      <c r="F28" s="51"/>
+      <c r="C28" s="50"/>
+      <c r="D28" s="50"/>
+      <c r="E28" s="50"/>
+      <c r="F28" s="50"/>
     </row>
     <row r="29" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="50"/>
-      <c r="B29" s="51" t="s">
+      <c r="A29" s="49"/>
+      <c r="B29" s="50" t="s">
         <v>17</v>
       </c>
-      <c r="C29" s="51"/>
-      <c r="D29" s="51"/>
-      <c r="E29" s="51"/>
-      <c r="F29" s="51"/>
+      <c r="C29" s="50"/>
+      <c r="D29" s="50"/>
+      <c r="E29" s="50"/>
+      <c r="F29" s="50"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="52" t="s">
+      <c r="A31" s="51" t="s">
         <v>85</v>
       </c>
-      <c r="B31" s="52" t="s">
+      <c r="B31" s="51" t="s">
         <v>44</v>
       </c>
-      <c r="C31" s="52" t="s">
+      <c r="C31" s="51" t="s">
         <v>86</v>
       </c>
-      <c r="D31" s="52" t="s">
+      <c r="D31" s="51" t="s">
         <v>87</v>
       </c>
-      <c r="E31" s="52" t="s">
+      <c r="E31" s="51" t="s">
         <v>88</v>
       </c>
-      <c r="F31" s="52" t="s">
+      <c r="F31" s="51" t="s">
         <v>63</v>
       </c>
-      <c r="G31" s="52" t="s">
+      <c r="G31" s="51" t="s">
         <v>89</v>
       </c>
-      <c r="H31" s="52" t="s">
+      <c r="H31" s="51" t="s">
         <v>90</v>
       </c>
-      <c r="I31" s="52" t="s">
+      <c r="I31" s="51" t="s">
         <v>91</v>
       </c>
     </row>
@@ -2281,18 +2246,8 @@
       <c r="R41" s="9"/>
       <c r="S41" s="9"/>
     </row>
-    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="L42" s="9"/>
-      <c r="M42" s="9"/>
-      <c r="N42" s="9"/>
-      <c r="O42" s="9"/>
-      <c r="P42" s="9"/>
-      <c r="Q42" s="9"/>
-      <c r="R42" s="9"/>
-      <c r="S42" s="9"/>
-    </row>
     <row r="43" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="53" t="s">
+      <c r="A43" s="52" t="s">
         <v>102</v>
       </c>
       <c r="B43" s="19" t="s">
@@ -2312,7 +2267,7 @@
       <c r="S43" s="9"/>
     </row>
     <row r="44" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="53"/>
+      <c r="A44" s="52"/>
       <c r="B44" s="19" t="s">
         <v>17</v>
       </c>
@@ -2329,283 +2284,267 @@
       <c r="R44" s="9"/>
       <c r="S44" s="9"/>
     </row>
-    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="L45" s="9"/>
-      <c r="M45" s="9"/>
-      <c r="N45" s="9"/>
-      <c r="O45" s="9"/>
-      <c r="P45" s="9"/>
-      <c r="Q45" s="9"/>
-      <c r="R45" s="9"/>
-      <c r="S45" s="9"/>
-    </row>
     <row r="46" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="54" t="s">
+      <c r="A46" s="53" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="55" t="s">
+      <c r="A47" s="54" t="s">
         <v>105</v>
       </c>
-      <c r="B47" s="55" t="s">
+      <c r="B47" s="54" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="56" t="n">
+      <c r="A48" s="55" t="n">
         <v>1</v>
       </c>
-      <c r="B48" s="57" t="s">
+      <c r="B48" s="56" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="56" t="n">
+      <c r="A49" s="55" t="n">
         <v>3</v>
       </c>
-      <c r="B49" s="57" t="s">
+      <c r="B49" s="56" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="56" t="n">
+      <c r="A50" s="55" t="n">
         <v>2</v>
       </c>
-      <c r="B50" s="57" t="s">
+      <c r="B50" s="56" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="56" t="n">
+      <c r="A51" s="55" t="n">
         <v>1</v>
       </c>
-      <c r="B51" s="57" t="s">
+      <c r="B51" s="56" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="50" t="s">
+      <c r="A53" s="49" t="s">
         <v>111</v>
       </c>
-      <c r="B53" s="51" t="s">
+      <c r="B53" s="50" t="s">
         <v>112</v>
       </c>
-      <c r="C53" s="51"/>
-      <c r="D53" s="51"/>
-      <c r="E53" s="51"/>
-      <c r="F53" s="51"/>
+      <c r="C53" s="50"/>
+      <c r="D53" s="50"/>
+      <c r="E53" s="50"/>
+      <c r="F53" s="50"/>
     </row>
     <row r="54" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="50"/>
-      <c r="B54" s="51" t="s">
+      <c r="A54" s="49"/>
+      <c r="B54" s="50" t="s">
         <v>17</v>
       </c>
-      <c r="C54" s="51"/>
-      <c r="D54" s="51"/>
-      <c r="E54" s="51"/>
-      <c r="F54" s="51"/>
+      <c r="C54" s="50"/>
+      <c r="D54" s="50"/>
+      <c r="E54" s="50"/>
+      <c r="F54" s="50"/>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="58" t="s">
+      <c r="A56" s="57" t="s">
         <v>113</v>
       </c>
-      <c r="B56" s="58" t="s">
+      <c r="B56" s="57" t="s">
         <v>44</v>
       </c>
-      <c r="C56" s="58" t="s">
+      <c r="C56" s="57" t="s">
         <v>86</v>
       </c>
-      <c r="D56" s="58" t="s">
+      <c r="D56" s="57" t="s">
         <v>87</v>
       </c>
-      <c r="E56" s="58" t="s">
+      <c r="E56" s="57" t="s">
         <v>88</v>
       </c>
-      <c r="F56" s="58" t="s">
+      <c r="F56" s="57" t="s">
         <v>63</v>
       </c>
-      <c r="G56" s="58" t="s">
+      <c r="G56" s="57" t="s">
         <v>89</v>
       </c>
-      <c r="H56" s="58" t="s">
+      <c r="H56" s="57" t="s">
         <v>90</v>
       </c>
-      <c r="I56" s="58" t="s">
+      <c r="I56" s="57" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="23.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A57" s="48" t="s">
+      <c r="A57" s="47" t="s">
         <v>46</v>
       </c>
-      <c r="B57" s="48"/>
-      <c r="C57" s="48"/>
-      <c r="D57" s="48"/>
-      <c r="E57" s="48"/>
-      <c r="F57" s="59" t="s">
+      <c r="B57" s="47"/>
+      <c r="C57" s="47"/>
+      <c r="D57" s="47"/>
+      <c r="E57" s="47"/>
+      <c r="F57" s="58" t="s">
         <v>114</v>
       </c>
-      <c r="G57" s="60"/>
-      <c r="H57" s="60"/>
-      <c r="I57" s="60"/>
+      <c r="G57" s="59"/>
+      <c r="H57" s="59"/>
+      <c r="I57" s="59"/>
     </row>
     <row r="58" customFormat="false" ht="23.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A58" s="48" t="s">
+      <c r="A58" s="47" t="s">
         <v>59</v>
       </c>
-      <c r="B58" s="48" t="s">
+      <c r="B58" s="47" t="s">
         <v>115</v>
       </c>
-      <c r="C58" s="48"/>
-      <c r="D58" s="48"/>
-      <c r="E58" s="48"/>
-      <c r="F58" s="48"/>
-      <c r="G58" s="60"/>
-      <c r="H58" s="60"/>
-      <c r="I58" s="60"/>
+      <c r="C58" s="47"/>
+      <c r="D58" s="47"/>
+      <c r="E58" s="47"/>
+      <c r="F58" s="47"/>
+      <c r="G58" s="59"/>
+      <c r="H58" s="59"/>
+      <c r="I58" s="59"/>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="48" t="s">
+      <c r="A59" s="47" t="s">
         <v>53</v>
       </c>
-      <c r="B59" s="48" t="s">
+      <c r="B59" s="47" t="s">
         <v>115</v>
       </c>
-      <c r="C59" s="48"/>
-      <c r="D59" s="48"/>
-      <c r="E59" s="48"/>
-      <c r="F59" s="48"/>
-      <c r="G59" s="60"/>
-      <c r="H59" s="60"/>
-      <c r="I59" s="60"/>
+      <c r="C59" s="47"/>
+      <c r="D59" s="47"/>
+      <c r="E59" s="47"/>
+      <c r="F59" s="47"/>
+      <c r="G59" s="59"/>
+      <c r="H59" s="59"/>
+      <c r="I59" s="59"/>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="48" t="s">
+      <c r="A60" s="47" t="s">
         <v>71</v>
       </c>
-      <c r="B60" s="48" t="s">
+      <c r="B60" s="47" t="s">
         <v>115</v>
       </c>
-      <c r="C60" s="48"/>
-      <c r="D60" s="48"/>
-      <c r="E60" s="48"/>
-      <c r="F60" s="48"/>
-      <c r="G60" s="60"/>
-      <c r="H60" s="60"/>
-      <c r="I60" s="60"/>
+      <c r="C60" s="47"/>
+      <c r="D60" s="47"/>
+      <c r="E60" s="47"/>
+      <c r="F60" s="47"/>
+      <c r="G60" s="59"/>
+      <c r="H60" s="59"/>
+      <c r="I60" s="59"/>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="48" t="s">
+      <c r="A61" s="47" t="s">
         <v>80</v>
       </c>
-      <c r="B61" s="48" t="s">
+      <c r="B61" s="47" t="s">
         <v>115</v>
       </c>
-      <c r="C61" s="48"/>
-      <c r="D61" s="48"/>
-      <c r="E61" s="48"/>
-      <c r="F61" s="48"/>
-      <c r="G61" s="60"/>
-      <c r="H61" s="60"/>
-      <c r="I61" s="60"/>
-    </row>
-    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="48"/>
-      <c r="B62" s="48"/>
-      <c r="C62" s="48"/>
-      <c r="D62" s="48"/>
-      <c r="E62" s="48"/>
-      <c r="F62" s="48"/>
-      <c r="G62" s="60"/>
-      <c r="H62" s="60"/>
-      <c r="I62" s="60"/>
+      <c r="C61" s="47"/>
+      <c r="D61" s="47"/>
+      <c r="E61" s="47"/>
+      <c r="F61" s="47"/>
+      <c r="G61" s="59"/>
+      <c r="H61" s="59"/>
+      <c r="I61" s="59"/>
+    </row>
+    <row r="63" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="49" t="s">
+        <v>116</v>
+      </c>
+      <c r="B63" s="50" t="s">
+        <v>117</v>
+      </c>
+      <c r="C63" s="50"/>
+      <c r="D63" s="50"/>
+      <c r="E63" s="50"/>
+      <c r="F63" s="50"/>
     </row>
     <row r="64" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="50" t="s">
-        <v>111</v>
-      </c>
-      <c r="B64" s="51" t="s">
-        <v>116</v>
-      </c>
-      <c r="C64" s="51"/>
-      <c r="D64" s="51"/>
-      <c r="E64" s="51"/>
-      <c r="F64" s="51"/>
-    </row>
-    <row r="65" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="50"/>
-      <c r="B65" s="51" t="s">
+      <c r="A64" s="49"/>
+      <c r="B64" s="50" t="s">
         <v>17</v>
       </c>
-      <c r="C65" s="51"/>
-      <c r="D65" s="51"/>
-      <c r="E65" s="51"/>
-      <c r="F65" s="51"/>
+      <c r="C64" s="50"/>
+      <c r="D64" s="50"/>
+      <c r="E64" s="50"/>
+      <c r="F64" s="50"/>
+    </row>
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="57" t="s">
+        <v>118</v>
+      </c>
+      <c r="B66" s="57" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="58" t="s">
-        <v>117</v>
-      </c>
-      <c r="B67" s="58" t="s">
-        <v>118</v>
+      <c r="A67" s="47" t="s">
+        <v>46</v>
+      </c>
+      <c r="B67" s="57" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="48" t="s">
-        <v>46</v>
-      </c>
-      <c r="B68" s="58" t="s">
-        <v>119</v>
-      </c>
+      <c r="A68" s="47" t="s">
+        <v>59</v>
+      </c>
+      <c r="B68" s="57"/>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="48" t="s">
-        <v>59</v>
-      </c>
-      <c r="B69" s="58"/>
+      <c r="A69" s="47" t="s">
+        <v>53</v>
+      </c>
+      <c r="B69" s="57"/>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="48" t="s">
-        <v>53</v>
-      </c>
-      <c r="B70" s="58"/>
+      <c r="A70" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="B70" s="57" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="48" t="s">
-        <v>71</v>
-      </c>
-      <c r="B71" s="58" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="48" t="s">
+      <c r="A71" s="47" t="s">
         <v>80</v>
       </c>
-      <c r="B72" s="60"/>
+      <c r="B71" s="59"/>
     </row>
   </sheetData>
-  <mergeCells count="19">
+  <mergeCells count="24">
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="B3:F3"/>
     <mergeCell ref="B4:F4"/>
     <mergeCell ref="B5:F5"/>
     <mergeCell ref="B6:F6"/>
+    <mergeCell ref="A11:A12"/>
     <mergeCell ref="B11:F11"/>
     <mergeCell ref="B12:F12"/>
     <mergeCell ref="A14:E14"/>
     <mergeCell ref="G14:K14"/>
     <mergeCell ref="M14:Q14"/>
     <mergeCell ref="R14:S14"/>
+    <mergeCell ref="A28:A29"/>
     <mergeCell ref="B28:F28"/>
     <mergeCell ref="B29:F29"/>
+    <mergeCell ref="A43:A44"/>
     <mergeCell ref="B43:F43"/>
     <mergeCell ref="B44:F44"/>
+    <mergeCell ref="A53:A54"/>
     <mergeCell ref="B53:F53"/>
     <mergeCell ref="B54:F54"/>
+    <mergeCell ref="A63:A64"/>
+    <mergeCell ref="B63:F63"/>
     <mergeCell ref="B64:F64"/>
-    <mergeCell ref="B65:F65"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -2639,198 +2578,198 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="61" t="s">
-        <v>120</v>
-      </c>
-      <c r="B1" s="61" t="s">
+      <c r="A1" s="60" t="s">
         <v>121</v>
       </c>
-      <c r="C1" s="61" t="s">
+      <c r="B1" s="60" t="s">
         <v>122</v>
       </c>
-      <c r="D1" s="61" t="s">
+      <c r="C1" s="60" t="s">
         <v>123</v>
       </c>
-      <c r="E1" s="61" t="s">
+      <c r="D1" s="60" t="s">
         <v>124</v>
       </c>
+      <c r="E1" s="60" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="62" t="s">
+      <c r="A2" s="61" t="s">
         <v>80</v>
       </c>
-      <c r="B2" s="62" t="s">
-        <v>125</v>
-      </c>
-      <c r="C2" s="63" t="s">
+      <c r="B2" s="61" t="s">
         <v>126</v>
       </c>
-      <c r="D2" s="63"/>
-      <c r="E2" s="62" t="s">
+      <c r="C2" s="62" t="s">
         <v>127</v>
       </c>
+      <c r="D2" s="62"/>
+      <c r="E2" s="61" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="62" t="s">
-        <v>128</v>
-      </c>
-      <c r="B3" s="62" t="s">
+      <c r="A3" s="61" t="s">
         <v>129</v>
       </c>
-      <c r="C3" s="62"/>
-      <c r="D3" s="62"/>
-      <c r="E3" s="63" t="s">
+      <c r="B3" s="61" t="s">
         <v>130</v>
       </c>
+      <c r="C3" s="61"/>
+      <c r="D3" s="61"/>
+      <c r="E3" s="62" t="s">
+        <v>131</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="62" t="s">
-        <v>131</v>
-      </c>
-      <c r="B4" s="62" t="s">
+      <c r="A4" s="61" t="s">
         <v>132</v>
       </c>
-      <c r="C4" s="62" t="s">
+      <c r="B4" s="61" t="s">
         <v>133</v>
       </c>
-      <c r="D4" s="62"/>
-      <c r="E4" s="62" t="s">
+      <c r="C4" s="61" t="s">
         <v>134</v>
       </c>
+      <c r="D4" s="61"/>
+      <c r="E4" s="61" t="s">
+        <v>135</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="62" t="s">
-        <v>135</v>
-      </c>
-      <c r="B5" s="62" t="s">
+      <c r="A5" s="61" t="s">
         <v>136</v>
       </c>
-      <c r="C5" s="62" t="s">
+      <c r="B5" s="61" t="s">
         <v>137</v>
       </c>
-      <c r="D5" s="62"/>
-      <c r="E5" s="62" t="s">
+      <c r="C5" s="61" t="s">
         <v>138</v>
       </c>
+      <c r="D5" s="61"/>
+      <c r="E5" s="61" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="62" t="s">
-        <v>139</v>
-      </c>
-      <c r="B6" s="62" t="s">
+      <c r="A6" s="61" t="s">
         <v>140</v>
       </c>
-      <c r="C6" s="62" t="s">
+      <c r="B6" s="61" t="s">
         <v>141</v>
       </c>
-      <c r="D6" s="62" t="s">
+      <c r="C6" s="61" t="s">
         <v>142</v>
       </c>
-      <c r="E6" s="63" t="s">
+      <c r="D6" s="61" t="s">
         <v>143</v>
       </c>
+      <c r="E6" s="62" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="62" t="s">
-        <v>144</v>
-      </c>
-      <c r="B7" s="62" t="s">
+      <c r="A7" s="61" t="s">
         <v>145</v>
       </c>
-      <c r="C7" s="63" t="s">
+      <c r="B7" s="61" t="s">
         <v>146</v>
       </c>
-      <c r="D7" s="63"/>
-      <c r="E7" s="62" t="s">
+      <c r="C7" s="62" t="s">
         <v>147</v>
       </c>
+      <c r="D7" s="62"/>
+      <c r="E7" s="61" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="62" t="s">
-        <v>148</v>
-      </c>
-      <c r="B8" s="62" t="s">
+      <c r="A8" s="61" t="s">
         <v>149</v>
       </c>
-      <c r="C8" s="63"/>
-      <c r="D8" s="63" t="s">
+      <c r="B8" s="61" t="s">
         <v>150</v>
       </c>
-      <c r="E8" s="62" t="s">
-        <v>148</v>
+      <c r="C8" s="62"/>
+      <c r="D8" s="62" t="s">
+        <v>151</v>
+      </c>
+      <c r="E8" s="61" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="62" t="s">
-        <v>151</v>
-      </c>
-      <c r="B9" s="62" t="s">
+      <c r="A9" s="61" t="s">
         <v>152</v>
       </c>
-      <c r="C9" s="62"/>
-      <c r="D9" s="62"/>
-      <c r="E9" s="62" t="s">
+      <c r="B9" s="61" t="s">
         <v>153</v>
       </c>
+      <c r="C9" s="61"/>
+      <c r="D9" s="61"/>
+      <c r="E9" s="61" t="s">
+        <v>154</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="62" t="s">
-        <v>154</v>
-      </c>
-      <c r="B10" s="62" t="s">
+      <c r="A10" s="61" t="s">
         <v>155</v>
       </c>
-      <c r="C10" s="62" t="s">
+      <c r="B10" s="61" t="s">
         <v>156</v>
       </c>
-      <c r="D10" s="62"/>
-      <c r="E10" s="63" t="s">
+      <c r="C10" s="61" t="s">
         <v>157</v>
       </c>
+      <c r="D10" s="61"/>
+      <c r="E10" s="62" t="s">
+        <v>158</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="62" t="s">
-        <v>158</v>
-      </c>
-      <c r="B11" s="62" t="s">
+      <c r="A11" s="61" t="s">
         <v>159</v>
       </c>
-      <c r="C11" s="62" t="s">
+      <c r="B11" s="61" t="s">
         <v>160</v>
       </c>
-      <c r="D11" s="62"/>
-      <c r="E11" s="63" t="s">
+      <c r="C11" s="61" t="s">
         <v>161</v>
       </c>
+      <c r="D11" s="61"/>
+      <c r="E11" s="62" t="s">
+        <v>162</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="62" t="s">
+      <c r="A12" s="61" t="s">
         <v>71</v>
       </c>
-      <c r="B12" s="62" t="s">
-        <v>162</v>
-      </c>
-      <c r="C12" s="62" t="s">
+      <c r="B12" s="61" t="s">
         <v>163</v>
       </c>
-      <c r="D12" s="62"/>
-      <c r="E12" s="63" t="s">
+      <c r="C12" s="61" t="s">
         <v>164</v>
       </c>
+      <c r="D12" s="61"/>
+      <c r="E12" s="62" t="s">
+        <v>165</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="62" t="s">
-        <v>165</v>
-      </c>
-      <c r="B13" s="63" t="s">
+      <c r="A13" s="61" t="s">
         <v>166</v>
       </c>
-      <c r="C13" s="62" t="s">
+      <c r="B13" s="62" t="s">
         <v>167</v>
       </c>
-      <c r="D13" s="62"/>
-      <c r="E13" s="63" t="s">
+      <c r="C13" s="61" t="s">
         <v>168</v>
+      </c>
+      <c r="D13" s="61"/>
+      <c r="E13" s="62" t="s">
+        <v>169</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se ajusta la programación para las matrices transpuestas
</commit_message>
<xml_diff>
--- a/Oficial/Patron_FL.xlsx
+++ b/Oficial/Patron_FL.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="430" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="311" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="BASE_SSE" sheetId="1" state="visible" r:id="rId2"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="169">
   <si>
     <t>SOLICITUD  DE SERVICIO EXTERNO A LABORATORIO</t>
   </si>
@@ -354,7 +354,7 @@
     <t>Cuadro 4</t>
   </si>
   <si>
-    <t>Agregar laboratorios y escribir en cada celda, relacionada con matriz, la observación en particular</t>
+    <t>Agregar todos los laboratorios y escribir en cada celda, relacionada con matriz, la observación en particular</t>
   </si>
   <si>
     <t>Observaciones\Lab</t>
@@ -370,13 +370,10 @@
     <t>Cuadro 5</t>
   </si>
   <si>
-    <t>Agregar todos los laboratorios involucrados y escribir en cada celda, solo 'si', si adjunta algún documento en particular</t>
+    <t>Escribir en cada celda, solo 'si', si adjunta algún documento en particular para cada matriz y laboratorio</t>
   </si>
   <si>
     <t>ADJUNTA</t>
-  </si>
-  <si>
-    <t>(si/no)</t>
   </si>
   <si>
     <t>si</t>
@@ -661,7 +658,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -708,6 +705,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF66FFFF"/>
         <bgColor rgb="FF99FFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF99"/>
+        <bgColor rgb="FFFFFFCC"/>
       </patternFill>
     </fill>
   </fills>
@@ -837,7 +840,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="65">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1046,6 +1049,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="7" fillId="9" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="12" fillId="2" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1075,6 +1082,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1209,10 +1220,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:S71"/>
+  <dimension ref="A1:S62"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A52" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B64" activeCellId="0" sqref="B64"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A34" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F59" activeCellId="0" sqref="F59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1222,7 +1233,7 @@
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.1887755102041"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.6275510204082"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.8775510204082"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="34.5510204081633"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="29.1938775510204"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.8979591836735"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="22.4540816326531"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="0" width="17.0918367346939"/>
@@ -1471,38 +1482,67 @@
       <c r="R12" s="9"/>
       <c r="S12" s="9"/>
     </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" s="20"/>
+      <c r="C13" s="20"/>
+      <c r="D13" s="20"/>
+      <c r="E13" s="20"/>
+      <c r="F13" s="20"/>
+      <c r="G13" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="H13" s="21"/>
+      <c r="I13" s="21"/>
+      <c r="J13" s="21"/>
+      <c r="K13" s="21"/>
+      <c r="L13" s="22"/>
+      <c r="M13" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="N13" s="23"/>
+      <c r="O13" s="23"/>
+      <c r="P13" s="23"/>
+      <c r="Q13" s="23"/>
+      <c r="R13" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="S13" s="24"/>
+    </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="20" t="s">
-        <v>18</v>
+      <c r="A14" s="25" t="s">
+        <v>22</v>
       </c>
       <c r="B14" s="20"/>
-      <c r="C14" s="20"/>
-      <c r="D14" s="20"/>
-      <c r="E14" s="20"/>
-      <c r="F14" s="20"/>
-      <c r="G14" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="H14" s="21"/>
-      <c r="I14" s="21"/>
-      <c r="J14" s="21"/>
-      <c r="K14" s="21"/>
-      <c r="L14" s="22"/>
-      <c r="M14" s="23" t="s">
-        <v>20</v>
-      </c>
-      <c r="N14" s="23"/>
-      <c r="O14" s="23"/>
-      <c r="P14" s="23"/>
-      <c r="Q14" s="23"/>
-      <c r="R14" s="24" t="s">
-        <v>21</v>
-      </c>
-      <c r="S14" s="24"/>
+      <c r="C14" s="26"/>
+      <c r="D14" s="26"/>
+      <c r="E14" s="26"/>
+      <c r="F14" s="26"/>
+      <c r="G14" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="H14" s="27"/>
+      <c r="I14" s="27"/>
+      <c r="J14" s="28"/>
+      <c r="K14" s="29"/>
+      <c r="L14" s="29"/>
+      <c r="M14" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="N14" s="31"/>
+      <c r="O14" s="32"/>
+      <c r="P14" s="32"/>
+      <c r="Q14" s="33"/>
+      <c r="R14" s="34" t="s">
+        <v>22</v>
+      </c>
+      <c r="S14" s="35"/>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="25" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B15" s="20"/>
       <c r="C15" s="26"/>
@@ -1510,7 +1550,7 @@
       <c r="E15" s="26"/>
       <c r="F15" s="26"/>
       <c r="G15" s="27" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H15" s="27"/>
       <c r="I15" s="27"/>
@@ -1518,111 +1558,127 @@
       <c r="K15" s="29"/>
       <c r="L15" s="29"/>
       <c r="M15" s="30" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="N15" s="31"/>
-      <c r="O15" s="32"/>
-      <c r="P15" s="32"/>
-      <c r="Q15" s="33"/>
+      <c r="O15" s="36"/>
+      <c r="P15" s="36"/>
+      <c r="Q15" s="37"/>
       <c r="R15" s="34" t="s">
-        <v>22</v>
-      </c>
-      <c r="S15" s="35"/>
-    </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="20"/>
-      <c r="C16" s="26"/>
-      <c r="D16" s="26"/>
-      <c r="E16" s="26"/>
-      <c r="F16" s="26"/>
-      <c r="G16" s="27" t="s">
-        <v>23</v>
-      </c>
-      <c r="H16" s="27"/>
-      <c r="I16" s="27"/>
-      <c r="J16" s="28"/>
-      <c r="K16" s="29"/>
-      <c r="L16" s="29"/>
-      <c r="M16" s="30" t="s">
-        <v>23</v>
-      </c>
-      <c r="N16" s="31"/>
-      <c r="O16" s="36"/>
-      <c r="P16" s="36"/>
-      <c r="Q16" s="37"/>
-      <c r="R16" s="34" t="s">
-        <v>23</v>
-      </c>
-      <c r="S16" s="24"/>
-    </row>
-    <row r="17" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="38" t="s">
+      <c r="S15" s="24"/>
+    </row>
+    <row r="16" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="38" t="s">
         <v>24</v>
       </c>
-      <c r="B17" s="38" t="s">
+      <c r="B16" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="C17" s="38" t="s">
+      <c r="C16" s="38" t="s">
         <v>26</v>
       </c>
-      <c r="D17" s="38" t="s">
+      <c r="D16" s="38" t="s">
         <v>27</v>
       </c>
-      <c r="E17" s="38" t="s">
+      <c r="E16" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="F17" s="38" t="s">
+      <c r="F16" s="38" t="s">
         <v>29</v>
       </c>
-      <c r="G17" s="39" t="s">
+      <c r="G16" s="39" t="s">
         <v>30</v>
       </c>
-      <c r="H17" s="39" t="s">
+      <c r="H16" s="39" t="s">
         <v>31</v>
       </c>
-      <c r="I17" s="39" t="s">
+      <c r="I16" s="39" t="s">
         <v>32</v>
       </c>
-      <c r="J17" s="39" t="s">
+      <c r="J16" s="39" t="s">
         <v>33</v>
       </c>
-      <c r="K17" s="39" t="s">
+      <c r="K16" s="39" t="s">
         <v>34</v>
       </c>
-      <c r="L17" s="40" t="s">
+      <c r="L16" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="M17" s="41" t="s">
+      <c r="M16" s="41" t="s">
         <v>36</v>
       </c>
-      <c r="N17" s="41" t="s">
+      <c r="N16" s="41" t="s">
         <v>37</v>
       </c>
-      <c r="O17" s="42" t="s">
+      <c r="O16" s="42" t="s">
         <v>38</v>
       </c>
-      <c r="P17" s="42" t="s">
+      <c r="P16" s="42" t="s">
         <v>39</v>
       </c>
-      <c r="Q17" s="42" t="s">
+      <c r="Q16" s="42" t="s">
         <v>40</v>
       </c>
-      <c r="R17" s="43" t="s">
+      <c r="R16" s="43" t="s">
         <v>41</v>
       </c>
-      <c r="S17" s="44" t="s">
+      <c r="S16" s="44" t="s">
         <v>42</v>
       </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="45" t="n">
+        <v>10</v>
+      </c>
+      <c r="B17" s="46" t="s">
+        <v>43</v>
+      </c>
+      <c r="C17" s="45" t="n">
+        <v>1</v>
+      </c>
+      <c r="D17" s="47" t="s">
+        <v>44</v>
+      </c>
+      <c r="E17" s="45" t="s">
+        <v>45</v>
+      </c>
+      <c r="F17" s="45" t="n">
+        <v>0</v>
+      </c>
+      <c r="G17" s="45" t="s">
+        <v>46</v>
+      </c>
+      <c r="H17" s="45" t="s">
+        <v>47</v>
+      </c>
+      <c r="I17" s="45" t="s">
+        <v>48</v>
+      </c>
+      <c r="J17" s="45" t="s">
+        <v>49</v>
+      </c>
+      <c r="K17" s="45" t="n">
+        <v>0.35</v>
+      </c>
+      <c r="L17" s="45" t="s">
+        <v>50</v>
+      </c>
+      <c r="M17" s="46"/>
+      <c r="N17" s="46"/>
+      <c r="O17" s="46"/>
+      <c r="P17" s="46"/>
+      <c r="Q17" s="46"/>
+      <c r="R17" s="46"/>
+      <c r="S17" s="46"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="45" t="n">
         <v>10</v>
       </c>
       <c r="B18" s="46" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="C18" s="45" t="n">
         <v>1</v>
@@ -1633,11 +1689,11 @@
       <c r="E18" s="45" t="s">
         <v>45</v>
       </c>
-      <c r="F18" s="45" t="n">
-        <v>0</v>
+      <c r="F18" s="45" t="s">
+        <v>52</v>
       </c>
       <c r="G18" s="45" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="H18" s="45" t="s">
         <v>47</v>
@@ -1645,14 +1701,14 @@
       <c r="I18" s="45" t="s">
         <v>48</v>
       </c>
-      <c r="J18" s="45" t="s">
-        <v>49</v>
+      <c r="J18" s="45" t="n">
+        <v>600</v>
       </c>
       <c r="K18" s="45" t="n">
-        <v>0.35</v>
+        <v>20</v>
       </c>
       <c r="L18" s="45" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="M18" s="46"/>
       <c r="N18" s="46"/>
@@ -1667,7 +1723,7 @@
         <v>10</v>
       </c>
       <c r="B19" s="46" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="C19" s="45" t="n">
         <v>1</v>
@@ -1679,10 +1735,10 @@
         <v>45</v>
       </c>
       <c r="F19" s="45" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="G19" s="45" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="H19" s="45" t="s">
         <v>47</v>
@@ -1690,14 +1746,14 @@
       <c r="I19" s="45" t="s">
         <v>48</v>
       </c>
-      <c r="J19" s="45" t="n">
-        <v>600</v>
+      <c r="J19" s="45" t="s">
+        <v>49</v>
       </c>
       <c r="K19" s="45" t="n">
-        <v>20</v>
+        <v>0.15</v>
       </c>
       <c r="L19" s="45" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="M19" s="46"/>
       <c r="N19" s="46"/>
@@ -1712,7 +1768,7 @@
         <v>10</v>
       </c>
       <c r="B20" s="46" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C20" s="45" t="n">
         <v>1</v>
@@ -1724,22 +1780,22 @@
         <v>45</v>
       </c>
       <c r="F20" s="45" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="G20" s="45" t="s">
-        <v>46</v>
+        <v>59</v>
       </c>
       <c r="H20" s="45" t="s">
-        <v>47</v>
+        <v>60</v>
       </c>
       <c r="I20" s="45" t="s">
-        <v>48</v>
-      </c>
-      <c r="J20" s="45" t="s">
-        <v>49</v>
+        <v>61</v>
+      </c>
+      <c r="J20" s="45" t="n">
+        <v>42</v>
       </c>
       <c r="K20" s="45" t="n">
-        <v>0.15</v>
+        <v>0.42</v>
       </c>
       <c r="L20" s="45" t="s">
         <v>50</v>
@@ -1754,37 +1810,37 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="45" t="n">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="B21" s="46" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="C21" s="45" t="n">
         <v>1</v>
       </c>
       <c r="D21" s="47" t="s">
-        <v>44</v>
+        <v>63</v>
       </c>
       <c r="E21" s="45" t="s">
         <v>45</v>
       </c>
       <c r="F21" s="45" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="G21" s="45" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="H21" s="45" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="I21" s="45" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="J21" s="45" t="n">
         <v>42</v>
       </c>
       <c r="K21" s="45" t="n">
-        <v>0.42</v>
+        <v>0.2</v>
       </c>
       <c r="L21" s="45" t="s">
         <v>50</v>
@@ -1802,7 +1858,7 @@
         <v>3</v>
       </c>
       <c r="B22" s="46" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="C22" s="45" t="n">
         <v>1</v>
@@ -1814,7 +1870,7 @@
         <v>45</v>
       </c>
       <c r="F22" s="45" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="G22" s="45" t="s">
         <v>46</v>
@@ -1829,7 +1885,7 @@
         <v>42</v>
       </c>
       <c r="K22" s="45" t="n">
-        <v>0.2</v>
+        <v>0.43</v>
       </c>
       <c r="L22" s="45" t="s">
         <v>50</v>
@@ -1844,40 +1900,40 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="45" t="n">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="B23" s="46" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C23" s="45" t="n">
         <v>1</v>
       </c>
       <c r="D23" s="47" t="s">
-        <v>63</v>
+        <v>44</v>
       </c>
       <c r="E23" s="45" t="s">
         <v>45</v>
       </c>
       <c r="F23" s="45" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="G23" s="45" t="s">
-        <v>46</v>
+        <v>71</v>
       </c>
       <c r="H23" s="45" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="I23" s="45" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="J23" s="45" t="n">
-        <v>42</v>
+        <v>8962</v>
       </c>
       <c r="K23" s="45" t="n">
-        <v>0.43</v>
+        <v>21580</v>
       </c>
       <c r="L23" s="45" t="s">
-        <v>50</v>
+        <v>74</v>
       </c>
       <c r="M23" s="46"/>
       <c r="N23" s="46"/>
@@ -1891,8 +1947,8 @@
       <c r="A24" s="45" t="n">
         <v>10</v>
       </c>
-      <c r="B24" s="46" t="s">
-        <v>69</v>
+      <c r="B24" s="48" t="s">
+        <v>75</v>
       </c>
       <c r="C24" s="45" t="n">
         <v>1</v>
@@ -1904,25 +1960,25 @@
         <v>45</v>
       </c>
       <c r="F24" s="45" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="G24" s="45" t="s">
-        <v>71</v>
-      </c>
-      <c r="H24" s="45" t="s">
-        <v>72</v>
+        <v>46</v>
+      </c>
+      <c r="H24" s="46" t="s">
+        <v>77</v>
       </c>
       <c r="I24" s="45" t="s">
-        <v>73</v>
-      </c>
-      <c r="J24" s="45" t="n">
-        <v>8962</v>
+        <v>78</v>
+      </c>
+      <c r="J24" s="45" t="s">
+        <v>49</v>
       </c>
       <c r="K24" s="45" t="n">
-        <v>21580</v>
+        <v>0.43</v>
       </c>
       <c r="L24" s="45" t="s">
-        <v>74</v>
+        <v>50</v>
       </c>
       <c r="M24" s="46"/>
       <c r="N24" s="46"/>
@@ -1937,7 +1993,7 @@
         <v>10</v>
       </c>
       <c r="B25" s="48" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="C25" s="45" t="n">
         <v>1</v>
@@ -1948,26 +2004,24 @@
       <c r="E25" s="45" t="s">
         <v>45</v>
       </c>
-      <c r="F25" s="45" t="s">
-        <v>76</v>
-      </c>
+      <c r="F25" s="46"/>
       <c r="G25" s="45" t="s">
-        <v>46</v>
-      </c>
-      <c r="H25" s="46" t="s">
-        <v>77</v>
+        <v>80</v>
+      </c>
+      <c r="H25" s="45" t="s">
+        <v>81</v>
       </c>
       <c r="I25" s="45" t="s">
-        <v>78</v>
-      </c>
-      <c r="J25" s="45" t="s">
-        <v>49</v>
+        <v>82</v>
+      </c>
+      <c r="J25" s="45" t="n">
+        <v>5632</v>
       </c>
       <c r="K25" s="45" t="n">
-        <v>0.43</v>
+        <v>9123</v>
       </c>
       <c r="L25" s="45" t="s">
-        <v>50</v>
+        <v>74</v>
       </c>
       <c r="M25" s="46"/>
       <c r="N25" s="46"/>
@@ -1977,108 +2031,116 @@
       <c r="R25" s="46"/>
       <c r="S25" s="46"/>
     </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="45" t="n">
-        <v>10</v>
-      </c>
-      <c r="B26" s="48" t="s">
-        <v>79</v>
-      </c>
-      <c r="C26" s="45" t="n">
+    <row r="26" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="49" t="s">
+        <v>83</v>
+      </c>
+      <c r="B26" s="50" t="s">
+        <v>84</v>
+      </c>
+      <c r="C26" s="50"/>
+      <c r="D26" s="50"/>
+      <c r="E26" s="50"/>
+      <c r="F26" s="50"/>
+    </row>
+    <row r="27" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="49"/>
+      <c r="B27" s="50" t="s">
+        <v>17</v>
+      </c>
+      <c r="C27" s="50"/>
+      <c r="D27" s="50"/>
+      <c r="E27" s="50"/>
+      <c r="F27" s="50"/>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="51" t="s">
+        <v>85</v>
+      </c>
+      <c r="B28" s="52" t="s">
+        <v>44</v>
+      </c>
+      <c r="C28" s="52" t="s">
+        <v>86</v>
+      </c>
+      <c r="D28" s="52" t="s">
+        <v>87</v>
+      </c>
+      <c r="E28" s="52" t="s">
+        <v>88</v>
+      </c>
+      <c r="F28" s="52" t="s">
+        <v>63</v>
+      </c>
+      <c r="G28" s="52" t="s">
+        <v>89</v>
+      </c>
+      <c r="H28" s="52" t="s">
+        <v>90</v>
+      </c>
+      <c r="I28" s="52" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="B29" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="D26" s="47" t="s">
-        <v>44</v>
-      </c>
-      <c r="E26" s="45" t="s">
-        <v>45</v>
-      </c>
-      <c r="F26" s="46"/>
-      <c r="G26" s="45" t="s">
-        <v>80</v>
-      </c>
-      <c r="H26" s="45" t="s">
-        <v>81</v>
-      </c>
-      <c r="I26" s="45" t="s">
-        <v>82</v>
-      </c>
-      <c r="J26" s="45" t="n">
-        <v>5632</v>
-      </c>
-      <c r="K26" s="45" t="n">
-        <v>9123</v>
-      </c>
-      <c r="L26" s="45" t="s">
-        <v>74</v>
-      </c>
-      <c r="M26" s="46"/>
-      <c r="N26" s="46"/>
-      <c r="O26" s="46"/>
-      <c r="P26" s="46"/>
-      <c r="Q26" s="46"/>
-      <c r="R26" s="46"/>
-      <c r="S26" s="46"/>
-    </row>
-    <row r="28" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="49" t="s">
-        <v>83</v>
-      </c>
-      <c r="B28" s="50" t="s">
-        <v>84</v>
-      </c>
-      <c r="C28" s="50"/>
-      <c r="D28" s="50"/>
-      <c r="E28" s="50"/>
-      <c r="F28" s="50"/>
-    </row>
-    <row r="29" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="49"/>
-      <c r="B29" s="50" t="s">
-        <v>17</v>
-      </c>
-      <c r="C29" s="50"/>
-      <c r="D29" s="50"/>
-      <c r="E29" s="50"/>
-      <c r="F29" s="50"/>
+      <c r="F29" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="L29" s="9"/>
+      <c r="M29" s="9"/>
+      <c r="N29" s="9"/>
+      <c r="O29" s="9"/>
+      <c r="P29" s="9"/>
+      <c r="Q29" s="9"/>
+      <c r="R29" s="9"/>
+      <c r="S29" s="9"/>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="B30" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F30" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="L30" s="9"/>
+      <c r="M30" s="9"/>
+      <c r="N30" s="9"/>
+      <c r="O30" s="9"/>
+      <c r="P30" s="9"/>
+      <c r="Q30" s="9"/>
+      <c r="R30" s="9"/>
+      <c r="S30" s="9"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="51" t="s">
-        <v>85</v>
-      </c>
-      <c r="B31" s="51" t="s">
-        <v>44</v>
-      </c>
-      <c r="C31" s="51" t="s">
-        <v>86</v>
-      </c>
-      <c r="D31" s="51" t="s">
-        <v>87</v>
-      </c>
-      <c r="E31" s="51" t="s">
-        <v>88</v>
-      </c>
-      <c r="F31" s="51" t="s">
-        <v>63</v>
-      </c>
-      <c r="G31" s="51" t="s">
-        <v>89</v>
-      </c>
-      <c r="H31" s="51" t="s">
-        <v>90</v>
-      </c>
-      <c r="I31" s="51" t="s">
-        <v>91</v>
-      </c>
+      <c r="A31" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="B31" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="L31" s="9"/>
+      <c r="M31" s="9"/>
+      <c r="N31" s="9"/>
+      <c r="O31" s="9"/>
+      <c r="P31" s="9"/>
+      <c r="Q31" s="9"/>
+      <c r="R31" s="9"/>
+      <c r="S31" s="9"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="B32" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="F32" s="0" t="n">
         <v>1</v>
       </c>
       <c r="L32" s="9"/>
@@ -2092,7 +2154,7 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="B33" s="0" t="n">
         <v>1</v>
@@ -2111,7 +2173,7 @@
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="B34" s="0" t="n">
         <v>1</v>
@@ -2127,7 +2189,7 @@
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="B35" s="0" t="n">
         <v>1</v>
@@ -2143,7 +2205,7 @@
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="B36" s="0" t="n">
         <v>1</v>
@@ -2162,7 +2224,7 @@
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="B37" s="0" t="n">
         <v>1</v>
@@ -2178,9 +2240,12 @@
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="B38" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F38" s="0" t="n">
         <v>1</v>
       </c>
       <c r="L38" s="9"/>
@@ -2192,16 +2257,17 @@
       <c r="R38" s="9"/>
       <c r="S38" s="9"/>
     </row>
-    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="0" t="s">
-        <v>99</v>
-      </c>
-      <c r="B39" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="F39" s="0" t="n">
-        <v>1</v>
-      </c>
+    <row r="39" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="53" t="s">
+        <v>102</v>
+      </c>
+      <c r="B39" s="19" t="s">
+        <v>103</v>
+      </c>
+      <c r="C39" s="19"/>
+      <c r="D39" s="19"/>
+      <c r="E39" s="19"/>
+      <c r="F39" s="19"/>
       <c r="L39" s="9"/>
       <c r="M39" s="9"/>
       <c r="N39" s="9"/>
@@ -2211,13 +2277,15 @@
       <c r="R39" s="9"/>
       <c r="S39" s="9"/>
     </row>
-    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="0" t="s">
-        <v>100</v>
-      </c>
-      <c r="B40" s="0" t="n">
-        <v>1</v>
-      </c>
+    <row r="40" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="53"/>
+      <c r="B40" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="C40" s="19"/>
+      <c r="D40" s="19"/>
+      <c r="E40" s="19"/>
+      <c r="F40" s="19"/>
       <c r="L40" s="9"/>
       <c r="M40" s="9"/>
       <c r="N40" s="9"/>
@@ -2227,297 +2295,262 @@
       <c r="R40" s="9"/>
       <c r="S40" s="9"/>
     </row>
-    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="0" t="s">
-        <v>101</v>
-      </c>
-      <c r="B41" s="0" t="n">
+    <row r="41" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="54" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="55" t="s">
+        <v>105</v>
+      </c>
+      <c r="B42" s="55" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="56" t="n">
         <v>1</v>
       </c>
-      <c r="F41" s="0" t="n">
+      <c r="B43" s="57" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="56" t="n">
+        <v>3</v>
+      </c>
+      <c r="B44" s="57" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="56" t="n">
+        <v>2</v>
+      </c>
+      <c r="B45" s="57" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="56" t="n">
         <v>1</v>
       </c>
-      <c r="L41" s="9"/>
-      <c r="M41" s="9"/>
-      <c r="N41" s="9"/>
-      <c r="O41" s="9"/>
-      <c r="P41" s="9"/>
-      <c r="Q41" s="9"/>
-      <c r="R41" s="9"/>
-      <c r="S41" s="9"/>
-    </row>
-    <row r="43" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="52" t="s">
-        <v>102</v>
-      </c>
-      <c r="B43" s="19" t="s">
-        <v>103</v>
-      </c>
-      <c r="C43" s="19"/>
-      <c r="D43" s="19"/>
-      <c r="E43" s="19"/>
-      <c r="F43" s="19"/>
-      <c r="L43" s="9"/>
-      <c r="M43" s="9"/>
-      <c r="N43" s="9"/>
-      <c r="O43" s="9"/>
-      <c r="P43" s="9"/>
-      <c r="Q43" s="9"/>
-      <c r="R43" s="9"/>
-      <c r="S43" s="9"/>
-    </row>
-    <row r="44" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="52"/>
-      <c r="B44" s="19" t="s">
+      <c r="B46" s="57" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="49" t="s">
+        <v>111</v>
+      </c>
+      <c r="B47" s="50" t="s">
+        <v>112</v>
+      </c>
+      <c r="C47" s="50"/>
+      <c r="D47" s="50"/>
+      <c r="E47" s="50"/>
+      <c r="F47" s="50"/>
+      <c r="G47" s="50"/>
+    </row>
+    <row r="48" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="49"/>
+      <c r="B48" s="50" t="s">
         <v>17</v>
       </c>
-      <c r="C44" s="19"/>
-      <c r="D44" s="19"/>
-      <c r="E44" s="19"/>
-      <c r="F44" s="19"/>
-      <c r="L44" s="9"/>
-      <c r="M44" s="9"/>
-      <c r="N44" s="9"/>
-      <c r="O44" s="9"/>
-      <c r="P44" s="9"/>
-      <c r="Q44" s="9"/>
-      <c r="R44" s="9"/>
-      <c r="S44" s="9"/>
-    </row>
-    <row r="46" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="53" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="54" t="s">
-        <v>105</v>
-      </c>
-      <c r="B47" s="54" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="55" t="n">
-        <v>1</v>
-      </c>
-      <c r="B48" s="56" t="s">
-        <v>107</v>
-      </c>
+      <c r="C48" s="50"/>
+      <c r="D48" s="50"/>
+      <c r="E48" s="50"/>
+      <c r="F48" s="50"/>
+      <c r="G48" s="50"/>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="55" t="n">
-        <v>3</v>
-      </c>
-      <c r="B49" s="56" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="55" t="n">
-        <v>2</v>
-      </c>
-      <c r="B50" s="56" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="55" t="n">
-        <v>1</v>
-      </c>
-      <c r="B51" s="56" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="53" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="49" t="s">
-        <v>111</v>
-      </c>
-      <c r="B53" s="50" t="s">
-        <v>112</v>
-      </c>
-      <c r="C53" s="50"/>
-      <c r="D53" s="50"/>
-      <c r="E53" s="50"/>
-      <c r="F53" s="50"/>
-    </row>
-    <row r="54" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="49"/>
-      <c r="B54" s="50" t="s">
+      <c r="A49" s="58" t="s">
+        <v>113</v>
+      </c>
+      <c r="B49" s="52" t="s">
+        <v>44</v>
+      </c>
+      <c r="C49" s="52" t="s">
+        <v>86</v>
+      </c>
+      <c r="D49" s="52" t="s">
+        <v>87</v>
+      </c>
+      <c r="E49" s="52" t="s">
+        <v>88</v>
+      </c>
+      <c r="F49" s="52" t="s">
+        <v>63</v>
+      </c>
+      <c r="G49" s="52" t="s">
+        <v>89</v>
+      </c>
+      <c r="H49" s="52" t="s">
+        <v>90</v>
+      </c>
+      <c r="I49" s="52" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="23.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A50" s="47" t="s">
+        <v>46</v>
+      </c>
+      <c r="B50" s="47"/>
+      <c r="C50" s="47"/>
+      <c r="D50" s="47"/>
+      <c r="E50" s="47"/>
+      <c r="F50" s="59" t="s">
+        <v>114</v>
+      </c>
+      <c r="G50" s="60"/>
+      <c r="H50" s="60"/>
+      <c r="I50" s="60"/>
+    </row>
+    <row r="51" customFormat="false" ht="23.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A51" s="47" t="s">
+        <v>59</v>
+      </c>
+      <c r="B51" s="47" t="s">
+        <v>115</v>
+      </c>
+      <c r="C51" s="47"/>
+      <c r="D51" s="47"/>
+      <c r="E51" s="47"/>
+      <c r="F51" s="47"/>
+      <c r="G51" s="60"/>
+      <c r="H51" s="60"/>
+      <c r="I51" s="60"/>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="47" t="s">
+        <v>53</v>
+      </c>
+      <c r="B52" s="47" t="s">
+        <v>115</v>
+      </c>
+      <c r="C52" s="47"/>
+      <c r="D52" s="47"/>
+      <c r="E52" s="47"/>
+      <c r="F52" s="47"/>
+      <c r="G52" s="60"/>
+      <c r="H52" s="60"/>
+      <c r="I52" s="60"/>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="B53" s="47" t="s">
+        <v>115</v>
+      </c>
+      <c r="C53" s="47"/>
+      <c r="D53" s="47"/>
+      <c r="E53" s="47"/>
+      <c r="F53" s="47"/>
+      <c r="G53" s="60"/>
+      <c r="H53" s="60"/>
+      <c r="I53" s="60"/>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="47" t="s">
+        <v>80</v>
+      </c>
+      <c r="B54" s="47" t="s">
+        <v>115</v>
+      </c>
+      <c r="C54" s="47"/>
+      <c r="D54" s="47"/>
+      <c r="E54" s="47"/>
+      <c r="F54" s="47"/>
+      <c r="G54" s="60"/>
+      <c r="H54" s="60"/>
+      <c r="I54" s="60"/>
+    </row>
+    <row r="55" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="49" t="s">
+        <v>116</v>
+      </c>
+      <c r="B55" s="50" t="s">
+        <v>117</v>
+      </c>
+      <c r="C55" s="50"/>
+      <c r="D55" s="50"/>
+      <c r="E55" s="50"/>
+      <c r="F55" s="50"/>
+      <c r="G55" s="50"/>
+    </row>
+    <row r="56" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="49"/>
+      <c r="B56" s="50" t="s">
         <v>17</v>
       </c>
-      <c r="C54" s="50"/>
-      <c r="D54" s="50"/>
-      <c r="E54" s="50"/>
-      <c r="F54" s="50"/>
-    </row>
-    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="57" t="s">
-        <v>113</v>
-      </c>
-      <c r="B56" s="57" t="s">
+      <c r="C56" s="50"/>
+      <c r="D56" s="50"/>
+      <c r="E56" s="50"/>
+      <c r="F56" s="50"/>
+      <c r="G56" s="50"/>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="61" t="s">
+        <v>118</v>
+      </c>
+      <c r="B57" s="52" t="s">
         <v>44</v>
       </c>
-      <c r="C56" s="57" t="s">
+      <c r="C57" s="52" t="s">
         <v>86</v>
       </c>
-      <c r="D56" s="57" t="s">
+      <c r="D57" s="52" t="s">
         <v>87</v>
       </c>
-      <c r="E56" s="57" t="s">
+      <c r="E57" s="52" t="s">
         <v>88</v>
       </c>
-      <c r="F56" s="57" t="s">
+      <c r="F57" s="52" t="s">
         <v>63</v>
       </c>
-      <c r="G56" s="57" t="s">
+      <c r="G57" s="52" t="s">
         <v>89</v>
       </c>
-      <c r="H56" s="57" t="s">
+      <c r="H57" s="52" t="s">
         <v>90</v>
       </c>
-      <c r="I56" s="57" t="s">
+      <c r="I57" s="52" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="23.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A57" s="47" t="s">
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="47" t="s">
         <v>46</v>
       </c>
-      <c r="B57" s="47"/>
-      <c r="C57" s="47"/>
-      <c r="D57" s="47"/>
-      <c r="E57" s="47"/>
-      <c r="F57" s="58" t="s">
-        <v>114</v>
-      </c>
-      <c r="G57" s="59"/>
-      <c r="H57" s="59"/>
-      <c r="I57" s="59"/>
-    </row>
-    <row r="58" customFormat="false" ht="23.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A58" s="47" t="s">
-        <v>59</v>
-      </c>
-      <c r="B58" s="47" t="s">
-        <v>115</v>
-      </c>
-      <c r="C58" s="47"/>
-      <c r="D58" s="47"/>
-      <c r="E58" s="47"/>
-      <c r="F58" s="47"/>
-      <c r="G58" s="59"/>
-      <c r="H58" s="59"/>
-      <c r="I58" s="59"/>
+      <c r="B58" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="F58" s="0" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="47" t="s">
-        <v>53</v>
-      </c>
-      <c r="B59" s="47" t="s">
-        <v>115</v>
-      </c>
-      <c r="C59" s="47"/>
-      <c r="D59" s="47"/>
-      <c r="E59" s="47"/>
-      <c r="F59" s="47"/>
-      <c r="G59" s="59"/>
-      <c r="H59" s="59"/>
-      <c r="I59" s="59"/>
+        <v>59</v>
+      </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="47" t="s">
-        <v>71</v>
-      </c>
-      <c r="B60" s="47" t="s">
-        <v>115</v>
-      </c>
-      <c r="C60" s="47"/>
-      <c r="D60" s="47"/>
-      <c r="E60" s="47"/>
-      <c r="F60" s="47"/>
-      <c r="G60" s="59"/>
-      <c r="H60" s="59"/>
-      <c r="I60" s="59"/>
+        <v>53</v>
+      </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="47" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="47" t="s">
         <v>80</v>
       </c>
-      <c r="B61" s="47" t="s">
-        <v>115</v>
-      </c>
-      <c r="C61" s="47"/>
-      <c r="D61" s="47"/>
-      <c r="E61" s="47"/>
-      <c r="F61" s="47"/>
-      <c r="G61" s="59"/>
-      <c r="H61" s="59"/>
-      <c r="I61" s="59"/>
-    </row>
-    <row r="63" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="49" t="s">
-        <v>116</v>
-      </c>
-      <c r="B63" s="50" t="s">
-        <v>117</v>
-      </c>
-      <c r="C63" s="50"/>
-      <c r="D63" s="50"/>
-      <c r="E63" s="50"/>
-      <c r="F63" s="50"/>
-    </row>
-    <row r="64" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="49"/>
-      <c r="B64" s="50" t="s">
-        <v>17</v>
-      </c>
-      <c r="C64" s="50"/>
-      <c r="D64" s="50"/>
-      <c r="E64" s="50"/>
-      <c r="F64" s="50"/>
-    </row>
-    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="57" t="s">
-        <v>118</v>
-      </c>
-      <c r="B66" s="57" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="47" t="s">
-        <v>46</v>
-      </c>
-      <c r="B67" s="57" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="47" t="s">
-        <v>59</v>
-      </c>
-      <c r="B68" s="57"/>
-    </row>
-    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="47" t="s">
-        <v>53</v>
-      </c>
-      <c r="B69" s="57"/>
-    </row>
-    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="47" t="s">
-        <v>71</v>
-      </c>
-      <c r="B70" s="57" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="47" t="s">
-        <v>80</v>
-      </c>
-      <c r="B71" s="59"/>
     </row>
   </sheetData>
   <mergeCells count="24">
@@ -2529,22 +2562,22 @@
     <mergeCell ref="A11:A12"/>
     <mergeCell ref="B11:F11"/>
     <mergeCell ref="B12:F12"/>
-    <mergeCell ref="A14:E14"/>
-    <mergeCell ref="G14:K14"/>
-    <mergeCell ref="M14:Q14"/>
-    <mergeCell ref="R14:S14"/>
-    <mergeCell ref="A28:A29"/>
-    <mergeCell ref="B28:F28"/>
-    <mergeCell ref="B29:F29"/>
-    <mergeCell ref="A43:A44"/>
-    <mergeCell ref="B43:F43"/>
-    <mergeCell ref="B44:F44"/>
-    <mergeCell ref="A53:A54"/>
-    <mergeCell ref="B53:F53"/>
-    <mergeCell ref="B54:F54"/>
-    <mergeCell ref="A63:A64"/>
-    <mergeCell ref="B63:F63"/>
-    <mergeCell ref="B64:F64"/>
+    <mergeCell ref="A13:E13"/>
+    <mergeCell ref="G13:K13"/>
+    <mergeCell ref="M13:Q13"/>
+    <mergeCell ref="R13:S13"/>
+    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="B26:F26"/>
+    <mergeCell ref="B27:F27"/>
+    <mergeCell ref="A39:A40"/>
+    <mergeCell ref="B39:F39"/>
+    <mergeCell ref="B40:F40"/>
+    <mergeCell ref="A47:A48"/>
+    <mergeCell ref="B47:G47"/>
+    <mergeCell ref="B48:G48"/>
+    <mergeCell ref="A55:A56"/>
+    <mergeCell ref="B55:G55"/>
+    <mergeCell ref="B56:G56"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -2564,8 +2597,8 @@
   </sheetPr>
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -2578,198 +2611,198 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="60" t="s">
+      <c r="A1" s="62" t="s">
+        <v>120</v>
+      </c>
+      <c r="B1" s="62" t="s">
         <v>121</v>
       </c>
-      <c r="B1" s="60" t="s">
+      <c r="C1" s="62" t="s">
         <v>122</v>
       </c>
-      <c r="C1" s="60" t="s">
+      <c r="D1" s="62" t="s">
         <v>123</v>
       </c>
-      <c r="D1" s="60" t="s">
+      <c r="E1" s="62" t="s">
         <v>124</v>
       </c>
-      <c r="E1" s="60" t="s">
+    </row>
+    <row r="2" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="63" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2" s="63" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="61" t="s">
-        <v>80</v>
-      </c>
-      <c r="B2" s="61" t="s">
+      <c r="C2" s="64" t="s">
         <v>126</v>
       </c>
-      <c r="C2" s="62" t="s">
+      <c r="D2" s="64"/>
+      <c r="E2" s="63" t="s">
         <v>127</v>
       </c>
-      <c r="D2" s="62"/>
-      <c r="E2" s="61" t="s">
+    </row>
+    <row r="3" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="63" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="61" t="s">
+      <c r="B3" s="63" t="s">
         <v>129</v>
       </c>
-      <c r="B3" s="61" t="s">
+      <c r="C3" s="63"/>
+      <c r="D3" s="63"/>
+      <c r="E3" s="64" t="s">
         <v>130</v>
       </c>
-      <c r="C3" s="61"/>
-      <c r="D3" s="61"/>
-      <c r="E3" s="62" t="s">
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="63" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="61" t="s">
+      <c r="B4" s="63" t="s">
         <v>132</v>
       </c>
-      <c r="B4" s="61" t="s">
+      <c r="C4" s="63" t="s">
         <v>133</v>
       </c>
-      <c r="C4" s="61" t="s">
+      <c r="D4" s="63"/>
+      <c r="E4" s="63" t="s">
         <v>134</v>
       </c>
-      <c r="D4" s="61"/>
-      <c r="E4" s="61" t="s">
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="63" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="61" t="s">
+      <c r="B5" s="63" t="s">
         <v>136</v>
       </c>
-      <c r="B5" s="61" t="s">
+      <c r="C5" s="63" t="s">
         <v>137</v>
       </c>
-      <c r="C5" s="61" t="s">
+      <c r="D5" s="63"/>
+      <c r="E5" s="63" t="s">
         <v>138</v>
       </c>
-      <c r="D5" s="61"/>
-      <c r="E5" s="61" t="s">
+    </row>
+    <row r="6" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="63" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="61" t="s">
+      <c r="B6" s="63" t="s">
         <v>140</v>
       </c>
-      <c r="B6" s="61" t="s">
+      <c r="C6" s="63" t="s">
         <v>141</v>
       </c>
-      <c r="C6" s="61" t="s">
+      <c r="D6" s="63" t="s">
         <v>142</v>
       </c>
-      <c r="D6" s="61" t="s">
+      <c r="E6" s="64" t="s">
         <v>143</v>
       </c>
-      <c r="E6" s="62" t="s">
+    </row>
+    <row r="7" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="63" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="7" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="61" t="s">
+      <c r="B7" s="63" t="s">
         <v>145</v>
       </c>
-      <c r="B7" s="61" t="s">
+      <c r="C7" s="64" t="s">
         <v>146</v>
       </c>
-      <c r="C7" s="62" t="s">
+      <c r="D7" s="64"/>
+      <c r="E7" s="63" t="s">
         <v>147</v>
       </c>
-      <c r="D7" s="62"/>
-      <c r="E7" s="61" t="s">
+    </row>
+    <row r="8" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="63" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="8" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="61" t="s">
+      <c r="B8" s="63" t="s">
         <v>149</v>
       </c>
-      <c r="B8" s="61" t="s">
+      <c r="C8" s="64"/>
+      <c r="D8" s="64" t="s">
         <v>150</v>
       </c>
-      <c r="C8" s="62"/>
-      <c r="D8" s="62" t="s">
+      <c r="E8" s="63" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="63" t="s">
         <v>151</v>
       </c>
-      <c r="E8" s="61" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="61" t="s">
+      <c r="B9" s="63" t="s">
         <v>152</v>
       </c>
-      <c r="B9" s="61" t="s">
+      <c r="C9" s="63"/>
+      <c r="D9" s="63"/>
+      <c r="E9" s="63" t="s">
         <v>153</v>
       </c>
-      <c r="C9" s="61"/>
-      <c r="D9" s="61"/>
-      <c r="E9" s="61" t="s">
+    </row>
+    <row r="10" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="63" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="10" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="61" t="s">
+      <c r="B10" s="63" t="s">
         <v>155</v>
       </c>
-      <c r="B10" s="61" t="s">
+      <c r="C10" s="63" t="s">
         <v>156</v>
       </c>
-      <c r="C10" s="61" t="s">
+      <c r="D10" s="63"/>
+      <c r="E10" s="64" t="s">
         <v>157</v>
       </c>
-      <c r="D10" s="61"/>
-      <c r="E10" s="62" t="s">
+    </row>
+    <row r="11" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="63" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="11" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="61" t="s">
+      <c r="B11" s="63" t="s">
         <v>159</v>
       </c>
-      <c r="B11" s="61" t="s">
+      <c r="C11" s="63" t="s">
         <v>160</v>
       </c>
-      <c r="C11" s="61" t="s">
+      <c r="D11" s="63"/>
+      <c r="E11" s="64" t="s">
         <v>161</v>
       </c>
-      <c r="D11" s="61"/>
-      <c r="E11" s="62" t="s">
+    </row>
+    <row r="12" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="63" t="s">
+        <v>71</v>
+      </c>
+      <c r="B12" s="63" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="12" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="61" t="s">
-        <v>71</v>
-      </c>
-      <c r="B12" s="61" t="s">
+      <c r="C12" s="63" t="s">
         <v>163</v>
       </c>
-      <c r="C12" s="61" t="s">
+      <c r="D12" s="63"/>
+      <c r="E12" s="64" t="s">
         <v>164</v>
       </c>
-      <c r="D12" s="61"/>
-      <c r="E12" s="62" t="s">
+    </row>
+    <row r="13" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="63" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="13" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="61" t="s">
+      <c r="B13" s="64" t="s">
         <v>166</v>
       </c>
-      <c r="B13" s="62" t="s">
+      <c r="C13" s="63" t="s">
         <v>167</v>
       </c>
-      <c r="C13" s="61" t="s">
+      <c r="D13" s="63"/>
+      <c r="E13" s="64" t="s">
         <v>168</v>
-      </c>
-      <c r="D13" s="61"/>
-      <c r="E13" s="62" t="s">
-        <v>169</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se ajustan los scripts para guardar el cuadro de adjuntos, leerlos en python y crear los archivos
</commit_message>
<xml_diff>
--- a/Oficial/Patron_FL.xlsx
+++ b/Oficial/Patron_FL.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="311" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="375" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="BASE_SSE" sheetId="1" state="visible" r:id="rId2"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="169">
   <si>
     <t>SOLICITUD  DE SERVICIO EXTERNO A LABORATORIO</t>
   </si>
@@ -1222,8 +1222,8 @@
   </sheetPr>
   <dimension ref="A1:S62"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A34" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F59" activeCellId="0" sqref="F59"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A54" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A62" activeCellId="0" sqref="A62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -2541,6 +2541,12 @@
       <c r="A60" s="47" t="s">
         <v>53</v>
       </c>
+      <c r="B60" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="F60" s="0" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="47" t="s">
@@ -2548,8 +2554,11 @@
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="47" t="s">
+      <c r="A62" s="48" t="s">
         <v>80</v>
+      </c>
+      <c r="F62" s="0" t="s">
+        <v>119</v>
       </c>
     </row>
   </sheetData>
@@ -2598,7 +2607,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="1" sqref="A62 A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>

</xml_diff>

<commit_message>
Correccion en la generacion del csv de observaciones, esto en los valores de OBS en el script bash
</commit_message>
<xml_diff>
--- a/Oficial/Patron_FL.xlsx
+++ b/Oficial/Patron_FL.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="375" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="417" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="BASE_SSE" sheetId="1" state="visible" r:id="rId2"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="166">
   <si>
     <t>SOLICITUD  DE SERVICIO EXTERNO A LABORATORIO</t>
   </si>
@@ -66,10 +66,7 @@
     <t>Cuadro 1</t>
   </si>
   <si>
-    <t>Llenar columnas de A a F (jefe proyecto) y G a L (jefe de área)</t>
-  </si>
-  <si>
-    <t>Si requiere más espacios agregue o inserte filas</t>
+    <t>Si requiere más espacios agregue o inserte filas (borre los datos que hay ahora)</t>
   </si>
   <si>
     <t>Campo responsabilidad Jefe de Proyecto</t>
@@ -177,7 +174,7 @@
     <t>5 mg/L</t>
   </si>
   <si>
-    <t>ALS</t>
+    <t>ALS-ANTOFA</t>
   </si>
   <si>
     <t>US$</t>
@@ -195,7 +192,7 @@
     <t>7 mg/L</t>
   </si>
   <si>
-    <t>SGS</t>
+    <t>SGS-SANTIAGO</t>
   </si>
   <si>
     <t>metales totales</t>
@@ -357,7 +354,7 @@
     <t>Agregar todos los laboratorios y escribir en cada celda, relacionada con matriz, la observación en particular</t>
   </si>
   <si>
-    <t>Observaciones\Lab</t>
+    <t>Lab\Observaciones</t>
   </si>
   <si>
     <t>Se dobla cantidad de muestras de nitrito
@@ -414,9 +411,6 @@
 GABRIELA FRANYOLA (muestras)</t>
   </si>
   <si>
-    <t>SGS-SANTIAGO</t>
-  </si>
-  <si>
     <t>PUERTO MADERO 130. PUDAHUEL</t>
   </si>
   <si>
@@ -436,9 +430,6 @@
   </si>
   <si>
     <t>CECILIA TAPIA</t>
-  </si>
-  <si>
-    <t>ALS-ANTOFA</t>
   </si>
   <si>
     <t>JUAN GUTEMBERG N°438, GALPÓN 9 Y 10. ANTOFAGASTA</t>
@@ -539,10 +530,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
-    <numFmt numFmtId="165" formatCode="DD/MM/YYYY"/>
-    <numFmt numFmtId="166" formatCode="0.00"/>
+    <numFmt numFmtId="165" formatCode="0.00"/>
   </numFmts>
   <fonts count="17">
     <font>
@@ -610,16 +600,16 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="12"/>
-      <name val="arial"/>
+      <sz val="14"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
-      <sz val="14"/>
+      <sz val="10"/>
+      <color rgb="FF17365D"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -840,7 +830,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="66">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -913,11 +903,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="10" fillId="2" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="2" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="2" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -993,31 +979,31 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="4" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="5" fillId="4" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="4" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="5" fillId="4" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="5" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="5" fillId="5" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="5" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="5" fillId="5" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="6" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="5" fillId="6" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="6" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="5" fillId="6" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1033,6 +1019,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1041,7 +1031,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="7" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="7" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1083,6 +1073,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -1178,15 +1172,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>523440</xdr:colOff>
+      <xdr:colOff>550440</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>7560</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1084320</xdr:colOff>
+      <xdr:colOff>1110960</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>776160</xdr:rowOff>
+      <xdr:rowOff>775800</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1199,8 +1193,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="523440" y="7560"/>
-          <a:ext cx="560880" cy="768600"/>
+          <a:off x="550440" y="7560"/>
+          <a:ext cx="560520" cy="768240"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1222,8 +1216,8 @@
   </sheetPr>
   <dimension ref="A1:S62"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A54" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A62" activeCellId="0" sqref="A62"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A37" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A51" activeCellId="1" sqref="A59 A51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1434,7 +1428,7 @@
       <c r="R9" s="9"/>
       <c r="S9" s="9"/>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="17" t="s">
         <v>15</v>
       </c>
@@ -1445,7 +1439,7 @@
       <c r="D11" s="18"/>
       <c r="E11" s="18"/>
       <c r="F11" s="18"/>
-      <c r="G11" s="16"/>
+      <c r="G11" s="18"/>
       <c r="H11" s="16"/>
       <c r="I11" s="16"/>
       <c r="J11" s="16"/>
@@ -1461,14 +1455,14 @@
     </row>
     <row r="12" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="17"/>
-      <c r="B12" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="C12" s="19"/>
-      <c r="D12" s="19"/>
-      <c r="E12" s="19"/>
-      <c r="F12" s="19"/>
-      <c r="G12" s="16"/>
+      <c r="B12" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="18"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="18"/>
       <c r="H12" s="16"/>
       <c r="I12" s="16"/>
       <c r="J12" s="16"/>
@@ -1483,608 +1477,610 @@
       <c r="S12" s="9"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="20" t="s">
+      <c r="A13" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="19"/>
+      <c r="C13" s="19"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="19"/>
+      <c r="F13" s="19"/>
+      <c r="G13" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="20"/>
-      <c r="C13" s="20"/>
-      <c r="D13" s="20"/>
-      <c r="E13" s="20"/>
-      <c r="F13" s="20"/>
-      <c r="G13" s="21" t="s">
+      <c r="H13" s="20"/>
+      <c r="I13" s="20"/>
+      <c r="J13" s="20"/>
+      <c r="K13" s="20"/>
+      <c r="L13" s="21"/>
+      <c r="M13" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="H13" s="21"/>
-      <c r="I13" s="21"/>
-      <c r="J13" s="21"/>
-      <c r="K13" s="21"/>
-      <c r="L13" s="22"/>
-      <c r="M13" s="23" t="s">
+      <c r="N13" s="22"/>
+      <c r="O13" s="22"/>
+      <c r="P13" s="22"/>
+      <c r="Q13" s="22"/>
+      <c r="R13" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="N13" s="23"/>
-      <c r="O13" s="23"/>
-      <c r="P13" s="23"/>
-      <c r="Q13" s="23"/>
-      <c r="R13" s="24" t="s">
+      <c r="S13" s="23"/>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="S13" s="24"/>
-    </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="25" t="s">
+      <c r="B14" s="19"/>
+      <c r="C14" s="25"/>
+      <c r="D14" s="25"/>
+      <c r="E14" s="25"/>
+      <c r="F14" s="25"/>
+      <c r="G14" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="H14" s="26"/>
+      <c r="I14" s="26"/>
+      <c r="J14" s="27"/>
+      <c r="K14" s="28"/>
+      <c r="L14" s="28"/>
+      <c r="M14" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="N14" s="30"/>
+      <c r="O14" s="31"/>
+      <c r="P14" s="31"/>
+      <c r="Q14" s="32"/>
+      <c r="R14" s="33" t="s">
+        <v>21</v>
+      </c>
+      <c r="S14" s="34"/>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="B14" s="20"/>
-      <c r="C14" s="26"/>
-      <c r="D14" s="26"/>
-      <c r="E14" s="26"/>
-      <c r="F14" s="26"/>
-      <c r="G14" s="27" t="s">
+      <c r="B15" s="19"/>
+      <c r="C15" s="25"/>
+      <c r="D15" s="25"/>
+      <c r="E15" s="25"/>
+      <c r="F15" s="25"/>
+      <c r="G15" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="H14" s="27"/>
-      <c r="I14" s="27"/>
-      <c r="J14" s="28"/>
-      <c r="K14" s="29"/>
-      <c r="L14" s="29"/>
-      <c r="M14" s="30" t="s">
+      <c r="H15" s="26"/>
+      <c r="I15" s="26"/>
+      <c r="J15" s="27"/>
+      <c r="K15" s="28"/>
+      <c r="L15" s="28"/>
+      <c r="M15" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="N14" s="31"/>
-      <c r="O14" s="32"/>
-      <c r="P14" s="32"/>
-      <c r="Q14" s="33"/>
-      <c r="R14" s="34" t="s">
+      <c r="N15" s="30"/>
+      <c r="O15" s="35"/>
+      <c r="P15" s="35"/>
+      <c r="Q15" s="36"/>
+      <c r="R15" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="S14" s="35"/>
-    </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="25" t="s">
+      <c r="S15" s="23"/>
+    </row>
+    <row r="16" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="37" t="s">
         <v>23</v>
       </c>
-      <c r="B15" s="20"/>
-      <c r="C15" s="26"/>
-      <c r="D15" s="26"/>
-      <c r="E15" s="26"/>
-      <c r="F15" s="26"/>
-      <c r="G15" s="27" t="s">
-        <v>23</v>
-      </c>
-      <c r="H15" s="27"/>
-      <c r="I15" s="27"/>
-      <c r="J15" s="28"/>
-      <c r="K15" s="29"/>
-      <c r="L15" s="29"/>
-      <c r="M15" s="30" t="s">
-        <v>23</v>
-      </c>
-      <c r="N15" s="31"/>
-      <c r="O15" s="36"/>
-      <c r="P15" s="36"/>
-      <c r="Q15" s="37"/>
-      <c r="R15" s="34" t="s">
-        <v>23</v>
-      </c>
-      <c r="S15" s="24"/>
-    </row>
-    <row r="16" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="38" t="s">
+      <c r="B16" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="B16" s="38" t="s">
+      <c r="C16" s="37" t="s">
         <v>25</v>
       </c>
-      <c r="C16" s="38" t="s">
+      <c r="D16" s="37" t="s">
         <v>26</v>
       </c>
-      <c r="D16" s="38" t="s">
+      <c r="E16" s="37" t="s">
         <v>27</v>
       </c>
-      <c r="E16" s="38" t="s">
+      <c r="F16" s="37" t="s">
         <v>28</v>
       </c>
-      <c r="F16" s="38" t="s">
+      <c r="G16" s="38" t="s">
         <v>29</v>
       </c>
-      <c r="G16" s="39" t="s">
+      <c r="H16" s="38" t="s">
         <v>30</v>
       </c>
-      <c r="H16" s="39" t="s">
+      <c r="I16" s="38" t="s">
         <v>31</v>
       </c>
-      <c r="I16" s="39" t="s">
+      <c r="J16" s="38" t="s">
         <v>32</v>
       </c>
-      <c r="J16" s="39" t="s">
+      <c r="K16" s="38" t="s">
         <v>33</v>
       </c>
-      <c r="K16" s="39" t="s">
+      <c r="L16" s="39" t="s">
         <v>34</v>
       </c>
-      <c r="L16" s="40" t="s">
+      <c r="M16" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="M16" s="41" t="s">
+      <c r="N16" s="40" t="s">
         <v>36</v>
       </c>
-      <c r="N16" s="41" t="s">
+      <c r="O16" s="41" t="s">
         <v>37</v>
       </c>
-      <c r="O16" s="42" t="s">
+      <c r="P16" s="41" t="s">
         <v>38</v>
       </c>
-      <c r="P16" s="42" t="s">
+      <c r="Q16" s="41" t="s">
         <v>39</v>
       </c>
-      <c r="Q16" s="42" t="s">
+      <c r="R16" s="42" t="s">
         <v>40</v>
       </c>
-      <c r="R16" s="43" t="s">
+      <c r="S16" s="43" t="s">
         <v>41</v>
       </c>
-      <c r="S16" s="44" t="s">
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="44" t="n">
+        <v>10</v>
+      </c>
+      <c r="B17" s="45" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="45" t="n">
+      <c r="C17" s="44" t="n">
+        <v>1</v>
+      </c>
+      <c r="D17" s="46" t="s">
+        <v>43</v>
+      </c>
+      <c r="E17" s="44" t="s">
+        <v>44</v>
+      </c>
+      <c r="F17" s="44" t="n">
+        <v>0</v>
+      </c>
+      <c r="G17" s="44" t="s">
+        <v>45</v>
+      </c>
+      <c r="H17" s="44" t="s">
+        <v>46</v>
+      </c>
+      <c r="I17" s="44" t="s">
+        <v>47</v>
+      </c>
+      <c r="J17" s="44" t="s">
+        <v>48</v>
+      </c>
+      <c r="K17" s="44" t="n">
+        <v>0.35</v>
+      </c>
+      <c r="L17" s="44" t="s">
+        <v>49</v>
+      </c>
+      <c r="M17" s="45"/>
+      <c r="N17" s="45"/>
+      <c r="O17" s="45"/>
+      <c r="P17" s="45"/>
+      <c r="Q17" s="45"/>
+      <c r="R17" s="45"/>
+      <c r="S17" s="45"/>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="44" t="n">
         <v>10</v>
       </c>
-      <c r="B17" s="46" t="s">
+      <c r="B18" s="45" t="s">
+        <v>50</v>
+      </c>
+      <c r="C18" s="44" t="n">
+        <v>1</v>
+      </c>
+      <c r="D18" s="46" t="s">
         <v>43</v>
       </c>
-      <c r="C17" s="45" t="n">
+      <c r="E18" s="44" t="s">
+        <v>44</v>
+      </c>
+      <c r="F18" s="44" t="s">
+        <v>51</v>
+      </c>
+      <c r="G18" s="47" t="s">
+        <v>52</v>
+      </c>
+      <c r="H18" s="44" t="s">
+        <v>46</v>
+      </c>
+      <c r="I18" s="44" t="s">
+        <v>47</v>
+      </c>
+      <c r="J18" s="44" t="n">
+        <v>600</v>
+      </c>
+      <c r="K18" s="44" t="n">
+        <v>20</v>
+      </c>
+      <c r="L18" s="44" t="s">
+        <v>53</v>
+      </c>
+      <c r="M18" s="45"/>
+      <c r="N18" s="45"/>
+      <c r="O18" s="45"/>
+      <c r="P18" s="45"/>
+      <c r="Q18" s="45"/>
+      <c r="R18" s="45"/>
+      <c r="S18" s="45"/>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="44" t="n">
+        <v>10</v>
+      </c>
+      <c r="B19" s="45" t="s">
+        <v>54</v>
+      </c>
+      <c r="C19" s="44" t="n">
         <v>1</v>
       </c>
-      <c r="D17" s="47" t="s">
+      <c r="D19" s="46" t="s">
+        <v>43</v>
+      </c>
+      <c r="E19" s="44" t="s">
         <v>44</v>
       </c>
-      <c r="E17" s="45" t="s">
+      <c r="F19" s="44" t="s">
+        <v>55</v>
+      </c>
+      <c r="G19" s="44" t="s">
         <v>45</v>
       </c>
-      <c r="F17" s="45" t="n">
-        <v>0</v>
-      </c>
-      <c r="G17" s="45" t="s">
+      <c r="H19" s="44" t="s">
         <v>46</v>
       </c>
-      <c r="H17" s="45" t="s">
+      <c r="I19" s="44" t="s">
         <v>47</v>
       </c>
-      <c r="I17" s="45" t="s">
+      <c r="J19" s="44" t="s">
         <v>48</v>
       </c>
-      <c r="J17" s="45" t="s">
+      <c r="K19" s="44" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="L19" s="44" t="s">
         <v>49</v>
       </c>
-      <c r="K17" s="45" t="n">
-        <v>0.35</v>
-      </c>
-      <c r="L17" s="45" t="s">
-        <v>50</v>
-      </c>
-      <c r="M17" s="46"/>
-      <c r="N17" s="46"/>
-      <c r="O17" s="46"/>
-      <c r="P17" s="46"/>
-      <c r="Q17" s="46"/>
-      <c r="R17" s="46"/>
-      <c r="S17" s="46"/>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="45" t="n">
+      <c r="M19" s="45"/>
+      <c r="N19" s="45"/>
+      <c r="O19" s="45"/>
+      <c r="P19" s="45"/>
+      <c r="Q19" s="45"/>
+      <c r="R19" s="45"/>
+      <c r="S19" s="45"/>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="44" t="n">
         <v>10</v>
       </c>
-      <c r="B18" s="46" t="s">
-        <v>51</v>
-      </c>
-      <c r="C18" s="45" t="n">
+      <c r="B20" s="45" t="s">
+        <v>56</v>
+      </c>
+      <c r="C20" s="44" t="n">
         <v>1</v>
       </c>
-      <c r="D18" s="47" t="s">
+      <c r="D20" s="46" t="s">
+        <v>43</v>
+      </c>
+      <c r="E20" s="44" t="s">
         <v>44</v>
       </c>
-      <c r="E18" s="45" t="s">
+      <c r="F20" s="44" t="s">
+        <v>57</v>
+      </c>
+      <c r="G20" s="47" t="s">
+        <v>58</v>
+      </c>
+      <c r="H20" s="44" t="s">
+        <v>59</v>
+      </c>
+      <c r="I20" s="44" t="s">
+        <v>60</v>
+      </c>
+      <c r="J20" s="44" t="n">
+        <v>42</v>
+      </c>
+      <c r="K20" s="44" t="n">
+        <v>0.42</v>
+      </c>
+      <c r="L20" s="44" t="s">
+        <v>49</v>
+      </c>
+      <c r="M20" s="45"/>
+      <c r="N20" s="45"/>
+      <c r="O20" s="45"/>
+      <c r="P20" s="45"/>
+      <c r="Q20" s="45"/>
+      <c r="R20" s="45"/>
+      <c r="S20" s="45"/>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="44" t="n">
+        <v>3</v>
+      </c>
+      <c r="B21" s="45" t="s">
+        <v>61</v>
+      </c>
+      <c r="C21" s="44" t="n">
+        <v>1</v>
+      </c>
+      <c r="D21" s="46" t="s">
+        <v>62</v>
+      </c>
+      <c r="E21" s="44" t="s">
+        <v>44</v>
+      </c>
+      <c r="F21" s="44" t="s">
+        <v>63</v>
+      </c>
+      <c r="G21" s="44" t="s">
         <v>45</v>
       </c>
-      <c r="F18" s="45" t="s">
-        <v>52</v>
-      </c>
-      <c r="G18" s="45" t="s">
-        <v>53</v>
-      </c>
-      <c r="H18" s="45" t="s">
-        <v>47</v>
-      </c>
-      <c r="I18" s="45" t="s">
+      <c r="H21" s="44" t="s">
+        <v>64</v>
+      </c>
+      <c r="I21" s="44" t="s">
+        <v>65</v>
+      </c>
+      <c r="J21" s="44" t="n">
+        <v>42</v>
+      </c>
+      <c r="K21" s="44" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="L21" s="44" t="s">
+        <v>49</v>
+      </c>
+      <c r="M21" s="45"/>
+      <c r="N21" s="45"/>
+      <c r="O21" s="45"/>
+      <c r="P21" s="45"/>
+      <c r="Q21" s="45"/>
+      <c r="R21" s="45"/>
+      <c r="S21" s="45"/>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="44" t="n">
+        <v>3</v>
+      </c>
+      <c r="B22" s="45" t="s">
+        <v>66</v>
+      </c>
+      <c r="C22" s="44" t="n">
+        <v>1</v>
+      </c>
+      <c r="D22" s="46" t="s">
+        <v>62</v>
+      </c>
+      <c r="E22" s="44" t="s">
+        <v>44</v>
+      </c>
+      <c r="F22" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="G22" s="44" t="s">
+        <v>45</v>
+      </c>
+      <c r="H22" s="44" t="s">
+        <v>64</v>
+      </c>
+      <c r="I22" s="44" t="s">
+        <v>65</v>
+      </c>
+      <c r="J22" s="44" t="n">
+        <v>42</v>
+      </c>
+      <c r="K22" s="44" t="n">
+        <v>0.43</v>
+      </c>
+      <c r="L22" s="44" t="s">
+        <v>49</v>
+      </c>
+      <c r="M22" s="45"/>
+      <c r="N22" s="45"/>
+      <c r="O22" s="45"/>
+      <c r="P22" s="45"/>
+      <c r="Q22" s="45"/>
+      <c r="R22" s="45"/>
+      <c r="S22" s="45"/>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="44" t="n">
+        <v>10</v>
+      </c>
+      <c r="B23" s="45" t="s">
+        <v>68</v>
+      </c>
+      <c r="C23" s="44" t="n">
+        <v>1</v>
+      </c>
+      <c r="D23" s="46" t="s">
+        <v>43</v>
+      </c>
+      <c r="E23" s="44" t="s">
+        <v>44</v>
+      </c>
+      <c r="F23" s="44" t="s">
+        <v>69</v>
+      </c>
+      <c r="G23" s="44" t="s">
+        <v>70</v>
+      </c>
+      <c r="H23" s="44" t="s">
+        <v>71</v>
+      </c>
+      <c r="I23" s="44" t="s">
+        <v>72</v>
+      </c>
+      <c r="J23" s="44" t="n">
+        <v>8962</v>
+      </c>
+      <c r="K23" s="44" t="n">
+        <v>21580</v>
+      </c>
+      <c r="L23" s="44" t="s">
+        <v>73</v>
+      </c>
+      <c r="M23" s="45"/>
+      <c r="N23" s="45"/>
+      <c r="O23" s="45"/>
+      <c r="P23" s="45"/>
+      <c r="Q23" s="45"/>
+      <c r="R23" s="45"/>
+      <c r="S23" s="45"/>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="44" t="n">
+        <v>10</v>
+      </c>
+      <c r="B24" s="48" t="s">
+        <v>74</v>
+      </c>
+      <c r="C24" s="44" t="n">
+        <v>1</v>
+      </c>
+      <c r="D24" s="46" t="s">
+        <v>43</v>
+      </c>
+      <c r="E24" s="44" t="s">
+        <v>44</v>
+      </c>
+      <c r="F24" s="44" t="s">
+        <v>75</v>
+      </c>
+      <c r="G24" s="44" t="s">
+        <v>45</v>
+      </c>
+      <c r="H24" s="45" t="s">
+        <v>76</v>
+      </c>
+      <c r="I24" s="44" t="s">
+        <v>77</v>
+      </c>
+      <c r="J24" s="44" t="s">
         <v>48</v>
       </c>
-      <c r="J18" s="45" t="n">
-        <v>600</v>
-      </c>
-      <c r="K18" s="45" t="n">
-        <v>20</v>
-      </c>
-      <c r="L18" s="45" t="s">
-        <v>54</v>
-      </c>
-      <c r="M18" s="46"/>
-      <c r="N18" s="46"/>
-      <c r="O18" s="46"/>
-      <c r="P18" s="46"/>
-      <c r="Q18" s="46"/>
-      <c r="R18" s="46"/>
-      <c r="S18" s="46"/>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="45" t="n">
+      <c r="K24" s="44" t="n">
+        <v>0.43</v>
+      </c>
+      <c r="L24" s="44" t="s">
+        <v>49</v>
+      </c>
+      <c r="M24" s="45"/>
+      <c r="N24" s="45"/>
+      <c r="O24" s="45"/>
+      <c r="P24" s="45"/>
+      <c r="Q24" s="45"/>
+      <c r="R24" s="45"/>
+      <c r="S24" s="45"/>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="44" t="n">
         <v>10</v>
       </c>
-      <c r="B19" s="46" t="s">
-        <v>55</v>
-      </c>
-      <c r="C19" s="45" t="n">
+      <c r="B25" s="48" t="s">
+        <v>78</v>
+      </c>
+      <c r="C25" s="44" t="n">
         <v>1</v>
       </c>
-      <c r="D19" s="47" t="s">
+      <c r="D25" s="46" t="s">
+        <v>43</v>
+      </c>
+      <c r="E25" s="44" t="s">
         <v>44</v>
       </c>
-      <c r="E19" s="45" t="s">
-        <v>45</v>
-      </c>
-      <c r="F19" s="45" t="s">
-        <v>56</v>
-      </c>
-      <c r="G19" s="45" t="s">
-        <v>46</v>
-      </c>
-      <c r="H19" s="45" t="s">
-        <v>47</v>
-      </c>
-      <c r="I19" s="45" t="s">
-        <v>48</v>
-      </c>
-      <c r="J19" s="45" t="s">
-        <v>49</v>
-      </c>
-      <c r="K19" s="45" t="n">
-        <v>0.15</v>
-      </c>
-      <c r="L19" s="45" t="s">
-        <v>50</v>
-      </c>
-      <c r="M19" s="46"/>
-      <c r="N19" s="46"/>
-      <c r="O19" s="46"/>
-      <c r="P19" s="46"/>
-      <c r="Q19" s="46"/>
-      <c r="R19" s="46"/>
-      <c r="S19" s="46"/>
-    </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="45" t="n">
-        <v>10</v>
-      </c>
-      <c r="B20" s="46" t="s">
-        <v>57</v>
-      </c>
-      <c r="C20" s="45" t="n">
-        <v>1</v>
-      </c>
-      <c r="D20" s="47" t="s">
-        <v>44</v>
-      </c>
-      <c r="E20" s="45" t="s">
-        <v>45</v>
-      </c>
-      <c r="F20" s="45" t="s">
-        <v>58</v>
-      </c>
-      <c r="G20" s="45" t="s">
-        <v>59</v>
-      </c>
-      <c r="H20" s="45" t="s">
-        <v>60</v>
-      </c>
-      <c r="I20" s="45" t="s">
-        <v>61</v>
-      </c>
-      <c r="J20" s="45" t="n">
-        <v>42</v>
-      </c>
-      <c r="K20" s="45" t="n">
-        <v>0.42</v>
-      </c>
-      <c r="L20" s="45" t="s">
-        <v>50</v>
-      </c>
-      <c r="M20" s="46"/>
-      <c r="N20" s="46"/>
-      <c r="O20" s="46"/>
-      <c r="P20" s="46"/>
-      <c r="Q20" s="46"/>
-      <c r="R20" s="46"/>
-      <c r="S20" s="46"/>
-    </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="45" t="n">
-        <v>3</v>
-      </c>
-      <c r="B21" s="46" t="s">
-        <v>62</v>
-      </c>
-      <c r="C21" s="45" t="n">
-        <v>1</v>
-      </c>
-      <c r="D21" s="47" t="s">
-        <v>63</v>
-      </c>
-      <c r="E21" s="45" t="s">
-        <v>45</v>
-      </c>
-      <c r="F21" s="45" t="s">
-        <v>64</v>
-      </c>
-      <c r="G21" s="45" t="s">
-        <v>46</v>
-      </c>
-      <c r="H21" s="45" t="s">
-        <v>65</v>
-      </c>
-      <c r="I21" s="45" t="s">
-        <v>66</v>
-      </c>
-      <c r="J21" s="45" t="n">
-        <v>42</v>
-      </c>
-      <c r="K21" s="45" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="L21" s="45" t="s">
-        <v>50</v>
-      </c>
-      <c r="M21" s="46"/>
-      <c r="N21" s="46"/>
-      <c r="O21" s="46"/>
-      <c r="P21" s="46"/>
-      <c r="Q21" s="46"/>
-      <c r="R21" s="46"/>
-      <c r="S21" s="46"/>
-    </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="45" t="n">
-        <v>3</v>
-      </c>
-      <c r="B22" s="46" t="s">
-        <v>67</v>
-      </c>
-      <c r="C22" s="45" t="n">
-        <v>1</v>
-      </c>
-      <c r="D22" s="47" t="s">
-        <v>63</v>
-      </c>
-      <c r="E22" s="45" t="s">
-        <v>45</v>
-      </c>
-      <c r="F22" s="45" t="s">
-        <v>68</v>
-      </c>
-      <c r="G22" s="45" t="s">
-        <v>46</v>
-      </c>
-      <c r="H22" s="45" t="s">
-        <v>65</v>
-      </c>
-      <c r="I22" s="45" t="s">
-        <v>66</v>
-      </c>
-      <c r="J22" s="45" t="n">
-        <v>42</v>
-      </c>
-      <c r="K22" s="45" t="n">
-        <v>0.43</v>
-      </c>
-      <c r="L22" s="45" t="s">
-        <v>50</v>
-      </c>
-      <c r="M22" s="46"/>
-      <c r="N22" s="46"/>
-      <c r="O22" s="46"/>
-      <c r="P22" s="46"/>
-      <c r="Q22" s="46"/>
-      <c r="R22" s="46"/>
-      <c r="S22" s="46"/>
-    </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="45" t="n">
-        <v>10</v>
-      </c>
-      <c r="B23" s="46" t="s">
-        <v>69</v>
-      </c>
-      <c r="C23" s="45" t="n">
-        <v>1</v>
-      </c>
-      <c r="D23" s="47" t="s">
-        <v>44</v>
-      </c>
-      <c r="E23" s="45" t="s">
-        <v>45</v>
-      </c>
-      <c r="F23" s="45" t="s">
-        <v>70</v>
-      </c>
-      <c r="G23" s="45" t="s">
-        <v>71</v>
-      </c>
-      <c r="H23" s="45" t="s">
-        <v>72</v>
-      </c>
-      <c r="I23" s="45" t="s">
+      <c r="F25" s="45"/>
+      <c r="G25" s="44" t="s">
+        <v>79</v>
+      </c>
+      <c r="H25" s="44" t="s">
+        <v>80</v>
+      </c>
+      <c r="I25" s="44" t="s">
+        <v>81</v>
+      </c>
+      <c r="J25" s="44" t="n">
+        <v>5632</v>
+      </c>
+      <c r="K25" s="44" t="n">
+        <v>9123</v>
+      </c>
+      <c r="L25" s="44" t="s">
         <v>73</v>
       </c>
-      <c r="J23" s="45" t="n">
-        <v>8962</v>
-      </c>
-      <c r="K23" s="45" t="n">
-        <v>21580</v>
-      </c>
-      <c r="L23" s="45" t="s">
-        <v>74</v>
-      </c>
-      <c r="M23" s="46"/>
-      <c r="N23" s="46"/>
-      <c r="O23" s="46"/>
-      <c r="P23" s="46"/>
-      <c r="Q23" s="46"/>
-      <c r="R23" s="46"/>
-      <c r="S23" s="46"/>
-    </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="45" t="n">
-        <v>10</v>
-      </c>
-      <c r="B24" s="48" t="s">
-        <v>75</v>
-      </c>
-      <c r="C24" s="45" t="n">
-        <v>1</v>
-      </c>
-      <c r="D24" s="47" t="s">
-        <v>44</v>
-      </c>
-      <c r="E24" s="45" t="s">
-        <v>45</v>
-      </c>
-      <c r="F24" s="45" t="s">
-        <v>76</v>
-      </c>
-      <c r="G24" s="45" t="s">
-        <v>46</v>
-      </c>
-      <c r="H24" s="46" t="s">
-        <v>77</v>
-      </c>
-      <c r="I24" s="45" t="s">
-        <v>78</v>
-      </c>
-      <c r="J24" s="45" t="s">
-        <v>49</v>
-      </c>
-      <c r="K24" s="45" t="n">
-        <v>0.43</v>
-      </c>
-      <c r="L24" s="45" t="s">
-        <v>50</v>
-      </c>
-      <c r="M24" s="46"/>
-      <c r="N24" s="46"/>
-      <c r="O24" s="46"/>
-      <c r="P24" s="46"/>
-      <c r="Q24" s="46"/>
-      <c r="R24" s="46"/>
-      <c r="S24" s="46"/>
-    </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="45" t="n">
-        <v>10</v>
-      </c>
-      <c r="B25" s="48" t="s">
-        <v>79</v>
-      </c>
-      <c r="C25" s="45" t="n">
-        <v>1</v>
-      </c>
-      <c r="D25" s="47" t="s">
-        <v>44</v>
-      </c>
-      <c r="E25" s="45" t="s">
-        <v>45</v>
-      </c>
-      <c r="F25" s="46"/>
-      <c r="G25" s="45" t="s">
-        <v>80</v>
-      </c>
-      <c r="H25" s="45" t="s">
-        <v>81</v>
-      </c>
-      <c r="I25" s="45" t="s">
-        <v>82</v>
-      </c>
-      <c r="J25" s="45" t="n">
-        <v>5632</v>
-      </c>
-      <c r="K25" s="45" t="n">
-        <v>9123</v>
-      </c>
-      <c r="L25" s="45" t="s">
-        <v>74</v>
-      </c>
-      <c r="M25" s="46"/>
-      <c r="N25" s="46"/>
-      <c r="O25" s="46"/>
-      <c r="P25" s="46"/>
-      <c r="Q25" s="46"/>
-      <c r="R25" s="46"/>
-      <c r="S25" s="46"/>
+      <c r="M25" s="45"/>
+      <c r="N25" s="45"/>
+      <c r="O25" s="45"/>
+      <c r="P25" s="45"/>
+      <c r="Q25" s="45"/>
+      <c r="R25" s="45"/>
+      <c r="S25" s="45"/>
     </row>
     <row r="26" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="49" t="s">
+        <v>82</v>
+      </c>
+      <c r="B26" s="50" t="s">
         <v>83</v>
-      </c>
-      <c r="B26" s="50" t="s">
-        <v>84</v>
       </c>
       <c r="C26" s="50"/>
       <c r="D26" s="50"/>
       <c r="E26" s="50"/>
       <c r="F26" s="50"/>
+      <c r="G26" s="50"/>
     </row>
     <row r="27" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="49"/>
       <c r="B27" s="50" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C27" s="50"/>
       <c r="D27" s="50"/>
       <c r="E27" s="50"/>
       <c r="F27" s="50"/>
+      <c r="G27" s="50"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="51" t="s">
+        <v>84</v>
+      </c>
+      <c r="B28" s="52" t="s">
+        <v>43</v>
+      </c>
+      <c r="C28" s="52" t="s">
         <v>85</v>
       </c>
-      <c r="B28" s="52" t="s">
-        <v>44</v>
-      </c>
-      <c r="C28" s="52" t="s">
+      <c r="D28" s="52" t="s">
         <v>86</v>
       </c>
-      <c r="D28" s="52" t="s">
+      <c r="E28" s="52" t="s">
         <v>87</v>
       </c>
-      <c r="E28" s="52" t="s">
+      <c r="F28" s="52" t="s">
+        <v>62</v>
+      </c>
+      <c r="G28" s="52" t="s">
         <v>88</v>
       </c>
-      <c r="F28" s="52" t="s">
-        <v>63</v>
-      </c>
-      <c r="G28" s="52" t="s">
+      <c r="H28" s="52" t="s">
         <v>89</v>
       </c>
-      <c r="H28" s="52" t="s">
+      <c r="I28" s="52" t="s">
         <v>90</v>
-      </c>
-      <c r="I28" s="52" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B29" s="0" t="n">
         <v>1</v>
@@ -2103,7 +2099,7 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B30" s="0" t="n">
         <v>1</v>
@@ -2122,7 +2118,7 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B31" s="0" t="n">
         <v>1</v>
@@ -2138,7 +2134,7 @@
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B32" s="0" t="n">
         <v>1</v>
@@ -2154,7 +2150,7 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B33" s="0" t="n">
         <v>1</v>
@@ -2173,7 +2169,7 @@
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B34" s="0" t="n">
         <v>1</v>
@@ -2189,7 +2185,7 @@
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B35" s="0" t="n">
         <v>1</v>
@@ -2205,7 +2201,7 @@
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B36" s="0" t="n">
         <v>1</v>
@@ -2224,7 +2220,7 @@
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B37" s="0" t="n">
         <v>1</v>
@@ -2240,7 +2236,7 @@
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B38" s="0" t="n">
         <v>1</v>
@@ -2259,15 +2255,16 @@
     </row>
     <row r="39" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="53" t="s">
+        <v>101</v>
+      </c>
+      <c r="B39" s="18" t="s">
         <v>102</v>
       </c>
-      <c r="B39" s="19" t="s">
-        <v>103</v>
-      </c>
-      <c r="C39" s="19"/>
-      <c r="D39" s="19"/>
-      <c r="E39" s="19"/>
-      <c r="F39" s="19"/>
+      <c r="C39" s="18"/>
+      <c r="D39" s="18"/>
+      <c r="E39" s="18"/>
+      <c r="F39" s="18"/>
+      <c r="G39" s="18"/>
       <c r="L39" s="9"/>
       <c r="M39" s="9"/>
       <c r="N39" s="9"/>
@@ -2279,13 +2276,14 @@
     </row>
     <row r="40" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="53"/>
-      <c r="B40" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="C40" s="19"/>
-      <c r="D40" s="19"/>
-      <c r="E40" s="19"/>
-      <c r="F40" s="19"/>
+      <c r="B40" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="C40" s="18"/>
+      <c r="D40" s="18"/>
+      <c r="E40" s="18"/>
+      <c r="F40" s="18"/>
+      <c r="G40" s="18"/>
       <c r="L40" s="9"/>
       <c r="M40" s="9"/>
       <c r="N40" s="9"/>
@@ -2297,15 +2295,15 @@
     </row>
     <row r="41" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="54" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="55" t="s">
+        <v>104</v>
+      </c>
+      <c r="B42" s="55" t="s">
         <v>105</v>
-      </c>
-      <c r="B42" s="55" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2313,7 +2311,7 @@
         <v>1</v>
       </c>
       <c r="B43" s="57" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2321,7 +2319,7 @@
         <v>3</v>
       </c>
       <c r="B44" s="57" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2329,7 +2327,7 @@
         <v>2</v>
       </c>
       <c r="B45" s="57" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2337,15 +2335,15 @@
         <v>1</v>
       </c>
       <c r="B46" s="57" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="49" t="s">
+        <v>110</v>
+      </c>
+      <c r="B47" s="50" t="s">
         <v>111</v>
-      </c>
-      <c r="B47" s="50" t="s">
-        <v>112</v>
       </c>
       <c r="C47" s="50"/>
       <c r="D47" s="50"/>
@@ -2356,7 +2354,7 @@
     <row r="48" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="49"/>
       <c r="B48" s="50" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C48" s="50"/>
       <c r="D48" s="50"/>
@@ -2366,199 +2364,199 @@
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="58" t="s">
+        <v>112</v>
+      </c>
+      <c r="B49" s="52" t="s">
+        <v>43</v>
+      </c>
+      <c r="C49" s="52" t="s">
+        <v>85</v>
+      </c>
+      <c r="D49" s="52" t="s">
+        <v>86</v>
+      </c>
+      <c r="E49" s="52" t="s">
+        <v>87</v>
+      </c>
+      <c r="F49" s="52" t="s">
+        <v>62</v>
+      </c>
+      <c r="G49" s="52" t="s">
+        <v>88</v>
+      </c>
+      <c r="H49" s="52" t="s">
+        <v>89</v>
+      </c>
+      <c r="I49" s="52" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="23.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A50" s="46" t="s">
+        <v>45</v>
+      </c>
+      <c r="B50" s="46"/>
+      <c r="C50" s="46"/>
+      <c r="D50" s="46"/>
+      <c r="E50" s="46"/>
+      <c r="F50" s="59" t="s">
         <v>113</v>
-      </c>
-      <c r="B49" s="52" t="s">
-        <v>44</v>
-      </c>
-      <c r="C49" s="52" t="s">
-        <v>86</v>
-      </c>
-      <c r="D49" s="52" t="s">
-        <v>87</v>
-      </c>
-      <c r="E49" s="52" t="s">
-        <v>88</v>
-      </c>
-      <c r="F49" s="52" t="s">
-        <v>63</v>
-      </c>
-      <c r="G49" s="52" t="s">
-        <v>89</v>
-      </c>
-      <c r="H49" s="52" t="s">
-        <v>90</v>
-      </c>
-      <c r="I49" s="52" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="50" customFormat="false" ht="23.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A50" s="47" t="s">
-        <v>46</v>
-      </c>
-      <c r="B50" s="47"/>
-      <c r="C50" s="47"/>
-      <c r="D50" s="47"/>
-      <c r="E50" s="47"/>
-      <c r="F50" s="59" t="s">
-        <v>114</v>
       </c>
       <c r="G50" s="60"/>
       <c r="H50" s="60"/>
       <c r="I50" s="60"/>
     </row>
     <row r="51" customFormat="false" ht="23.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A51" s="47" t="s">
-        <v>59</v>
-      </c>
-      <c r="B51" s="47" t="s">
-        <v>115</v>
-      </c>
-      <c r="C51" s="47"/>
-      <c r="D51" s="47"/>
-      <c r="E51" s="47"/>
-      <c r="F51" s="47"/>
+      <c r="A51" s="61" t="s">
+        <v>58</v>
+      </c>
+      <c r="B51" s="46" t="s">
+        <v>114</v>
+      </c>
+      <c r="C51" s="46"/>
+      <c r="D51" s="46"/>
+      <c r="E51" s="46"/>
+      <c r="F51" s="46"/>
       <c r="G51" s="60"/>
       <c r="H51" s="60"/>
       <c r="I51" s="60"/>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="47" t="s">
-        <v>53</v>
-      </c>
-      <c r="B52" s="47" t="s">
-        <v>115</v>
-      </c>
-      <c r="C52" s="47"/>
-      <c r="D52" s="47"/>
-      <c r="E52" s="47"/>
-      <c r="F52" s="47"/>
+      <c r="A52" s="61" t="s">
+        <v>52</v>
+      </c>
+      <c r="B52" s="46" t="s">
+        <v>114</v>
+      </c>
+      <c r="C52" s="46"/>
+      <c r="D52" s="46"/>
+      <c r="E52" s="46"/>
+      <c r="F52" s="46"/>
       <c r="G52" s="60"/>
       <c r="H52" s="60"/>
       <c r="I52" s="60"/>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="47" t="s">
-        <v>71</v>
-      </c>
-      <c r="B53" s="47" t="s">
-        <v>115</v>
-      </c>
-      <c r="C53" s="47"/>
-      <c r="D53" s="47"/>
-      <c r="E53" s="47"/>
-      <c r="F53" s="47"/>
+      <c r="A53" s="46" t="s">
+        <v>70</v>
+      </c>
+      <c r="B53" s="46" t="s">
+        <v>114</v>
+      </c>
+      <c r="C53" s="46"/>
+      <c r="D53" s="46"/>
+      <c r="E53" s="46"/>
+      <c r="F53" s="46"/>
       <c r="G53" s="60"/>
       <c r="H53" s="60"/>
       <c r="I53" s="60"/>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="47" t="s">
-        <v>80</v>
-      </c>
-      <c r="B54" s="47" t="s">
-        <v>115</v>
-      </c>
-      <c r="C54" s="47"/>
-      <c r="D54" s="47"/>
-      <c r="E54" s="47"/>
-      <c r="F54" s="47"/>
+      <c r="A54" s="46" t="s">
+        <v>79</v>
+      </c>
+      <c r="B54" s="46" t="s">
+        <v>114</v>
+      </c>
+      <c r="C54" s="46"/>
+      <c r="D54" s="46"/>
+      <c r="E54" s="46"/>
+      <c r="F54" s="46"/>
       <c r="G54" s="60"/>
       <c r="H54" s="60"/>
       <c r="I54" s="60"/>
     </row>
     <row r="55" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="49" t="s">
+      <c r="A55" s="53" t="s">
+        <v>115</v>
+      </c>
+      <c r="B55" s="18" t="s">
         <v>116</v>
       </c>
-      <c r="B55" s="50" t="s">
+      <c r="C55" s="18"/>
+      <c r="D55" s="18"/>
+      <c r="E55" s="18"/>
+      <c r="F55" s="18"/>
+      <c r="G55" s="18"/>
+    </row>
+    <row r="56" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="53"/>
+      <c r="B56" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="C56" s="18"/>
+      <c r="D56" s="18"/>
+      <c r="E56" s="18"/>
+      <c r="F56" s="18"/>
+      <c r="G56" s="18"/>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="62" t="s">
         <v>117</v>
       </c>
-      <c r="C55" s="50"/>
-      <c r="D55" s="50"/>
-      <c r="E55" s="50"/>
-      <c r="F55" s="50"/>
-      <c r="G55" s="50"/>
-    </row>
-    <row r="56" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="49"/>
-      <c r="B56" s="50" t="s">
-        <v>17</v>
-      </c>
-      <c r="C56" s="50"/>
-      <c r="D56" s="50"/>
-      <c r="E56" s="50"/>
-      <c r="F56" s="50"/>
-      <c r="G56" s="50"/>
-    </row>
-    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="61" t="s">
+      <c r="B57" s="52" t="s">
+        <v>43</v>
+      </c>
+      <c r="C57" s="52" t="s">
+        <v>85</v>
+      </c>
+      <c r="D57" s="52" t="s">
+        <v>86</v>
+      </c>
+      <c r="E57" s="52" t="s">
+        <v>87</v>
+      </c>
+      <c r="F57" s="52" t="s">
+        <v>62</v>
+      </c>
+      <c r="G57" s="52" t="s">
+        <v>88</v>
+      </c>
+      <c r="H57" s="52" t="s">
+        <v>89</v>
+      </c>
+      <c r="I57" s="52" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="46" t="s">
+        <v>45</v>
+      </c>
+      <c r="B58" s="0" t="s">
         <v>118</v>
       </c>
-      <c r="B57" s="52" t="s">
-        <v>44</v>
-      </c>
-      <c r="C57" s="52" t="s">
-        <v>86</v>
-      </c>
-      <c r="D57" s="52" t="s">
-        <v>87</v>
-      </c>
-      <c r="E57" s="52" t="s">
-        <v>88</v>
-      </c>
-      <c r="F57" s="52" t="s">
-        <v>63</v>
-      </c>
-      <c r="G57" s="52" t="s">
-        <v>89</v>
-      </c>
-      <c r="H57" s="52" t="s">
-        <v>90</v>
-      </c>
-      <c r="I57" s="52" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="47" t="s">
-        <v>46</v>
-      </c>
-      <c r="B58" s="0" t="s">
-        <v>119</v>
-      </c>
       <c r="F58" s="0" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="47" t="s">
-        <v>59</v>
+      <c r="A59" s="61" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="47" t="s">
-        <v>53</v>
+      <c r="A60" s="61" t="s">
+        <v>52</v>
       </c>
       <c r="B60" s="0" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F60" s="0" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="47" t="s">
-        <v>71</v>
+      <c r="A61" s="46" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="48" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F62" s="0" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
   </sheetData>
@@ -2569,18 +2567,18 @@
     <mergeCell ref="B5:F5"/>
     <mergeCell ref="B6:F6"/>
     <mergeCell ref="A11:A12"/>
-    <mergeCell ref="B11:F11"/>
-    <mergeCell ref="B12:F12"/>
+    <mergeCell ref="B11:G11"/>
+    <mergeCell ref="B12:G12"/>
     <mergeCell ref="A13:E13"/>
     <mergeCell ref="G13:K13"/>
     <mergeCell ref="M13:Q13"/>
     <mergeCell ref="R13:S13"/>
     <mergeCell ref="A26:A27"/>
-    <mergeCell ref="B26:F26"/>
-    <mergeCell ref="B27:F27"/>
+    <mergeCell ref="B26:G26"/>
+    <mergeCell ref="B27:G27"/>
     <mergeCell ref="A39:A40"/>
-    <mergeCell ref="B39:F39"/>
-    <mergeCell ref="B40:F40"/>
+    <mergeCell ref="B39:G39"/>
+    <mergeCell ref="B40:G40"/>
     <mergeCell ref="A47:A48"/>
     <mergeCell ref="B47:G47"/>
     <mergeCell ref="B48:G48"/>
@@ -2606,8 +2604,8 @@
   </sheetPr>
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="1" sqref="A62 A4"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A4" activeCellId="2" sqref="A59 A51 A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -2620,198 +2618,198 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="62" t="s">
+      <c r="A1" s="63" t="s">
+        <v>119</v>
+      </c>
+      <c r="B1" s="63" t="s">
         <v>120</v>
       </c>
-      <c r="B1" s="62" t="s">
+      <c r="C1" s="63" t="s">
         <v>121</v>
       </c>
-      <c r="C1" s="62" t="s">
+      <c r="D1" s="63" t="s">
         <v>122</v>
       </c>
-      <c r="D1" s="62" t="s">
+      <c r="E1" s="63" t="s">
         <v>123</v>
       </c>
-      <c r="E1" s="62" t="s">
+    </row>
+    <row r="2" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="64" t="s">
+        <v>79</v>
+      </c>
+      <c r="B2" s="64" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="63" t="s">
-        <v>80</v>
-      </c>
-      <c r="B2" s="63" t="s">
+      <c r="C2" s="65" t="s">
         <v>125</v>
       </c>
-      <c r="C2" s="64" t="s">
+      <c r="D2" s="65"/>
+      <c r="E2" s="64" t="s">
         <v>126</v>
       </c>
-      <c r="D2" s="64"/>
-      <c r="E2" s="63" t="s">
+    </row>
+    <row r="3" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="64" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="63" t="s">
+      <c r="B3" s="64" t="s">
         <v>128</v>
       </c>
-      <c r="B3" s="63" t="s">
+      <c r="C3" s="64"/>
+      <c r="D3" s="64"/>
+      <c r="E3" s="65" t="s">
         <v>129</v>
       </c>
-      <c r="C3" s="63"/>
-      <c r="D3" s="63"/>
-      <c r="E3" s="64" t="s">
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="64" t="s">
+        <v>58</v>
+      </c>
+      <c r="B4" s="64" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="63" t="s">
+      <c r="C4" s="64" t="s">
         <v>131</v>
       </c>
-      <c r="B4" s="63" t="s">
+      <c r="D4" s="64"/>
+      <c r="E4" s="64" t="s">
         <v>132</v>
       </c>
-      <c r="C4" s="63" t="s">
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="64" t="s">
         <v>133</v>
       </c>
-      <c r="D4" s="63"/>
-      <c r="E4" s="63" t="s">
+      <c r="B5" s="64" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="63" t="s">
+      <c r="C5" s="64" t="s">
         <v>135</v>
       </c>
-      <c r="B5" s="63" t="s">
+      <c r="D5" s="64"/>
+      <c r="E5" s="64" t="s">
         <v>136</v>
       </c>
-      <c r="C5" s="63" t="s">
+    </row>
+    <row r="6" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="64" t="s">
+        <v>52</v>
+      </c>
+      <c r="B6" s="64" t="s">
         <v>137</v>
       </c>
-      <c r="D5" s="63"/>
-      <c r="E5" s="63" t="s">
+      <c r="C6" s="64" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="63" t="s">
+      <c r="D6" s="64" t="s">
         <v>139</v>
       </c>
-      <c r="B6" s="63" t="s">
+      <c r="E6" s="65" t="s">
         <v>140</v>
       </c>
-      <c r="C6" s="63" t="s">
+    </row>
+    <row r="7" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="64" t="s">
         <v>141</v>
       </c>
-      <c r="D6" s="63" t="s">
+      <c r="B7" s="64" t="s">
         <v>142</v>
       </c>
-      <c r="E6" s="64" t="s">
+      <c r="C7" s="65" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="7" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="63" t="s">
+      <c r="D7" s="65"/>
+      <c r="E7" s="64" t="s">
         <v>144</v>
       </c>
-      <c r="B7" s="63" t="s">
+    </row>
+    <row r="8" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="64" t="s">
         <v>145</v>
       </c>
-      <c r="C7" s="64" t="s">
+      <c r="B8" s="64" t="s">
         <v>146</v>
       </c>
-      <c r="D7" s="64"/>
-      <c r="E7" s="63" t="s">
+      <c r="C8" s="65"/>
+      <c r="D8" s="65" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="8" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="63" t="s">
+      <c r="E8" s="64" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="64" t="s">
         <v>148</v>
       </c>
-      <c r="B8" s="63" t="s">
+      <c r="B9" s="64" t="s">
         <v>149</v>
       </c>
-      <c r="C8" s="64"/>
-      <c r="D8" s="64" t="s">
+      <c r="C9" s="64"/>
+      <c r="D9" s="64"/>
+      <c r="E9" s="64" t="s">
         <v>150</v>
       </c>
-      <c r="E8" s="63" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="63" t="s">
+    </row>
+    <row r="10" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="64" t="s">
         <v>151</v>
       </c>
-      <c r="B9" s="63" t="s">
+      <c r="B10" s="64" t="s">
         <v>152</v>
       </c>
-      <c r="C9" s="63"/>
-      <c r="D9" s="63"/>
-      <c r="E9" s="63" t="s">
+      <c r="C10" s="64" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="10" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="63" t="s">
+      <c r="D10" s="64"/>
+      <c r="E10" s="65" t="s">
         <v>154</v>
       </c>
-      <c r="B10" s="63" t="s">
+    </row>
+    <row r="11" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="64" t="s">
         <v>155</v>
       </c>
-      <c r="C10" s="63" t="s">
+      <c r="B11" s="64" t="s">
         <v>156</v>
       </c>
-      <c r="D10" s="63"/>
-      <c r="E10" s="64" t="s">
+      <c r="C11" s="64" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="11" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="63" t="s">
+      <c r="D11" s="64"/>
+      <c r="E11" s="65" t="s">
         <v>158</v>
       </c>
-      <c r="B11" s="63" t="s">
+    </row>
+    <row r="12" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="64" t="s">
+        <v>70</v>
+      </c>
+      <c r="B12" s="64" t="s">
         <v>159</v>
       </c>
-      <c r="C11" s="63" t="s">
+      <c r="C12" s="64" t="s">
         <v>160</v>
       </c>
-      <c r="D11" s="63"/>
-      <c r="E11" s="64" t="s">
+      <c r="D12" s="64"/>
+      <c r="E12" s="65" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="63" t="s">
-        <v>71</v>
-      </c>
-      <c r="B12" s="63" t="s">
+    <row r="13" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="64" t="s">
         <v>162</v>
       </c>
-      <c r="C12" s="63" t="s">
+      <c r="B13" s="65" t="s">
         <v>163</v>
       </c>
-      <c r="D12" s="63"/>
-      <c r="E12" s="64" t="s">
+      <c r="C13" s="64" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="13" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="63" t="s">
+      <c r="D13" s="64"/>
+      <c r="E13" s="65" t="s">
         <v>165</v>
-      </c>
-      <c r="B13" s="64" t="s">
-        <v>166</v>
-      </c>
-      <c r="C13" s="63" t="s">
-        <v>167</v>
-      </c>
-      <c r="D13" s="63"/>
-      <c r="E13" s="64" t="s">
-        <v>168</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se añade lista de parámetros, en base al filtrado de una lista irregular de estos asociados a laboratorios
</commit_message>
<xml_diff>
--- a/Oficial/Patron_FL.xlsx
+++ b/Oficial/Patron_FL.xlsx
@@ -5,18 +5,19 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="417" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="375" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="BASE_SSE" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Labs" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Parametros" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="279">
   <si>
     <t>SOLICITUD  DE SERVICIO EXTERNO A LABORATORIO</t>
   </si>
@@ -411,6 +412,9 @@
 GABRIELA FRANYOLA (muestras)</t>
   </si>
   <si>
+    <t>SGS SANTIAGO</t>
+  </si>
+  <si>
     <t>PUERTO MADERO 130. PUDAHUEL</t>
   </si>
   <si>
@@ -420,7 +424,7 @@
     <t>LEYDI CORTÉS</t>
   </si>
   <si>
-    <t>SGS-ANTOFA</t>
+    <t>SGS ANTOFAGASTA</t>
   </si>
   <si>
     <t>PEDRO AGUIRRE CERDA N°7367. ANTOFAGASTA</t>
@@ -432,6 +436,9 @@
     <t>CECILIA TAPIA</t>
   </si>
   <si>
+    <t>ALS ANTOFAGASTA</t>
+  </si>
+  <si>
     <t>JUAN GUTEMBERG N°438, GALPÓN 9 Y 10. ANTOFAGASTA</t>
   </si>
   <si>
@@ -444,7 +451,7 @@
     <t>JOHANNA GONZALEZ</t>
   </si>
   <si>
-    <t>ALS-SANTIAGO</t>
+    <t>ALS SANTIAGO</t>
   </si>
   <si>
     <t>HERMANOS CARRERA PINTO 159, PAQUE INDUSTRIAL LOS LIBERTADOSRES COLINA</t>
@@ -524,6 +531,339 @@
   </si>
   <si>
     <t>JUAN MANDUCHER (Administración)</t>
+  </si>
+  <si>
+    <t>Nombre Parámetro</t>
+  </si>
+  <si>
+    <t>Conductividad total</t>
+  </si>
+  <si>
+    <t>Conductividad  disuelto</t>
+  </si>
+  <si>
+    <t>Feofitina total</t>
+  </si>
+  <si>
+    <t>Feofitina  disuelto</t>
+  </si>
+  <si>
+    <t>Fósforo total</t>
+  </si>
+  <si>
+    <t>Fósforo  disuelto</t>
+  </si>
+  <si>
+    <t>nitrato total</t>
+  </si>
+  <si>
+    <t>nitrato  disuelto</t>
+  </si>
+  <si>
+    <t>nitrito total</t>
+  </si>
+  <si>
+    <t>nitrito  disuelto</t>
+  </si>
+  <si>
+    <t>Oxígeno total</t>
+  </si>
+  <si>
+    <t>Oxígeno  disuelto</t>
+  </si>
+  <si>
+    <t>pH total</t>
+  </si>
+  <si>
+    <t>pH  disuelto</t>
+  </si>
+  <si>
+    <t>Salinidad total</t>
+  </si>
+  <si>
+    <t>Salinidad  disuelto</t>
+  </si>
+  <si>
+    <t>Sólidos total</t>
+  </si>
+  <si>
+    <t>Sólidos  disuelto</t>
+  </si>
+  <si>
+    <t>Sulfato total</t>
+  </si>
+  <si>
+    <t>Sulfato  disuelto</t>
+  </si>
+  <si>
+    <t>Temperatura total</t>
+  </si>
+  <si>
+    <t>Temperatura  disuelto</t>
+  </si>
+  <si>
+    <t>Turbiedad total</t>
+  </si>
+  <si>
+    <t>Turbiedad  disuelto</t>
+  </si>
+  <si>
+    <t>Clorofila total</t>
+  </si>
+  <si>
+    <t>Clorofila  disuelto</t>
+  </si>
+  <si>
+    <t>Cromo total</t>
+  </si>
+  <si>
+    <t>Cromo  disuelto</t>
+  </si>
+  <si>
+    <t>Color total</t>
+  </si>
+  <si>
+    <t>Color  disuelto</t>
+  </si>
+  <si>
+    <t>HAMs total</t>
+  </si>
+  <si>
+    <t>HAMs  disuelto</t>
+  </si>
+  <si>
+    <t>HAPs total</t>
+  </si>
+  <si>
+    <t>SGSSANTIAGO</t>
+  </si>
+  <si>
+    <t>HAPs  disuelto</t>
+  </si>
+  <si>
+    <t>Detergentes total</t>
+  </si>
+  <si>
+    <t>Detergentes  disuelto</t>
+  </si>
+  <si>
+    <t>Índice total</t>
+  </si>
+  <si>
+    <t>Índice  disuelto</t>
+  </si>
+  <si>
+    <t>Hidrocarburos total</t>
+  </si>
+  <si>
+    <t>Hidrocarburos  disuelto</t>
+  </si>
+  <si>
+    <t>Coliformes total</t>
+  </si>
+  <si>
+    <t>Coliformes  disuelto</t>
+  </si>
+  <si>
+    <t>DBO5 total</t>
+  </si>
+  <si>
+    <t>DBO5  disuelto</t>
+  </si>
+  <si>
+    <t>Nitrógeno total</t>
+  </si>
+  <si>
+    <t>Nitrógeno  disuelto</t>
+  </si>
+  <si>
+    <t>Cianuro total</t>
+  </si>
+  <si>
+    <t>Cianuro  disuelto</t>
+  </si>
+  <si>
+    <t>Fluoruro total</t>
+  </si>
+  <si>
+    <t>Fluoruro  disuelto</t>
+  </si>
+  <si>
+    <t>Aceites total</t>
+  </si>
+  <si>
+    <t>Aceites  disuelto</t>
+  </si>
+  <si>
+    <t>Cadmio total</t>
+  </si>
+  <si>
+    <t>U.CONCE</t>
+  </si>
+  <si>
+    <t>Cadmio  disuelto</t>
+  </si>
+  <si>
+    <t>Cobre total</t>
+  </si>
+  <si>
+    <t>Cobre  disuelto</t>
+  </si>
+  <si>
+    <t>Estaño total</t>
+  </si>
+  <si>
+    <t>Estaño  disuelto</t>
+  </si>
+  <si>
+    <t>Hierro total</t>
+  </si>
+  <si>
+    <t>Hierro  disuelto</t>
+  </si>
+  <si>
+    <t>Manganeso total</t>
+  </si>
+  <si>
+    <t>Manganeso  disuelto</t>
+  </si>
+  <si>
+    <t>Mercurio total</t>
+  </si>
+  <si>
+    <t>Mercurio  disuelto</t>
+  </si>
+  <si>
+    <t>Molibdeno total</t>
+  </si>
+  <si>
+    <t>Molibdeno  disuelto</t>
+  </si>
+  <si>
+    <t>Plomo total</t>
+  </si>
+  <si>
+    <t>Plomo  disuelto</t>
+  </si>
+  <si>
+    <t>Selenio total</t>
+  </si>
+  <si>
+    <t>Selenio  disuelto</t>
+  </si>
+  <si>
+    <t>Zinc total</t>
+  </si>
+  <si>
+    <t>Zinc  disuelto</t>
+  </si>
+  <si>
+    <t>Aluminio total</t>
+  </si>
+  <si>
+    <t>Aluminio  disuelto</t>
+  </si>
+  <si>
+    <t>Arsénico  disuelto</t>
+  </si>
+  <si>
+    <t>ALSSANTIAGO</t>
+  </si>
+  <si>
+    <t>COT total</t>
+  </si>
+  <si>
+    <t>COT  disuelto</t>
+  </si>
+  <si>
+    <t>GRANULOMETRIA total</t>
+  </si>
+  <si>
+    <t>AQUAGESTION</t>
+  </si>
+  <si>
+    <t>GRANULOMETRIA  disuelto</t>
+  </si>
+  <si>
+    <t>MATERIA total</t>
+  </si>
+  <si>
+    <t>MATERIA  disuelto</t>
+  </si>
+  <si>
+    <t>ACEITES total</t>
+  </si>
+  <si>
+    <t>ACEITES  disuelto</t>
+  </si>
+  <si>
+    <t>HIDROCARBUROS total</t>
+  </si>
+  <si>
+    <t>HIDROCARBUROS  disuelto</t>
+  </si>
+  <si>
+    <t>As total</t>
+  </si>
+  <si>
+    <t>As  disuelto</t>
+  </si>
+  <si>
+    <t>Cd total</t>
+  </si>
+  <si>
+    <t>Cd  disuelto</t>
+  </si>
+  <si>
+    <t>Cu total</t>
+  </si>
+  <si>
+    <t>Cu  disuelto</t>
+  </si>
+  <si>
+    <t>Cr total</t>
+  </si>
+  <si>
+    <t>Cr  disuelto</t>
+  </si>
+  <si>
+    <t>Hg total</t>
+  </si>
+  <si>
+    <t>Hg  disuelto</t>
+  </si>
+  <si>
+    <t>Mo total</t>
+  </si>
+  <si>
+    <t>Mo  disuelto</t>
+  </si>
+  <si>
+    <t>Pb total</t>
+  </si>
+  <si>
+    <t>Pb  disuelto</t>
+  </si>
+  <si>
+    <t>Se total</t>
+  </si>
+  <si>
+    <t>Se  disuelto</t>
+  </si>
+  <si>
+    <t>Zn total</t>
+  </si>
+  <si>
+    <t>Zn  disuelto</t>
+  </si>
+  <si>
+    <t>NITRÓGENO total</t>
+  </si>
+  <si>
+    <t>SGS</t>
+  </si>
+  <si>
+    <t>NITRÓGENO  disuelto</t>
   </si>
 </sst>
 </file>
@@ -830,7 +1170,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="67">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1093,6 +1433,10 @@
     </xf>
     <xf numFmtId="164" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -1216,8 +1560,8 @@
   </sheetPr>
   <dimension ref="A1:S62"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A37" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A51" activeCellId="1" sqref="A59 A51"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A31" activeCellId="0" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -2605,7 +2949,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="2" sqref="A59 A51 A4"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -2664,122 +3008,122 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="64" t="s">
-        <v>58</v>
+        <v>130</v>
       </c>
       <c r="B4" s="64" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C4" s="64" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D4" s="64"/>
       <c r="E4" s="64" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="64" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B5" s="64" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C5" s="64" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D5" s="64"/>
       <c r="E5" s="64" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="64" t="s">
-        <v>52</v>
+        <v>138</v>
       </c>
       <c r="B6" s="64" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C6" s="64" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="D6" s="64" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="E6" s="65" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="64" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="B7" s="64" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C7" s="65" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="D7" s="65"/>
       <c r="E7" s="64" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="64" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="B8" s="64" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="C8" s="65"/>
       <c r="D8" s="65" t="s">
+        <v>149</v>
+      </c>
+      <c r="E8" s="64" t="s">
         <v>147</v>
-      </c>
-      <c r="E8" s="64" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="64" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="B9" s="64" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="C9" s="64"/>
       <c r="D9" s="64"/>
       <c r="E9" s="64" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="64" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="B10" s="64" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="C10" s="64" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="D10" s="64"/>
       <c r="E10" s="65" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="64" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="B11" s="64" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="C11" s="64" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="D11" s="64"/>
       <c r="E11" s="65" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2787,29 +3131,1023 @@
         <v>70</v>
       </c>
       <c r="B12" s="64" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="C12" s="64" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="D12" s="64"/>
       <c r="E12" s="65" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="64" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="B13" s="65" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="C13" s="64" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="D13" s="64"/>
       <c r="E13" s="65" t="s">
-        <v>165</v>
+        <v>167</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B121"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E97" activeCellId="0" sqref="E97"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.265306122449"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.5561224489796"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="62" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>169</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>170</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>171</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>173</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>174</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>175</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>176</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>177</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>178</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>179</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>180</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>181</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>182</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>183</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>184</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>185</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>186</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>187</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>188</v>
+      </c>
+      <c r="B21" s="0" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>189</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>190</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>191</v>
+      </c>
+      <c r="B24" s="0" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>192</v>
+      </c>
+      <c r="B25" s="0" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>193</v>
+      </c>
+      <c r="B26" s="0" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>194</v>
+      </c>
+      <c r="B27" s="0" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>195</v>
+      </c>
+      <c r="B28" s="0" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>196</v>
+      </c>
+      <c r="B29" s="0" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
+        <v>197</v>
+      </c>
+      <c r="B30" s="0" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="s">
+        <v>198</v>
+      </c>
+      <c r="B31" s="0" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="s">
+        <v>199</v>
+      </c>
+      <c r="B32" s="0" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="s">
+        <v>200</v>
+      </c>
+      <c r="B33" s="0" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
+        <v>201</v>
+      </c>
+      <c r="B34" s="0" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="s">
+        <v>203</v>
+      </c>
+      <c r="B35" s="0" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="s">
+        <v>204</v>
+      </c>
+      <c r="B36" s="0" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="s">
+        <v>205</v>
+      </c>
+      <c r="B37" s="0" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="s">
+        <v>206</v>
+      </c>
+      <c r="B38" s="0" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="s">
+        <v>207</v>
+      </c>
+      <c r="B39" s="0" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0" t="s">
+        <v>208</v>
+      </c>
+      <c r="B40" s="0" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0" t="s">
+        <v>209</v>
+      </c>
+      <c r="B41" s="0" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="s">
+        <v>208</v>
+      </c>
+      <c r="B42" s="0" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0" t="s">
+        <v>209</v>
+      </c>
+      <c r="B43" s="0" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="0" t="s">
+        <v>208</v>
+      </c>
+      <c r="B44" s="0" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0" t="s">
+        <v>209</v>
+      </c>
+      <c r="B45" s="0" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="0" t="s">
+        <v>210</v>
+      </c>
+      <c r="B46" s="0" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="0" t="s">
+        <v>211</v>
+      </c>
+      <c r="B47" s="0" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="0" t="s">
+        <v>210</v>
+      </c>
+      <c r="B48" s="0" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="0" t="s">
+        <v>211</v>
+      </c>
+      <c r="B49" s="0" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="0" t="s">
+        <v>212</v>
+      </c>
+      <c r="B50" s="0" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="0" t="s">
+        <v>213</v>
+      </c>
+      <c r="B51" s="0" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="0" t="s">
+        <v>185</v>
+      </c>
+      <c r="B52" s="0" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="0" t="s">
+        <v>186</v>
+      </c>
+      <c r="B53" s="0" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="0" t="s">
+        <v>214</v>
+      </c>
+      <c r="B54" s="0" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="0" t="s">
+        <v>215</v>
+      </c>
+      <c r="B55" s="0" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="0" t="s">
+        <v>216</v>
+      </c>
+      <c r="B56" s="0" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="0" t="s">
+        <v>217</v>
+      </c>
+      <c r="B57" s="0" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="0" t="s">
+        <v>218</v>
+      </c>
+      <c r="B58" s="0" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="0" t="s">
+        <v>219</v>
+      </c>
+      <c r="B59" s="0" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="0" t="s">
+        <v>220</v>
+      </c>
+      <c r="B60" s="0" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="0" t="s">
+        <v>221</v>
+      </c>
+      <c r="B61" s="0" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="0" t="s">
+        <v>208</v>
+      </c>
+      <c r="B62" s="0" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="0" t="s">
+        <v>209</v>
+      </c>
+      <c r="B63" s="0" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="0" t="s">
+        <v>222</v>
+      </c>
+      <c r="B64" s="0" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="0" t="s">
+        <v>224</v>
+      </c>
+      <c r="B65" s="0" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="0" t="s">
+        <v>225</v>
+      </c>
+      <c r="B66" s="0" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="0" t="s">
+        <v>226</v>
+      </c>
+      <c r="B67" s="0" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="0" t="s">
+        <v>195</v>
+      </c>
+      <c r="B68" s="0" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="0" t="s">
+        <v>196</v>
+      </c>
+      <c r="B69" s="0" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="0" t="s">
+        <v>227</v>
+      </c>
+      <c r="B70" s="0" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="0" t="s">
+        <v>228</v>
+      </c>
+      <c r="B71" s="0" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="0" t="s">
+        <v>229</v>
+      </c>
+      <c r="B72" s="0" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="0" t="s">
+        <v>230</v>
+      </c>
+      <c r="B73" s="0" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="0" t="s">
+        <v>231</v>
+      </c>
+      <c r="B74" s="0" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="0" t="s">
+        <v>232</v>
+      </c>
+      <c r="B75" s="0" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="0" t="s">
+        <v>233</v>
+      </c>
+      <c r="B76" s="0" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="0" t="s">
+        <v>234</v>
+      </c>
+      <c r="B77" s="0" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="0" t="s">
+        <v>235</v>
+      </c>
+      <c r="B78" s="0" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="0" t="s">
+        <v>236</v>
+      </c>
+      <c r="B79" s="0" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="0" t="s">
+        <v>237</v>
+      </c>
+      <c r="B80" s="0" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="0" t="s">
+        <v>238</v>
+      </c>
+      <c r="B81" s="0" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="0" t="s">
+        <v>239</v>
+      </c>
+      <c r="B82" s="0" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="0" t="s">
+        <v>240</v>
+      </c>
+      <c r="B83" s="0" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="0" t="s">
+        <v>241</v>
+      </c>
+      <c r="B84" s="0" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="0" t="s">
+        <v>242</v>
+      </c>
+      <c r="B85" s="0" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="0" t="s">
+        <v>243</v>
+      </c>
+      <c r="B86" s="0" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="0" t="s">
+        <v>244</v>
+      </c>
+      <c r="B87" s="0" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="B88" s="0" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="0" t="s">
+        <v>245</v>
+      </c>
+      <c r="B89" s="0" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="0" t="s">
+        <v>201</v>
+      </c>
+      <c r="B90" s="0" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="0" t="s">
+        <v>203</v>
+      </c>
+      <c r="B91" s="0" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A92" s="0" t="s">
+        <v>247</v>
+      </c>
+      <c r="B92" s="0" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A93" s="0" t="s">
+        <v>248</v>
+      </c>
+      <c r="B93" s="0" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A94" s="0" t="s">
+        <v>249</v>
+      </c>
+      <c r="B94" s="0" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A95" s="0" t="s">
+        <v>251</v>
+      </c>
+      <c r="B95" s="0" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A96" s="0" t="s">
+        <v>252</v>
+      </c>
+      <c r="B96" s="0" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A97" s="0" t="s">
+        <v>253</v>
+      </c>
+      <c r="B97" s="0" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A98" s="0" t="s">
+        <v>254</v>
+      </c>
+      <c r="B98" s="0" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A99" s="0" t="s">
+        <v>255</v>
+      </c>
+      <c r="B99" s="0" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A100" s="0" t="s">
+        <v>256</v>
+      </c>
+      <c r="B100" s="0" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A101" s="0" t="s">
+        <v>257</v>
+      </c>
+      <c r="B101" s="0" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A102" s="0" t="s">
+        <v>258</v>
+      </c>
+      <c r="B102" s="66" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A103" s="0" t="s">
+        <v>259</v>
+      </c>
+      <c r="B103" s="66" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A104" s="0" t="s">
+        <v>260</v>
+      </c>
+      <c r="B104" s="66" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A105" s="0" t="s">
+        <v>261</v>
+      </c>
+      <c r="B105" s="66" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A106" s="0" t="s">
+        <v>262</v>
+      </c>
+      <c r="B106" s="66" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A107" s="0" t="s">
+        <v>263</v>
+      </c>
+      <c r="B107" s="66" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A108" s="0" t="s">
+        <v>264</v>
+      </c>
+      <c r="B108" s="66" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A109" s="0" t="s">
+        <v>265</v>
+      </c>
+      <c r="B109" s="66" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A110" s="0" t="s">
+        <v>266</v>
+      </c>
+      <c r="B110" s="66" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A111" s="0" t="s">
+        <v>267</v>
+      </c>
+      <c r="B111" s="66" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A112" s="0" t="s">
+        <v>268</v>
+      </c>
+      <c r="B112" s="66" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A113" s="0" t="s">
+        <v>269</v>
+      </c>
+      <c r="B113" s="66" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A114" s="0" t="s">
+        <v>270</v>
+      </c>
+      <c r="B114" s="66" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A115" s="0" t="s">
+        <v>271</v>
+      </c>
+      <c r="B115" s="66" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A116" s="0" t="s">
+        <v>272</v>
+      </c>
+      <c r="B116" s="66" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A117" s="0" t="s">
+        <v>273</v>
+      </c>
+      <c r="B117" s="66" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A118" s="0" t="s">
+        <v>274</v>
+      </c>
+      <c r="B118" s="66" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A119" s="0" t="s">
+        <v>275</v>
+      </c>
+      <c r="B119" s="66" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A120" s="0" t="s">
+        <v>276</v>
+      </c>
+      <c r="B120" s="0" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A121" s="0" t="s">
+        <v>278</v>
+      </c>
+      <c r="B121" s="0" t="s">
+        <v>277</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se hacen nuevos test, con las matrices que se toman en proyecto, se añade matriz de matrices medibles y sus relaciones agua-sedimento
</commit_message>
<xml_diff>
--- a/Oficial/Patron_FL.xlsx
+++ b/Oficial/Patron_FL.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="375" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="249" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="BASE_SSE" sheetId="1" state="visible" r:id="rId2"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="245">
   <si>
     <t>SOLICITUD  DE SERVICIO EXTERNO A LABORATORIO</t>
   </si>
@@ -151,18 +151,21 @@
     <t>Agua Marina</t>
   </si>
   <si>
+    <t>in situ</t>
+  </si>
+  <si>
+    <t>CEA-1</t>
+  </si>
+  <si>
+    <t>Feofitina total</t>
+  </si>
+  <si>
+    <t>Sedimento Marino</t>
+  </si>
+  <si>
     <t>SM 4020E</t>
   </si>
   <si>
-    <t>in situ</t>
-  </si>
-  <si>
-    <t>CEA-1</t>
-  </si>
-  <si>
-    <t>Feofitina total</t>
-  </si>
-  <si>
     <t>Fósforo  disuelto</t>
   </si>
   <si>
@@ -188,27 +191,6 @@
   </si>
   <si>
     <t>Estaciones\Matriz</t>
-  </si>
-  <si>
-    <t>Agua Salar</t>
-  </si>
-  <si>
-    <t>Agua Salar Dulce</t>
-  </si>
-  <si>
-    <t>Agua Dulce</t>
-  </si>
-  <si>
-    <t>Sedimento Marino</t>
-  </si>
-  <si>
-    <t>Sedimento Salar</t>
-  </si>
-  <si>
-    <t>Sedimento Salar Dulce</t>
-  </si>
-  <si>
-    <t>Sedimento Dulce</t>
   </si>
   <si>
     <t>RCA-01</t>
@@ -284,31 +266,37 @@
 Se dobla cantidad de muestras de nitrato</t>
   </si>
   <si>
+    <t>SGS SANTIAGO</t>
+  </si>
+  <si>
+    <t>Se solicita debido a que entrega es mas rapida</t>
+  </si>
+  <si>
+    <t>ALS ANTOFAGASTA</t>
+  </si>
+  <si>
+    <t>BIODIVERSA</t>
+  </si>
+  <si>
+    <t>HIDROLAB</t>
+  </si>
+  <si>
+    <t>Cuadro 5</t>
+  </si>
+  <si>
+    <t>Escribir en cada celda, solo 'si', si adjunta algún documento en particular para cada matriz y laboratorio</t>
+  </si>
+  <si>
+    <t>ADJUNTA</t>
+  </si>
+  <si>
+    <t>si</t>
+  </si>
+  <si>
     <t>SGS-SANTIAGO</t>
   </si>
   <si>
-    <t>Se solicita debido a que entrega es mas rapida</t>
-  </si>
-  <si>
     <t>ALS-ANTOFA</t>
-  </si>
-  <si>
-    <t>BIODIVERSA</t>
-  </si>
-  <si>
-    <t>HIDROLAB</t>
-  </si>
-  <si>
-    <t>Cuadro 5</t>
-  </si>
-  <si>
-    <t>Escribir en cada celda, solo 'si', si adjunta algún documento en particular para cada matriz y laboratorio</t>
-  </si>
-  <si>
-    <t>ADJUNTA</t>
-  </si>
-  <si>
-    <t>si</t>
   </si>
   <si>
     <t>LABORATORIO</t>
@@ -346,9 +334,6 @@
 GABRIELA FRANYOLA (muestras)</t>
   </si>
   <si>
-    <t>SGS SANTIAGO</t>
-  </si>
-  <si>
     <t>PUERTO MADERO 130. PUDAHUEL</t>
   </si>
   <si>
@@ -368,9 +353,6 @@
   </si>
   <si>
     <t>CECILIA TAPIA</t>
-  </si>
-  <si>
-    <t>ALS ANTOFAGASTA</t>
   </si>
   <si>
     <t>JUAN GUTEMBERG N°438, GALPÓN 9 Y 10. ANTOFAGASTA</t>
@@ -790,7 +772,7 @@
     <numFmt numFmtId="164" formatCode="GENERAL"/>
     <numFmt numFmtId="165" formatCode="0.00"/>
   </numFmts>
-  <fonts count="16">
+  <fonts count="17">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -897,6 +879,13 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF1F497D"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="10">
     <fill>
@@ -937,6 +926,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF99"/>
+        <bgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FF99FFFF"/>
         <bgColor rgb="FF66FFFF"/>
       </patternFill>
@@ -945,12 +940,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF66FFFF"/>
         <bgColor rgb="FF99FFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF99"/>
-        <bgColor rgb="FFFFFFCC"/>
       </patternFill>
     </fill>
   </fills>
@@ -1273,16 +1262,16 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="7" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="7" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="8" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="7" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="8" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="8" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="9" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
@@ -1317,7 +1306,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1325,10 +1318,6 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1337,7 +1326,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1426,15 +1415,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>577440</xdr:colOff>
+      <xdr:colOff>712440</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>7560</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1137600</xdr:colOff>
+      <xdr:colOff>1270800</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>775440</xdr:rowOff>
+      <xdr:rowOff>773640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1447,8 +1436,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="577440" y="7560"/>
-          <a:ext cx="560160" cy="767880"/>
+          <a:off x="712440" y="7560"/>
+          <a:ext cx="558360" cy="766080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1470,8 +1459,8 @@
   </sheetPr>
   <dimension ref="A1:S62"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D60" activeCellId="0" sqref="D60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1884,13 +1873,13 @@
         <v>42</v>
       </c>
       <c r="C17" s="44" t="n">
-        <v>1</v>
+        <v>-3</v>
       </c>
       <c r="D17" s="45" t="s">
         <v>43</v>
       </c>
-      <c r="E17" s="44" t="s">
-        <v>44</v>
+      <c r="E17" s="44" t="n">
+        <v>-1</v>
       </c>
       <c r="F17" s="44" t="n">
         <v>0</v>
@@ -1900,10 +1889,10 @@
         <v>CEA</v>
       </c>
       <c r="H17" s="44" t="s">
+        <v>44</v>
+      </c>
+      <c r="I17" s="44" t="s">
         <v>45</v>
-      </c>
-      <c r="I17" s="44" t="s">
-        <v>46</v>
       </c>
       <c r="J17" s="46" t="n">
         <f aca="false">+VLOOKUP(B17,Parametros!A$1:D$121,3,)</f>
@@ -1925,14 +1914,22 @@
       <c r="R17" s="47"/>
       <c r="S17" s="47"/>
     </row>
-    <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="44"/>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="44" t="n">
+        <v>11</v>
+      </c>
       <c r="B18" s="47" t="s">
+        <v>46</v>
+      </c>
+      <c r="C18" s="44" t="n">
+        <v>2</v>
+      </c>
+      <c r="D18" s="48" t="s">
         <v>47</v>
       </c>
-      <c r="C18" s="44"/>
-      <c r="D18" s="45"/>
-      <c r="E18" s="44"/>
+      <c r="E18" s="44" t="s">
+        <v>48</v>
+      </c>
       <c r="F18" s="44"/>
       <c r="G18" s="46" t="str">
         <f aca="false">+VLOOKUP(B18,Parametros!A$1:B$121,2,)</f>
@@ -1951,14 +1948,22 @@
       <c r="R18" s="47"/>
       <c r="S18" s="47"/>
     </row>
-    <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="44"/>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="44" t="n">
+        <v>12</v>
+      </c>
       <c r="B19" s="47" t="s">
+        <v>49</v>
+      </c>
+      <c r="C19" s="44" t="n">
+        <v>3</v>
+      </c>
+      <c r="D19" s="45" t="s">
+        <v>43</v>
+      </c>
+      <c r="E19" s="44" t="s">
         <v>48</v>
       </c>
-      <c r="C19" s="44"/>
-      <c r="D19" s="45"/>
-      <c r="E19" s="44"/>
       <c r="F19" s="44"/>
       <c r="G19" s="46" t="str">
         <f aca="false">+VLOOKUP(B19,Parametros!A$1:B$121,2,)</f>
@@ -1977,14 +1982,22 @@
       <c r="R19" s="47"/>
       <c r="S19" s="47"/>
     </row>
-    <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="44"/>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="44" t="n">
+        <v>13</v>
+      </c>
       <c r="B20" s="47" t="s">
         <v>42</v>
       </c>
-      <c r="C20" s="44"/>
-      <c r="D20" s="45"/>
-      <c r="E20" s="44"/>
+      <c r="C20" s="44" t="n">
+        <v>4</v>
+      </c>
+      <c r="D20" s="45" t="s">
+        <v>43</v>
+      </c>
+      <c r="E20" s="44" t="s">
+        <v>48</v>
+      </c>
       <c r="F20" s="44"/>
       <c r="G20" s="46" t="str">
         <f aca="false">+VLOOKUP(B20,Parametros!A$1:B$121,2,)</f>
@@ -2003,14 +2016,22 @@
       <c r="R20" s="47"/>
       <c r="S20" s="47"/>
     </row>
-    <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="44"/>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="44" t="n">
+        <v>14</v>
+      </c>
       <c r="B21" s="47" t="s">
-        <v>49</v>
-      </c>
-      <c r="C21" s="44"/>
-      <c r="D21" s="45"/>
-      <c r="E21" s="44"/>
+        <v>50</v>
+      </c>
+      <c r="C21" s="44" t="n">
+        <v>5</v>
+      </c>
+      <c r="D21" s="45" t="s">
+        <v>43</v>
+      </c>
+      <c r="E21" s="44" t="s">
+        <v>48</v>
+      </c>
       <c r="F21" s="44"/>
       <c r="G21" s="46" t="str">
         <f aca="false">+VLOOKUP(B21,Parametros!A$1:B$121,2,)</f>
@@ -2029,14 +2050,22 @@
       <c r="R21" s="47"/>
       <c r="S21" s="47"/>
     </row>
-    <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="44"/>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="44" t="n">
+        <v>15</v>
+      </c>
       <c r="B22" s="47" t="s">
-        <v>50</v>
-      </c>
-      <c r="C22" s="44"/>
-      <c r="D22" s="45"/>
-      <c r="E22" s="44"/>
+        <v>51</v>
+      </c>
+      <c r="C22" s="44" t="n">
+        <v>6</v>
+      </c>
+      <c r="D22" s="45" t="s">
+        <v>43</v>
+      </c>
+      <c r="E22" s="44" t="s">
+        <v>48</v>
+      </c>
       <c r="F22" s="44"/>
       <c r="G22" s="46" t="str">
         <f aca="false">+VLOOKUP(B22,Parametros!A$1:B$121,2,)</f>
@@ -2055,14 +2084,22 @@
       <c r="R22" s="47"/>
       <c r="S22" s="47"/>
     </row>
-    <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="44"/>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="44" t="n">
+        <v>16</v>
+      </c>
       <c r="B23" s="47" t="s">
-        <v>51</v>
-      </c>
-      <c r="C23" s="44"/>
-      <c r="D23" s="45"/>
-      <c r="E23" s="44"/>
+        <v>52</v>
+      </c>
+      <c r="C23" s="44" t="n">
+        <v>7</v>
+      </c>
+      <c r="D23" s="48" t="s">
+        <v>47</v>
+      </c>
+      <c r="E23" s="44" t="s">
+        <v>48</v>
+      </c>
       <c r="F23" s="44"/>
       <c r="G23" s="46" t="str">
         <f aca="false">+VLOOKUP(B23,Parametros!A$1:B$121,2,)</f>
@@ -2081,14 +2118,22 @@
       <c r="R23" s="47"/>
       <c r="S23" s="47"/>
     </row>
-    <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="44"/>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="44" t="n">
+        <v>17</v>
+      </c>
       <c r="B24" s="47" t="s">
-        <v>52</v>
-      </c>
-      <c r="C24" s="44"/>
-      <c r="D24" s="45"/>
-      <c r="E24" s="44"/>
+        <v>53</v>
+      </c>
+      <c r="C24" s="44" t="n">
+        <v>8</v>
+      </c>
+      <c r="D24" s="45" t="s">
+        <v>43</v>
+      </c>
+      <c r="E24" s="44" t="s">
+        <v>48</v>
+      </c>
       <c r="F24" s="44"/>
       <c r="G24" s="46" t="str">
         <f aca="false">+VLOOKUP(B24,Parametros!A$1:B$121,2,)</f>
@@ -2108,13 +2153,21 @@
       <c r="S24" s="47"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="44"/>
+      <c r="A25" s="44" t="n">
+        <v>18</v>
+      </c>
       <c r="B25" s="47" t="s">
-        <v>53</v>
-      </c>
-      <c r="C25" s="44"/>
-      <c r="D25" s="45"/>
-      <c r="E25" s="44"/>
+        <v>54</v>
+      </c>
+      <c r="C25" s="44" t="n">
+        <v>9</v>
+      </c>
+      <c r="D25" s="48" t="s">
+        <v>47</v>
+      </c>
+      <c r="E25" s="44" t="s">
+        <v>48</v>
+      </c>
       <c r="F25" s="47"/>
       <c r="G25" s="46" t="str">
         <f aca="false">+VLOOKUP(B25,Parametros!A$1:B$121,2,)</f>
@@ -2134,66 +2187,48 @@
       <c r="S25" s="47"/>
     </row>
     <row r="26" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="48" t="s">
-        <v>54</v>
-      </c>
-      <c r="B26" s="49" t="s">
+      <c r="A26" s="49" t="s">
         <v>55</v>
       </c>
-      <c r="C26" s="49"/>
-      <c r="D26" s="49"/>
-      <c r="E26" s="49"/>
-      <c r="F26" s="49"/>
-      <c r="G26" s="49"/>
+      <c r="B26" s="50" t="s">
+        <v>56</v>
+      </c>
+      <c r="C26" s="50"/>
+      <c r="D26" s="50"/>
+      <c r="E26" s="50"/>
+      <c r="F26" s="50"/>
+      <c r="G26" s="50"/>
     </row>
     <row r="27" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="48"/>
-      <c r="B27" s="49" t="s">
+      <c r="A27" s="49"/>
+      <c r="B27" s="50" t="s">
         <v>16</v>
       </c>
-      <c r="C27" s="49"/>
-      <c r="D27" s="49"/>
-      <c r="E27" s="49"/>
-      <c r="F27" s="49"/>
-      <c r="G27" s="49"/>
-    </row>
-    <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="50" t="s">
-        <v>56</v>
-      </c>
-      <c r="B28" s="51" t="s">
+      <c r="C27" s="50"/>
+      <c r="D27" s="50"/>
+      <c r="E27" s="50"/>
+      <c r="F27" s="50"/>
+      <c r="G27" s="50"/>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="51" t="s">
+        <v>57</v>
+      </c>
+      <c r="B28" s="48" t="s">
         <v>43</v>
       </c>
-      <c r="C28" s="51" t="s">
-        <v>57</v>
-      </c>
-      <c r="D28" s="51" t="s">
+      <c r="C28" s="48" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
         <v>58</v>
-      </c>
-      <c r="E28" s="51" t="s">
-        <v>59</v>
-      </c>
-      <c r="F28" s="51" t="s">
-        <v>60</v>
-      </c>
-      <c r="G28" s="51" t="s">
-        <v>61</v>
-      </c>
-      <c r="H28" s="51" t="s">
-        <v>62</v>
-      </c>
-      <c r="I28" s="51" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="s">
-        <v>64</v>
       </c>
       <c r="B29" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="F29" s="0" t="n">
+      <c r="C29" s="0" t="n">
         <v>1</v>
       </c>
       <c r="L29" s="9"/>
@@ -2205,14 +2240,14 @@
       <c r="R29" s="9"/>
       <c r="S29" s="9"/>
     </row>
-    <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="B30" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="F30" s="0" t="n">
+      <c r="C30" s="0" t="n">
         <v>1</v>
       </c>
       <c r="L30" s="9"/>
@@ -2224,9 +2259,9 @@
       <c r="R30" s="9"/>
       <c r="S30" s="9"/>
     </row>
-    <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="B31" s="0" t="n">
         <v>1</v>
@@ -2240,9 +2275,9 @@
       <c r="R31" s="9"/>
       <c r="S31" s="9"/>
     </row>
-    <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="B32" s="0" t="n">
         <v>1</v>
@@ -2256,14 +2291,14 @@
       <c r="R32" s="9"/>
       <c r="S32" s="9"/>
     </row>
-    <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="B33" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="F33" s="0" t="n">
+      <c r="C33" s="0" t="n">
         <v>1</v>
       </c>
       <c r="L33" s="9"/>
@@ -2275,9 +2310,9 @@
       <c r="R33" s="9"/>
       <c r="S33" s="9"/>
     </row>
-    <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="B34" s="0" t="n">
         <v>1</v>
@@ -2291,9 +2326,9 @@
       <c r="R34" s="9"/>
       <c r="S34" s="9"/>
     </row>
-    <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="B35" s="0" t="n">
         <v>1</v>
@@ -2307,14 +2342,14 @@
       <c r="R35" s="9"/>
       <c r="S35" s="9"/>
     </row>
-    <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="B36" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="F36" s="0" t="n">
+      <c r="C36" s="0" t="n">
         <v>1</v>
       </c>
       <c r="L36" s="9"/>
@@ -2326,9 +2361,9 @@
       <c r="R36" s="9"/>
       <c r="S36" s="9"/>
     </row>
-    <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B37" s="0" t="n">
         <v>1</v>
@@ -2342,14 +2377,14 @@
       <c r="R37" s="9"/>
       <c r="S37" s="9"/>
     </row>
-    <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="B38" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="F38" s="0" t="n">
+      <c r="C38" s="0" t="n">
         <v>1</v>
       </c>
       <c r="L38" s="9"/>
@@ -2363,10 +2398,10 @@
     </row>
     <row r="39" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="52" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="B39" s="18" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="C39" s="18"/>
       <c r="D39" s="18"/>
@@ -2403,15 +2438,15 @@
     </row>
     <row r="41" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="53" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="54" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="B42" s="54" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2419,7 +2454,7 @@
         <v>1</v>
       </c>
       <c r="B43" s="56" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2427,7 +2462,7 @@
         <v>3</v>
       </c>
       <c r="B44" s="56" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2435,7 +2470,7 @@
         <v>2</v>
       </c>
       <c r="B45" s="56" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2443,143 +2478,94 @@
         <v>1</v>
       </c>
       <c r="B46" s="56" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="48" t="s">
-        <v>83</v>
-      </c>
-      <c r="B47" s="49" t="s">
-        <v>84</v>
-      </c>
-      <c r="C47" s="49"/>
-      <c r="D47" s="49"/>
-      <c r="E47" s="49"/>
-      <c r="F47" s="49"/>
-      <c r="G47" s="49"/>
+      <c r="A47" s="49" t="s">
+        <v>77</v>
+      </c>
+      <c r="B47" s="50" t="s">
+        <v>78</v>
+      </c>
+      <c r="C47" s="50"/>
+      <c r="D47" s="50"/>
+      <c r="E47" s="50"/>
+      <c r="F47" s="50"/>
+      <c r="G47" s="50"/>
     </row>
     <row r="48" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="48"/>
-      <c r="B48" s="49" t="s">
+      <c r="A48" s="49"/>
+      <c r="B48" s="50" t="s">
         <v>16</v>
       </c>
-      <c r="C48" s="49"/>
-      <c r="D48" s="49"/>
-      <c r="E48" s="49"/>
-      <c r="F48" s="49"/>
-      <c r="G48" s="49"/>
-    </row>
-    <row r="49" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C48" s="50"/>
+      <c r="D48" s="50"/>
+      <c r="E48" s="50"/>
+      <c r="F48" s="50"/>
+      <c r="G48" s="50"/>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="57" t="s">
-        <v>85</v>
-      </c>
-      <c r="B49" s="51" t="s">
+        <v>79</v>
+      </c>
+      <c r="B49" s="48" t="s">
         <v>43</v>
       </c>
-      <c r="C49" s="51" t="s">
-        <v>57</v>
-      </c>
-      <c r="D49" s="51" t="s">
-        <v>58</v>
-      </c>
-      <c r="E49" s="51" t="s">
-        <v>59</v>
-      </c>
-      <c r="F49" s="51" t="s">
-        <v>60</v>
-      </c>
-      <c r="G49" s="51" t="s">
-        <v>61</v>
-      </c>
-      <c r="H49" s="51" t="s">
-        <v>62</v>
-      </c>
-      <c r="I49" s="51" t="s">
-        <v>63</v>
+      <c r="C49" s="48" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="23.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="45" t="s">
+        <v>80</v>
+      </c>
+      <c r="B50" s="58" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="23.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A51" s="59" t="s">
+        <v>82</v>
+      </c>
+      <c r="B51" s="45" t="s">
+        <v>83</v>
+      </c>
+      <c r="C51" s="45"/>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="59" t="s">
+        <v>84</v>
+      </c>
+      <c r="B52" s="45" t="s">
+        <v>83</v>
+      </c>
+      <c r="C52" s="45"/>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="45" t="s">
+        <v>85</v>
+      </c>
+      <c r="B53" s="45" t="s">
+        <v>83</v>
+      </c>
+      <c r="C53" s="45"/>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="45" t="s">
         <v>86</v>
       </c>
-      <c r="B50" s="45"/>
-      <c r="C50" s="45"/>
-      <c r="D50" s="45"/>
-      <c r="E50" s="45"/>
-      <c r="F50" s="58" t="s">
-        <v>87</v>
-      </c>
-      <c r="G50" s="59"/>
-      <c r="H50" s="59"/>
-      <c r="I50" s="59"/>
-    </row>
-    <row r="51" customFormat="false" ht="23.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A51" s="60" t="s">
-        <v>88</v>
-      </c>
-      <c r="B51" s="45" t="s">
-        <v>89</v>
-      </c>
-      <c r="C51" s="45"/>
-      <c r="D51" s="45"/>
-      <c r="E51" s="45"/>
-      <c r="F51" s="45"/>
-      <c r="G51" s="59"/>
-      <c r="H51" s="59"/>
-      <c r="I51" s="59"/>
-    </row>
-    <row r="52" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="60" t="s">
-        <v>90</v>
-      </c>
-      <c r="B52" s="45" t="s">
-        <v>89</v>
-      </c>
-      <c r="C52" s="45"/>
-      <c r="D52" s="45"/>
-      <c r="E52" s="45"/>
-      <c r="F52" s="45"/>
-      <c r="G52" s="59"/>
-      <c r="H52" s="59"/>
-      <c r="I52" s="59"/>
-    </row>
-    <row r="53" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="45" t="s">
-        <v>91</v>
-      </c>
-      <c r="B53" s="45" t="s">
-        <v>89</v>
-      </c>
-      <c r="C53" s="45"/>
-      <c r="D53" s="45"/>
-      <c r="E53" s="45"/>
-      <c r="F53" s="45"/>
-      <c r="G53" s="59"/>
-      <c r="H53" s="59"/>
-      <c r="I53" s="59"/>
-    </row>
-    <row r="54" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="45" t="s">
-        <v>92</v>
-      </c>
       <c r="B54" s="45" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="C54" s="45"/>
-      <c r="D54" s="45"/>
-      <c r="E54" s="45"/>
-      <c r="F54" s="45"/>
-      <c r="G54" s="59"/>
-      <c r="H54" s="59"/>
-      <c r="I54" s="59"/>
     </row>
     <row r="55" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="52" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="B55" s="18" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="C55" s="18"/>
       <c r="D55" s="18"/>
@@ -2598,73 +2584,55 @@
       <c r="F56" s="18"/>
       <c r="G56" s="18"/>
     </row>
-    <row r="57" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="61" t="s">
-        <v>95</v>
-      </c>
-      <c r="B57" s="51" t="s">
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="60" t="s">
+        <v>89</v>
+      </c>
+      <c r="B57" s="48" t="s">
         <v>43</v>
       </c>
-      <c r="C57" s="51" t="s">
-        <v>57</v>
-      </c>
-      <c r="D57" s="51" t="s">
-        <v>58</v>
-      </c>
-      <c r="E57" s="51" t="s">
-        <v>59</v>
-      </c>
-      <c r="F57" s="51" t="s">
-        <v>60</v>
-      </c>
-      <c r="G57" s="51" t="s">
-        <v>61</v>
-      </c>
-      <c r="H57" s="51" t="s">
-        <v>62</v>
-      </c>
-      <c r="I57" s="51" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="58" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C57" s="48" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="45" t="s">
+        <v>80</v>
+      </c>
+      <c r="B58" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="C58" s="0" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="61" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="61" t="s">
+        <v>92</v>
+      </c>
+      <c r="B60" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="C60" s="0" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="45" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="62" t="s">
         <v>86</v>
       </c>
-      <c r="B58" s="0" t="s">
-        <v>96</v>
-      </c>
-      <c r="F58" s="0" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="59" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="60" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="60" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="60" t="s">
+      <c r="C62" s="0" t="s">
         <v>90</v>
-      </c>
-      <c r="B60" s="0" t="s">
-        <v>96</v>
-      </c>
-      <c r="F60" s="0" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="61" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="45" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="62" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="62" t="s">
-        <v>92</v>
-      </c>
-      <c r="F62" s="0" t="s">
-        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -2710,10 +2678,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -2727,197 +2695,206 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="63" t="s">
+        <v>93</v>
+      </c>
+      <c r="B1" s="63" t="s">
+        <v>94</v>
+      </c>
+      <c r="C1" s="63" t="s">
+        <v>95</v>
+      </c>
+      <c r="D1" s="63" t="s">
+        <v>96</v>
+      </c>
+      <c r="E1" s="63" t="s">
         <v>97</v>
       </c>
-      <c r="B1" s="63" t="s">
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="64" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2" s="63"/>
+      <c r="C2" s="63"/>
+      <c r="D2" s="63"/>
+      <c r="E2" s="63"/>
+    </row>
+    <row r="3" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="59" t="s">
+        <v>86</v>
+      </c>
+      <c r="B3" s="59" t="s">
         <v>98</v>
       </c>
-      <c r="C1" s="63" t="s">
+      <c r="C3" s="65" t="s">
         <v>99</v>
       </c>
-      <c r="D1" s="63" t="s">
+      <c r="D3" s="65"/>
+      <c r="E3" s="59" t="s">
         <v>100</v>
       </c>
-      <c r="E1" s="63" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="64" t="s">
-        <v>92</v>
-      </c>
-      <c r="B2" s="64" t="s">
+    </row>
+    <row r="4" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="59" t="s">
+        <v>101</v>
+      </c>
+      <c r="B4" s="59" t="s">
         <v>102</v>
       </c>
-      <c r="C2" s="65" t="s">
+      <c r="C4" s="59"/>
+      <c r="D4" s="59"/>
+      <c r="E4" s="65" t="s">
         <v>103</v>
       </c>
-      <c r="D2" s="65"/>
-      <c r="E2" s="64" t="s">
+    </row>
+    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="59" t="s">
+        <v>82</v>
+      </c>
+      <c r="B5" s="59" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="64" t="s">
+      <c r="C5" s="59" t="s">
         <v>105</v>
       </c>
-      <c r="B3" s="64" t="s">
+      <c r="D5" s="59"/>
+      <c r="E5" s="59" t="s">
         <v>106</v>
       </c>
-      <c r="C3" s="64"/>
-      <c r="D3" s="64"/>
-      <c r="E3" s="65" t="s">
+    </row>
+    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="59" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="64" t="s">
+      <c r="B6" s="59" t="s">
         <v>108</v>
       </c>
-      <c r="B4" s="64" t="s">
+      <c r="C6" s="59" t="s">
         <v>109</v>
       </c>
-      <c r="C4" s="64" t="s">
+      <c r="D6" s="59"/>
+      <c r="E6" s="59" t="s">
         <v>110</v>
       </c>
-      <c r="D4" s="64"/>
-      <c r="E4" s="64" t="s">
+    </row>
+    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="59" t="s">
+        <v>84</v>
+      </c>
+      <c r="B7" s="59" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="64" t="s">
+      <c r="C7" s="59" t="s">
         <v>112</v>
       </c>
-      <c r="B5" s="64" t="s">
+      <c r="D7" s="59" t="s">
         <v>113</v>
       </c>
-      <c r="C5" s="64" t="s">
+      <c r="E7" s="65" t="s">
         <v>114</v>
       </c>
-      <c r="D5" s="64"/>
-      <c r="E5" s="64" t="s">
+    </row>
+    <row r="8" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="59" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="64" t="s">
+      <c r="B8" s="59" t="s">
         <v>116</v>
       </c>
-      <c r="B6" s="64" t="s">
+      <c r="C8" s="65" t="s">
         <v>117</v>
       </c>
-      <c r="C6" s="64" t="s">
+      <c r="D8" s="65"/>
+      <c r="E8" s="59" t="s">
         <v>118</v>
       </c>
-      <c r="D6" s="64" t="s">
+    </row>
+    <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="59" t="s">
         <v>119</v>
       </c>
-      <c r="E6" s="65" t="s">
+      <c r="B9" s="59" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="7" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="64" t="s">
+      <c r="C9" s="65"/>
+      <c r="D9" s="65" t="s">
         <v>121</v>
       </c>
-      <c r="B7" s="64" t="s">
+      <c r="E9" s="59" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="59" t="s">
         <v>122</v>
       </c>
-      <c r="C7" s="65" t="s">
+      <c r="B10" s="59" t="s">
         <v>123</v>
       </c>
-      <c r="D7" s="65"/>
-      <c r="E7" s="64" t="s">
+      <c r="C10" s="59"/>
+      <c r="D10" s="59"/>
+      <c r="E10" s="59" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="64" t="s">
+    <row r="11" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="59" t="s">
         <v>125</v>
       </c>
-      <c r="B8" s="64" t="s">
+      <c r="B11" s="59" t="s">
         <v>126</v>
       </c>
-      <c r="C8" s="65"/>
-      <c r="D8" s="65" t="s">
+      <c r="C11" s="59" t="s">
         <v>127</v>
       </c>
-      <c r="E8" s="64" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="64" t="s">
+      <c r="D11" s="59"/>
+      <c r="E11" s="65" t="s">
         <v>128</v>
       </c>
-      <c r="B9" s="64" t="s">
+    </row>
+    <row r="12" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="59" t="s">
         <v>129</v>
       </c>
-      <c r="C9" s="64"/>
-      <c r="D9" s="64"/>
-      <c r="E9" s="64" t="s">
+      <c r="B12" s="59" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="10" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="64" t="s">
+      <c r="C12" s="59" t="s">
         <v>131</v>
       </c>
-      <c r="B10" s="64" t="s">
+      <c r="D12" s="59"/>
+      <c r="E12" s="65" t="s">
         <v>132</v>
       </c>
-      <c r="C10" s="64" t="s">
+    </row>
+    <row r="13" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="59" t="s">
+        <v>85</v>
+      </c>
+      <c r="B13" s="59" t="s">
         <v>133</v>
       </c>
-      <c r="D10" s="64"/>
-      <c r="E10" s="65" t="s">
+      <c r="C13" s="59" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="11" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="64" t="s">
+      <c r="D13" s="59"/>
+      <c r="E13" s="65" t="s">
         <v>135</v>
       </c>
-      <c r="B11" s="64" t="s">
+    </row>
+    <row r="14" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="59" t="s">
         <v>136</v>
       </c>
-      <c r="C11" s="64" t="s">
+      <c r="B14" s="65" t="s">
         <v>137</v>
       </c>
-      <c r="D11" s="64"/>
-      <c r="E11" s="65" t="s">
+      <c r="C14" s="59" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="12" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="64" t="s">
-        <v>91</v>
-      </c>
-      <c r="B12" s="64" t="s">
+      <c r="D14" s="59"/>
+      <c r="E14" s="65" t="s">
         <v>139</v>
-      </c>
-      <c r="C12" s="64" t="s">
-        <v>140</v>
-      </c>
-      <c r="D12" s="64"/>
-      <c r="E12" s="65" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="64" t="s">
-        <v>142</v>
-      </c>
-      <c r="B13" s="65" t="s">
-        <v>143</v>
-      </c>
-      <c r="C13" s="64" t="s">
-        <v>144</v>
-      </c>
-      <c r="D13" s="64"/>
-      <c r="E13" s="65" t="s">
-        <v>145</v>
       </c>
     </row>
   </sheetData>
@@ -2954,175 +2931,175 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="61" t="s">
-        <v>146</v>
-      </c>
-      <c r="B1" s="61" t="s">
-        <v>147</v>
-      </c>
-      <c r="C1" s="61" t="s">
-        <v>148</v>
-      </c>
-      <c r="D1" s="61" t="s">
-        <v>149</v>
-      </c>
-      <c r="E1" s="61" t="s">
-        <v>150</v>
-      </c>
-      <c r="F1" s="61" t="s">
-        <v>151</v>
+      <c r="A1" s="60" t="s">
+        <v>140</v>
+      </c>
+      <c r="B1" s="60" t="s">
+        <v>141</v>
+      </c>
+      <c r="C1" s="60" t="s">
+        <v>142</v>
+      </c>
+      <c r="D1" s="60" t="s">
+        <v>143</v>
+      </c>
+      <c r="E1" s="60" t="s">
+        <v>144</v>
+      </c>
+      <c r="F1" s="60" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3130,266 +3107,266 @@
         <v>42</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>108</v>
+        <v>82</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>108</v>
+        <v>82</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>108</v>
+        <v>82</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>108</v>
+        <v>82</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>108</v>
+        <v>82</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>108</v>
+        <v>82</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>108</v>
+        <v>82</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>108</v>
+        <v>82</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>108</v>
+        <v>82</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>108</v>
+        <v>82</v>
       </c>
       <c r="D53" s="0" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="E53" s="0" t="str">
         <f aca="false">+VLOOKUP(D53,A1:B121,1)</f>
@@ -3398,546 +3375,546 @@
     </row>
     <row r="54" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>108</v>
+        <v>82</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>108</v>
+        <v>82</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>108</v>
+        <v>82</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>108</v>
+        <v>82</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="B58" s="0" t="s">
-        <v>108</v>
+        <v>82</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="B59" s="0" t="s">
-        <v>108</v>
+        <v>82</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="B60" s="0" t="s">
-        <v>108</v>
+        <v>82</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>108</v>
+        <v>82</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="B62" s="0" t="s">
-        <v>108</v>
+        <v>82</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="B63" s="0" t="s">
-        <v>108</v>
+        <v>82</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="B64" s="66" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="B65" s="66" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="B66" s="66" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="B67" s="66" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B68" s="66" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="B69" s="66" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="B70" s="66" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="B71" s="66" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="B72" s="66" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="B73" s="66" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="B74" s="66" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="B75" s="66" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="B76" s="66" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="B77" s="66" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="B78" s="66" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="B79" s="66" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="B80" s="66" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="B81" s="66" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="B82" s="66" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="B83" s="66" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="B84" s="66" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="B85" s="66" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="B86" s="66" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="B87" s="66" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="B88" s="66" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="B89" s="66" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="B90" s="0" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="B91" s="0" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="B92" s="0" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="B93" s="0" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="B94" s="0" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="B95" s="0" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="0" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="B96" s="0" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="0" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="B97" s="0" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="0" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="B98" s="0" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="0" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="B99" s="0" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="0" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="B100" s="0" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="0" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="B101" s="0" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="0" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="B102" s="66" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="0" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="B103" s="66" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="0" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="B104" s="66" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="0" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="B105" s="66" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="0" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="B106" s="66" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="0" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="B107" s="66" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="0" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="B108" s="66" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="0" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="B109" s="66" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="0" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="B110" s="66" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="0" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="B111" s="66" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="0" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="B112" s="66" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="0" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="B113" s="66" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="0" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="B114" s="66" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="0" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="B115" s="66" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="0" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="B116" s="66" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="0" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="B117" s="66" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="0" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="B118" s="66" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="0" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="B119" s="66" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="0" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="B120" s="0" t="s">
-        <v>108</v>
+        <v>82</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="0" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="B121" s="0" t="s">
-        <v>108</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Mejoras en indicaciones de planilla
</commit_message>
<xml_diff>
--- a/Oficial/Patron_FL.xlsx
+++ b/Oficial/Patron_FL.xlsx
@@ -11,13 +11,14 @@
     <sheet name="BASE_SSE" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Labs" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="Parametros" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Matrices" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="446" uniqueCount="251">
   <si>
     <t>SOLICITUD  DE SERVICIO EXTERNO A LABORATORIO</t>
   </si>
@@ -55,13 +56,16 @@
     <t>Fecha Solicitud</t>
   </si>
   <si>
-    <t>10-03-2015</t>
+    <t>(DD/MM/AA)</t>
   </si>
   <si>
     <t>Fecha Entrega de Material</t>
   </si>
   <si>
-    <t>15-03-2015</t>
+    <t>Quedan</t>
+  </si>
+  <si>
+    <t>Días</t>
   </si>
   <si>
     <t>Cuadro 1</t>
@@ -291,12 +295,6 @@
   </si>
   <si>
     <t>si</t>
-  </si>
-  <si>
-    <t>SGS-SANTIAGO</t>
-  </si>
-  <si>
-    <t>ALS-ANTOFA</t>
   </si>
   <si>
     <t>LABORATORIO</t>
@@ -762,22 +760,43 @@
   </si>
   <si>
     <t>NITRÓGENO  disuelto</t>
+  </si>
+  <si>
+    <t>Matrices-Agua\Matrices-Sedimento</t>
+  </si>
+  <si>
+    <t>Sedimento Salar</t>
+  </si>
+  <si>
+    <t>Sedimento Salar Dulce</t>
+  </si>
+  <si>
+    <t>Sedimento Dulce</t>
+  </si>
+  <si>
+    <t>Agua Salar</t>
+  </si>
+  <si>
+    <t>Agua Salar Dulce</t>
+  </si>
+  <si>
+    <t>Agua Dulce</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
-    <numFmt numFmtId="165" formatCode="0.00"/>
+    <numFmt numFmtId="165" formatCode="DD/MM/YY"/>
+    <numFmt numFmtId="166" formatCode="0.00"/>
   </numFmts>
-  <fonts count="17">
+  <fonts count="24">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -799,7 +818,6 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -807,69 +825,87 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="11"/>
+      <color rgb="FF3333FF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="12"/>
       <name val="arial"/>
       <family val="2"/>
-      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FFCC0066"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FF3333FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="1"/>
-      <charset val="1"/>
+      <sz val="14"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="16"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="14"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="14"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="14"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="12"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF17365D"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -877,17 +913,38 @@
       <color rgb="FF1F497D"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF1F497D"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FFFF3300"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <i val="true"/>
+      <sz val="10"/>
+      <color rgb="FF801900"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <i val="true"/>
+      <sz val="10"/>
+      <color rgb="FF0000CC"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -927,7 +984,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF99"/>
-        <bgColor rgb="FFFFFFCC"/>
+        <bgColor rgb="FFFFFF66"/>
       </patternFill>
     </fill>
     <fill>
@@ -940,6 +997,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF66FFFF"/>
         <bgColor rgb="FF99FFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF66"/>
+        <bgColor rgb="FFFFFF99"/>
       </patternFill>
     </fill>
   </fills>
@@ -1069,7 +1132,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="76">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1110,39 +1173,67 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="2" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="2" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="2" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="2" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1218,31 +1309,31 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="4" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="5" fillId="4" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="4" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="5" fillId="4" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="5" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="5" fillId="5" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="5" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="5" fillId="5" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="6" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="5" fillId="6" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="6" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="5" fillId="6" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1262,31 +1353,31 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="7" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="7" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="8" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="8" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="8" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="8" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="9" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="9" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="2" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="2" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1298,44 +1389,52 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="21" fillId="10" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="23" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -1353,15 +1452,15 @@
       <rgbColor rgb="FFFFFFFF"/>
       <rgbColor rgb="FFFF0000"/>
       <rgbColor rgb="FF00FF00"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF0000CC"/>
+      <rgbColor rgb="FFFFFF66"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF801900"/>
       <rgbColor rgb="FF008000"/>
       <rgbColor rgb="FF00000A"/>
       <rgbColor rgb="FF808000"/>
-      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FFCC0066"/>
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FFD9D9D9"/>
       <rgbColor rgb="FF808080"/>
@@ -1389,12 +1488,12 @@
       <rgbColor rgb="FFFF99CC"/>
       <rgbColor rgb="FFCC99FF"/>
       <rgbColor rgb="FFFFCCCC"/>
-      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF3333FF"/>
       <rgbColor rgb="FF66FFFF"/>
       <rgbColor rgb="FF99CC00"/>
       <rgbColor rgb="FFFFCC00"/>
       <rgbColor rgb="FFFF9900"/>
-      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FFFF3300"/>
       <rgbColor rgb="FF666699"/>
       <rgbColor rgb="FF969696"/>
       <rgbColor rgb="FF17365D"/>
@@ -1459,8 +1558,8 @@
   </sheetPr>
   <dimension ref="A1:S62"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D60" activeCellId="0" sqref="D60"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D19" activeCellId="0" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1521,7 +1620,7 @@
       <c r="R3" s="9"/>
       <c r="S3" s="9"/>
     </row>
-    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="10" t="s">
         <v>3</v>
       </c>
@@ -1546,7 +1645,7 @@
       <c r="R4" s="9"/>
       <c r="S4" s="9"/>
     </row>
-    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="12" t="s">
         <v>5</v>
       </c>
@@ -1571,8 +1670,8 @@
       <c r="R5" s="9"/>
       <c r="S5" s="9"/>
     </row>
-    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="12" t="s">
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="13" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="11" t="s">
@@ -1596,11 +1695,11 @@
       <c r="R6" s="9"/>
       <c r="S6" s="9"/>
     </row>
-    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="13" t="s">
+      <c r="B7" s="14" t="s">
         <v>10</v>
       </c>
       <c r="C7" s="8"/>
@@ -1622,13 +1721,15 @@
       <c r="S7" s="9"/>
     </row>
     <row r="8" customFormat="false" ht="15.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="12" t="s">
+      <c r="A8" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="15" t="n">
+        <v>42073</v>
+      </c>
+      <c r="C8" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="8"/>
       <c r="D8" s="8"/>
       <c r="E8" s="8"/>
       <c r="F8" s="8"/>
@@ -1646,22 +1747,31 @@
       <c r="R8" s="9"/>
       <c r="S8" s="9"/>
     </row>
-    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="15" t="s">
+    <row r="9" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="13" t="s">
+      <c r="B9" s="18" t="n">
+        <v>42083</v>
+      </c>
+      <c r="C9" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="16"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="16"/>
-      <c r="G9" s="16"/>
-      <c r="H9" s="16"/>
-      <c r="I9" s="16"/>
-      <c r="J9" s="16"/>
-      <c r="K9" s="16"/>
+      <c r="E9" s="21" t="n">
+        <f aca="false">+B9-B8</f>
+        <v>10</v>
+      </c>
+      <c r="F9" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="G9" s="23"/>
+      <c r="H9" s="23"/>
+      <c r="I9" s="23"/>
+      <c r="J9" s="23"/>
+      <c r="K9" s="23"/>
       <c r="L9" s="9"/>
       <c r="M9" s="9"/>
       <c r="N9" s="9"/>
@@ -1672,21 +1782,21 @@
       <c r="S9" s="9"/>
     </row>
     <row r="11" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="B11" s="18" t="s">
+      <c r="A11" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="18"/>
-      <c r="D11" s="18"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="18"/>
-      <c r="G11" s="18"/>
-      <c r="H11" s="16"/>
-      <c r="I11" s="16"/>
-      <c r="J11" s="16"/>
-      <c r="K11" s="16"/>
+      <c r="B11" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" s="25"/>
+      <c r="D11" s="25"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="25"/>
+      <c r="G11" s="25"/>
+      <c r="H11" s="23"/>
+      <c r="I11" s="23"/>
+      <c r="J11" s="23"/>
+      <c r="K11" s="23"/>
       <c r="L11" s="9"/>
       <c r="M11" s="9"/>
       <c r="N11" s="9"/>
@@ -1697,19 +1807,19 @@
       <c r="S11" s="9"/>
     </row>
     <row r="12" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="17"/>
-      <c r="B12" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="C12" s="18"/>
-      <c r="D12" s="18"/>
-      <c r="E12" s="18"/>
-      <c r="F12" s="18"/>
-      <c r="G12" s="18"/>
-      <c r="H12" s="16"/>
-      <c r="I12" s="16"/>
-      <c r="J12" s="16"/>
-      <c r="K12" s="16"/>
+      <c r="A12" s="24"/>
+      <c r="B12" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" s="25"/>
+      <c r="D12" s="25"/>
+      <c r="E12" s="25"/>
+      <c r="F12" s="25"/>
+      <c r="G12" s="25"/>
+      <c r="H12" s="23"/>
+      <c r="I12" s="23"/>
+      <c r="J12" s="23"/>
+      <c r="K12" s="23"/>
       <c r="L12" s="9"/>
       <c r="M12" s="9"/>
       <c r="N12" s="9"/>
@@ -1720,510 +1830,510 @@
       <c r="S12" s="9"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="B13" s="19"/>
-      <c r="C13" s="19"/>
-      <c r="D13" s="19"/>
-      <c r="E13" s="19"/>
-      <c r="F13" s="19"/>
-      <c r="G13" s="20" t="s">
+      <c r="A13" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="H13" s="20"/>
-      <c r="I13" s="20"/>
-      <c r="J13" s="20"/>
-      <c r="K13" s="20"/>
-      <c r="L13" s="21"/>
-      <c r="M13" s="22" t="s">
+      <c r="B13" s="26"/>
+      <c r="C13" s="26"/>
+      <c r="D13" s="26"/>
+      <c r="E13" s="26"/>
+      <c r="F13" s="26"/>
+      <c r="G13" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="N13" s="22"/>
-      <c r="O13" s="22"/>
-      <c r="P13" s="22"/>
-      <c r="Q13" s="22"/>
-      <c r="R13" s="23" t="s">
+      <c r="H13" s="27"/>
+      <c r="I13" s="27"/>
+      <c r="J13" s="27"/>
+      <c r="K13" s="27"/>
+      <c r="L13" s="28"/>
+      <c r="M13" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="S13" s="23"/>
+      <c r="N13" s="29"/>
+      <c r="O13" s="29"/>
+      <c r="P13" s="29"/>
+      <c r="Q13" s="29"/>
+      <c r="R13" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="S13" s="30"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="24" t="s">
-        <v>21</v>
-      </c>
-      <c r="B14" s="19"/>
-      <c r="C14" s="25"/>
-      <c r="D14" s="25"/>
-      <c r="E14" s="25"/>
-      <c r="F14" s="25"/>
-      <c r="G14" s="26" t="s">
-        <v>21</v>
-      </c>
-      <c r="H14" s="26"/>
-      <c r="I14" s="26"/>
-      <c r="J14" s="27"/>
-      <c r="K14" s="28"/>
-      <c r="L14" s="28"/>
-      <c r="M14" s="29" t="s">
-        <v>21</v>
-      </c>
-      <c r="N14" s="30"/>
-      <c r="O14" s="31"/>
-      <c r="P14" s="31"/>
-      <c r="Q14" s="32"/>
-      <c r="R14" s="33" t="s">
-        <v>21</v>
-      </c>
-      <c r="S14" s="34"/>
+      <c r="A14" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" s="26"/>
+      <c r="C14" s="32"/>
+      <c r="D14" s="32"/>
+      <c r="E14" s="32"/>
+      <c r="F14" s="32"/>
+      <c r="G14" s="33" t="s">
+        <v>22</v>
+      </c>
+      <c r="H14" s="33"/>
+      <c r="I14" s="33"/>
+      <c r="J14" s="34"/>
+      <c r="K14" s="35"/>
+      <c r="L14" s="35"/>
+      <c r="M14" s="36" t="s">
+        <v>22</v>
+      </c>
+      <c r="N14" s="37"/>
+      <c r="O14" s="38"/>
+      <c r="P14" s="38"/>
+      <c r="Q14" s="39"/>
+      <c r="R14" s="40" t="s">
+        <v>22</v>
+      </c>
+      <c r="S14" s="41"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="24" t="s">
-        <v>22</v>
-      </c>
-      <c r="B15" s="19"/>
-      <c r="C15" s="25"/>
-      <c r="D15" s="25"/>
-      <c r="E15" s="25"/>
-      <c r="F15" s="25"/>
-      <c r="G15" s="26" t="s">
-        <v>22</v>
-      </c>
-      <c r="H15" s="26"/>
-      <c r="I15" s="26"/>
-      <c r="J15" s="27"/>
-      <c r="K15" s="28"/>
-      <c r="L15" s="28"/>
-      <c r="M15" s="29" t="s">
-        <v>22</v>
-      </c>
-      <c r="N15" s="30"/>
-      <c r="O15" s="35"/>
-      <c r="P15" s="35"/>
-      <c r="Q15" s="36"/>
-      <c r="R15" s="33" t="s">
-        <v>22</v>
-      </c>
-      <c r="S15" s="23"/>
+      <c r="A15" s="31" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" s="26"/>
+      <c r="C15" s="32"/>
+      <c r="D15" s="32"/>
+      <c r="E15" s="32"/>
+      <c r="F15" s="32"/>
+      <c r="G15" s="33" t="s">
+        <v>23</v>
+      </c>
+      <c r="H15" s="33"/>
+      <c r="I15" s="33"/>
+      <c r="J15" s="34"/>
+      <c r="K15" s="35"/>
+      <c r="L15" s="35"/>
+      <c r="M15" s="36" t="s">
+        <v>23</v>
+      </c>
+      <c r="N15" s="37"/>
+      <c r="O15" s="42"/>
+      <c r="P15" s="42"/>
+      <c r="Q15" s="43"/>
+      <c r="R15" s="40" t="s">
+        <v>23</v>
+      </c>
+      <c r="S15" s="30"/>
     </row>
     <row r="16" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="37" t="s">
-        <v>23</v>
-      </c>
-      <c r="B16" s="37" t="s">
+      <c r="A16" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="C16" s="37" t="s">
+      <c r="B16" s="44" t="s">
         <v>25</v>
       </c>
-      <c r="D16" s="37" t="s">
+      <c r="C16" s="44" t="s">
         <v>26</v>
       </c>
-      <c r="E16" s="37" t="s">
+      <c r="D16" s="44" t="s">
         <v>27</v>
       </c>
-      <c r="F16" s="37" t="s">
+      <c r="E16" s="44" t="s">
         <v>28</v>
       </c>
-      <c r="G16" s="38" t="s">
+      <c r="F16" s="44" t="s">
         <v>29</v>
       </c>
-      <c r="H16" s="38" t="s">
+      <c r="G16" s="45" t="s">
         <v>30</v>
       </c>
-      <c r="I16" s="38" t="s">
+      <c r="H16" s="45" t="s">
         <v>31</v>
       </c>
-      <c r="J16" s="38" t="s">
+      <c r="I16" s="45" t="s">
         <v>32</v>
       </c>
-      <c r="K16" s="38" t="s">
+      <c r="J16" s="45" t="s">
         <v>33</v>
       </c>
-      <c r="L16" s="39" t="s">
+      <c r="K16" s="45" t="s">
         <v>34</v>
       </c>
-      <c r="M16" s="40" t="s">
+      <c r="L16" s="46" t="s">
         <v>35</v>
       </c>
-      <c r="N16" s="40" t="s">
+      <c r="M16" s="47" t="s">
         <v>36</v>
       </c>
-      <c r="O16" s="41" t="s">
+      <c r="N16" s="47" t="s">
         <v>37</v>
       </c>
-      <c r="P16" s="41" t="s">
+      <c r="O16" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="Q16" s="41" t="s">
+      <c r="P16" s="48" t="s">
         <v>39</v>
       </c>
-      <c r="R16" s="42" t="s">
+      <c r="Q16" s="48" t="s">
         <v>40</v>
       </c>
-      <c r="S16" s="43" t="s">
+      <c r="R16" s="49" t="s">
         <v>41</v>
       </c>
+      <c r="S16" s="50" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="44" t="n">
+      <c r="A17" s="51" t="n">
         <v>10</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="C17" s="44" t="n">
+        <v>43</v>
+      </c>
+      <c r="C17" s="51" t="n">
         <v>-3</v>
       </c>
-      <c r="D17" s="45" t="s">
-        <v>43</v>
-      </c>
-      <c r="E17" s="44" t="n">
+      <c r="D17" s="52" t="s">
+        <v>44</v>
+      </c>
+      <c r="E17" s="51" t="n">
         <v>-1</v>
       </c>
-      <c r="F17" s="44" t="n">
+      <c r="F17" s="51" t="n">
         <v>0</v>
       </c>
-      <c r="G17" s="46" t="str">
+      <c r="G17" s="53" t="str">
         <f aca="false">+VLOOKUP(B17,Parametros!A$1:B$121,2,)</f>
         <v>CEA</v>
       </c>
-      <c r="H17" s="44" t="s">
-        <v>44</v>
-      </c>
-      <c r="I17" s="44" t="s">
+      <c r="H17" s="51" t="s">
         <v>45</v>
       </c>
-      <c r="J17" s="46" t="n">
+      <c r="I17" s="51" t="s">
+        <v>46</v>
+      </c>
+      <c r="J17" s="53" t="n">
         <f aca="false">+VLOOKUP(B17,Parametros!A$1:D$121,3,)</f>
         <v>0</v>
       </c>
-      <c r="K17" s="46" t="n">
+      <c r="K17" s="53" t="n">
         <f aca="false">+VLOOKUP(B17,Parametros!A$1:E$121,4,)</f>
         <v>0</v>
       </c>
-      <c r="L17" s="46" t="n">
+      <c r="L17" s="53" t="n">
         <f aca="false">+VLOOKUP(B17,Parametros!A$1:G$121,5,)</f>
         <v>0</v>
       </c>
-      <c r="M17" s="47"/>
-      <c r="N17" s="47"/>
-      <c r="O17" s="47"/>
-      <c r="P17" s="47"/>
-      <c r="Q17" s="47"/>
-      <c r="R17" s="47"/>
-      <c r="S17" s="47"/>
+      <c r="M17" s="54"/>
+      <c r="N17" s="54"/>
+      <c r="O17" s="54"/>
+      <c r="P17" s="54"/>
+      <c r="Q17" s="54"/>
+      <c r="R17" s="54"/>
+      <c r="S17" s="54"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="44" t="n">
+      <c r="A18" s="51" t="n">
         <v>11</v>
       </c>
-      <c r="B18" s="47" t="s">
-        <v>46</v>
-      </c>
-      <c r="C18" s="44" t="n">
+      <c r="B18" s="54" t="s">
+        <v>47</v>
+      </c>
+      <c r="C18" s="51" t="n">
         <v>2</v>
       </c>
-      <c r="D18" s="48" t="s">
-        <v>47</v>
-      </c>
-      <c r="E18" s="44" t="s">
+      <c r="D18" s="55" t="s">
         <v>48</v>
       </c>
-      <c r="F18" s="44"/>
-      <c r="G18" s="46" t="str">
+      <c r="E18" s="51" t="s">
+        <v>49</v>
+      </c>
+      <c r="F18" s="51"/>
+      <c r="G18" s="53" t="str">
         <f aca="false">+VLOOKUP(B18,Parametros!A$1:B$121,2,)</f>
         <v>CEA</v>
       </c>
-      <c r="H18" s="44"/>
-      <c r="I18" s="44"/>
-      <c r="J18" s="44"/>
-      <c r="K18" s="44"/>
-      <c r="L18" s="44"/>
-      <c r="M18" s="47"/>
-      <c r="N18" s="47"/>
-      <c r="O18" s="47"/>
-      <c r="P18" s="47"/>
-      <c r="Q18" s="47"/>
-      <c r="R18" s="47"/>
-      <c r="S18" s="47"/>
+      <c r="H18" s="51"/>
+      <c r="I18" s="51"/>
+      <c r="J18" s="51"/>
+      <c r="K18" s="51"/>
+      <c r="L18" s="51"/>
+      <c r="M18" s="54"/>
+      <c r="N18" s="54"/>
+      <c r="O18" s="54"/>
+      <c r="P18" s="54"/>
+      <c r="Q18" s="54"/>
+      <c r="R18" s="54"/>
+      <c r="S18" s="54"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="44" t="n">
+      <c r="A19" s="51" t="n">
         <v>12</v>
       </c>
-      <c r="B19" s="47" t="s">
+      <c r="B19" s="54" t="s">
+        <v>50</v>
+      </c>
+      <c r="C19" s="51" t="n">
+        <v>3</v>
+      </c>
+      <c r="D19" s="52" t="s">
+        <v>44</v>
+      </c>
+      <c r="E19" s="51" t="s">
         <v>49</v>
       </c>
-      <c r="C19" s="44" t="n">
-        <v>3</v>
-      </c>
-      <c r="D19" s="45" t="s">
-        <v>43</v>
-      </c>
-      <c r="E19" s="44" t="s">
-        <v>48</v>
-      </c>
-      <c r="F19" s="44"/>
-      <c r="G19" s="46" t="str">
+      <c r="F19" s="51"/>
+      <c r="G19" s="53" t="str">
         <f aca="false">+VLOOKUP(B19,Parametros!A$1:B$121,2,)</f>
         <v>CEA</v>
       </c>
-      <c r="H19" s="44"/>
-      <c r="I19" s="44"/>
-      <c r="J19" s="44"/>
-      <c r="K19" s="44"/>
-      <c r="L19" s="44"/>
-      <c r="M19" s="47"/>
-      <c r="N19" s="47"/>
-      <c r="O19" s="47"/>
-      <c r="P19" s="47"/>
-      <c r="Q19" s="47"/>
-      <c r="R19" s="47"/>
-      <c r="S19" s="47"/>
+      <c r="H19" s="51"/>
+      <c r="I19" s="51"/>
+      <c r="J19" s="51"/>
+      <c r="K19" s="51"/>
+      <c r="L19" s="51"/>
+      <c r="M19" s="54"/>
+      <c r="N19" s="54"/>
+      <c r="O19" s="54"/>
+      <c r="P19" s="54"/>
+      <c r="Q19" s="54"/>
+      <c r="R19" s="54"/>
+      <c r="S19" s="54"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="44" t="n">
+      <c r="A20" s="51" t="n">
         <v>13</v>
       </c>
-      <c r="B20" s="47" t="s">
-        <v>42</v>
-      </c>
-      <c r="C20" s="44" t="n">
+      <c r="B20" s="54" t="s">
+        <v>43</v>
+      </c>
+      <c r="C20" s="51" t="n">
         <v>4</v>
       </c>
-      <c r="D20" s="45" t="s">
-        <v>43</v>
-      </c>
-      <c r="E20" s="44" t="s">
-        <v>48</v>
-      </c>
-      <c r="F20" s="44"/>
-      <c r="G20" s="46" t="str">
+      <c r="D20" s="52" t="s">
+        <v>44</v>
+      </c>
+      <c r="E20" s="51" t="s">
+        <v>49</v>
+      </c>
+      <c r="F20" s="51"/>
+      <c r="G20" s="53" t="str">
         <f aca="false">+VLOOKUP(B20,Parametros!A$1:B$121,2,)</f>
         <v>CEA</v>
       </c>
-      <c r="H20" s="44"/>
-      <c r="I20" s="44"/>
-      <c r="J20" s="44"/>
-      <c r="K20" s="44"/>
-      <c r="L20" s="44"/>
-      <c r="M20" s="47"/>
-      <c r="N20" s="47"/>
-      <c r="O20" s="47"/>
-      <c r="P20" s="47"/>
-      <c r="Q20" s="47"/>
-      <c r="R20" s="47"/>
-      <c r="S20" s="47"/>
+      <c r="H20" s="51"/>
+      <c r="I20" s="51"/>
+      <c r="J20" s="51"/>
+      <c r="K20" s="51"/>
+      <c r="L20" s="51"/>
+      <c r="M20" s="54"/>
+      <c r="N20" s="54"/>
+      <c r="O20" s="54"/>
+      <c r="P20" s="54"/>
+      <c r="Q20" s="54"/>
+      <c r="R20" s="54"/>
+      <c r="S20" s="54"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="44" t="n">
+      <c r="A21" s="51" t="n">
         <v>14</v>
       </c>
-      <c r="B21" s="47" t="s">
-        <v>50</v>
-      </c>
-      <c r="C21" s="44" t="n">
+      <c r="B21" s="54" t="s">
+        <v>51</v>
+      </c>
+      <c r="C21" s="51" t="n">
         <v>5</v>
       </c>
-      <c r="D21" s="45" t="s">
-        <v>43</v>
-      </c>
-      <c r="E21" s="44" t="s">
-        <v>48</v>
-      </c>
-      <c r="F21" s="44"/>
-      <c r="G21" s="46" t="str">
+      <c r="D21" s="52" t="s">
+        <v>44</v>
+      </c>
+      <c r="E21" s="51" t="s">
+        <v>49</v>
+      </c>
+      <c r="F21" s="51"/>
+      <c r="G21" s="53" t="str">
         <f aca="false">+VLOOKUP(B21,Parametros!A$1:B$121,2,)</f>
         <v>HIDROLAB</v>
       </c>
-      <c r="H21" s="44"/>
-      <c r="I21" s="44"/>
-      <c r="J21" s="44"/>
-      <c r="K21" s="44"/>
-      <c r="L21" s="44"/>
-      <c r="M21" s="47"/>
-      <c r="N21" s="47"/>
-      <c r="O21" s="47"/>
-      <c r="P21" s="47"/>
-      <c r="Q21" s="47"/>
-      <c r="R21" s="47"/>
-      <c r="S21" s="47"/>
+      <c r="H21" s="51"/>
+      <c r="I21" s="51"/>
+      <c r="J21" s="51"/>
+      <c r="K21" s="51"/>
+      <c r="L21" s="51"/>
+      <c r="M21" s="54"/>
+      <c r="N21" s="54"/>
+      <c r="O21" s="54"/>
+      <c r="P21" s="54"/>
+      <c r="Q21" s="54"/>
+      <c r="R21" s="54"/>
+      <c r="S21" s="54"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="44" t="n">
+      <c r="A22" s="51" t="n">
         <v>15</v>
       </c>
-      <c r="B22" s="47" t="s">
-        <v>51</v>
-      </c>
-      <c r="C22" s="44" t="n">
+      <c r="B22" s="54" t="s">
+        <v>52</v>
+      </c>
+      <c r="C22" s="51" t="n">
         <v>6</v>
       </c>
-      <c r="D22" s="45" t="s">
-        <v>43</v>
-      </c>
-      <c r="E22" s="44" t="s">
-        <v>48</v>
-      </c>
-      <c r="F22" s="44"/>
-      <c r="G22" s="46" t="str">
+      <c r="D22" s="52" t="s">
+        <v>44</v>
+      </c>
+      <c r="E22" s="51" t="s">
+        <v>49</v>
+      </c>
+      <c r="F22" s="51"/>
+      <c r="G22" s="53" t="str">
         <f aca="false">+VLOOKUP(B22,Parametros!A$1:B$121,2,)</f>
         <v>CEA</v>
       </c>
-      <c r="H22" s="44"/>
-      <c r="I22" s="44"/>
-      <c r="J22" s="44"/>
-      <c r="K22" s="44"/>
-      <c r="L22" s="44"/>
-      <c r="M22" s="47"/>
-      <c r="N22" s="47"/>
-      <c r="O22" s="47"/>
-      <c r="P22" s="47"/>
-      <c r="Q22" s="47"/>
-      <c r="R22" s="47"/>
-      <c r="S22" s="47"/>
+      <c r="H22" s="51"/>
+      <c r="I22" s="51"/>
+      <c r="J22" s="51"/>
+      <c r="K22" s="51"/>
+      <c r="L22" s="51"/>
+      <c r="M22" s="54"/>
+      <c r="N22" s="54"/>
+      <c r="O22" s="54"/>
+      <c r="P22" s="54"/>
+      <c r="Q22" s="54"/>
+      <c r="R22" s="54"/>
+      <c r="S22" s="54"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="44" t="n">
+      <c r="A23" s="51" t="n">
         <v>16</v>
       </c>
-      <c r="B23" s="47" t="s">
-        <v>52</v>
-      </c>
-      <c r="C23" s="44" t="n">
+      <c r="B23" s="54" t="s">
+        <v>53</v>
+      </c>
+      <c r="C23" s="51" t="n">
         <v>7</v>
       </c>
-      <c r="D23" s="48" t="s">
-        <v>47</v>
-      </c>
-      <c r="E23" s="44" t="s">
+      <c r="D23" s="55" t="s">
         <v>48</v>
       </c>
-      <c r="F23" s="44"/>
-      <c r="G23" s="46" t="str">
+      <c r="E23" s="51" t="s">
+        <v>49</v>
+      </c>
+      <c r="F23" s="51"/>
+      <c r="G23" s="53" t="str">
         <f aca="false">+VLOOKUP(B23,Parametros!A$1:B$121,2,)</f>
         <v>ANAM</v>
       </c>
-      <c r="H23" s="44"/>
-      <c r="I23" s="44"/>
-      <c r="J23" s="44"/>
-      <c r="K23" s="44"/>
-      <c r="L23" s="44"/>
-      <c r="M23" s="47"/>
-      <c r="N23" s="47"/>
-      <c r="O23" s="47"/>
-      <c r="P23" s="47"/>
-      <c r="Q23" s="47"/>
-      <c r="R23" s="47"/>
-      <c r="S23" s="47"/>
+      <c r="H23" s="51"/>
+      <c r="I23" s="51"/>
+      <c r="J23" s="51"/>
+      <c r="K23" s="51"/>
+      <c r="L23" s="51"/>
+      <c r="M23" s="54"/>
+      <c r="N23" s="54"/>
+      <c r="O23" s="54"/>
+      <c r="P23" s="54"/>
+      <c r="Q23" s="54"/>
+      <c r="R23" s="54"/>
+      <c r="S23" s="54"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="44" t="n">
+      <c r="A24" s="51" t="n">
         <v>17</v>
       </c>
-      <c r="B24" s="47" t="s">
-        <v>53</v>
-      </c>
-      <c r="C24" s="44" t="n">
+      <c r="B24" s="54" t="s">
+        <v>54</v>
+      </c>
+      <c r="C24" s="51" t="n">
         <v>8</v>
       </c>
-      <c r="D24" s="45" t="s">
-        <v>43</v>
-      </c>
-      <c r="E24" s="44" t="s">
-        <v>48</v>
-      </c>
-      <c r="F24" s="44"/>
-      <c r="G24" s="46" t="str">
+      <c r="D24" s="52" t="s">
+        <v>44</v>
+      </c>
+      <c r="E24" s="51" t="s">
+        <v>49</v>
+      </c>
+      <c r="F24" s="51"/>
+      <c r="G24" s="53" t="str">
         <f aca="false">+VLOOKUP(B24,Parametros!A$1:B$121,2,)</f>
         <v>CEA</v>
       </c>
-      <c r="H24" s="47"/>
-      <c r="I24" s="44"/>
-      <c r="J24" s="44"/>
-      <c r="K24" s="44"/>
-      <c r="L24" s="44"/>
-      <c r="M24" s="47"/>
-      <c r="N24" s="47"/>
-      <c r="O24" s="47"/>
-      <c r="P24" s="47"/>
-      <c r="Q24" s="47"/>
-      <c r="R24" s="47"/>
-      <c r="S24" s="47"/>
+      <c r="H24" s="54"/>
+      <c r="I24" s="51"/>
+      <c r="J24" s="51"/>
+      <c r="K24" s="51"/>
+      <c r="L24" s="51"/>
+      <c r="M24" s="54"/>
+      <c r="N24" s="54"/>
+      <c r="O24" s="54"/>
+      <c r="P24" s="54"/>
+      <c r="Q24" s="54"/>
+      <c r="R24" s="54"/>
+      <c r="S24" s="54"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="44" t="n">
+      <c r="A25" s="51" t="n">
         <v>18</v>
       </c>
-      <c r="B25" s="47" t="s">
-        <v>54</v>
-      </c>
-      <c r="C25" s="44" t="n">
+      <c r="B25" s="54" t="s">
+        <v>55</v>
+      </c>
+      <c r="C25" s="51" t="n">
         <v>9</v>
       </c>
-      <c r="D25" s="48" t="s">
-        <v>47</v>
-      </c>
-      <c r="E25" s="44" t="s">
+      <c r="D25" s="55" t="s">
         <v>48</v>
       </c>
-      <c r="F25" s="47"/>
-      <c r="G25" s="46" t="str">
+      <c r="E25" s="51" t="s">
+        <v>49</v>
+      </c>
+      <c r="F25" s="54"/>
+      <c r="G25" s="53" t="str">
         <f aca="false">+VLOOKUP(B25,Parametros!A$1:B$121,2,)</f>
         <v>ALS SANTIAGO</v>
       </c>
-      <c r="H25" s="44"/>
-      <c r="I25" s="44"/>
-      <c r="J25" s="44"/>
-      <c r="K25" s="44"/>
-      <c r="L25" s="44"/>
-      <c r="M25" s="47"/>
-      <c r="N25" s="47"/>
-      <c r="O25" s="47"/>
-      <c r="P25" s="47"/>
-      <c r="Q25" s="47"/>
-      <c r="R25" s="47"/>
-      <c r="S25" s="47"/>
+      <c r="H25" s="51"/>
+      <c r="I25" s="51"/>
+      <c r="J25" s="51"/>
+      <c r="K25" s="51"/>
+      <c r="L25" s="51"/>
+      <c r="M25" s="54"/>
+      <c r="N25" s="54"/>
+      <c r="O25" s="54"/>
+      <c r="P25" s="54"/>
+      <c r="Q25" s="54"/>
+      <c r="R25" s="54"/>
+      <c r="S25" s="54"/>
     </row>
     <row r="26" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="49" t="s">
-        <v>55</v>
-      </c>
-      <c r="B26" s="50" t="s">
+      <c r="A26" s="56" t="s">
         <v>56</v>
       </c>
-      <c r="C26" s="50"/>
-      <c r="D26" s="50"/>
-      <c r="E26" s="50"/>
-      <c r="F26" s="50"/>
-      <c r="G26" s="50"/>
+      <c r="B26" s="57" t="s">
+        <v>57</v>
+      </c>
+      <c r="C26" s="57"/>
+      <c r="D26" s="57"/>
+      <c r="E26" s="57"/>
+      <c r="F26" s="57"/>
+      <c r="G26" s="57"/>
     </row>
     <row r="27" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="49"/>
-      <c r="B27" s="50" t="s">
-        <v>16</v>
-      </c>
-      <c r="C27" s="50"/>
-      <c r="D27" s="50"/>
-      <c r="E27" s="50"/>
-      <c r="F27" s="50"/>
-      <c r="G27" s="50"/>
+      <c r="A27" s="56"/>
+      <c r="B27" s="57" t="s">
+        <v>17</v>
+      </c>
+      <c r="C27" s="57"/>
+      <c r="D27" s="57"/>
+      <c r="E27" s="57"/>
+      <c r="F27" s="57"/>
+      <c r="G27" s="57"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="51" t="s">
-        <v>57</v>
-      </c>
-      <c r="B28" s="48" t="s">
-        <v>43</v>
-      </c>
-      <c r="C28" s="48" t="s">
-        <v>47</v>
+      <c r="A28" s="58" t="s">
+        <v>58</v>
+      </c>
+      <c r="B28" s="55" t="s">
+        <v>44</v>
+      </c>
+      <c r="C28" s="55" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B29" s="0" t="n">
         <v>1</v>
@@ -2242,7 +2352,7 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B30" s="0" t="n">
         <v>1</v>
@@ -2261,7 +2371,7 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B31" s="0" t="n">
         <v>1</v>
@@ -2277,7 +2387,7 @@
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B32" s="0" t="n">
         <v>1</v>
@@ -2293,7 +2403,7 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B33" s="0" t="n">
         <v>1</v>
@@ -2312,7 +2422,7 @@
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B34" s="0" t="n">
         <v>1</v>
@@ -2328,7 +2438,7 @@
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B35" s="0" t="n">
         <v>1</v>
@@ -2344,7 +2454,7 @@
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B36" s="0" t="n">
         <v>1</v>
@@ -2363,7 +2473,7 @@
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B37" s="0" t="n">
         <v>1</v>
@@ -2379,7 +2489,7 @@
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B38" s="0" t="n">
         <v>1</v>
@@ -2397,17 +2507,17 @@
       <c r="S38" s="9"/>
     </row>
     <row r="39" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="52" t="s">
-        <v>68</v>
-      </c>
-      <c r="B39" s="18" t="s">
+      <c r="A39" s="59" t="s">
         <v>69</v>
       </c>
-      <c r="C39" s="18"/>
-      <c r="D39" s="18"/>
-      <c r="E39" s="18"/>
-      <c r="F39" s="18"/>
-      <c r="G39" s="18"/>
+      <c r="B39" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="C39" s="25"/>
+      <c r="D39" s="25"/>
+      <c r="E39" s="25"/>
+      <c r="F39" s="25"/>
+      <c r="G39" s="25"/>
       <c r="L39" s="9"/>
       <c r="M39" s="9"/>
       <c r="N39" s="9"/>
@@ -2418,15 +2528,15 @@
       <c r="S39" s="9"/>
     </row>
     <row r="40" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="52"/>
-      <c r="B40" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="C40" s="18"/>
-      <c r="D40" s="18"/>
-      <c r="E40" s="18"/>
-      <c r="F40" s="18"/>
-      <c r="G40" s="18"/>
+      <c r="A40" s="59"/>
+      <c r="B40" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="C40" s="25"/>
+      <c r="D40" s="25"/>
+      <c r="E40" s="25"/>
+      <c r="F40" s="25"/>
+      <c r="G40" s="25"/>
       <c r="L40" s="9"/>
       <c r="M40" s="9"/>
       <c r="N40" s="9"/>
@@ -2437,202 +2547,202 @@
       <c r="S40" s="9"/>
     </row>
     <row r="41" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="53" t="s">
-        <v>70</v>
+      <c r="A41" s="60" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="54" t="s">
-        <v>71</v>
-      </c>
-      <c r="B42" s="54" t="s">
+      <c r="A42" s="61" t="s">
         <v>72</v>
       </c>
+      <c r="B42" s="61" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="43" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="55" t="n">
+      <c r="A43" s="62" t="n">
         <v>1</v>
       </c>
-      <c r="B43" s="56" t="s">
-        <v>73</v>
+      <c r="B43" s="63" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="55" t="n">
+      <c r="A44" s="62" t="n">
         <v>3</v>
       </c>
-      <c r="B44" s="56" t="s">
-        <v>74</v>
+      <c r="B44" s="63" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="55" t="n">
+      <c r="A45" s="62" t="n">
         <v>2</v>
       </c>
-      <c r="B45" s="56" t="s">
-        <v>75</v>
+      <c r="B45" s="63" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="55" t="n">
+      <c r="A46" s="62" t="n">
         <v>1</v>
       </c>
-      <c r="B46" s="56" t="s">
-        <v>76</v>
+      <c r="B46" s="63" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="49" t="s">
-        <v>77</v>
-      </c>
-      <c r="B47" s="50" t="s">
+      <c r="A47" s="56" t="s">
         <v>78</v>
       </c>
-      <c r="C47" s="50"/>
-      <c r="D47" s="50"/>
-      <c r="E47" s="50"/>
-      <c r="F47" s="50"/>
-      <c r="G47" s="50"/>
+      <c r="B47" s="57" t="s">
+        <v>79</v>
+      </c>
+      <c r="C47" s="57"/>
+      <c r="D47" s="57"/>
+      <c r="E47" s="57"/>
+      <c r="F47" s="57"/>
+      <c r="G47" s="57"/>
     </row>
     <row r="48" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="49"/>
-      <c r="B48" s="50" t="s">
-        <v>16</v>
-      </c>
-      <c r="C48" s="50"/>
-      <c r="D48" s="50"/>
-      <c r="E48" s="50"/>
-      <c r="F48" s="50"/>
-      <c r="G48" s="50"/>
+      <c r="A48" s="56"/>
+      <c r="B48" s="57" t="s">
+        <v>17</v>
+      </c>
+      <c r="C48" s="57"/>
+      <c r="D48" s="57"/>
+      <c r="E48" s="57"/>
+      <c r="F48" s="57"/>
+      <c r="G48" s="57"/>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="57" t="s">
-        <v>79</v>
-      </c>
-      <c r="B49" s="48" t="s">
-        <v>43</v>
-      </c>
-      <c r="C49" s="48" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="50" customFormat="false" ht="23.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A50" s="45" t="s">
+      <c r="A49" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="B50" s="58" t="s">
+      <c r="B49" s="55" t="s">
+        <v>44</v>
+      </c>
+      <c r="C49" s="55" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="45.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="64" t="s">
         <v>81</v>
       </c>
+      <c r="B50" s="65" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="51" customFormat="false" ht="23.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A51" s="59" t="s">
-        <v>82</v>
-      </c>
-      <c r="B51" s="45" t="s">
+      <c r="A51" s="66" t="s">
         <v>83</v>
       </c>
-      <c r="C51" s="45"/>
+      <c r="B51" s="52" t="s">
+        <v>84</v>
+      </c>
+      <c r="C51" s="52"/>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="59" t="s">
+      <c r="A52" s="66" t="s">
+        <v>85</v>
+      </c>
+      <c r="B52" s="52" t="s">
         <v>84</v>
       </c>
-      <c r="B52" s="45" t="s">
+      <c r="C52" s="52"/>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="52" t="s">
+        <v>86</v>
+      </c>
+      <c r="B53" s="52" t="s">
+        <v>84</v>
+      </c>
+      <c r="C53" s="52"/>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="52" t="s">
+        <v>87</v>
+      </c>
+      <c r="B54" s="52" t="s">
+        <v>84</v>
+      </c>
+      <c r="C54" s="52"/>
+    </row>
+    <row r="55" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="59" t="s">
+        <v>88</v>
+      </c>
+      <c r="B55" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="C55" s="25"/>
+      <c r="D55" s="25"/>
+      <c r="E55" s="25"/>
+      <c r="F55" s="25"/>
+      <c r="G55" s="25"/>
+    </row>
+    <row r="56" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="59"/>
+      <c r="B56" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="C56" s="25"/>
+      <c r="D56" s="25"/>
+      <c r="E56" s="25"/>
+      <c r="F56" s="25"/>
+      <c r="G56" s="25"/>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="67" t="s">
+        <v>90</v>
+      </c>
+      <c r="B57" s="55" t="s">
+        <v>44</v>
+      </c>
+      <c r="C57" s="55" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="52" t="s">
+        <v>81</v>
+      </c>
+      <c r="B58" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="C58" s="0" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="66" t="s">
         <v>83</v>
       </c>
-      <c r="C52" s="45"/>
-    </row>
-    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="45" t="s">
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="66" t="s">
         <v>85</v>
       </c>
-      <c r="B53" s="45" t="s">
-        <v>83</v>
-      </c>
-      <c r="C53" s="45"/>
-    </row>
-    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="45" t="s">
+      <c r="B60" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="C60" s="0" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="52" t="s">
         <v>86</v>
       </c>
-      <c r="B54" s="45" t="s">
-        <v>83</v>
-      </c>
-      <c r="C54" s="45"/>
-    </row>
-    <row r="55" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="52" t="s">
+    </row>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="52" t="s">
         <v>87</v>
       </c>
-      <c r="B55" s="18" t="s">
-        <v>88</v>
-      </c>
-      <c r="C55" s="18"/>
-      <c r="D55" s="18"/>
-      <c r="E55" s="18"/>
-      <c r="F55" s="18"/>
-      <c r="G55" s="18"/>
-    </row>
-    <row r="56" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="52"/>
-      <c r="B56" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="C56" s="18"/>
-      <c r="D56" s="18"/>
-      <c r="E56" s="18"/>
-      <c r="F56" s="18"/>
-      <c r="G56" s="18"/>
-    </row>
-    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="60" t="s">
-        <v>89</v>
-      </c>
-      <c r="B57" s="48" t="s">
-        <v>43</v>
-      </c>
-      <c r="C57" s="48" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="45" t="s">
-        <v>80</v>
-      </c>
-      <c r="B58" s="0" t="s">
-        <v>90</v>
-      </c>
-      <c r="C58" s="0" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="61" t="s">
+      <c r="C62" s="0" t="s">
         <v>91</v>
-      </c>
-    </row>
-    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="61" t="s">
-        <v>92</v>
-      </c>
-      <c r="B60" s="0" t="s">
-        <v>90</v>
-      </c>
-      <c r="C60" s="0" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="45" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="62" t="s">
-        <v>86</v>
-      </c>
-      <c r="C62" s="0" t="s">
-        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -2680,7 +2790,7 @@
   </sheetPr>
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
@@ -2694,207 +2804,207 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="63" t="s">
+      <c r="A1" s="68" t="s">
+        <v>92</v>
+      </c>
+      <c r="B1" s="68" t="s">
         <v>93</v>
       </c>
-      <c r="B1" s="63" t="s">
+      <c r="C1" s="68" t="s">
         <v>94</v>
       </c>
-      <c r="C1" s="63" t="s">
+      <c r="D1" s="68" t="s">
         <v>95</v>
       </c>
-      <c r="D1" s="63" t="s">
+      <c r="E1" s="68" t="s">
         <v>96</v>
       </c>
-      <c r="E1" s="63" t="s">
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="69" t="s">
+        <v>81</v>
+      </c>
+      <c r="B2" s="68"/>
+      <c r="C2" s="68"/>
+      <c r="D2" s="68"/>
+      <c r="E2" s="68"/>
+    </row>
+    <row r="3" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="66" t="s">
+        <v>87</v>
+      </c>
+      <c r="B3" s="66" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="64" t="s">
-        <v>80</v>
-      </c>
-      <c r="B2" s="63"/>
-      <c r="C2" s="63"/>
-      <c r="D2" s="63"/>
-      <c r="E2" s="63"/>
-    </row>
-    <row r="3" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="59" t="s">
+      <c r="C3" s="70" t="s">
+        <v>98</v>
+      </c>
+      <c r="D3" s="70"/>
+      <c r="E3" s="66" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="66" t="s">
+        <v>100</v>
+      </c>
+      <c r="B4" s="66" t="s">
+        <v>101</v>
+      </c>
+      <c r="C4" s="66"/>
+      <c r="D4" s="66"/>
+      <c r="E4" s="70" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="66" t="s">
+        <v>83</v>
+      </c>
+      <c r="B5" s="66" t="s">
+        <v>103</v>
+      </c>
+      <c r="C5" s="66" t="s">
+        <v>104</v>
+      </c>
+      <c r="D5" s="66"/>
+      <c r="E5" s="66" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="66" t="s">
+        <v>106</v>
+      </c>
+      <c r="B6" s="66" t="s">
+        <v>107</v>
+      </c>
+      <c r="C6" s="66" t="s">
+        <v>108</v>
+      </c>
+      <c r="D6" s="66"/>
+      <c r="E6" s="66" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="66" t="s">
+        <v>85</v>
+      </c>
+      <c r="B7" s="66" t="s">
+        <v>110</v>
+      </c>
+      <c r="C7" s="66" t="s">
+        <v>111</v>
+      </c>
+      <c r="D7" s="66" t="s">
+        <v>112</v>
+      </c>
+      <c r="E7" s="70" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="66" t="s">
+        <v>114</v>
+      </c>
+      <c r="B8" s="66" t="s">
+        <v>115</v>
+      </c>
+      <c r="C8" s="70" t="s">
+        <v>116</v>
+      </c>
+      <c r="D8" s="70"/>
+      <c r="E8" s="66" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="66" t="s">
+        <v>118</v>
+      </c>
+      <c r="B9" s="66" t="s">
+        <v>119</v>
+      </c>
+      <c r="C9" s="70"/>
+      <c r="D9" s="70" t="s">
+        <v>120</v>
+      </c>
+      <c r="E9" s="66" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="66" t="s">
+        <v>121</v>
+      </c>
+      <c r="B10" s="66" t="s">
+        <v>122</v>
+      </c>
+      <c r="C10" s="66"/>
+      <c r="D10" s="66"/>
+      <c r="E10" s="66" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="66" t="s">
+        <v>124</v>
+      </c>
+      <c r="B11" s="66" t="s">
+        <v>125</v>
+      </c>
+      <c r="C11" s="66" t="s">
+        <v>126</v>
+      </c>
+      <c r="D11" s="66"/>
+      <c r="E11" s="70" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="66" t="s">
+        <v>128</v>
+      </c>
+      <c r="B12" s="66" t="s">
+        <v>129</v>
+      </c>
+      <c r="C12" s="66" t="s">
+        <v>130</v>
+      </c>
+      <c r="D12" s="66"/>
+      <c r="E12" s="70" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="66" t="s">
         <v>86</v>
       </c>
-      <c r="B3" s="59" t="s">
-        <v>98</v>
-      </c>
-      <c r="C3" s="65" t="s">
-        <v>99</v>
-      </c>
-      <c r="D3" s="65"/>
-      <c r="E3" s="59" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="59" t="s">
-        <v>101</v>
-      </c>
-      <c r="B4" s="59" t="s">
-        <v>102</v>
-      </c>
-      <c r="C4" s="59"/>
-      <c r="D4" s="59"/>
-      <c r="E4" s="65" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="59" t="s">
-        <v>82</v>
-      </c>
-      <c r="B5" s="59" t="s">
-        <v>104</v>
-      </c>
-      <c r="C5" s="59" t="s">
-        <v>105</v>
-      </c>
-      <c r="D5" s="59"/>
-      <c r="E5" s="59" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="59" t="s">
-        <v>107</v>
-      </c>
-      <c r="B6" s="59" t="s">
-        <v>108</v>
-      </c>
-      <c r="C6" s="59" t="s">
-        <v>109</v>
-      </c>
-      <c r="D6" s="59"/>
-      <c r="E6" s="59" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="59" t="s">
-        <v>84</v>
-      </c>
-      <c r="B7" s="59" t="s">
-        <v>111</v>
-      </c>
-      <c r="C7" s="59" t="s">
-        <v>112</v>
-      </c>
-      <c r="D7" s="59" t="s">
-        <v>113</v>
-      </c>
-      <c r="E7" s="65" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="59" t="s">
-        <v>115</v>
-      </c>
-      <c r="B8" s="59" t="s">
-        <v>116</v>
-      </c>
-      <c r="C8" s="65" t="s">
-        <v>117</v>
-      </c>
-      <c r="D8" s="65"/>
-      <c r="E8" s="59" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="59" t="s">
-        <v>119</v>
-      </c>
-      <c r="B9" s="59" t="s">
-        <v>120</v>
-      </c>
-      <c r="C9" s="65"/>
-      <c r="D9" s="65" t="s">
-        <v>121</v>
-      </c>
-      <c r="E9" s="59" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="59" t="s">
-        <v>122</v>
-      </c>
-      <c r="B10" s="59" t="s">
-        <v>123</v>
-      </c>
-      <c r="C10" s="59"/>
-      <c r="D10" s="59"/>
-      <c r="E10" s="59" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="59" t="s">
-        <v>125</v>
-      </c>
-      <c r="B11" s="59" t="s">
-        <v>126</v>
-      </c>
-      <c r="C11" s="59" t="s">
-        <v>127</v>
-      </c>
-      <c r="D11" s="59"/>
-      <c r="E11" s="65" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="59" t="s">
-        <v>129</v>
-      </c>
-      <c r="B12" s="59" t="s">
-        <v>130</v>
-      </c>
-      <c r="C12" s="59" t="s">
-        <v>131</v>
-      </c>
-      <c r="D12" s="59"/>
-      <c r="E12" s="65" t="s">
+      <c r="B13" s="66" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="13" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="59" t="s">
-        <v>85</v>
-      </c>
-      <c r="B13" s="59" t="s">
+      <c r="C13" s="66" t="s">
         <v>133</v>
       </c>
-      <c r="C13" s="59" t="s">
+      <c r="D13" s="66"/>
+      <c r="E13" s="70" t="s">
         <v>134</v>
       </c>
-      <c r="D13" s="59"/>
-      <c r="E13" s="65" t="s">
+    </row>
+    <row r="14" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="66" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="14" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="59" t="s">
+      <c r="B14" s="70" t="s">
         <v>136</v>
       </c>
-      <c r="B14" s="65" t="s">
+      <c r="C14" s="66" t="s">
         <v>137</v>
       </c>
-      <c r="C14" s="59" t="s">
+      <c r="D14" s="66"/>
+      <c r="E14" s="70" t="s">
         <v>138</v>
-      </c>
-      <c r="D14" s="59"/>
-      <c r="E14" s="65" t="s">
-        <v>139</v>
       </c>
     </row>
   </sheetData>
@@ -2915,7 +3025,7 @@
   </sheetPr>
   <dimension ref="A1:F121"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A21" activeCellId="0" sqref="A21"/>
     </sheetView>
   </sheetViews>
@@ -2931,990 +3041,990 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="60" t="s">
+      <c r="A1" s="67" t="s">
+        <v>139</v>
+      </c>
+      <c r="B1" s="67" t="s">
         <v>140</v>
       </c>
-      <c r="B1" s="60" t="s">
+      <c r="C1" s="67" t="s">
         <v>141</v>
       </c>
-      <c r="C1" s="60" t="s">
+      <c r="D1" s="67" t="s">
         <v>142</v>
       </c>
-      <c r="D1" s="60" t="s">
+      <c r="E1" s="67" t="s">
         <v>143</v>
       </c>
-      <c r="E1" s="60" t="s">
+      <c r="F1" s="67" t="s">
         <v>144</v>
-      </c>
-      <c r="F1" s="60" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D53" s="0" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E53" s="0" t="str">
         <f aca="false">+VLOOKUP(D53,A1:B121,1)</f>
-        <v>Cromo  disuelto</v>
+        <v>Conductividad  disuelto</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B58" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B59" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B60" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B62" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B63" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>190</v>
-      </c>
-      <c r="B64" s="66" t="s">
-        <v>101</v>
+        <v>189</v>
+      </c>
+      <c r="B64" s="71" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>191</v>
-      </c>
-      <c r="B65" s="66" t="s">
-        <v>101</v>
+        <v>190</v>
+      </c>
+      <c r="B65" s="71" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>192</v>
-      </c>
-      <c r="B66" s="66" t="s">
-        <v>101</v>
+        <v>191</v>
+      </c>
+      <c r="B66" s="71" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>193</v>
-      </c>
-      <c r="B67" s="66" t="s">
-        <v>101</v>
+        <v>192</v>
+      </c>
+      <c r="B67" s="71" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="B68" s="66" t="s">
-        <v>101</v>
+        <v>55</v>
+      </c>
+      <c r="B68" s="71" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>167</v>
-      </c>
-      <c r="B69" s="66" t="s">
-        <v>101</v>
+        <v>166</v>
+      </c>
+      <c r="B69" s="71" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>194</v>
-      </c>
-      <c r="B70" s="66" t="s">
-        <v>101</v>
+        <v>193</v>
+      </c>
+      <c r="B70" s="71" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>195</v>
-      </c>
-      <c r="B71" s="66" t="s">
-        <v>101</v>
+        <v>194</v>
+      </c>
+      <c r="B71" s="71" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>196</v>
-      </c>
-      <c r="B72" s="66" t="s">
-        <v>101</v>
+        <v>195</v>
+      </c>
+      <c r="B72" s="71" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
-        <v>197</v>
-      </c>
-      <c r="B73" s="66" t="s">
-        <v>101</v>
+        <v>196</v>
+      </c>
+      <c r="B73" s="71" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
-        <v>198</v>
-      </c>
-      <c r="B74" s="66" t="s">
-        <v>101</v>
+        <v>197</v>
+      </c>
+      <c r="B74" s="71" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
-        <v>199</v>
-      </c>
-      <c r="B75" s="66" t="s">
-        <v>101</v>
+        <v>198</v>
+      </c>
+      <c r="B75" s="71" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
-        <v>200</v>
-      </c>
-      <c r="B76" s="66" t="s">
-        <v>101</v>
+        <v>199</v>
+      </c>
+      <c r="B76" s="71" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
-        <v>201</v>
-      </c>
-      <c r="B77" s="66" t="s">
-        <v>101</v>
+        <v>200</v>
+      </c>
+      <c r="B77" s="71" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
-        <v>202</v>
-      </c>
-      <c r="B78" s="66" t="s">
-        <v>101</v>
+        <v>201</v>
+      </c>
+      <c r="B78" s="71" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
-        <v>203</v>
-      </c>
-      <c r="B79" s="66" t="s">
-        <v>101</v>
+        <v>202</v>
+      </c>
+      <c r="B79" s="71" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
-        <v>204</v>
-      </c>
-      <c r="B80" s="66" t="s">
-        <v>101</v>
+        <v>203</v>
+      </c>
+      <c r="B80" s="71" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
-        <v>205</v>
-      </c>
-      <c r="B81" s="66" t="s">
-        <v>101</v>
+        <v>204</v>
+      </c>
+      <c r="B81" s="71" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
-        <v>206</v>
-      </c>
-      <c r="B82" s="66" t="s">
-        <v>101</v>
+        <v>205</v>
+      </c>
+      <c r="B82" s="71" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
-        <v>207</v>
-      </c>
-      <c r="B83" s="66" t="s">
-        <v>101</v>
+        <v>206</v>
+      </c>
+      <c r="B83" s="71" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
-        <v>208</v>
-      </c>
-      <c r="B84" s="66" t="s">
-        <v>101</v>
+        <v>207</v>
+      </c>
+      <c r="B84" s="71" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="s">
-        <v>209</v>
-      </c>
-      <c r="B85" s="66" t="s">
-        <v>101</v>
+        <v>208</v>
+      </c>
+      <c r="B85" s="71" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
-        <v>210</v>
-      </c>
-      <c r="B86" s="66" t="s">
-        <v>101</v>
+        <v>209</v>
+      </c>
+      <c r="B86" s="71" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
-        <v>211</v>
-      </c>
-      <c r="B87" s="66" t="s">
-        <v>101</v>
+        <v>210</v>
+      </c>
+      <c r="B87" s="71" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
-        <v>212</v>
-      </c>
-      <c r="B88" s="66" t="s">
-        <v>101</v>
+        <v>211</v>
+      </c>
+      <c r="B88" s="71" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
-        <v>213</v>
-      </c>
-      <c r="B89" s="66" t="s">
-        <v>101</v>
+        <v>212</v>
+      </c>
+      <c r="B89" s="71" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B90" s="0" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B91" s="0" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B92" s="0" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B93" s="0" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="s">
+        <v>215</v>
+      </c>
+      <c r="B94" s="0" t="s">
         <v>216</v>
-      </c>
-      <c r="B94" s="0" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B95" s="0" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="0" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B96" s="0" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="0" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B97" s="0" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="0" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B98" s="0" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="0" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B99" s="0" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="0" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B100" s="0" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="0" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B101" s="0" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="0" t="s">
-        <v>225</v>
-      </c>
-      <c r="B102" s="66" t="s">
-        <v>101</v>
+        <v>224</v>
+      </c>
+      <c r="B102" s="71" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="0" t="s">
-        <v>226</v>
-      </c>
-      <c r="B103" s="66" t="s">
-        <v>101</v>
+        <v>225</v>
+      </c>
+      <c r="B103" s="71" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="0" t="s">
-        <v>227</v>
-      </c>
-      <c r="B104" s="66" t="s">
-        <v>101</v>
+        <v>226</v>
+      </c>
+      <c r="B104" s="71" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="0" t="s">
-        <v>228</v>
-      </c>
-      <c r="B105" s="66" t="s">
-        <v>101</v>
+        <v>227</v>
+      </c>
+      <c r="B105" s="71" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="0" t="s">
-        <v>229</v>
-      </c>
-      <c r="B106" s="66" t="s">
-        <v>101</v>
+        <v>228</v>
+      </c>
+      <c r="B106" s="71" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="0" t="s">
-        <v>230</v>
-      </c>
-      <c r="B107" s="66" t="s">
-        <v>101</v>
+        <v>229</v>
+      </c>
+      <c r="B107" s="71" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="0" t="s">
-        <v>231</v>
-      </c>
-      <c r="B108" s="66" t="s">
-        <v>101</v>
+        <v>230</v>
+      </c>
+      <c r="B108" s="71" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="0" t="s">
-        <v>232</v>
-      </c>
-      <c r="B109" s="66" t="s">
-        <v>101</v>
+        <v>231</v>
+      </c>
+      <c r="B109" s="71" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="0" t="s">
-        <v>233</v>
-      </c>
-      <c r="B110" s="66" t="s">
-        <v>101</v>
+        <v>232</v>
+      </c>
+      <c r="B110" s="71" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="0" t="s">
-        <v>234</v>
-      </c>
-      <c r="B111" s="66" t="s">
-        <v>101</v>
+        <v>233</v>
+      </c>
+      <c r="B111" s="71" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="0" t="s">
-        <v>235</v>
-      </c>
-      <c r="B112" s="66" t="s">
-        <v>101</v>
+        <v>234</v>
+      </c>
+      <c r="B112" s="71" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="0" t="s">
-        <v>236</v>
-      </c>
-      <c r="B113" s="66" t="s">
-        <v>101</v>
+        <v>235</v>
+      </c>
+      <c r="B113" s="71" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="0" t="s">
-        <v>237</v>
-      </c>
-      <c r="B114" s="66" t="s">
-        <v>101</v>
+        <v>236</v>
+      </c>
+      <c r="B114" s="71" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="0" t="s">
-        <v>238</v>
-      </c>
-      <c r="B115" s="66" t="s">
-        <v>101</v>
+        <v>237</v>
+      </c>
+      <c r="B115" s="71" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="0" t="s">
-        <v>239</v>
-      </c>
-      <c r="B116" s="66" t="s">
-        <v>101</v>
+        <v>238</v>
+      </c>
+      <c r="B116" s="71" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="0" t="s">
-        <v>240</v>
-      </c>
-      <c r="B117" s="66" t="s">
-        <v>101</v>
+        <v>239</v>
+      </c>
+      <c r="B117" s="71" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="0" t="s">
-        <v>241</v>
-      </c>
-      <c r="B118" s="66" t="s">
-        <v>101</v>
+        <v>240</v>
+      </c>
+      <c r="B118" s="71" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="0" t="s">
-        <v>242</v>
-      </c>
-      <c r="B119" s="66" t="s">
-        <v>101</v>
+        <v>241</v>
+      </c>
+      <c r="B119" s="71" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="0" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B120" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="0" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B121" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -3926,4 +4036,97 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.1377551020408"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.7755102040816"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.9132653061224"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.4081632653061"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="72" t="s">
+        <v>244</v>
+      </c>
+      <c r="B1" s="73" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" s="73" t="s">
+        <v>245</v>
+      </c>
+      <c r="D1" s="73" t="s">
+        <v>246</v>
+      </c>
+      <c r="E1" s="73" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="74" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" s="75" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" s="75"/>
+      <c r="D2" s="75"/>
+      <c r="E2" s="75"/>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="74" t="s">
+        <v>248</v>
+      </c>
+      <c r="B3" s="75"/>
+      <c r="C3" s="75" t="n">
+        <v>1</v>
+      </c>
+      <c r="D3" s="75"/>
+      <c r="E3" s="75"/>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="74" t="s">
+        <v>249</v>
+      </c>
+      <c r="B4" s="75"/>
+      <c r="C4" s="75"/>
+      <c r="D4" s="75" t="n">
+        <v>1</v>
+      </c>
+      <c r="E4" s="75"/>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="74" t="s">
+        <v>250</v>
+      </c>
+      <c r="B5" s="75"/>
+      <c r="C5" s="75"/>
+      <c r="D5" s="75"/>
+      <c r="E5" s="75" t="n">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;A</oddHeader>
+    <oddFooter>&amp;CPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Se crean las configuraciones para crear las matrices, dado que appy no soporta creacion de columnas en una plantilla se cambia a libreria ezodf
</commit_message>
<xml_diff>
--- a/Oficial/Patron_FL.xlsx
+++ b/Oficial/Patron_FL.xlsx
@@ -30,6 +30,7 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t>Formato: DD/MM/AA</t>
         </r>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="258">
   <si>
     <t>SOLICITUD  DE SERVICIO EXTERNO A LABORATORIO</t>
   </si>
@@ -189,25 +190,49 @@
     <t>HIDROLAB</t>
   </si>
   <si>
+    <t>CEA0</t>
+  </si>
+  <si>
     <t>Fósforo  disuelto</t>
   </si>
   <si>
     <t>U DE CONCEPCIÓN</t>
   </si>
   <si>
+    <t>CEA1</t>
+  </si>
+  <si>
+    <t>CEA2</t>
+  </si>
+  <si>
     <t>Índice total</t>
   </si>
   <si>
+    <t>CEA3</t>
+  </si>
+  <si>
     <t>nitrito total</t>
   </si>
   <si>
+    <t>CEA4</t>
+  </si>
+  <si>
     <t>HAMs total</t>
   </si>
   <si>
+    <t>CEA5</t>
+  </si>
+  <si>
     <t>nitrato  disuelto</t>
   </si>
   <si>
+    <t>CEA6</t>
+  </si>
+  <si>
     <t>Cromo total</t>
+  </si>
+  <si>
+    <t>CEA7</t>
   </si>
   <si>
     <t>Códigos de
@@ -814,11 +839,12 @@
     <numFmt numFmtId="166" formatCode="0.00"/>
     <numFmt numFmtId="167" formatCode="0;[RED]\-0"/>
   </numFmts>
-  <fonts count="24">
+  <fonts count="23">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -840,6 +866,7 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -853,42 +880,41 @@
       <sz val="12"/>
       <name val="arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF3333FF"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FFCC0066"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="14"/>
       <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="14"/>
-      <color rgb="FFFF0000"/>
-      <name val="Arial"/>
-      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -896,41 +922,48 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF1F497D"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF17365D"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="14"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="14"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="12"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <i val="true"/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -938,6 +971,7 @@
       <color rgb="FF1F497D"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -945,6 +979,7 @@
       <color rgb="FFFF3300"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -953,6 +988,7 @@
       <color rgb="FF801900"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -961,6 +997,7 @@
       <color rgb="FF0000CC"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="13">
@@ -1149,7 +1186,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="93">
+  <cellXfs count="89">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1242,111 +1279,107 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="2" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="2" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="3" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="3" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="3" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="3" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="4" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="4" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="5" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="5" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="2" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="2" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="2" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="2" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="3" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="3" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="3" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="3" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="3" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="3" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="4" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="4" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="4" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="4" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="4" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="4" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="4" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="4" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="5" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="5" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="5" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="5" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="4" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="4" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="4" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="4" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="13" fillId="2" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="12" fillId="2" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="13" fillId="3" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="12" fillId="3" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="13" fillId="3" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="12" fillId="3" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="13" fillId="4" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="12" fillId="4" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="13" fillId="4" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="12" fillId="4" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="13" fillId="5" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="12" fillId="5" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="13" fillId="5" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="12" fillId="5" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1362,35 +1395,35 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="14" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="7" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="7" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="7" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="7" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="6" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="6" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="6" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="6" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1414,23 +1447,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1443,10 +1468,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1458,7 +1479,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="11" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="18" fillId="11" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1474,11 +1495,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="8" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="18" fillId="8" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="10" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="10" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1490,15 +1511,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="10" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="10" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1506,19 +1527,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="12" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="20" fillId="12" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="22" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="23" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1599,15 +1620,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>712440</xdr:colOff>
+      <xdr:colOff>739440</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>7560</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1270800</xdr:colOff>
+      <xdr:colOff>1297440</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>773640</xdr:rowOff>
+      <xdr:rowOff>773280</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1620,8 +1641,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="712440" y="7560"/>
-          <a:ext cx="558360" cy="766080"/>
+          <a:off x="739440" y="7560"/>
+          <a:ext cx="558000" cy="765720"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1643,8 +1664,8 @@
   </sheetPr>
   <dimension ref="A1:S69"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G22" activeCellId="0" sqref="G22"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I17" activeCellId="0" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1812,7 +1833,7 @@
       </c>
       <c r="B8" s="14" t="n">
         <f aca="true">+TODAY()</f>
-        <v>42082</v>
+        <v>42083</v>
       </c>
       <c r="C8" s="15"/>
       <c r="D8" s="16"/>
@@ -1863,7 +1884,7 @@
       </c>
       <c r="B10" s="20" t="n">
         <f aca="false">+B9-B8</f>
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C10" s="21" t="s">
         <v>14</v>
@@ -1872,624 +1893,639 @@
       <c r="E10" s="16"/>
       <c r="F10" s="16"/>
     </row>
-    <row r="11" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="22"/>
-      <c r="B11" s="23"/>
-      <c r="C11" s="24"/>
+      <c r="C11" s="23"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="25" t="s">
+      <c r="A12" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="25"/>
-      <c r="C12" s="25"/>
-      <c r="D12" s="25"/>
-      <c r="E12" s="25"/>
-      <c r="F12" s="25"/>
-      <c r="G12" s="26" t="s">
+      <c r="B12" s="24"/>
+      <c r="C12" s="24"/>
+      <c r="D12" s="24"/>
+      <c r="E12" s="24"/>
+      <c r="F12" s="24"/>
+      <c r="G12" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="H12" s="26"/>
-      <c r="I12" s="26"/>
-      <c r="J12" s="26"/>
-      <c r="K12" s="26"/>
-      <c r="L12" s="27"/>
-      <c r="M12" s="28" t="s">
+      <c r="H12" s="25"/>
+      <c r="I12" s="25"/>
+      <c r="J12" s="25"/>
+      <c r="K12" s="25"/>
+      <c r="L12" s="26"/>
+      <c r="M12" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="N12" s="28"/>
-      <c r="O12" s="28"/>
-      <c r="P12" s="28"/>
-      <c r="Q12" s="28"/>
-      <c r="R12" s="29" t="s">
+      <c r="N12" s="27"/>
+      <c r="O12" s="27"/>
+      <c r="P12" s="27"/>
+      <c r="Q12" s="27"/>
+      <c r="R12" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="S12" s="29"/>
+      <c r="S12" s="28"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="30" t="s">
+      <c r="A13" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="25"/>
-      <c r="C13" s="31"/>
-      <c r="D13" s="31"/>
-      <c r="E13" s="31"/>
-      <c r="F13" s="31"/>
-      <c r="G13" s="32" t="s">
+      <c r="B13" s="24"/>
+      <c r="C13" s="30"/>
+      <c r="D13" s="30"/>
+      <c r="E13" s="30"/>
+      <c r="F13" s="30"/>
+      <c r="G13" s="31" t="s">
         <v>19</v>
       </c>
-      <c r="H13" s="32"/>
-      <c r="I13" s="32"/>
-      <c r="J13" s="33"/>
-      <c r="K13" s="34"/>
-      <c r="L13" s="34"/>
-      <c r="M13" s="35" t="s">
+      <c r="H13" s="31"/>
+      <c r="I13" s="31"/>
+      <c r="J13" s="32"/>
+      <c r="K13" s="33"/>
+      <c r="L13" s="33"/>
+      <c r="M13" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="N13" s="36"/>
-      <c r="O13" s="37"/>
-      <c r="P13" s="37"/>
-      <c r="Q13" s="38"/>
-      <c r="R13" s="39" t="s">
+      <c r="N13" s="35"/>
+      <c r="O13" s="36"/>
+      <c r="P13" s="36"/>
+      <c r="Q13" s="37"/>
+      <c r="R13" s="38" t="s">
         <v>19</v>
       </c>
-      <c r="S13" s="40"/>
+      <c r="S13" s="39"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="30" t="s">
+      <c r="A14" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="25"/>
-      <c r="C14" s="31"/>
-      <c r="D14" s="31"/>
-      <c r="E14" s="31"/>
-      <c r="F14" s="31"/>
-      <c r="G14" s="32" t="s">
+      <c r="B14" s="24"/>
+      <c r="C14" s="30"/>
+      <c r="D14" s="30"/>
+      <c r="E14" s="30"/>
+      <c r="F14" s="30"/>
+      <c r="G14" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="H14" s="32"/>
-      <c r="I14" s="32"/>
-      <c r="J14" s="33"/>
-      <c r="K14" s="34"/>
-      <c r="L14" s="34"/>
-      <c r="M14" s="35" t="s">
+      <c r="H14" s="31"/>
+      <c r="I14" s="31"/>
+      <c r="J14" s="32"/>
+      <c r="K14" s="33"/>
+      <c r="L14" s="33"/>
+      <c r="M14" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="N14" s="36"/>
-      <c r="O14" s="41"/>
-      <c r="P14" s="41"/>
-      <c r="Q14" s="42"/>
-      <c r="R14" s="39" t="s">
+      <c r="N14" s="35"/>
+      <c r="O14" s="40"/>
+      <c r="P14" s="40"/>
+      <c r="Q14" s="41"/>
+      <c r="R14" s="38" t="s">
         <v>20</v>
       </c>
-      <c r="S14" s="29"/>
+      <c r="S14" s="28"/>
     </row>
     <row r="15" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="43" t="s">
+      <c r="A15" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="B15" s="43" t="s">
+      <c r="B15" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="C15" s="43" t="s">
+      <c r="C15" s="42" t="s">
         <v>23</v>
       </c>
-      <c r="D15" s="43" t="s">
+      <c r="D15" s="42" t="s">
         <v>24</v>
       </c>
-      <c r="E15" s="43" t="s">
+      <c r="E15" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="F15" s="43" t="s">
+      <c r="F15" s="42" t="s">
         <v>26</v>
       </c>
-      <c r="G15" s="44" t="s">
+      <c r="G15" s="43" t="s">
         <v>27</v>
       </c>
-      <c r="H15" s="44" t="s">
+      <c r="H15" s="43" t="s">
         <v>28</v>
       </c>
-      <c r="I15" s="44" t="s">
+      <c r="I15" s="43" t="s">
         <v>29</v>
       </c>
-      <c r="J15" s="44" t="s">
+      <c r="J15" s="43" t="s">
         <v>30</v>
       </c>
-      <c r="K15" s="44" t="s">
+      <c r="K15" s="43" t="s">
         <v>31</v>
       </c>
-      <c r="L15" s="45" t="s">
+      <c r="L15" s="44" t="s">
         <v>32</v>
       </c>
-      <c r="M15" s="46" t="s">
+      <c r="M15" s="45" t="s">
         <v>33</v>
       </c>
-      <c r="N15" s="46" t="s">
+      <c r="N15" s="45" t="s">
         <v>34</v>
       </c>
-      <c r="O15" s="47" t="s">
+      <c r="O15" s="46" t="s">
         <v>35</v>
       </c>
-      <c r="P15" s="47" t="s">
+      <c r="P15" s="46" t="s">
         <v>36</v>
       </c>
-      <c r="Q15" s="47" t="s">
+      <c r="Q15" s="46" t="s">
         <v>37</v>
       </c>
-      <c r="R15" s="48" t="s">
+      <c r="R15" s="47" t="s">
         <v>38</v>
       </c>
-      <c r="S15" s="49" t="s">
+      <c r="S15" s="48" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="50" t="n">
+      <c r="A16" s="49" t="n">
         <v>10</v>
       </c>
       <c r="B16" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="C16" s="50" t="n">
+      <c r="C16" s="49" t="n">
         <v>5</v>
       </c>
-      <c r="D16" s="51" t="s">
+      <c r="D16" s="50" t="s">
         <v>41</v>
       </c>
-      <c r="E16" s="52" t="s">
+      <c r="E16" s="51" t="s">
         <v>42</v>
       </c>
-      <c r="F16" s="52" t="n">
+      <c r="F16" s="51" t="n">
         <v>0</v>
       </c>
-      <c r="G16" s="53" t="s">
+      <c r="G16" s="52" t="s">
         <v>43</v>
       </c>
-      <c r="H16" s="52" t="s">
+      <c r="H16" s="51" t="s">
         <v>44</v>
       </c>
-      <c r="I16" s="52" t="s">
+      <c r="I16" s="51" t="s">
         <v>45</v>
       </c>
-      <c r="J16" s="54" t="n">
+      <c r="J16" s="53" t="n">
         <f aca="false">+VLOOKUP(B16,Parametros!A$1:D$121,3,)</f>
         <v>0</v>
       </c>
-      <c r="K16" s="54" t="n">
+      <c r="K16" s="53" t="n">
         <f aca="false">+VLOOKUP(B16,Parametros!A$1:E$121,4,)</f>
         <v>0</v>
       </c>
-      <c r="L16" s="54" t="n">
+      <c r="L16" s="53" t="n">
         <f aca="false">+VLOOKUP(B16,Parametros!A$1:G$121,5,)</f>
         <v>0</v>
       </c>
-      <c r="M16" s="55"/>
-      <c r="N16" s="55"/>
-      <c r="O16" s="55"/>
-      <c r="P16" s="55"/>
-      <c r="Q16" s="55"/>
-      <c r="R16" s="55"/>
-      <c r="S16" s="55"/>
+      <c r="M16" s="54"/>
+      <c r="N16" s="54"/>
+      <c r="O16" s="54"/>
+      <c r="P16" s="54"/>
+      <c r="Q16" s="54"/>
+      <c r="R16" s="54"/>
+      <c r="S16" s="54"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="50" t="n">
+      <c r="A17" s="49" t="n">
         <v>11</v>
       </c>
-      <c r="B17" s="55" t="s">
+      <c r="B17" s="54" t="s">
         <v>46</v>
       </c>
-      <c r="C17" s="50" t="n">
+      <c r="C17" s="49" t="n">
         <v>5</v>
       </c>
-      <c r="D17" s="51" t="s">
+      <c r="D17" s="50" t="s">
         <v>47</v>
       </c>
-      <c r="E17" s="52" t="s">
+      <c r="E17" s="51" t="s">
         <v>42</v>
       </c>
-      <c r="F17" s="52"/>
-      <c r="G17" s="56" t="s">
+      <c r="F17" s="51"/>
+      <c r="G17" s="55" t="s">
         <v>48</v>
       </c>
-      <c r="H17" s="52"/>
-      <c r="I17" s="52"/>
-      <c r="J17" s="54" t="n">
+      <c r="H17" s="51"/>
+      <c r="I17" s="51" t="s">
+        <v>49</v>
+      </c>
+      <c r="J17" s="53" t="n">
         <f aca="false">+VLOOKUP(B17,Parametros!A$1:D$121,3,)</f>
         <v>0</v>
       </c>
-      <c r="K17" s="54" t="n">
+      <c r="K17" s="53" t="n">
         <f aca="false">+VLOOKUP(B17,Parametros!A$1:E$121,4,)</f>
         <v>0</v>
       </c>
-      <c r="L17" s="54" t="n">
+      <c r="L17" s="53" t="n">
         <f aca="false">+VLOOKUP(B17,Parametros!A$1:G$121,5,)</f>
         <v>0</v>
       </c>
-      <c r="M17" s="55"/>
-      <c r="N17" s="55"/>
-      <c r="O17" s="55"/>
-      <c r="P17" s="55"/>
-      <c r="Q17" s="55"/>
-      <c r="R17" s="55"/>
-      <c r="S17" s="55"/>
+      <c r="M17" s="54"/>
+      <c r="N17" s="54"/>
+      <c r="O17" s="54"/>
+      <c r="P17" s="54"/>
+      <c r="Q17" s="54"/>
+      <c r="R17" s="54"/>
+      <c r="S17" s="54"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="50" t="n">
+      <c r="A18" s="49" t="n">
         <v>12</v>
       </c>
-      <c r="B18" s="55" t="s">
-        <v>49</v>
-      </c>
-      <c r="C18" s="50" t="n">
+      <c r="B18" s="54" t="s">
+        <v>50</v>
+      </c>
+      <c r="C18" s="49" t="n">
         <v>3</v>
       </c>
-      <c r="D18" s="51" t="s">
+      <c r="D18" s="50" t="s">
         <v>41</v>
       </c>
-      <c r="E18" s="52" t="s">
+      <c r="E18" s="51" t="s">
         <v>42</v>
       </c>
-      <c r="F18" s="52"/>
-      <c r="G18" s="56" t="s">
-        <v>50</v>
-      </c>
-      <c r="H18" s="52"/>
-      <c r="I18" s="52"/>
-      <c r="J18" s="54" t="n">
+      <c r="F18" s="51"/>
+      <c r="G18" s="55" t="s">
+        <v>51</v>
+      </c>
+      <c r="H18" s="51"/>
+      <c r="I18" s="51" t="s">
+        <v>52</v>
+      </c>
+      <c r="J18" s="53" t="n">
         <f aca="false">+VLOOKUP(B18,Parametros!A$1:D$121,3,)</f>
         <v>0</v>
       </c>
-      <c r="K18" s="54" t="n">
+      <c r="K18" s="53" t="n">
         <f aca="false">+VLOOKUP(B18,Parametros!A$1:E$121,4,)</f>
         <v>0</v>
       </c>
-      <c r="L18" s="54" t="n">
+      <c r="L18" s="53" t="n">
         <f aca="false">+VLOOKUP(B18,Parametros!A$1:G$121,5,)</f>
         <v>0</v>
       </c>
-      <c r="M18" s="55"/>
-      <c r="N18" s="55"/>
-      <c r="O18" s="55"/>
-      <c r="P18" s="55"/>
-      <c r="Q18" s="55"/>
-      <c r="R18" s="55"/>
-      <c r="S18" s="55"/>
+      <c r="M18" s="54"/>
+      <c r="N18" s="54"/>
+      <c r="O18" s="54"/>
+      <c r="P18" s="54"/>
+      <c r="Q18" s="54"/>
+      <c r="R18" s="54"/>
+      <c r="S18" s="54"/>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="50" t="n">
+      <c r="A19" s="49" t="n">
         <v>13</v>
       </c>
-      <c r="B19" s="55" t="s">
+      <c r="B19" s="54" t="s">
         <v>40</v>
       </c>
-      <c r="C19" s="50" t="n">
+      <c r="C19" s="49" t="n">
         <v>4</v>
       </c>
-      <c r="D19" s="51" t="s">
+      <c r="D19" s="50" t="s">
         <v>41</v>
       </c>
-      <c r="E19" s="52" t="s">
+      <c r="E19" s="51" t="s">
         <v>42</v>
       </c>
-      <c r="F19" s="52"/>
-      <c r="G19" s="53" t="s">
+      <c r="F19" s="51"/>
+      <c r="G19" s="52" t="s">
         <v>43</v>
       </c>
-      <c r="H19" s="52"/>
-      <c r="I19" s="52"/>
-      <c r="J19" s="54" t="n">
+      <c r="H19" s="51"/>
+      <c r="I19" s="51" t="s">
+        <v>53</v>
+      </c>
+      <c r="J19" s="53" t="n">
         <f aca="false">+VLOOKUP(B19,Parametros!A$1:D$121,3,)</f>
         <v>0</v>
       </c>
-      <c r="K19" s="54" t="n">
+      <c r="K19" s="53" t="n">
         <f aca="false">+VLOOKUP(B19,Parametros!A$1:E$121,4,)</f>
         <v>0</v>
       </c>
-      <c r="L19" s="54" t="n">
+      <c r="L19" s="53" t="n">
         <f aca="false">+VLOOKUP(B19,Parametros!A$1:G$121,5,)</f>
         <v>0</v>
       </c>
-      <c r="M19" s="55"/>
-      <c r="N19" s="55"/>
-      <c r="O19" s="55"/>
-      <c r="P19" s="55"/>
-      <c r="Q19" s="55"/>
-      <c r="R19" s="55"/>
-      <c r="S19" s="55"/>
+      <c r="M19" s="54"/>
+      <c r="N19" s="54"/>
+      <c r="O19" s="54"/>
+      <c r="P19" s="54"/>
+      <c r="Q19" s="54"/>
+      <c r="R19" s="54"/>
+      <c r="S19" s="54"/>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="50" t="n">
+      <c r="A20" s="49" t="n">
         <v>14</v>
       </c>
-      <c r="B20" s="55" t="s">
-        <v>51</v>
-      </c>
-      <c r="C20" s="50" t="n">
+      <c r="B20" s="54" t="s">
+        <v>54</v>
+      </c>
+      <c r="C20" s="49" t="n">
         <v>5</v>
       </c>
-      <c r="D20" s="51" t="s">
+      <c r="D20" s="50" t="s">
         <v>41</v>
       </c>
-      <c r="E20" s="52" t="s">
+      <c r="E20" s="51" t="s">
         <v>42</v>
       </c>
-      <c r="F20" s="52"/>
-      <c r="G20" s="53" t="s">
+      <c r="F20" s="51"/>
+      <c r="G20" s="52" t="s">
         <v>43</v>
       </c>
-      <c r="H20" s="52"/>
-      <c r="I20" s="52"/>
-      <c r="J20" s="54" t="n">
+      <c r="H20" s="51"/>
+      <c r="I20" s="51" t="s">
+        <v>55</v>
+      </c>
+      <c r="J20" s="53" t="n">
         <f aca="false">+VLOOKUP(B20,Parametros!A$1:D$121,3,)</f>
         <v>0</v>
       </c>
-      <c r="K20" s="54" t="n">
+      <c r="K20" s="53" t="n">
         <f aca="false">+VLOOKUP(B20,Parametros!A$1:E$121,4,)</f>
         <v>0</v>
       </c>
-      <c r="L20" s="54" t="n">
+      <c r="L20" s="53" t="n">
         <f aca="false">+VLOOKUP(B20,Parametros!A$1:G$121,5,)</f>
         <v>0</v>
       </c>
-      <c r="M20" s="55"/>
-      <c r="N20" s="55"/>
-      <c r="O20" s="55"/>
-      <c r="P20" s="55"/>
-      <c r="Q20" s="55"/>
-      <c r="R20" s="55"/>
-      <c r="S20" s="55"/>
+      <c r="M20" s="54"/>
+      <c r="N20" s="54"/>
+      <c r="O20" s="54"/>
+      <c r="P20" s="54"/>
+      <c r="Q20" s="54"/>
+      <c r="R20" s="54"/>
+      <c r="S20" s="54"/>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="50" t="n">
+      <c r="A21" s="49" t="n">
         <v>15</v>
       </c>
-      <c r="B21" s="55" t="s">
-        <v>52</v>
-      </c>
-      <c r="C21" s="50" t="n">
+      <c r="B21" s="54" t="s">
+        <v>56</v>
+      </c>
+      <c r="C21" s="49" t="n">
         <v>6</v>
       </c>
-      <c r="D21" s="51" t="s">
+      <c r="D21" s="50" t="s">
         <v>41</v>
       </c>
-      <c r="E21" s="52" t="s">
+      <c r="E21" s="51" t="s">
         <v>42</v>
       </c>
-      <c r="F21" s="52"/>
-      <c r="G21" s="53" t="s">
+      <c r="F21" s="51"/>
+      <c r="G21" s="52" t="s">
         <v>43</v>
       </c>
-      <c r="H21" s="52"/>
-      <c r="I21" s="52"/>
-      <c r="J21" s="54" t="n">
+      <c r="H21" s="51"/>
+      <c r="I21" s="51" t="s">
+        <v>57</v>
+      </c>
+      <c r="J21" s="53" t="n">
         <f aca="false">+VLOOKUP(B21,Parametros!A$1:D$121,3,)</f>
         <v>0</v>
       </c>
-      <c r="K21" s="54" t="n">
+      <c r="K21" s="53" t="n">
         <f aca="false">+VLOOKUP(B21,Parametros!A$1:E$121,4,)</f>
         <v>0</v>
       </c>
-      <c r="L21" s="54" t="n">
+      <c r="L21" s="53" t="n">
         <f aca="false">+VLOOKUP(B21,Parametros!A$1:G$121,5,)</f>
         <v>0</v>
       </c>
-      <c r="M21" s="55"/>
-      <c r="N21" s="55"/>
-      <c r="O21" s="55"/>
-      <c r="P21" s="55"/>
-      <c r="Q21" s="55"/>
-      <c r="R21" s="55"/>
-      <c r="S21" s="55"/>
+      <c r="M21" s="54"/>
+      <c r="N21" s="54"/>
+      <c r="O21" s="54"/>
+      <c r="P21" s="54"/>
+      <c r="Q21" s="54"/>
+      <c r="R21" s="54"/>
+      <c r="S21" s="54"/>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="50" t="n">
+      <c r="A22" s="49" t="n">
         <v>16</v>
       </c>
-      <c r="B22" s="55" t="s">
-        <v>53</v>
-      </c>
-      <c r="C22" s="50" t="n">
+      <c r="B22" s="54" t="s">
+        <v>58</v>
+      </c>
+      <c r="C22" s="49" t="n">
         <v>7</v>
       </c>
-      <c r="D22" s="51" t="s">
+      <c r="D22" s="50" t="s">
         <v>47</v>
       </c>
-      <c r="E22" s="52" t="s">
+      <c r="E22" s="51" t="s">
         <v>42</v>
       </c>
-      <c r="F22" s="52"/>
-      <c r="G22" s="53" t="s">
+      <c r="F22" s="51"/>
+      <c r="G22" s="52" t="s">
         <v>43</v>
       </c>
-      <c r="H22" s="52"/>
-      <c r="I22" s="52"/>
-      <c r="J22" s="54" t="n">
+      <c r="H22" s="51"/>
+      <c r="I22" s="51" t="s">
+        <v>59</v>
+      </c>
+      <c r="J22" s="53" t="n">
         <f aca="false">+VLOOKUP(B22,Parametros!A$1:D$121,3,)</f>
         <v>0</v>
       </c>
-      <c r="K22" s="54" t="n">
+      <c r="K22" s="53" t="n">
         <f aca="false">+VLOOKUP(B22,Parametros!A$1:E$121,4,)</f>
         <v>0</v>
       </c>
-      <c r="L22" s="54" t="n">
+      <c r="L22" s="53" t="n">
         <f aca="false">+VLOOKUP(B22,Parametros!A$1:G$121,5,)</f>
         <v>0</v>
       </c>
-      <c r="M22" s="55"/>
-      <c r="N22" s="55"/>
-      <c r="O22" s="55"/>
-      <c r="P22" s="55"/>
-      <c r="Q22" s="55"/>
-      <c r="R22" s="55"/>
-      <c r="S22" s="55"/>
+      <c r="M22" s="54"/>
+      <c r="N22" s="54"/>
+      <c r="O22" s="54"/>
+      <c r="P22" s="54"/>
+      <c r="Q22" s="54"/>
+      <c r="R22" s="54"/>
+      <c r="S22" s="54"/>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="50" t="n">
+      <c r="A23" s="49" t="n">
         <v>17</v>
       </c>
-      <c r="B23" s="55" t="s">
-        <v>54</v>
-      </c>
-      <c r="C23" s="50" t="n">
+      <c r="B23" s="54" t="s">
+        <v>60</v>
+      </c>
+      <c r="C23" s="49" t="n">
         <v>8</v>
       </c>
-      <c r="D23" s="51" t="s">
+      <c r="D23" s="50" t="s">
         <v>41</v>
       </c>
-      <c r="E23" s="52" t="s">
+      <c r="E23" s="51" t="s">
         <v>42</v>
       </c>
-      <c r="F23" s="52"/>
-      <c r="G23" s="53" t="s">
+      <c r="F23" s="51"/>
+      <c r="G23" s="52" t="s">
         <v>43</v>
       </c>
-      <c r="H23" s="55"/>
-      <c r="I23" s="52"/>
-      <c r="J23" s="54" t="n">
+      <c r="H23" s="54"/>
+      <c r="I23" s="51" t="s">
+        <v>61</v>
+      </c>
+      <c r="J23" s="53" t="n">
         <f aca="false">+VLOOKUP(B23,Parametros!A$1:D$121,3,)</f>
         <v>0</v>
       </c>
-      <c r="K23" s="54" t="n">
+      <c r="K23" s="53" t="n">
         <f aca="false">+VLOOKUP(B23,Parametros!A$1:E$121,4,)</f>
         <v>0</v>
       </c>
-      <c r="L23" s="54" t="n">
+      <c r="L23" s="53" t="n">
         <f aca="false">+VLOOKUP(B23,Parametros!A$1:G$121,5,)</f>
         <v>0</v>
       </c>
-      <c r="M23" s="55"/>
-      <c r="N23" s="55"/>
-      <c r="O23" s="55"/>
-      <c r="P23" s="55"/>
-      <c r="Q23" s="55"/>
-      <c r="R23" s="55"/>
-      <c r="S23" s="55"/>
+      <c r="M23" s="54"/>
+      <c r="N23" s="54"/>
+      <c r="O23" s="54"/>
+      <c r="P23" s="54"/>
+      <c r="Q23" s="54"/>
+      <c r="R23" s="54"/>
+      <c r="S23" s="54"/>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="50" t="n">
+      <c r="A24" s="49" t="n">
         <v>18</v>
       </c>
-      <c r="B24" s="55" t="s">
-        <v>55</v>
-      </c>
-      <c r="C24" s="50" t="n">
+      <c r="B24" s="54" t="s">
+        <v>62</v>
+      </c>
+      <c r="C24" s="49" t="n">
         <v>9</v>
       </c>
-      <c r="D24" s="51" t="s">
+      <c r="D24" s="50" t="s">
         <v>47</v>
       </c>
-      <c r="E24" s="52" t="s">
+      <c r="E24" s="51" t="s">
         <v>42</v>
       </c>
-      <c r="F24" s="55"/>
-      <c r="G24" s="53" t="s">
+      <c r="F24" s="54"/>
+      <c r="G24" s="52" t="s">
         <v>43</v>
       </c>
-      <c r="H24" s="52"/>
-      <c r="I24" s="52"/>
-      <c r="J24" s="54" t="n">
+      <c r="H24" s="51"/>
+      <c r="I24" s="51" t="s">
+        <v>63</v>
+      </c>
+      <c r="J24" s="53" t="n">
         <f aca="false">+VLOOKUP(B24,Parametros!A$1:D$121,3,)</f>
         <v>0</v>
       </c>
-      <c r="K24" s="54" t="n">
+      <c r="K24" s="53" t="n">
         <f aca="false">+VLOOKUP(B24,Parametros!A$1:E$121,4,)</f>
         <v>0</v>
       </c>
-      <c r="L24" s="54" t="n">
+      <c r="L24" s="53" t="n">
         <f aca="false">+VLOOKUP(B24,Parametros!A$1:G$121,5,)</f>
         <v>0</v>
       </c>
-      <c r="M24" s="55"/>
-      <c r="N24" s="55"/>
-      <c r="O24" s="55"/>
-      <c r="P24" s="55"/>
-      <c r="Q24" s="55"/>
-      <c r="R24" s="55"/>
-      <c r="S24" s="55"/>
+      <c r="M24" s="54"/>
+      <c r="N24" s="54"/>
+      <c r="O24" s="54"/>
+      <c r="P24" s="54"/>
+      <c r="Q24" s="54"/>
+      <c r="R24" s="54"/>
+      <c r="S24" s="54"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="26" customFormat="false" ht="17.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="57" t="s">
-        <v>56</v>
-      </c>
-      <c r="B26" s="58" t="s">
-        <v>57</v>
-      </c>
-      <c r="C26" s="58"/>
-      <c r="D26" s="58"/>
-      <c r="E26" s="58"/>
-      <c r="F26" s="58"/>
-      <c r="G26" s="58"/>
-      <c r="H26" s="58"/>
-      <c r="I26" s="58"/>
+      <c r="A26" s="56" t="s">
+        <v>64</v>
+      </c>
+      <c r="B26" s="57" t="s">
+        <v>65</v>
+      </c>
+      <c r="C26" s="57"/>
+      <c r="D26" s="57"/>
+      <c r="E26" s="57"/>
+      <c r="F26" s="57"/>
+      <c r="G26" s="57"/>
+      <c r="H26" s="57"/>
+      <c r="I26" s="57"/>
     </row>
     <row r="27" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="57"/>
-      <c r="B27" s="58" t="s">
-        <v>58</v>
-      </c>
-      <c r="C27" s="58"/>
-      <c r="D27" s="58"/>
-      <c r="E27" s="58"/>
-      <c r="F27" s="58"/>
-      <c r="G27" s="58"/>
-      <c r="H27" s="58"/>
-      <c r="I27" s="58"/>
-    </row>
-    <row r="28" s="61" customFormat="true" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="59"/>
-      <c r="B28" s="60"/>
-      <c r="C28" s="60"/>
-      <c r="D28" s="60"/>
-      <c r="E28" s="60"/>
-      <c r="F28" s="60"/>
-      <c r="G28" s="60"/>
+      <c r="A27" s="56"/>
+      <c r="B27" s="57" t="s">
+        <v>66</v>
+      </c>
+      <c r="C27" s="57"/>
+      <c r="D27" s="57"/>
+      <c r="E27" s="57"/>
+      <c r="F27" s="57"/>
+      <c r="G27" s="57"/>
+      <c r="H27" s="57"/>
+      <c r="I27" s="57"/>
+    </row>
+    <row r="28" s="60" customFormat="true" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="58"/>
+      <c r="B28" s="59"/>
+      <c r="C28" s="59"/>
+      <c r="D28" s="59"/>
+      <c r="E28" s="59"/>
+      <c r="F28" s="59"/>
+      <c r="G28" s="59"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="62" t="s">
-        <v>59</v>
-      </c>
-      <c r="B29" s="63" t="s">
+      <c r="A29" s="61" t="s">
+        <v>67</v>
+      </c>
+      <c r="B29" s="62" t="s">
         <v>41</v>
       </c>
-      <c r="C29" s="63" t="s">
+      <c r="C29" s="62" t="s">
         <v>47</v>
       </c>
-      <c r="D29" s="63" t="s">
-        <v>60</v>
-      </c>
-      <c r="E29" s="63" t="s">
-        <v>61</v>
-      </c>
-      <c r="F29" s="63" t="s">
-        <v>62</v>
-      </c>
-      <c r="G29" s="63" t="s">
-        <v>63</v>
-      </c>
-      <c r="H29" s="63" t="s">
-        <v>64</v>
-      </c>
-      <c r="I29" s="63" t="s">
-        <v>65</v>
+      <c r="D29" s="62" t="s">
+        <v>68</v>
+      </c>
+      <c r="E29" s="62" t="s">
+        <v>69</v>
+      </c>
+      <c r="F29" s="62" t="s">
+        <v>70</v>
+      </c>
+      <c r="G29" s="62" t="s">
+        <v>71</v>
+      </c>
+      <c r="H29" s="62" t="s">
+        <v>72</v>
+      </c>
+      <c r="I29" s="62" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="64" t="s">
-        <v>66</v>
-      </c>
-      <c r="B30" s="65" t="n">
+      <c r="A30" s="63" t="s">
+        <v>74</v>
+      </c>
+      <c r="B30" s="64" t="n">
         <v>1</v>
       </c>
-      <c r="C30" s="65" t="n">
+      <c r="C30" s="64" t="n">
         <v>1</v>
       </c>
-      <c r="D30" s="65"/>
-      <c r="E30" s="65"/>
-      <c r="F30" s="65"/>
-      <c r="G30" s="65"/>
-      <c r="H30" s="65"/>
-      <c r="I30" s="65"/>
+      <c r="D30" s="64"/>
+      <c r="E30" s="64"/>
+      <c r="F30" s="64"/>
+      <c r="G30" s="64"/>
+      <c r="H30" s="64"/>
+      <c r="I30" s="64"/>
       <c r="L30" s="8"/>
       <c r="M30" s="8"/>
       <c r="N30" s="8"/>
@@ -2500,21 +2536,21 @@
       <c r="S30" s="8"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="64" t="s">
-        <v>67</v>
-      </c>
-      <c r="B31" s="65" t="n">
+      <c r="A31" s="63" t="s">
+        <v>75</v>
+      </c>
+      <c r="B31" s="64" t="n">
         <v>1</v>
       </c>
-      <c r="C31" s="65" t="n">
+      <c r="C31" s="64" t="n">
         <v>1</v>
       </c>
-      <c r="D31" s="65"/>
-      <c r="E31" s="65"/>
-      <c r="F31" s="65"/>
-      <c r="G31" s="65"/>
-      <c r="H31" s="65"/>
-      <c r="I31" s="65"/>
+      <c r="D31" s="64"/>
+      <c r="E31" s="64"/>
+      <c r="F31" s="64"/>
+      <c r="G31" s="64"/>
+      <c r="H31" s="64"/>
+      <c r="I31" s="64"/>
       <c r="L31" s="8"/>
       <c r="M31" s="8"/>
       <c r="N31" s="8"/>
@@ -2525,19 +2561,19 @@
       <c r="S31" s="8"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="64" t="s">
-        <v>68</v>
-      </c>
-      <c r="B32" s="65" t="n">
+      <c r="A32" s="63" t="s">
+        <v>76</v>
+      </c>
+      <c r="B32" s="64" t="n">
         <v>1</v>
       </c>
-      <c r="C32" s="65"/>
-      <c r="D32" s="65"/>
-      <c r="E32" s="65"/>
-      <c r="F32" s="65"/>
-      <c r="G32" s="65"/>
-      <c r="H32" s="65"/>
-      <c r="I32" s="65"/>
+      <c r="C32" s="64"/>
+      <c r="D32" s="64"/>
+      <c r="E32" s="64"/>
+      <c r="F32" s="64"/>
+      <c r="G32" s="64"/>
+      <c r="H32" s="64"/>
+      <c r="I32" s="64"/>
       <c r="L32" s="8"/>
       <c r="M32" s="8"/>
       <c r="N32" s="8"/>
@@ -2548,19 +2584,19 @@
       <c r="S32" s="8"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="64" t="s">
-        <v>69</v>
-      </c>
-      <c r="B33" s="65" t="n">
+      <c r="A33" s="63" t="s">
+        <v>77</v>
+      </c>
+      <c r="B33" s="64" t="n">
         <v>1</v>
       </c>
-      <c r="C33" s="65"/>
-      <c r="D33" s="65"/>
-      <c r="E33" s="65"/>
-      <c r="F33" s="65"/>
-      <c r="G33" s="65"/>
-      <c r="H33" s="65"/>
-      <c r="I33" s="65"/>
+      <c r="C33" s="64"/>
+      <c r="D33" s="64"/>
+      <c r="E33" s="64"/>
+      <c r="F33" s="64"/>
+      <c r="G33" s="64"/>
+      <c r="H33" s="64"/>
+      <c r="I33" s="64"/>
       <c r="L33" s="8"/>
       <c r="M33" s="8"/>
       <c r="N33" s="8"/>
@@ -2571,21 +2607,21 @@
       <c r="S33" s="8"/>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="64" t="s">
-        <v>70</v>
-      </c>
-      <c r="B34" s="65" t="n">
+      <c r="A34" s="63" t="s">
+        <v>78</v>
+      </c>
+      <c r="B34" s="64" t="n">
         <v>1</v>
       </c>
-      <c r="C34" s="65" t="n">
+      <c r="C34" s="64" t="n">
         <v>1</v>
       </c>
-      <c r="D34" s="65"/>
-      <c r="E34" s="65"/>
-      <c r="F34" s="65"/>
-      <c r="G34" s="65"/>
-      <c r="H34" s="65"/>
-      <c r="I34" s="65"/>
+      <c r="D34" s="64"/>
+      <c r="E34" s="64"/>
+      <c r="F34" s="64"/>
+      <c r="G34" s="64"/>
+      <c r="H34" s="64"/>
+      <c r="I34" s="64"/>
       <c r="L34" s="8"/>
       <c r="M34" s="8"/>
       <c r="N34" s="8"/>
@@ -2596,19 +2632,19 @@
       <c r="S34" s="8"/>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="64" t="s">
-        <v>71</v>
-      </c>
-      <c r="B35" s="65" t="n">
+      <c r="A35" s="63" t="s">
+        <v>79</v>
+      </c>
+      <c r="B35" s="64" t="n">
         <v>1</v>
       </c>
-      <c r="C35" s="65"/>
-      <c r="D35" s="65"/>
-      <c r="E35" s="65"/>
-      <c r="F35" s="65"/>
-      <c r="G35" s="65"/>
-      <c r="H35" s="65"/>
-      <c r="I35" s="65"/>
+      <c r="C35" s="64"/>
+      <c r="D35" s="64"/>
+      <c r="E35" s="64"/>
+      <c r="F35" s="64"/>
+      <c r="G35" s="64"/>
+      <c r="H35" s="64"/>
+      <c r="I35" s="64"/>
       <c r="L35" s="8"/>
       <c r="M35" s="8"/>
       <c r="N35" s="8"/>
@@ -2619,19 +2655,19 @@
       <c r="S35" s="8"/>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="64" t="s">
-        <v>72</v>
-      </c>
-      <c r="B36" s="65" t="n">
+      <c r="A36" s="63" t="s">
+        <v>80</v>
+      </c>
+      <c r="B36" s="64" t="n">
         <v>1</v>
       </c>
-      <c r="C36" s="65"/>
-      <c r="D36" s="65"/>
-      <c r="E36" s="65"/>
-      <c r="F36" s="65"/>
-      <c r="G36" s="65"/>
-      <c r="H36" s="65"/>
-      <c r="I36" s="65"/>
+      <c r="C36" s="64"/>
+      <c r="D36" s="64"/>
+      <c r="E36" s="64"/>
+      <c r="F36" s="64"/>
+      <c r="G36" s="64"/>
+      <c r="H36" s="64"/>
+      <c r="I36" s="64"/>
       <c r="L36" s="8"/>
       <c r="M36" s="8"/>
       <c r="N36" s="8"/>
@@ -2642,21 +2678,21 @@
       <c r="S36" s="8"/>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="64" t="s">
-        <v>73</v>
-      </c>
-      <c r="B37" s="65" t="n">
+      <c r="A37" s="63" t="s">
+        <v>81</v>
+      </c>
+      <c r="B37" s="64" t="n">
         <v>1</v>
       </c>
-      <c r="C37" s="65" t="n">
+      <c r="C37" s="64" t="n">
         <v>1</v>
       </c>
-      <c r="D37" s="65"/>
-      <c r="E37" s="65"/>
-      <c r="F37" s="65"/>
-      <c r="G37" s="65"/>
-      <c r="H37" s="65"/>
-      <c r="I37" s="65"/>
+      <c r="D37" s="64"/>
+      <c r="E37" s="64"/>
+      <c r="F37" s="64"/>
+      <c r="G37" s="64"/>
+      <c r="H37" s="64"/>
+      <c r="I37" s="64"/>
       <c r="L37" s="8"/>
       <c r="M37" s="8"/>
       <c r="N37" s="8"/>
@@ -2667,19 +2703,19 @@
       <c r="S37" s="8"/>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="64" t="s">
-        <v>74</v>
-      </c>
-      <c r="B38" s="65" t="n">
+      <c r="A38" s="63" t="s">
+        <v>82</v>
+      </c>
+      <c r="B38" s="64" t="n">
         <v>1</v>
       </c>
-      <c r="C38" s="65"/>
-      <c r="D38" s="65"/>
-      <c r="E38" s="65"/>
-      <c r="F38" s="65"/>
-      <c r="G38" s="65"/>
-      <c r="H38" s="65"/>
-      <c r="I38" s="65"/>
+      <c r="C38" s="64"/>
+      <c r="D38" s="64"/>
+      <c r="E38" s="64"/>
+      <c r="F38" s="64"/>
+      <c r="G38" s="64"/>
+      <c r="H38" s="64"/>
+      <c r="I38" s="64"/>
       <c r="L38" s="8"/>
       <c r="M38" s="8"/>
       <c r="N38" s="8"/>
@@ -2690,21 +2726,21 @@
       <c r="S38" s="8"/>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="64" t="s">
-        <v>75</v>
-      </c>
-      <c r="B39" s="65" t="n">
+      <c r="A39" s="63" t="s">
+        <v>83</v>
+      </c>
+      <c r="B39" s="64" t="n">
         <v>1</v>
       </c>
-      <c r="C39" s="65" t="n">
+      <c r="C39" s="64" t="n">
         <v>1</v>
       </c>
-      <c r="D39" s="65"/>
-      <c r="E39" s="65"/>
-      <c r="F39" s="65"/>
-      <c r="G39" s="65"/>
-      <c r="H39" s="65"/>
-      <c r="I39" s="65"/>
+      <c r="D39" s="64"/>
+      <c r="E39" s="64"/>
+      <c r="F39" s="64"/>
+      <c r="G39" s="64"/>
+      <c r="H39" s="64"/>
+      <c r="I39" s="64"/>
       <c r="L39" s="8"/>
       <c r="M39" s="8"/>
       <c r="N39" s="8"/>
@@ -2725,17 +2761,17 @@
       <c r="S40" s="8"/>
     </row>
     <row r="41" customFormat="false" ht="17.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A41" s="57" t="s">
-        <v>76</v>
-      </c>
-      <c r="B41" s="58" t="s">
-        <v>77</v>
-      </c>
-      <c r="C41" s="58"/>
-      <c r="D41" s="58"/>
-      <c r="E41" s="58"/>
-      <c r="F41" s="66"/>
-      <c r="G41" s="66"/>
+      <c r="A41" s="56" t="s">
+        <v>84</v>
+      </c>
+      <c r="B41" s="57" t="s">
+        <v>85</v>
+      </c>
+      <c r="C41" s="57"/>
+      <c r="D41" s="57"/>
+      <c r="E41" s="57"/>
+      <c r="F41" s="65"/>
+      <c r="G41" s="65"/>
       <c r="L41" s="8"/>
       <c r="M41" s="8"/>
       <c r="N41" s="8"/>
@@ -2746,15 +2782,15 @@
       <c r="S41" s="8"/>
     </row>
     <row r="42" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="57"/>
-      <c r="B42" s="58" t="s">
-        <v>58</v>
-      </c>
-      <c r="C42" s="58"/>
-      <c r="D42" s="58"/>
-      <c r="E42" s="58"/>
-      <c r="F42" s="66"/>
-      <c r="G42" s="66"/>
+      <c r="A42" s="56"/>
+      <c r="B42" s="57" t="s">
+        <v>66</v>
+      </c>
+      <c r="C42" s="57"/>
+      <c r="D42" s="57"/>
+      <c r="E42" s="57"/>
+      <c r="F42" s="65"/>
+      <c r="G42" s="65"/>
       <c r="L42" s="8"/>
       <c r="M42" s="8"/>
       <c r="N42" s="8"/>
@@ -2764,372 +2800,372 @@
       <c r="R42" s="8"/>
       <c r="S42" s="8"/>
     </row>
-    <row r="43" s="68" customFormat="true" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="67"/>
-      <c r="B43" s="66"/>
-      <c r="C43" s="66"/>
-      <c r="D43" s="66"/>
-      <c r="E43" s="66"/>
-      <c r="F43" s="66"/>
-      <c r="G43" s="66"/>
-      <c r="L43" s="69"/>
-      <c r="M43" s="69"/>
-      <c r="N43" s="69"/>
-      <c r="O43" s="69"/>
-      <c r="P43" s="69"/>
-      <c r="Q43" s="69"/>
-      <c r="R43" s="69"/>
-      <c r="S43" s="69"/>
+    <row r="43" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="66"/>
+      <c r="B43" s="65"/>
+      <c r="C43" s="65"/>
+      <c r="D43" s="65"/>
+      <c r="E43" s="65"/>
+      <c r="F43" s="65"/>
+      <c r="G43" s="65"/>
+      <c r="L43" s="8"/>
+      <c r="M43" s="8"/>
+      <c r="N43" s="8"/>
+      <c r="O43" s="8"/>
+      <c r="P43" s="8"/>
+      <c r="Q43" s="8"/>
+      <c r="R43" s="8"/>
+      <c r="S43" s="8"/>
     </row>
     <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="70" t="s">
-        <v>78</v>
-      </c>
-      <c r="B44" s="70" t="s">
-        <v>79</v>
+      <c r="A44" s="67" t="s">
+        <v>86</v>
+      </c>
+      <c r="B44" s="67" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="71" t="n">
+      <c r="A45" s="68" t="n">
         <v>1</v>
       </c>
-      <c r="B45" s="72" t="s">
-        <v>80</v>
+      <c r="B45" s="69" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="71" t="n">
+      <c r="A46" s="68" t="n">
         <v>3</v>
       </c>
-      <c r="B46" s="72" t="s">
-        <v>81</v>
+      <c r="B46" s="69" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="71" t="n">
+      <c r="A47" s="68" t="n">
         <v>2</v>
       </c>
-      <c r="B47" s="72" t="s">
-        <v>82</v>
+      <c r="B47" s="69" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="71" t="n">
+      <c r="A48" s="68" t="n">
         <v>1</v>
       </c>
-      <c r="B48" s="72" t="s">
-        <v>83</v>
+      <c r="B48" s="69" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="71" t="n">
+      <c r="A49" s="68" t="n">
         <v>2</v>
       </c>
-      <c r="B49" s="72" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="50" s="68" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="73"/>
-      <c r="B50" s="74"/>
+      <c r="B49" s="69" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="13"/>
+      <c r="B50" s="70"/>
     </row>
     <row r="51" customFormat="false" ht="17.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A51" s="57" t="s">
-        <v>85</v>
-      </c>
-      <c r="B51" s="58" t="s">
-        <v>86</v>
-      </c>
-      <c r="C51" s="58"/>
-      <c r="D51" s="58"/>
-      <c r="E51" s="58"/>
-      <c r="F51" s="58"/>
-      <c r="G51" s="58"/>
-      <c r="H51" s="58"/>
-      <c r="I51" s="58"/>
+      <c r="A51" s="56" t="s">
+        <v>93</v>
+      </c>
+      <c r="B51" s="57" t="s">
+        <v>94</v>
+      </c>
+      <c r="C51" s="57"/>
+      <c r="D51" s="57"/>
+      <c r="E51" s="57"/>
+      <c r="F51" s="57"/>
+      <c r="G51" s="57"/>
+      <c r="H51" s="57"/>
+      <c r="I51" s="57"/>
     </row>
     <row r="52" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="57"/>
-      <c r="B52" s="58" t="s">
-        <v>58</v>
-      </c>
-      <c r="C52" s="58"/>
-      <c r="D52" s="58"/>
-      <c r="E52" s="58"/>
-      <c r="F52" s="58"/>
-      <c r="G52" s="58"/>
-      <c r="H52" s="58"/>
-      <c r="I52" s="58"/>
-    </row>
-    <row r="53" s="68" customFormat="true" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="67"/>
-      <c r="B53" s="66"/>
-      <c r="C53" s="66"/>
-      <c r="D53" s="66"/>
-      <c r="E53" s="66"/>
-      <c r="F53" s="66"/>
-      <c r="G53" s="66"/>
-      <c r="H53" s="75"/>
-      <c r="I53" s="75"/>
+      <c r="A52" s="56"/>
+      <c r="B52" s="57" t="s">
+        <v>66</v>
+      </c>
+      <c r="C52" s="57"/>
+      <c r="D52" s="57"/>
+      <c r="E52" s="57"/>
+      <c r="F52" s="57"/>
+      <c r="G52" s="57"/>
+      <c r="H52" s="57"/>
+      <c r="I52" s="57"/>
+    </row>
+    <row r="53" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="66"/>
+      <c r="B53" s="65"/>
+      <c r="C53" s="65"/>
+      <c r="D53" s="65"/>
+      <c r="E53" s="65"/>
+      <c r="F53" s="65"/>
+      <c r="G53" s="65"/>
+      <c r="H53" s="71"/>
+      <c r="I53" s="71"/>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="62" t="s">
-        <v>87</v>
-      </c>
-      <c r="B54" s="76" t="s">
+      <c r="A54" s="61" t="s">
+        <v>95</v>
+      </c>
+      <c r="B54" s="72" t="s">
         <v>27</v>
       </c>
-      <c r="C54" s="63" t="s">
+      <c r="C54" s="62" t="s">
         <v>41</v>
       </c>
-      <c r="D54" s="63" t="s">
+      <c r="D54" s="62" t="s">
         <v>47</v>
       </c>
-      <c r="E54" s="63" t="s">
-        <v>60</v>
-      </c>
-      <c r="F54" s="63" t="s">
-        <v>61</v>
-      </c>
-      <c r="G54" s="63" t="s">
-        <v>62</v>
-      </c>
-      <c r="H54" s="63" t="s">
-        <v>63</v>
-      </c>
-      <c r="I54" s="63" t="s">
-        <v>64</v>
-      </c>
-      <c r="J54" s="63" t="s">
-        <v>65</v>
+      <c r="E54" s="62" t="s">
+        <v>68</v>
+      </c>
+      <c r="F54" s="62" t="s">
+        <v>69</v>
+      </c>
+      <c r="G54" s="62" t="s">
+        <v>70</v>
+      </c>
+      <c r="H54" s="62" t="s">
+        <v>71</v>
+      </c>
+      <c r="I54" s="62" t="s">
+        <v>72</v>
+      </c>
+      <c r="J54" s="62" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="46.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="77" t="s">
-        <v>88</v>
-      </c>
-      <c r="B55" s="78" t="s">
+      <c r="A55" s="73" t="s">
+        <v>96</v>
+      </c>
+      <c r="B55" s="74" t="s">
         <v>43</v>
       </c>
-      <c r="C55" s="79" t="s">
-        <v>89</v>
-      </c>
-      <c r="D55" s="80"/>
-      <c r="E55" s="80"/>
-      <c r="F55" s="80"/>
-      <c r="G55" s="80"/>
-      <c r="H55" s="80"/>
-      <c r="I55" s="80"/>
-      <c r="J55" s="80"/>
+      <c r="C55" s="75" t="s">
+        <v>97</v>
+      </c>
+      <c r="D55" s="76"/>
+      <c r="E55" s="76"/>
+      <c r="F55" s="76"/>
+      <c r="G55" s="76"/>
+      <c r="H55" s="76"/>
+      <c r="I55" s="76"/>
+      <c r="J55" s="76"/>
     </row>
     <row r="56" customFormat="false" ht="23.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A56" s="81" t="s">
-        <v>90</v>
-      </c>
-      <c r="B56" s="82" t="s">
-        <v>91</v>
-      </c>
-      <c r="C56" s="65"/>
-      <c r="D56" s="83" t="s">
-        <v>92</v>
-      </c>
-      <c r="E56" s="65"/>
-      <c r="F56" s="65"/>
-      <c r="G56" s="65"/>
-      <c r="H56" s="65"/>
-      <c r="I56" s="65"/>
-      <c r="J56" s="65"/>
+      <c r="A56" s="77" t="s">
+        <v>98</v>
+      </c>
+      <c r="B56" s="78" t="s">
+        <v>99</v>
+      </c>
+      <c r="C56" s="64"/>
+      <c r="D56" s="79" t="s">
+        <v>100</v>
+      </c>
+      <c r="E56" s="64"/>
+      <c r="F56" s="64"/>
+      <c r="G56" s="64"/>
+      <c r="H56" s="64"/>
+      <c r="I56" s="64"/>
+      <c r="J56" s="64"/>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="81" t="s">
-        <v>90</v>
-      </c>
-      <c r="B57" s="82" t="s">
-        <v>93</v>
-      </c>
-      <c r="C57" s="65"/>
-      <c r="D57" s="83" t="s">
-        <v>92</v>
-      </c>
-      <c r="E57" s="65"/>
-      <c r="F57" s="65"/>
-      <c r="G57" s="65"/>
-      <c r="H57" s="65"/>
-      <c r="I57" s="65"/>
-      <c r="J57" s="65"/>
+      <c r="A57" s="77" t="s">
+        <v>98</v>
+      </c>
+      <c r="B57" s="78" t="s">
+        <v>101</v>
+      </c>
+      <c r="C57" s="64"/>
+      <c r="D57" s="79" t="s">
+        <v>100</v>
+      </c>
+      <c r="E57" s="64"/>
+      <c r="F57" s="64"/>
+      <c r="G57" s="64"/>
+      <c r="H57" s="64"/>
+      <c r="I57" s="64"/>
+      <c r="J57" s="64"/>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="81" t="s">
-        <v>90</v>
-      </c>
-      <c r="B58" s="84" t="s">
-        <v>94</v>
-      </c>
-      <c r="C58" s="65"/>
-      <c r="D58" s="83" t="s">
-        <v>92</v>
-      </c>
-      <c r="E58" s="65"/>
-      <c r="F58" s="65"/>
-      <c r="G58" s="65"/>
-      <c r="H58" s="65"/>
-      <c r="I58" s="65"/>
-      <c r="J58" s="65"/>
+      <c r="A58" s="77" t="s">
+        <v>98</v>
+      </c>
+      <c r="B58" s="80" t="s">
+        <v>102</v>
+      </c>
+      <c r="C58" s="64"/>
+      <c r="D58" s="79" t="s">
+        <v>100</v>
+      </c>
+      <c r="E58" s="64"/>
+      <c r="F58" s="64"/>
+      <c r="G58" s="64"/>
+      <c r="H58" s="64"/>
+      <c r="I58" s="64"/>
+      <c r="J58" s="64"/>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="81" t="s">
-        <v>90</v>
-      </c>
-      <c r="B59" s="84" t="s">
+      <c r="A59" s="77" t="s">
+        <v>98</v>
+      </c>
+      <c r="B59" s="80" t="s">
         <v>48</v>
       </c>
-      <c r="C59" s="65"/>
-      <c r="D59" s="83" t="s">
-        <v>92</v>
-      </c>
-      <c r="E59" s="65"/>
-      <c r="F59" s="65"/>
-      <c r="G59" s="65"/>
-      <c r="H59" s="65"/>
-      <c r="I59" s="65"/>
-      <c r="J59" s="65"/>
+      <c r="C59" s="64"/>
+      <c r="D59" s="79" t="s">
+        <v>100</v>
+      </c>
+      <c r="E59" s="64"/>
+      <c r="F59" s="64"/>
+      <c r="G59" s="64"/>
+      <c r="H59" s="64"/>
+      <c r="I59" s="64"/>
+      <c r="J59" s="64"/>
     </row>
     <row r="61" customFormat="false" ht="17.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A61" s="57" t="s">
-        <v>95</v>
-      </c>
-      <c r="B61" s="58" t="s">
-        <v>96</v>
-      </c>
-      <c r="C61" s="58"/>
-      <c r="D61" s="58"/>
-      <c r="E61" s="58"/>
-      <c r="F61" s="58"/>
-      <c r="G61" s="58"/>
+      <c r="A61" s="56" t="s">
+        <v>103</v>
+      </c>
+      <c r="B61" s="57" t="s">
+        <v>104</v>
+      </c>
+      <c r="C61" s="57"/>
+      <c r="D61" s="57"/>
+      <c r="E61" s="57"/>
+      <c r="F61" s="57"/>
+      <c r="G61" s="57"/>
     </row>
     <row r="62" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="57"/>
-      <c r="B62" s="58" t="s">
-        <v>58</v>
-      </c>
-      <c r="C62" s="58"/>
-      <c r="D62" s="58"/>
-      <c r="E62" s="58"/>
-      <c r="F62" s="58"/>
-      <c r="G62" s="58"/>
-    </row>
-    <row r="63" s="68" customFormat="true" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="67"/>
-      <c r="B63" s="66"/>
-      <c r="C63" s="66"/>
-      <c r="D63" s="66"/>
-      <c r="E63" s="66"/>
-      <c r="F63" s="66"/>
-      <c r="G63" s="66"/>
+      <c r="A62" s="56"/>
+      <c r="B62" s="57" t="s">
+        <v>66</v>
+      </c>
+      <c r="C62" s="57"/>
+      <c r="D62" s="57"/>
+      <c r="E62" s="57"/>
+      <c r="F62" s="57"/>
+      <c r="G62" s="57"/>
+    </row>
+    <row r="63" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="66"/>
+      <c r="B63" s="65"/>
+      <c r="C63" s="65"/>
+      <c r="D63" s="65"/>
+      <c r="E63" s="65"/>
+      <c r="F63" s="65"/>
+      <c r="G63" s="65"/>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="76" t="s">
+      <c r="A64" s="72" t="s">
         <v>27</v>
       </c>
-      <c r="B64" s="63" t="s">
+      <c r="B64" s="62" t="s">
         <v>41</v>
       </c>
-      <c r="C64" s="63" t="s">
+      <c r="C64" s="62" t="s">
         <v>47</v>
       </c>
-      <c r="D64" s="63" t="s">
-        <v>60</v>
-      </c>
-      <c r="E64" s="63" t="s">
-        <v>61</v>
-      </c>
-      <c r="F64" s="63" t="s">
-        <v>62</v>
-      </c>
-      <c r="G64" s="63" t="s">
-        <v>63</v>
-      </c>
-      <c r="H64" s="63" t="s">
-        <v>64</v>
-      </c>
-      <c r="I64" s="63" t="s">
-        <v>65</v>
+      <c r="D64" s="62" t="s">
+        <v>68</v>
+      </c>
+      <c r="E64" s="62" t="s">
+        <v>69</v>
+      </c>
+      <c r="F64" s="62" t="s">
+        <v>70</v>
+      </c>
+      <c r="G64" s="62" t="s">
+        <v>71</v>
+      </c>
+      <c r="H64" s="62" t="s">
+        <v>72</v>
+      </c>
+      <c r="I64" s="62" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="84" t="s">
+      <c r="A65" s="80" t="s">
         <v>43</v>
       </c>
-      <c r="B65" s="65" t="s">
-        <v>97</v>
-      </c>
-      <c r="C65" s="65" t="s">
-        <v>97</v>
-      </c>
-      <c r="D65" s="65"/>
-      <c r="E65" s="65"/>
-      <c r="F65" s="65"/>
-      <c r="G65" s="65"/>
-      <c r="H65" s="65"/>
-      <c r="I65" s="65"/>
+      <c r="B65" s="64" t="s">
+        <v>105</v>
+      </c>
+      <c r="C65" s="64" t="s">
+        <v>105</v>
+      </c>
+      <c r="D65" s="64"/>
+      <c r="E65" s="64"/>
+      <c r="F65" s="64"/>
+      <c r="G65" s="64"/>
+      <c r="H65" s="64"/>
+      <c r="I65" s="64"/>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="85" t="s">
-        <v>91</v>
-      </c>
-      <c r="B66" s="65"/>
-      <c r="C66" s="65"/>
-      <c r="D66" s="65"/>
-      <c r="E66" s="65"/>
-      <c r="F66" s="65"/>
-      <c r="G66" s="65"/>
-      <c r="H66" s="65"/>
-      <c r="I66" s="65"/>
+      <c r="A66" s="81" t="s">
+        <v>99</v>
+      </c>
+      <c r="B66" s="64"/>
+      <c r="C66" s="64"/>
+      <c r="D66" s="64"/>
+      <c r="E66" s="64"/>
+      <c r="F66" s="64"/>
+      <c r="G66" s="64"/>
+      <c r="H66" s="64"/>
+      <c r="I66" s="64"/>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="85" t="s">
-        <v>93</v>
-      </c>
-      <c r="B67" s="65" t="s">
-        <v>97</v>
-      </c>
-      <c r="C67" s="65" t="s">
-        <v>97</v>
-      </c>
-      <c r="D67" s="65"/>
-      <c r="E67" s="65"/>
-      <c r="F67" s="65"/>
-      <c r="G67" s="65"/>
-      <c r="H67" s="65"/>
-      <c r="I67" s="65"/>
+      <c r="A67" s="81" t="s">
+        <v>101</v>
+      </c>
+      <c r="B67" s="64" t="s">
+        <v>105</v>
+      </c>
+      <c r="C67" s="64" t="s">
+        <v>105</v>
+      </c>
+      <c r="D67" s="64"/>
+      <c r="E67" s="64"/>
+      <c r="F67" s="64"/>
+      <c r="G67" s="64"/>
+      <c r="H67" s="64"/>
+      <c r="I67" s="64"/>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="84" t="s">
-        <v>94</v>
-      </c>
-      <c r="B68" s="65"/>
-      <c r="C68" s="65"/>
-      <c r="D68" s="65"/>
-      <c r="E68" s="65"/>
-      <c r="F68" s="65"/>
-      <c r="G68" s="65"/>
-      <c r="H68" s="65"/>
-      <c r="I68" s="65"/>
+      <c r="A68" s="80" t="s">
+        <v>102</v>
+      </c>
+      <c r="B68" s="64"/>
+      <c r="C68" s="64"/>
+      <c r="D68" s="64"/>
+      <c r="E68" s="64"/>
+      <c r="F68" s="64"/>
+      <c r="G68" s="64"/>
+      <c r="H68" s="64"/>
+      <c r="I68" s="64"/>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="84" t="s">
+      <c r="A69" s="80" t="s">
         <v>48</v>
       </c>
-      <c r="B69" s="65"/>
-      <c r="C69" s="65" t="s">
-        <v>97</v>
-      </c>
-      <c r="D69" s="65"/>
-      <c r="E69" s="65"/>
-      <c r="F69" s="65"/>
-      <c r="G69" s="65"/>
-      <c r="H69" s="65"/>
-      <c r="I69" s="65"/>
+      <c r="B69" s="64"/>
+      <c r="C69" s="64" t="s">
+        <v>105</v>
+      </c>
+      <c r="D69" s="64"/>
+      <c r="E69" s="64"/>
+      <c r="F69" s="64"/>
+      <c r="G69" s="64"/>
+      <c r="H69" s="64"/>
+      <c r="I69" s="64"/>
     </row>
   </sheetData>
   <mergeCells count="19">
@@ -3186,207 +3222,207 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="86" t="s">
-        <v>98</v>
-      </c>
-      <c r="B1" s="86" t="s">
+      <c r="A1" s="82" t="s">
+        <v>106</v>
+      </c>
+      <c r="B1" s="82" t="s">
+        <v>107</v>
+      </c>
+      <c r="C1" s="82" t="s">
+        <v>108</v>
+      </c>
+      <c r="D1" s="82" t="s">
+        <v>109</v>
+      </c>
+      <c r="E1" s="82" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="52" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" s="82"/>
+      <c r="C2" s="82"/>
+      <c r="D2" s="82"/>
+      <c r="E2" s="82"/>
+    </row>
+    <row r="3" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="55" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3" s="55" t="s">
+        <v>111</v>
+      </c>
+      <c r="C3" s="83" t="s">
+        <v>112</v>
+      </c>
+      <c r="D3" s="83"/>
+      <c r="E3" s="55" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="55" t="s">
+        <v>51</v>
+      </c>
+      <c r="B4" s="55" t="s">
+        <v>114</v>
+      </c>
+      <c r="C4" s="55"/>
+      <c r="D4" s="55"/>
+      <c r="E4" s="83" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="55" t="s">
         <v>99</v>
       </c>
-      <c r="C1" s="86" t="s">
-        <v>100</v>
-      </c>
-      <c r="D1" s="86" t="s">
+      <c r="B5" s="55" t="s">
+        <v>116</v>
+      </c>
+      <c r="C5" s="55" t="s">
+        <v>117</v>
+      </c>
+      <c r="D5" s="55"/>
+      <c r="E5" s="55" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="55" t="s">
+        <v>119</v>
+      </c>
+      <c r="B6" s="55" t="s">
+        <v>120</v>
+      </c>
+      <c r="C6" s="55" t="s">
+        <v>121</v>
+      </c>
+      <c r="D6" s="55"/>
+      <c r="E6" s="55" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="55" t="s">
         <v>101</v>
       </c>
-      <c r="E1" s="86" t="s">
+      <c r="B7" s="55" t="s">
+        <v>123</v>
+      </c>
+      <c r="C7" s="55" t="s">
+        <v>124</v>
+      </c>
+      <c r="D7" s="55" t="s">
+        <v>125</v>
+      </c>
+      <c r="E7" s="83" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="55" t="s">
+        <v>127</v>
+      </c>
+      <c r="B8" s="55" t="s">
+        <v>128</v>
+      </c>
+      <c r="C8" s="83" t="s">
+        <v>129</v>
+      </c>
+      <c r="D8" s="83"/>
+      <c r="E8" s="55" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="55" t="s">
+        <v>131</v>
+      </c>
+      <c r="B9" s="55" t="s">
+        <v>132</v>
+      </c>
+      <c r="C9" s="83"/>
+      <c r="D9" s="83" t="s">
+        <v>133</v>
+      </c>
+      <c r="E9" s="55" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="55" t="s">
+        <v>134</v>
+      </c>
+      <c r="B10" s="55" t="s">
+        <v>135</v>
+      </c>
+      <c r="C10" s="55"/>
+      <c r="D10" s="55"/>
+      <c r="E10" s="55" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="55" t="s">
+        <v>137</v>
+      </c>
+      <c r="B11" s="55" t="s">
+        <v>138</v>
+      </c>
+      <c r="C11" s="55" t="s">
+        <v>139</v>
+      </c>
+      <c r="D11" s="55"/>
+      <c r="E11" s="83" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="55" t="s">
+        <v>141</v>
+      </c>
+      <c r="B12" s="55" t="s">
+        <v>142</v>
+      </c>
+      <c r="C12" s="55" t="s">
+        <v>143</v>
+      </c>
+      <c r="D12" s="55"/>
+      <c r="E12" s="83" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="55" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="53" t="s">
-        <v>43</v>
-      </c>
-      <c r="B2" s="86"/>
-      <c r="C2" s="86"/>
-      <c r="D2" s="86"/>
-      <c r="E2" s="86"/>
-    </row>
-    <row r="3" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="56" t="s">
-        <v>48</v>
-      </c>
-      <c r="B3" s="56" t="s">
-        <v>103</v>
-      </c>
-      <c r="C3" s="87" t="s">
-        <v>104</v>
-      </c>
-      <c r="D3" s="87"/>
-      <c r="E3" s="56" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="56" t="s">
-        <v>50</v>
-      </c>
-      <c r="B4" s="56" t="s">
-        <v>106</v>
-      </c>
-      <c r="C4" s="56"/>
-      <c r="D4" s="56"/>
-      <c r="E4" s="87" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="56" t="s">
-        <v>91</v>
-      </c>
-      <c r="B5" s="56" t="s">
-        <v>108</v>
-      </c>
-      <c r="C5" s="56" t="s">
-        <v>109</v>
-      </c>
-      <c r="D5" s="56"/>
-      <c r="E5" s="56" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="56" t="s">
-        <v>111</v>
-      </c>
-      <c r="B6" s="56" t="s">
-        <v>112</v>
-      </c>
-      <c r="C6" s="56" t="s">
-        <v>113</v>
-      </c>
-      <c r="D6" s="56"/>
-      <c r="E6" s="56" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="56" t="s">
-        <v>93</v>
-      </c>
-      <c r="B7" s="56" t="s">
-        <v>115</v>
-      </c>
-      <c r="C7" s="56" t="s">
-        <v>116</v>
-      </c>
-      <c r="D7" s="56" t="s">
-        <v>117</v>
-      </c>
-      <c r="E7" s="87" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="56" t="s">
-        <v>119</v>
-      </c>
-      <c r="B8" s="56" t="s">
-        <v>120</v>
-      </c>
-      <c r="C8" s="87" t="s">
-        <v>121</v>
-      </c>
-      <c r="D8" s="87"/>
-      <c r="E8" s="56" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="56" t="s">
-        <v>123</v>
-      </c>
-      <c r="B9" s="56" t="s">
-        <v>124</v>
-      </c>
-      <c r="C9" s="87"/>
-      <c r="D9" s="87" t="s">
-        <v>125</v>
-      </c>
-      <c r="E9" s="56" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="56" t="s">
-        <v>126</v>
-      </c>
-      <c r="B10" s="56" t="s">
-        <v>127</v>
-      </c>
-      <c r="C10" s="56"/>
-      <c r="D10" s="56"/>
-      <c r="E10" s="56" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="56" t="s">
-        <v>129</v>
-      </c>
-      <c r="B11" s="56" t="s">
-        <v>130</v>
-      </c>
-      <c r="C11" s="56" t="s">
-        <v>131</v>
-      </c>
-      <c r="D11" s="56"/>
-      <c r="E11" s="87" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="56" t="s">
-        <v>133</v>
-      </c>
-      <c r="B12" s="56" t="s">
-        <v>134</v>
-      </c>
-      <c r="C12" s="56" t="s">
-        <v>135</v>
-      </c>
-      <c r="D12" s="56"/>
-      <c r="E12" s="87" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="56" t="s">
-        <v>94</v>
-      </c>
-      <c r="B13" s="56" t="s">
-        <v>137</v>
-      </c>
-      <c r="C13" s="56" t="s">
-        <v>138</v>
-      </c>
-      <c r="D13" s="56"/>
-      <c r="E13" s="87" t="s">
-        <v>139</v>
+      <c r="B13" s="55" t="s">
+        <v>145</v>
+      </c>
+      <c r="C13" s="55" t="s">
+        <v>146</v>
+      </c>
+      <c r="D13" s="55"/>
+      <c r="E13" s="83" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="56" t="s">
-        <v>140</v>
-      </c>
-      <c r="B14" s="87" t="s">
-        <v>141</v>
-      </c>
-      <c r="C14" s="56" t="s">
-        <v>142</v>
-      </c>
-      <c r="D14" s="56"/>
-      <c r="E14" s="87" t="s">
-        <v>143</v>
+      <c r="A14" s="55" t="s">
+        <v>148</v>
+      </c>
+      <c r="B14" s="83" t="s">
+        <v>149</v>
+      </c>
+      <c r="C14" s="55" t="s">
+        <v>150</v>
+      </c>
+      <c r="D14" s="55"/>
+      <c r="E14" s="83" t="s">
+        <v>151</v>
       </c>
     </row>
   </sheetData>
@@ -3423,28 +3459,28 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="88" t="s">
-        <v>144</v>
-      </c>
-      <c r="B1" s="88" t="s">
-        <v>145</v>
-      </c>
-      <c r="C1" s="88" t="s">
-        <v>146</v>
-      </c>
-      <c r="D1" s="88" t="s">
-        <v>147</v>
-      </c>
-      <c r="E1" s="88" t="s">
-        <v>148</v>
-      </c>
-      <c r="F1" s="88" t="s">
-        <v>149</v>
+      <c r="A1" s="84" t="s">
+        <v>152</v>
+      </c>
+      <c r="B1" s="84" t="s">
+        <v>153</v>
+      </c>
+      <c r="C1" s="84" t="s">
+        <v>154</v>
+      </c>
+      <c r="D1" s="84" t="s">
+        <v>155</v>
+      </c>
+      <c r="E1" s="84" t="s">
+        <v>156</v>
+      </c>
+      <c r="F1" s="84" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>150</v>
+        <v>158</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>43</v>
@@ -3452,7 +3488,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>43</v>
@@ -3468,7 +3504,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
       <c r="B5" s="0" t="s">
         <v>43</v>
@@ -3476,7 +3512,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>153</v>
+        <v>161</v>
       </c>
       <c r="B6" s="0" t="s">
         <v>43</v>
@@ -3484,7 +3520,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B7" s="0" t="s">
         <v>43</v>
@@ -3492,7 +3528,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>154</v>
+        <v>162</v>
       </c>
       <c r="B8" s="0" t="s">
         <v>43</v>
@@ -3500,7 +3536,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="B9" s="0" t="s">
         <v>43</v>
@@ -3508,7 +3544,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="B10" s="0" t="s">
         <v>43</v>
@@ -3516,7 +3552,7 @@
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="B11" s="0" t="s">
         <v>43</v>
@@ -3524,7 +3560,7 @@
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>156</v>
+        <v>164</v>
       </c>
       <c r="B12" s="0" t="s">
         <v>43</v>
@@ -3532,7 +3568,7 @@
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>157</v>
+        <v>165</v>
       </c>
       <c r="B13" s="0" t="s">
         <v>43</v>
@@ -3540,7 +3576,7 @@
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>158</v>
+        <v>166</v>
       </c>
       <c r="B14" s="0" t="s">
         <v>43</v>
@@ -3548,7 +3584,7 @@
     </row>
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>159</v>
+        <v>167</v>
       </c>
       <c r="B15" s="0" t="s">
         <v>43</v>
@@ -3556,7 +3592,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>160</v>
+        <v>168</v>
       </c>
       <c r="B16" s="0" t="s">
         <v>43</v>
@@ -3564,7 +3600,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>161</v>
+        <v>169</v>
       </c>
       <c r="B17" s="0" t="s">
         <v>43</v>
@@ -3572,7 +3608,7 @@
     </row>
     <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>162</v>
+        <v>170</v>
       </c>
       <c r="B18" s="0" t="s">
         <v>43</v>
@@ -3580,7 +3616,7 @@
     </row>
     <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>163</v>
+        <v>171</v>
       </c>
       <c r="B19" s="0" t="s">
         <v>43</v>
@@ -3588,7 +3624,7 @@
     </row>
     <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>164</v>
+        <v>172</v>
       </c>
       <c r="B20" s="0" t="s">
         <v>43</v>
@@ -3604,7 +3640,7 @@
     </row>
     <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>165</v>
+        <v>173</v>
       </c>
       <c r="B22" s="0" t="s">
         <v>43</v>
@@ -3612,7 +3648,7 @@
     </row>
     <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>166</v>
+        <v>174</v>
       </c>
       <c r="B23" s="0" t="s">
         <v>43</v>
@@ -3620,7 +3656,7 @@
     </row>
     <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>167</v>
+        <v>175</v>
       </c>
       <c r="B24" s="0" t="s">
         <v>43</v>
@@ -3628,7 +3664,7 @@
     </row>
     <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>168</v>
+        <v>176</v>
       </c>
       <c r="B25" s="0" t="s">
         <v>43</v>
@@ -3636,87 +3672,87 @@
     </row>
     <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>169</v>
+        <v>177</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>94</v>
+        <v>102</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>170</v>
+        <v>178</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>94</v>
+        <v>102</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>119</v>
+        <v>127</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>171</v>
+        <v>179</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>119</v>
+        <v>127</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>172</v>
+        <v>180</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>119</v>
+        <v>127</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>173</v>
+        <v>181</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>119</v>
+        <v>127</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>174</v>
+        <v>182</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>175</v>
+        <v>183</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>176</v>
+        <v>184</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>177</v>
+        <v>185</v>
       </c>
       <c r="B36" s="0" t="s">
         <v>48</v>
@@ -3724,7 +3760,7 @@
     </row>
     <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>178</v>
+        <v>186</v>
       </c>
       <c r="B37" s="0" t="s">
         <v>48</v>
@@ -3732,7 +3768,7 @@
     </row>
     <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="B38" s="0" t="s">
         <v>48</v>
@@ -3740,7 +3776,7 @@
     </row>
     <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>179</v>
+        <v>187</v>
       </c>
       <c r="B39" s="0" t="s">
         <v>48</v>
@@ -3748,7 +3784,7 @@
     </row>
     <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>180</v>
+        <v>188</v>
       </c>
       <c r="B40" s="0" t="s">
         <v>48</v>
@@ -3756,7 +3792,7 @@
     </row>
     <row r="41" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>181</v>
+        <v>189</v>
       </c>
       <c r="B41" s="0" t="s">
         <v>48</v>
@@ -3764,7 +3800,7 @@
     </row>
     <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>180</v>
+        <v>188</v>
       </c>
       <c r="B42" s="0" t="s">
         <v>48</v>
@@ -3772,7 +3808,7 @@
     </row>
     <row r="43" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>181</v>
+        <v>189</v>
       </c>
       <c r="B43" s="0" t="s">
         <v>48</v>
@@ -3780,7 +3816,7 @@
     </row>
     <row r="44" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>180</v>
+        <v>188</v>
       </c>
       <c r="B44" s="0" t="s">
         <v>48</v>
@@ -3788,7 +3824,7 @@
     </row>
     <row r="45" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>181</v>
+        <v>189</v>
       </c>
       <c r="B45" s="0" t="s">
         <v>48</v>
@@ -3796,69 +3832,69 @@
     </row>
     <row r="46" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>182</v>
+        <v>190</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>183</v>
+        <v>191</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>182</v>
+        <v>190</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>183</v>
+        <v>191</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>184</v>
+        <v>192</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>185</v>
+        <v>193</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>162</v>
+        <v>170</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>163</v>
+        <v>171</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="D53" s="0" t="s">
-        <v>184</v>
+        <v>192</v>
       </c>
       <c r="E53" s="0" t="str">
         <f aca="false">+VLOOKUP(D53,A1:B121,1)</f>
@@ -3867,546 +3903,546 @@
     </row>
     <row r="54" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>186</v>
+        <v>194</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>187</v>
+        <v>195</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>188</v>
+        <v>196</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>189</v>
+        <v>197</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>190</v>
+        <v>198</v>
       </c>
       <c r="B58" s="0" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>191</v>
+        <v>199</v>
       </c>
       <c r="B59" s="0" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>192</v>
+        <v>200</v>
       </c>
       <c r="B60" s="0" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>193</v>
+        <v>201</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>180</v>
+        <v>188</v>
       </c>
       <c r="B62" s="0" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>181</v>
+        <v>189</v>
       </c>
       <c r="B63" s="0" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>194</v>
-      </c>
-      <c r="B64" s="89" t="s">
-        <v>50</v>
+        <v>202</v>
+      </c>
+      <c r="B64" s="85" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>195</v>
-      </c>
-      <c r="B65" s="89" t="s">
-        <v>50</v>
+        <v>203</v>
+      </c>
+      <c r="B65" s="85" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>196</v>
-      </c>
-      <c r="B66" s="89" t="s">
-        <v>50</v>
+        <v>204</v>
+      </c>
+      <c r="B66" s="85" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>197</v>
-      </c>
-      <c r="B67" s="89" t="s">
-        <v>50</v>
+        <v>205</v>
+      </c>
+      <c r="B67" s="85" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="B68" s="89" t="s">
-        <v>50</v>
+        <v>62</v>
+      </c>
+      <c r="B68" s="85" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>171</v>
-      </c>
-      <c r="B69" s="89" t="s">
-        <v>50</v>
+        <v>179</v>
+      </c>
+      <c r="B69" s="85" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>198</v>
-      </c>
-      <c r="B70" s="89" t="s">
-        <v>50</v>
+        <v>206</v>
+      </c>
+      <c r="B70" s="85" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>199</v>
-      </c>
-      <c r="B71" s="89" t="s">
-        <v>50</v>
+        <v>207</v>
+      </c>
+      <c r="B71" s="85" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>200</v>
-      </c>
-      <c r="B72" s="89" t="s">
-        <v>50</v>
+        <v>208</v>
+      </c>
+      <c r="B72" s="85" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
-        <v>201</v>
-      </c>
-      <c r="B73" s="89" t="s">
-        <v>50</v>
+        <v>209</v>
+      </c>
+      <c r="B73" s="85" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
-        <v>202</v>
-      </c>
-      <c r="B74" s="89" t="s">
-        <v>50</v>
+        <v>210</v>
+      </c>
+      <c r="B74" s="85" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
-        <v>203</v>
-      </c>
-      <c r="B75" s="89" t="s">
-        <v>50</v>
+        <v>211</v>
+      </c>
+      <c r="B75" s="85" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
-        <v>204</v>
-      </c>
-      <c r="B76" s="89" t="s">
-        <v>50</v>
+        <v>212</v>
+      </c>
+      <c r="B76" s="85" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
-        <v>205</v>
-      </c>
-      <c r="B77" s="89" t="s">
-        <v>50</v>
+        <v>213</v>
+      </c>
+      <c r="B77" s="85" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
-        <v>206</v>
-      </c>
-      <c r="B78" s="89" t="s">
-        <v>50</v>
+        <v>214</v>
+      </c>
+      <c r="B78" s="85" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
-        <v>207</v>
-      </c>
-      <c r="B79" s="89" t="s">
-        <v>50</v>
+        <v>215</v>
+      </c>
+      <c r="B79" s="85" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
-        <v>208</v>
-      </c>
-      <c r="B80" s="89" t="s">
-        <v>50</v>
+        <v>216</v>
+      </c>
+      <c r="B80" s="85" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
-        <v>209</v>
-      </c>
-      <c r="B81" s="89" t="s">
-        <v>50</v>
+        <v>217</v>
+      </c>
+      <c r="B81" s="85" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
-        <v>210</v>
-      </c>
-      <c r="B82" s="89" t="s">
-        <v>50</v>
+        <v>218</v>
+      </c>
+      <c r="B82" s="85" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
-        <v>211</v>
-      </c>
-      <c r="B83" s="89" t="s">
-        <v>50</v>
+        <v>219</v>
+      </c>
+      <c r="B83" s="85" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
-        <v>212</v>
-      </c>
-      <c r="B84" s="89" t="s">
-        <v>50</v>
+        <v>220</v>
+      </c>
+      <c r="B84" s="85" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="s">
-        <v>213</v>
-      </c>
-      <c r="B85" s="89" t="s">
-        <v>50</v>
+        <v>221</v>
+      </c>
+      <c r="B85" s="85" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
-        <v>214</v>
-      </c>
-      <c r="B86" s="89" t="s">
-        <v>50</v>
+        <v>222</v>
+      </c>
+      <c r="B86" s="85" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
-        <v>215</v>
-      </c>
-      <c r="B87" s="89" t="s">
-        <v>50</v>
+        <v>223</v>
+      </c>
+      <c r="B87" s="85" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
-        <v>216</v>
-      </c>
-      <c r="B88" s="89" t="s">
-        <v>50</v>
+        <v>224</v>
+      </c>
+      <c r="B88" s="85" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
-        <v>217</v>
-      </c>
-      <c r="B89" s="89" t="s">
-        <v>50</v>
+        <v>225</v>
+      </c>
+      <c r="B89" s="85" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
-        <v>175</v>
+        <v>183</v>
       </c>
       <c r="B90" s="0" t="s">
-        <v>119</v>
+        <v>127</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="s">
-        <v>176</v>
+        <v>184</v>
       </c>
       <c r="B91" s="0" t="s">
-        <v>119</v>
+        <v>127</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="B92" s="0" t="s">
-        <v>119</v>
+        <v>127</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="s">
-        <v>219</v>
+        <v>227</v>
       </c>
       <c r="B93" s="0" t="s">
-        <v>119</v>
+        <v>127</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="s">
-        <v>220</v>
+        <v>228</v>
       </c>
       <c r="B94" s="0" t="s">
-        <v>221</v>
+        <v>229</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="s">
-        <v>222</v>
+        <v>230</v>
       </c>
       <c r="B95" s="0" t="s">
-        <v>221</v>
+        <v>229</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="0" t="s">
-        <v>223</v>
+        <v>231</v>
       </c>
       <c r="B96" s="0" t="s">
-        <v>221</v>
+        <v>229</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="0" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="B97" s="0" t="s">
-        <v>221</v>
+        <v>229</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="0" t="s">
-        <v>225</v>
+        <v>233</v>
       </c>
       <c r="B98" s="0" t="s">
-        <v>129</v>
+        <v>137</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="0" t="s">
-        <v>226</v>
+        <v>234</v>
       </c>
       <c r="B99" s="0" t="s">
-        <v>129</v>
+        <v>137</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="0" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="B100" s="0" t="s">
-        <v>123</v>
+        <v>131</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="0" t="s">
-        <v>228</v>
+        <v>236</v>
       </c>
       <c r="B101" s="0" t="s">
-        <v>123</v>
+        <v>131</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="0" t="s">
-        <v>229</v>
-      </c>
-      <c r="B102" s="89" t="s">
-        <v>50</v>
+        <v>237</v>
+      </c>
+      <c r="B102" s="85" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="0" t="s">
-        <v>230</v>
-      </c>
-      <c r="B103" s="89" t="s">
-        <v>50</v>
+        <v>238</v>
+      </c>
+      <c r="B103" s="85" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="0" t="s">
-        <v>231</v>
-      </c>
-      <c r="B104" s="89" t="s">
-        <v>50</v>
+        <v>239</v>
+      </c>
+      <c r="B104" s="85" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="0" t="s">
-        <v>232</v>
-      </c>
-      <c r="B105" s="89" t="s">
-        <v>50</v>
+        <v>240</v>
+      </c>
+      <c r="B105" s="85" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="0" t="s">
-        <v>233</v>
-      </c>
-      <c r="B106" s="89" t="s">
-        <v>50</v>
+        <v>241</v>
+      </c>
+      <c r="B106" s="85" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="0" t="s">
-        <v>234</v>
-      </c>
-      <c r="B107" s="89" t="s">
-        <v>50</v>
+        <v>242</v>
+      </c>
+      <c r="B107" s="85" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="0" t="s">
-        <v>235</v>
-      </c>
-      <c r="B108" s="89" t="s">
-        <v>50</v>
+        <v>243</v>
+      </c>
+      <c r="B108" s="85" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="0" t="s">
-        <v>236</v>
-      </c>
-      <c r="B109" s="89" t="s">
-        <v>50</v>
+        <v>244</v>
+      </c>
+      <c r="B109" s="85" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="0" t="s">
-        <v>237</v>
-      </c>
-      <c r="B110" s="89" t="s">
-        <v>50</v>
+        <v>245</v>
+      </c>
+      <c r="B110" s="85" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="0" t="s">
-        <v>238</v>
-      </c>
-      <c r="B111" s="89" t="s">
-        <v>50</v>
+        <v>246</v>
+      </c>
+      <c r="B111" s="85" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="0" t="s">
-        <v>239</v>
-      </c>
-      <c r="B112" s="89" t="s">
-        <v>50</v>
+        <v>247</v>
+      </c>
+      <c r="B112" s="85" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="0" t="s">
-        <v>240</v>
-      </c>
-      <c r="B113" s="89" t="s">
-        <v>50</v>
+        <v>248</v>
+      </c>
+      <c r="B113" s="85" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="0" t="s">
-        <v>241</v>
-      </c>
-      <c r="B114" s="89" t="s">
-        <v>50</v>
+        <v>249</v>
+      </c>
+      <c r="B114" s="85" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="0" t="s">
-        <v>242</v>
-      </c>
-      <c r="B115" s="89" t="s">
-        <v>50</v>
+        <v>250</v>
+      </c>
+      <c r="B115" s="85" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="0" t="s">
-        <v>243</v>
-      </c>
-      <c r="B116" s="89" t="s">
-        <v>50</v>
+        <v>251</v>
+      </c>
+      <c r="B116" s="85" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="0" t="s">
-        <v>244</v>
-      </c>
-      <c r="B117" s="89" t="s">
-        <v>50</v>
+        <v>252</v>
+      </c>
+      <c r="B117" s="85" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="0" t="s">
-        <v>245</v>
-      </c>
-      <c r="B118" s="89" t="s">
-        <v>50</v>
+        <v>253</v>
+      </c>
+      <c r="B118" s="85" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="0" t="s">
-        <v>246</v>
-      </c>
-      <c r="B119" s="89" t="s">
-        <v>50</v>
+        <v>254</v>
+      </c>
+      <c r="B119" s="85" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="0" t="s">
-        <v>247</v>
+        <v>255</v>
       </c>
       <c r="B120" s="0" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="0" t="s">
-        <v>248</v>
+        <v>256</v>
       </c>
       <c r="B121" s="0" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -4442,63 +4478,63 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="90" t="s">
-        <v>249</v>
-      </c>
-      <c r="B1" s="91" t="s">
+      <c r="A1" s="86" t="s">
+        <v>257</v>
+      </c>
+      <c r="B1" s="87" t="s">
         <v>47</v>
       </c>
-      <c r="C1" s="91" t="s">
-        <v>61</v>
-      </c>
-      <c r="D1" s="91" t="s">
-        <v>63</v>
-      </c>
-      <c r="E1" s="91" t="s">
-        <v>65</v>
+      <c r="C1" s="87" t="s">
+        <v>69</v>
+      </c>
+      <c r="D1" s="87" t="s">
+        <v>71</v>
+      </c>
+      <c r="E1" s="87" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="92" t="s">
+      <c r="A2" s="88" t="s">
         <v>41</v>
       </c>
-      <c r="B2" s="65" t="n">
+      <c r="B2" s="64" t="n">
         <v>1</v>
       </c>
-      <c r="C2" s="65"/>
-      <c r="D2" s="65"/>
-      <c r="E2" s="65"/>
+      <c r="C2" s="64"/>
+      <c r="D2" s="64"/>
+      <c r="E2" s="64"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="92" t="s">
-        <v>60</v>
-      </c>
-      <c r="B3" s="65"/>
-      <c r="C3" s="65" t="n">
+      <c r="A3" s="88" t="s">
+        <v>68</v>
+      </c>
+      <c r="B3" s="64"/>
+      <c r="C3" s="64" t="n">
         <v>1</v>
       </c>
-      <c r="D3" s="65"/>
-      <c r="E3" s="65"/>
+      <c r="D3" s="64"/>
+      <c r="E3" s="64"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="92" t="s">
-        <v>62</v>
-      </c>
-      <c r="B4" s="65"/>
-      <c r="C4" s="65"/>
-      <c r="D4" s="65" t="n">
+      <c r="A4" s="88" t="s">
+        <v>70</v>
+      </c>
+      <c r="B4" s="64"/>
+      <c r="C4" s="64"/>
+      <c r="D4" s="64" t="n">
         <v>1</v>
       </c>
-      <c r="E4" s="65"/>
+      <c r="E4" s="64"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="92" t="s">
-        <v>64</v>
-      </c>
-      <c r="B5" s="65"/>
-      <c r="C5" s="65"/>
-      <c r="D5" s="65"/>
-      <c r="E5" s="65" t="n">
+      <c r="A5" s="88" t="s">
+        <v>72</v>
+      </c>
+      <c r="B5" s="64"/>
+      <c r="C5" s="64"/>
+      <c r="D5" s="64"/>
+      <c r="E5" s="64" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Correcciones al codigo generador de los csv
</commit_message>
<xml_diff>
--- a/Oficial/Patron_FL.xlsx
+++ b/Oficial/Patron_FL.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="384" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="426" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="BASE_SSE" sheetId="1" state="visible" r:id="rId2"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="258">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="261">
   <si>
     <t>SOLICITUD  DE SERVICIO EXTERNO A LABORATORIO</t>
   </si>
@@ -181,6 +181,9 @@
     <t>CEA-1</t>
   </si>
   <si>
+    <t>UF</t>
+  </si>
+  <si>
     <t>Feofitina total</t>
   </si>
   <si>
@@ -193,6 +196,9 @@
     <t>CEA0</t>
   </si>
   <si>
+    <t>US</t>
+  </si>
+  <si>
     <t>Fósforo  disuelto</t>
   </si>
   <si>
@@ -200,6 +206,9 @@
   </si>
   <si>
     <t>CEA1</t>
+  </si>
+  <si>
+    <t>CLP$</t>
   </si>
   <si>
     <t>CEA2</t>
@@ -1620,15 +1629,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>739440</xdr:colOff>
+      <xdr:colOff>766440</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>7560</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1297440</xdr:colOff>
+      <xdr:colOff>1324080</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>773280</xdr:rowOff>
+      <xdr:rowOff>772920</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1641,8 +1650,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="739440" y="7560"/>
-          <a:ext cx="558000" cy="765720"/>
+          <a:off x="766440" y="7560"/>
+          <a:ext cx="557640" cy="765360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1664,8 +1673,8 @@
   </sheetPr>
   <dimension ref="A1:S69"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I17" activeCellId="0" sqref="I17"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A16" activeCellId="0" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1833,7 +1842,7 @@
       </c>
       <c r="B8" s="14" t="n">
         <f aca="true">+TODAY()</f>
-        <v>42083</v>
+        <v>42087</v>
       </c>
       <c r="C8" s="15"/>
       <c r="D8" s="16"/>
@@ -1884,7 +1893,7 @@
       </c>
       <c r="B10" s="20" t="n">
         <f aca="false">+B9-B8</f>
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C10" s="21" t="s">
         <v>14</v>
@@ -2076,12 +2085,10 @@
         <v>0</v>
       </c>
       <c r="K16" s="53" t="n">
-        <f aca="false">+VLOOKUP(B16,Parametros!A$1:E$121,4,)</f>
-        <v>0</v>
-      </c>
-      <c r="L16" s="53" t="n">
-        <f aca="false">+VLOOKUP(B16,Parametros!A$1:G$121,5,)</f>
-        <v>0</v>
+        <v>100</v>
+      </c>
+      <c r="L16" s="53" t="s">
+        <v>46</v>
       </c>
       <c r="M16" s="54"/>
       <c r="N16" s="54"/>
@@ -2096,36 +2103,34 @@
         <v>11</v>
       </c>
       <c r="B17" s="54" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C17" s="49" t="n">
         <v>5</v>
       </c>
       <c r="D17" s="50" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E17" s="51" t="s">
         <v>42</v>
       </c>
       <c r="F17" s="51"/>
       <c r="G17" s="55" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H17" s="51"/>
       <c r="I17" s="51" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="J17" s="53" t="n">
         <f aca="false">+VLOOKUP(B17,Parametros!A$1:D$121,3,)</f>
         <v>0</v>
       </c>
       <c r="K17" s="53" t="n">
-        <f aca="false">+VLOOKUP(B17,Parametros!A$1:E$121,4,)</f>
-        <v>0</v>
-      </c>
-      <c r="L17" s="53" t="n">
-        <f aca="false">+VLOOKUP(B17,Parametros!A$1:G$121,5,)</f>
-        <v>0</v>
+        <v>101</v>
+      </c>
+      <c r="L17" s="53" t="s">
+        <v>51</v>
       </c>
       <c r="M17" s="54"/>
       <c r="N17" s="54"/>
@@ -2140,7 +2145,7 @@
         <v>12</v>
       </c>
       <c r="B18" s="54" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C18" s="49" t="n">
         <v>3</v>
@@ -2153,23 +2158,21 @@
       </c>
       <c r="F18" s="51"/>
       <c r="G18" s="55" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H18" s="51"/>
       <c r="I18" s="51" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="J18" s="53" t="n">
         <f aca="false">+VLOOKUP(B18,Parametros!A$1:D$121,3,)</f>
         <v>0</v>
       </c>
       <c r="K18" s="53" t="n">
-        <f aca="false">+VLOOKUP(B18,Parametros!A$1:E$121,4,)</f>
-        <v>0</v>
-      </c>
-      <c r="L18" s="53" t="n">
-        <f aca="false">+VLOOKUP(B18,Parametros!A$1:G$121,5,)</f>
-        <v>0</v>
+        <v>102</v>
+      </c>
+      <c r="L18" s="53" t="s">
+        <v>55</v>
       </c>
       <c r="M18" s="54"/>
       <c r="N18" s="54"/>
@@ -2201,19 +2204,17 @@
       </c>
       <c r="H19" s="51"/>
       <c r="I19" s="51" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="J19" s="53" t="n">
         <f aca="false">+VLOOKUP(B19,Parametros!A$1:D$121,3,)</f>
         <v>0</v>
       </c>
       <c r="K19" s="53" t="n">
-        <f aca="false">+VLOOKUP(B19,Parametros!A$1:E$121,4,)</f>
-        <v>0</v>
-      </c>
-      <c r="L19" s="53" t="n">
-        <f aca="false">+VLOOKUP(B19,Parametros!A$1:G$121,5,)</f>
-        <v>0</v>
+        <v>103</v>
+      </c>
+      <c r="L19" s="53" t="s">
+        <v>55</v>
       </c>
       <c r="M19" s="54"/>
       <c r="N19" s="54"/>
@@ -2228,7 +2229,7 @@
         <v>14</v>
       </c>
       <c r="B20" s="54" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="C20" s="49" t="n">
         <v>5</v>
@@ -2245,19 +2246,17 @@
       </c>
       <c r="H20" s="51"/>
       <c r="I20" s="51" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="J20" s="53" t="n">
         <f aca="false">+VLOOKUP(B20,Parametros!A$1:D$121,3,)</f>
         <v>0</v>
       </c>
       <c r="K20" s="53" t="n">
-        <f aca="false">+VLOOKUP(B20,Parametros!A$1:E$121,4,)</f>
-        <v>0</v>
-      </c>
-      <c r="L20" s="53" t="n">
-        <f aca="false">+VLOOKUP(B20,Parametros!A$1:G$121,5,)</f>
-        <v>0</v>
+        <v>104</v>
+      </c>
+      <c r="L20" s="53" t="s">
+        <v>55</v>
       </c>
       <c r="M20" s="54"/>
       <c r="N20" s="54"/>
@@ -2272,7 +2271,7 @@
         <v>15</v>
       </c>
       <c r="B21" s="54" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="C21" s="49" t="n">
         <v>6</v>
@@ -2289,19 +2288,17 @@
       </c>
       <c r="H21" s="51"/>
       <c r="I21" s="51" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="J21" s="53" t="n">
         <f aca="false">+VLOOKUP(B21,Parametros!A$1:D$121,3,)</f>
         <v>0</v>
       </c>
       <c r="K21" s="53" t="n">
-        <f aca="false">+VLOOKUP(B21,Parametros!A$1:E$121,4,)</f>
-        <v>0</v>
-      </c>
-      <c r="L21" s="53" t="n">
-        <f aca="false">+VLOOKUP(B21,Parametros!A$1:G$121,5,)</f>
-        <v>0</v>
+        <v>105</v>
+      </c>
+      <c r="L21" s="53" t="s">
+        <v>55</v>
       </c>
       <c r="M21" s="54"/>
       <c r="N21" s="54"/>
@@ -2316,13 +2313,13 @@
         <v>16</v>
       </c>
       <c r="B22" s="54" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="C22" s="49" t="n">
         <v>7</v>
       </c>
       <c r="D22" s="50" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E22" s="51" t="s">
         <v>42</v>
@@ -2333,19 +2330,17 @@
       </c>
       <c r="H22" s="51"/>
       <c r="I22" s="51" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="J22" s="53" t="n">
         <f aca="false">+VLOOKUP(B22,Parametros!A$1:D$121,3,)</f>
         <v>0</v>
       </c>
       <c r="K22" s="53" t="n">
-        <f aca="false">+VLOOKUP(B22,Parametros!A$1:E$121,4,)</f>
-        <v>0</v>
-      </c>
-      <c r="L22" s="53" t="n">
-        <f aca="false">+VLOOKUP(B22,Parametros!A$1:G$121,5,)</f>
-        <v>0</v>
+        <v>106</v>
+      </c>
+      <c r="L22" s="53" t="s">
+        <v>55</v>
       </c>
       <c r="M22" s="54"/>
       <c r="N22" s="54"/>
@@ -2360,7 +2355,7 @@
         <v>17</v>
       </c>
       <c r="B23" s="54" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="C23" s="49" t="n">
         <v>8</v>
@@ -2377,19 +2372,17 @@
       </c>
       <c r="H23" s="54"/>
       <c r="I23" s="51" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="J23" s="53" t="n">
         <f aca="false">+VLOOKUP(B23,Parametros!A$1:D$121,3,)</f>
         <v>0</v>
       </c>
       <c r="K23" s="53" t="n">
-        <f aca="false">+VLOOKUP(B23,Parametros!A$1:E$121,4,)</f>
-        <v>0</v>
-      </c>
-      <c r="L23" s="53" t="n">
-        <f aca="false">+VLOOKUP(B23,Parametros!A$1:G$121,5,)</f>
-        <v>0</v>
+        <v>107</v>
+      </c>
+      <c r="L23" s="53" t="s">
+        <v>55</v>
       </c>
       <c r="M23" s="54"/>
       <c r="N23" s="54"/>
@@ -2404,13 +2397,13 @@
         <v>18</v>
       </c>
       <c r="B24" s="54" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="C24" s="49" t="n">
         <v>9</v>
       </c>
       <c r="D24" s="50" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E24" s="51" t="s">
         <v>42</v>
@@ -2421,19 +2414,17 @@
       </c>
       <c r="H24" s="51"/>
       <c r="I24" s="51" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="J24" s="53" t="n">
         <f aca="false">+VLOOKUP(B24,Parametros!A$1:D$121,3,)</f>
         <v>0</v>
       </c>
       <c r="K24" s="53" t="n">
-        <f aca="false">+VLOOKUP(B24,Parametros!A$1:E$121,4,)</f>
-        <v>0</v>
-      </c>
-      <c r="L24" s="53" t="n">
-        <f aca="false">+VLOOKUP(B24,Parametros!A$1:G$121,5,)</f>
-        <v>0</v>
+        <v>108</v>
+      </c>
+      <c r="L24" s="53" t="s">
+        <v>55</v>
       </c>
       <c r="M24" s="54"/>
       <c r="N24" s="54"/>
@@ -2446,10 +2437,10 @@
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="26" customFormat="false" ht="17.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="56" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="B26" s="57" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="C26" s="57"/>
       <c r="D26" s="57"/>
@@ -2462,7 +2453,7 @@
     <row r="27" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="56"/>
       <c r="B27" s="57" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="C27" s="57"/>
       <c r="D27" s="57"/>
@@ -2483,36 +2474,36 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="61" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="B29" s="62" t="s">
         <v>41</v>
       </c>
       <c r="C29" s="62" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D29" s="62" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="E29" s="62" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="F29" s="62" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="G29" s="62" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="H29" s="62" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="I29" s="62" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="63" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="B30" s="64" t="n">
         <v>1</v>
@@ -2537,7 +2528,7 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="63" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="B31" s="64" t="n">
         <v>1</v>
@@ -2562,7 +2553,7 @@
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="63" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="B32" s="64" t="n">
         <v>1</v>
@@ -2585,7 +2576,7 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="63" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="B33" s="64" t="n">
         <v>1</v>
@@ -2608,7 +2599,7 @@
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="63" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="B34" s="64" t="n">
         <v>1</v>
@@ -2633,7 +2624,7 @@
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="63" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="B35" s="64" t="n">
         <v>1</v>
@@ -2656,7 +2647,7 @@
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="63" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="B36" s="64" t="n">
         <v>1</v>
@@ -2679,7 +2670,7 @@
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="63" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="B37" s="64" t="n">
         <v>1</v>
@@ -2704,7 +2695,7 @@
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="63" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="B38" s="64" t="n">
         <v>1</v>
@@ -2727,7 +2718,7 @@
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="63" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="B39" s="64" t="n">
         <v>1</v>
@@ -2762,10 +2753,10 @@
     </row>
     <row r="41" customFormat="false" ht="17.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="56" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="B41" s="57" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="C41" s="57"/>
       <c r="D41" s="57"/>
@@ -2784,7 +2775,7 @@
     <row r="42" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="56"/>
       <c r="B42" s="57" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="C42" s="57"/>
       <c r="D42" s="57"/>
@@ -2819,10 +2810,10 @@
     </row>
     <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="67" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="B44" s="67" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2830,7 +2821,7 @@
         <v>1</v>
       </c>
       <c r="B45" s="69" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2838,7 +2829,7 @@
         <v>3</v>
       </c>
       <c r="B46" s="69" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2846,7 +2837,7 @@
         <v>2</v>
       </c>
       <c r="B47" s="69" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2854,7 +2845,7 @@
         <v>1</v>
       </c>
       <c r="B48" s="69" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2862,7 +2853,7 @@
         <v>2</v>
       </c>
       <c r="B49" s="69" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2871,10 +2862,10 @@
     </row>
     <row r="51" customFormat="false" ht="17.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="56" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="B51" s="57" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="C51" s="57"/>
       <c r="D51" s="57"/>
@@ -2887,7 +2878,7 @@
     <row r="52" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="56"/>
       <c r="B52" s="57" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="C52" s="57"/>
       <c r="D52" s="57"/>
@@ -2910,7 +2901,7 @@
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="61" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="B54" s="72" t="s">
         <v>27</v>
@@ -2919,36 +2910,36 @@
         <v>41</v>
       </c>
       <c r="D54" s="62" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E54" s="62" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="F54" s="62" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="G54" s="62" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="H54" s="62" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="I54" s="62" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="J54" s="62" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="46.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="73" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="B55" s="74" t="s">
         <v>43</v>
       </c>
       <c r="C55" s="75" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="D55" s="76"/>
       <c r="E55" s="76"/>
@@ -2960,14 +2951,14 @@
     </row>
     <row r="56" customFormat="false" ht="23.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="77" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="B56" s="78" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="C56" s="64"/>
       <c r="D56" s="79" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="E56" s="64"/>
       <c r="F56" s="64"/>
@@ -2978,14 +2969,14 @@
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="77" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="B57" s="78" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="C57" s="64"/>
       <c r="D57" s="79" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="E57" s="64"/>
       <c r="F57" s="64"/>
@@ -2996,14 +2987,14 @@
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="77" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="B58" s="80" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="C58" s="64"/>
       <c r="D58" s="79" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="E58" s="64"/>
       <c r="F58" s="64"/>
@@ -3014,14 +3005,14 @@
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="77" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="B59" s="80" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C59" s="64"/>
       <c r="D59" s="79" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="E59" s="64"/>
       <c r="F59" s="64"/>
@@ -3032,10 +3023,10 @@
     </row>
     <row r="61" customFormat="false" ht="17.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="56" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="B61" s="57" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="C61" s="57"/>
       <c r="D61" s="57"/>
@@ -3046,7 +3037,7 @@
     <row r="62" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="56"/>
       <c r="B62" s="57" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="C62" s="57"/>
       <c r="D62" s="57"/>
@@ -3071,25 +3062,25 @@
         <v>41</v>
       </c>
       <c r="C64" s="62" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D64" s="62" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="E64" s="62" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="F64" s="62" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="G64" s="62" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="H64" s="62" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="I64" s="62" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3097,10 +3088,10 @@
         <v>43</v>
       </c>
       <c r="B65" s="64" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="C65" s="64" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="D65" s="64"/>
       <c r="E65" s="64"/>
@@ -3111,7 +3102,7 @@
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="81" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="B66" s="64"/>
       <c r="C66" s="64"/>
@@ -3124,13 +3115,13 @@
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="81" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="B67" s="64" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="C67" s="64" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="D67" s="64"/>
       <c r="E67" s="64"/>
@@ -3141,7 +3132,7 @@
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="80" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="B68" s="64"/>
       <c r="C68" s="64"/>
@@ -3154,11 +3145,11 @@
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="80" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B69" s="64"/>
       <c r="C69" s="64" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="D69" s="64"/>
       <c r="E69" s="64"/>
@@ -3208,8 +3199,8 @@
   </sheetPr>
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -3223,19 +3214,19 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="82" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="B1" s="82" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="C1" s="82" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="D1" s="82" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="E1" s="82" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3249,180 +3240,180 @@
     </row>
     <row r="3" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="55" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B3" s="55" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="C3" s="83" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="D3" s="83"/>
       <c r="E3" s="55" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="55" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B4" s="55" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="C4" s="55"/>
       <c r="D4" s="55"/>
       <c r="E4" s="83" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="55" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="B5" s="55" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="C5" s="55" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="D5" s="55"/>
       <c r="E5" s="55" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="55" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="B6" s="55" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="C6" s="55" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="D6" s="55"/>
       <c r="E6" s="55" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="55" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="B7" s="55" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="C7" s="55" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="D7" s="55" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="E7" s="83" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="55" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="B8" s="55" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="C8" s="83" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="D8" s="83"/>
       <c r="E8" s="55" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="55" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="B9" s="55" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="C9" s="83"/>
       <c r="D9" s="83" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="E9" s="55" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="55" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="B10" s="55" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="C10" s="55"/>
       <c r="D10" s="55"/>
       <c r="E10" s="55" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="55" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="B11" s="55" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="C11" s="55" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="D11" s="55"/>
       <c r="E11" s="83" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="55" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="B12" s="55" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="C12" s="55" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="D12" s="55"/>
       <c r="E12" s="83" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="55" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="B13" s="55" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="C13" s="55" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="D13" s="55"/>
       <c r="E13" s="83" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="55" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="B14" s="83" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="C14" s="55" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="D14" s="55"/>
       <c r="E14" s="83" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
     </row>
   </sheetData>
@@ -3443,7 +3434,7 @@
   </sheetPr>
   <dimension ref="A1:F121"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -3460,27 +3451,27 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="84" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="B1" s="84" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="C1" s="84" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="D1" s="84" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="E1" s="84" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="F1" s="84" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>43</v>
@@ -3488,7 +3479,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>43</v>
@@ -3496,7 +3487,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>43</v>
@@ -3504,7 +3495,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="B5" s="0" t="s">
         <v>43</v>
@@ -3512,7 +3503,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="B6" s="0" t="s">
         <v>43</v>
@@ -3520,7 +3511,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B7" s="0" t="s">
         <v>43</v>
@@ -3528,7 +3519,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="B8" s="0" t="s">
         <v>43</v>
@@ -3536,7 +3527,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="B9" s="0" t="s">
         <v>43</v>
@@ -3544,7 +3535,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B10" s="0" t="s">
         <v>43</v>
@@ -3552,7 +3543,7 @@
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="B11" s="0" t="s">
         <v>43</v>
@@ -3560,7 +3551,7 @@
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="B12" s="0" t="s">
         <v>43</v>
@@ -3568,7 +3559,7 @@
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="B13" s="0" t="s">
         <v>43</v>
@@ -3576,7 +3567,7 @@
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="B14" s="0" t="s">
         <v>43</v>
@@ -3584,7 +3575,7 @@
     </row>
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="B15" s="0" t="s">
         <v>43</v>
@@ -3592,7 +3583,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="B16" s="0" t="s">
         <v>43</v>
@@ -3600,7 +3591,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="B17" s="0" t="s">
         <v>43</v>
@@ -3608,7 +3599,7 @@
     </row>
     <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="B18" s="0" t="s">
         <v>43</v>
@@ -3616,7 +3607,7 @@
     </row>
     <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="B19" s="0" t="s">
         <v>43</v>
@@ -3624,7 +3615,7 @@
     </row>
     <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="B20" s="0" t="s">
         <v>43</v>
@@ -3640,7 +3631,7 @@
     </row>
     <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="B22" s="0" t="s">
         <v>43</v>
@@ -3648,7 +3639,7 @@
     </row>
     <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="B23" s="0" t="s">
         <v>43</v>
@@ -3656,7 +3647,7 @@
     </row>
     <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="B24" s="0" t="s">
         <v>43</v>
@@ -3664,7 +3655,7 @@
     </row>
     <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="B25" s="0" t="s">
         <v>43</v>
@@ -3672,229 +3663,229 @@
     </row>
     <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="D53" s="0" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="E53" s="0" t="str">
         <f aca="false">+VLOOKUP(D53,A1:B121,1)</f>
@@ -3903,546 +3894,546 @@
     </row>
     <row r="54" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="B58" s="0" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="B59" s="0" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="B60" s="0" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="B62" s="0" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="B63" s="0" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="B64" s="85" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="B65" s="85" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="B66" s="85" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="B67" s="85" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="B68" s="85" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="B69" s="85" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="B70" s="85" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="B71" s="85" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="B72" s="85" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="B73" s="85" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="B74" s="85" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="B75" s="85" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="B76" s="85" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="B77" s="85" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="B78" s="85" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="B79" s="85" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="B80" s="85" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="B81" s="85" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="B82" s="85" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="B83" s="85" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="B84" s="85" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="B85" s="85" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="B86" s="85" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="B87" s="85" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="B88" s="85" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="B89" s="85" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="B90" s="0" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="B91" s="0" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="B92" s="0" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="B93" s="0" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="B94" s="0" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="B95" s="0" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="0" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="B96" s="0" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="0" t="s">
+        <v>235</v>
+      </c>
+      <c r="B97" s="0" t="s">
         <v>232</v>
-      </c>
-      <c r="B97" s="0" t="s">
-        <v>229</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="0" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="B98" s="0" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="0" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="B99" s="0" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="0" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="B100" s="0" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="0" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="B101" s="0" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="0" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="B102" s="85" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="0" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="B103" s="85" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="0" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="B104" s="85" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="0" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
       <c r="B105" s="85" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="0" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="B106" s="85" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="0" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="B107" s="85" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="0" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="B108" s="85" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="0" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="B109" s="85" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="0" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="B110" s="85" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="0" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="B111" s="85" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="0" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="B112" s="85" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="0" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="B113" s="85" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="0" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="B114" s="85" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="0" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="B115" s="85" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="0" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="B116" s="85" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="0" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="B117" s="85" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="0" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
       <c r="B118" s="85" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="0" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="B119" s="85" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="0" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
       <c r="B120" s="0" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="0" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
       <c r="B121" s="0" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -4463,7 +4454,7 @@
   </sheetPr>
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -4479,19 +4470,19 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="86" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
       <c r="B1" s="87" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C1" s="87" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="D1" s="87" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="E1" s="87" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4507,7 +4498,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="88" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="B3" s="64"/>
       <c r="C3" s="64" t="n">
@@ -4518,7 +4509,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="88" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="B4" s="64"/>
       <c r="C4" s="64"/>
@@ -4529,7 +4520,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="88" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="B5" s="64"/>
       <c r="C5" s="64"/>

</xml_diff>

<commit_message>
Se genera borrador de manual de user dev y de usuario normal, además de general las opciones para manejar el script en modo usuario o produccion
</commit_message>
<xml_diff>
--- a/Oficial/Patron_FL.xlsx
+++ b/Oficial/Patron_FL.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="426" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="474" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="BASE_SSE" sheetId="1" state="visible" r:id="rId2"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="261">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="482" uniqueCount="262">
   <si>
     <t>SOLICITUD  DE SERVICIO EXTERNO A LABORATORIO</t>
   </si>
@@ -368,6 +368,9 @@
   </si>
   <si>
     <t>Escribir en cada celda, solo 'si', si adjunta algún documento en particular para cada matriz y laboratorio</t>
+  </si>
+  <si>
+    <t>Hay adjuntos?</t>
   </si>
   <si>
     <t>si</t>
@@ -848,7 +851,7 @@
     <numFmt numFmtId="166" formatCode="0.00"/>
     <numFmt numFmtId="167" formatCode="0;[RED]\-0"/>
   </numFmts>
-  <fonts count="23">
+  <fonts count="24">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -874,6 +877,12 @@
       <sz val="20"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="20"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
@@ -1195,7 +1204,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="89">
+  <cellXfs count="93">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1212,6 +1221,10 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1220,7 +1233,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1232,19 +1245,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1252,23 +1265,23 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1276,119 +1289,119 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="2" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="2" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="3" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="3" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="3" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="3" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="4" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="4" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="5" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="5" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="2" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="2" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="2" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="2" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="3" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="3" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="3" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="3" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="3" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="3" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="4" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="4" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="4" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="4" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="4" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="4" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="4" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="4" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="5" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="5" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="5" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="5" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="4" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="4" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="4" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="4" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="12" fillId="2" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="13" fillId="2" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="12" fillId="3" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="13" fillId="3" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="12" fillId="3" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="13" fillId="3" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="12" fillId="4" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="13" fillId="4" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="12" fillId="4" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="13" fillId="4" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="12" fillId="5" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="13" fillId="5" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="12" fillId="5" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="13" fillId="5" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1404,7 +1417,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1416,23 +1429,23 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="7" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="7" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="7" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="7" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="6" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="6" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="6" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="6" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1440,11 +1453,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="8" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="8" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="9" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="9" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1456,15 +1469,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1484,11 +1497,11 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="10" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="10" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="11" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="19" fillId="11" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1504,11 +1517,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="8" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="19" fillId="8" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="10" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="10" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1520,35 +1533,47 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="10" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="10" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="12" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="21" fillId="12" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="23" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1629,15 +1654,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>766440</xdr:colOff>
+      <xdr:colOff>793440</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>7560</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1324080</xdr:colOff>
+      <xdr:colOff>1350720</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>772920</xdr:rowOff>
+      <xdr:rowOff>772560</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1650,8 +1675,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="766440" y="7560"/>
-          <a:ext cx="557640" cy="765360"/>
+          <a:off x="793440" y="7560"/>
+          <a:ext cx="557280" cy="765000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1673,8 +1698,8 @@
   </sheetPr>
   <dimension ref="A1:S69"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A16" activeCellId="0" sqref="A16"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1702,1461 +1727,1479 @@
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
+      <c r="G1" s="4" t="n">
+        <v>100</v>
+      </c>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="6"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="7"/>
-      <c r="J3" s="7"/>
-      <c r="K3" s="7"/>
-      <c r="L3" s="8"/>
-      <c r="M3" s="8"/>
-      <c r="N3" s="8"/>
-      <c r="O3" s="8"/>
-      <c r="P3" s="8"/>
-      <c r="Q3" s="8"/>
-      <c r="R3" s="8"/>
-      <c r="S3" s="8"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="8"/>
+      <c r="L3" s="9"/>
+      <c r="M3" s="9"/>
+      <c r="N3" s="9"/>
+      <c r="O3" s="9"/>
+      <c r="P3" s="9"/>
+      <c r="Q3" s="9"/>
+      <c r="R3" s="9"/>
+      <c r="S3" s="9"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7"/>
-      <c r="I4" s="7"/>
-      <c r="J4" s="7"/>
-      <c r="K4" s="7"/>
-      <c r="L4" s="8"/>
-      <c r="M4" s="8"/>
-      <c r="N4" s="8"/>
-      <c r="O4" s="8"/>
-      <c r="P4" s="8"/>
-      <c r="Q4" s="8"/>
-      <c r="R4" s="8"/>
-      <c r="S4" s="8"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="8"/>
+      <c r="K4" s="8"/>
+      <c r="L4" s="9"/>
+      <c r="M4" s="9"/>
+      <c r="N4" s="9"/>
+      <c r="O4" s="9"/>
+      <c r="P4" s="9"/>
+      <c r="Q4" s="9"/>
+      <c r="R4" s="9"/>
+      <c r="S4" s="9"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7"/>
-      <c r="I5" s="7"/>
-      <c r="J5" s="7"/>
-      <c r="K5" s="7"/>
-      <c r="L5" s="8"/>
-      <c r="M5" s="8"/>
-      <c r="N5" s="8"/>
-      <c r="O5" s="8"/>
-      <c r="P5" s="8"/>
-      <c r="Q5" s="8"/>
-      <c r="R5" s="8"/>
-      <c r="S5" s="8"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="8"/>
+      <c r="K5" s="8"/>
+      <c r="L5" s="9"/>
+      <c r="M5" s="9"/>
+      <c r="N5" s="9"/>
+      <c r="O5" s="9"/>
+      <c r="P5" s="9"/>
+      <c r="Q5" s="9"/>
+      <c r="R5" s="9"/>
+      <c r="S5" s="9"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="7"/>
-      <c r="J6" s="7"/>
-      <c r="K6" s="7"/>
-      <c r="L6" s="8"/>
-      <c r="M6" s="8"/>
-      <c r="N6" s="8"/>
-      <c r="O6" s="8"/>
-      <c r="P6" s="8"/>
-      <c r="Q6" s="8"/>
-      <c r="R6" s="8"/>
-      <c r="S6" s="8"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="8"/>
+      <c r="J6" s="8"/>
+      <c r="K6" s="8"/>
+      <c r="L6" s="9"/>
+      <c r="M6" s="9"/>
+      <c r="N6" s="9"/>
+      <c r="O6" s="9"/>
+      <c r="P6" s="9"/>
+      <c r="Q6" s="9"/>
+      <c r="R6" s="9"/>
+      <c r="S6" s="9"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="12" t="s">
+      <c r="B7" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="13"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="13"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
-      <c r="I7" s="7"/>
-      <c r="J7" s="7"/>
-      <c r="K7" s="7"/>
-      <c r="L7" s="8"/>
-      <c r="M7" s="8"/>
-      <c r="N7" s="8"/>
-      <c r="O7" s="8"/>
-      <c r="P7" s="8"/>
-      <c r="Q7" s="8"/>
-      <c r="R7" s="8"/>
-      <c r="S7" s="8"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="8"/>
+      <c r="K7" s="8"/>
+      <c r="L7" s="9"/>
+      <c r="M7" s="9"/>
+      <c r="N7" s="9"/>
+      <c r="O7" s="9"/>
+      <c r="P7" s="9"/>
+      <c r="Q7" s="9"/>
+      <c r="R7" s="9"/>
+      <c r="S7" s="9"/>
     </row>
     <row r="8" customFormat="false" ht="15.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="14" t="n">
+      <c r="B8" s="15" t="n">
         <f aca="true">+TODAY()</f>
-        <v>42087</v>
-      </c>
-      <c r="C8" s="15"/>
-      <c r="D8" s="16"/>
-      <c r="E8" s="16"/>
-      <c r="F8" s="16"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
-      <c r="J8" s="7"/>
-      <c r="K8" s="7"/>
-      <c r="L8" s="8"/>
-      <c r="M8" s="8"/>
-      <c r="N8" s="8"/>
-      <c r="O8" s="8"/>
-      <c r="P8" s="8"/>
-      <c r="Q8" s="8"/>
-      <c r="R8" s="8"/>
-      <c r="S8" s="8"/>
+        <v>42089</v>
+      </c>
+      <c r="C8" s="16"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="17"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="8"/>
+      <c r="J8" s="8"/>
+      <c r="K8" s="8"/>
+      <c r="L8" s="9"/>
+      <c r="M8" s="9"/>
+      <c r="N8" s="9"/>
+      <c r="O8" s="9"/>
+      <c r="P8" s="9"/>
+      <c r="Q8" s="9"/>
+      <c r="R8" s="9"/>
+      <c r="S8" s="9"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="9" t="s">
+      <c r="A9" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="17" t="n">
+      <c r="B9" s="18" t="n">
         <v>42095</v>
       </c>
-      <c r="C9" s="18"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="16"/>
-      <c r="G9" s="19"/>
-      <c r="H9" s="19"/>
-      <c r="I9" s="19"/>
-      <c r="J9" s="19"/>
-      <c r="K9" s="19"/>
-      <c r="L9" s="8"/>
-      <c r="M9" s="8"/>
-      <c r="N9" s="8"/>
-      <c r="O9" s="8"/>
-      <c r="P9" s="8"/>
-      <c r="Q9" s="8"/>
-      <c r="R9" s="8"/>
-      <c r="S9" s="8"/>
+      <c r="C9" s="19"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="17"/>
+      <c r="G9" s="20"/>
+      <c r="H9" s="20"/>
+      <c r="I9" s="20"/>
+      <c r="J9" s="20"/>
+      <c r="K9" s="20"/>
+      <c r="L9" s="9"/>
+      <c r="M9" s="9"/>
+      <c r="N9" s="9"/>
+      <c r="O9" s="9"/>
+      <c r="P9" s="9"/>
+      <c r="Q9" s="9"/>
+      <c r="R9" s="9"/>
+      <c r="S9" s="9"/>
     </row>
     <row r="10" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="20" t="n">
+      <c r="B10" s="21" t="n">
         <f aca="false">+B9-B8</f>
-        <v>8</v>
-      </c>
-      <c r="C10" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="16"/>
-      <c r="E10" s="16"/>
-      <c r="F10" s="16"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="17"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="22"/>
-      <c r="C11" s="23"/>
+      <c r="A11" s="23"/>
+      <c r="C11" s="24"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="24" t="s">
+      <c r="A12" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="24"/>
-      <c r="C12" s="24"/>
-      <c r="D12" s="24"/>
-      <c r="E12" s="24"/>
-      <c r="F12" s="24"/>
-      <c r="G12" s="25" t="s">
+      <c r="B12" s="25"/>
+      <c r="C12" s="25"/>
+      <c r="D12" s="25"/>
+      <c r="E12" s="25"/>
+      <c r="F12" s="25"/>
+      <c r="G12" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="H12" s="25"/>
-      <c r="I12" s="25"/>
-      <c r="J12" s="25"/>
-      <c r="K12" s="25"/>
-      <c r="L12" s="26"/>
-      <c r="M12" s="27" t="s">
+      <c r="H12" s="26"/>
+      <c r="I12" s="26"/>
+      <c r="J12" s="26"/>
+      <c r="K12" s="26"/>
+      <c r="L12" s="27"/>
+      <c r="M12" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="N12" s="27"/>
-      <c r="O12" s="27"/>
-      <c r="P12" s="27"/>
-      <c r="Q12" s="27"/>
-      <c r="R12" s="28" t="s">
+      <c r="N12" s="28"/>
+      <c r="O12" s="28"/>
+      <c r="P12" s="28"/>
+      <c r="Q12" s="28"/>
+      <c r="R12" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="S12" s="28"/>
+      <c r="S12" s="29"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="29" t="s">
+      <c r="A13" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="24"/>
-      <c r="C13" s="30"/>
-      <c r="D13" s="30"/>
-      <c r="E13" s="30"/>
-      <c r="F13" s="30"/>
-      <c r="G13" s="31" t="s">
+      <c r="B13" s="25"/>
+      <c r="C13" s="31"/>
+      <c r="D13" s="31"/>
+      <c r="E13" s="31"/>
+      <c r="F13" s="31"/>
+      <c r="G13" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="H13" s="31"/>
-      <c r="I13" s="31"/>
-      <c r="J13" s="32"/>
-      <c r="K13" s="33"/>
-      <c r="L13" s="33"/>
-      <c r="M13" s="34" t="s">
+      <c r="H13" s="32"/>
+      <c r="I13" s="32"/>
+      <c r="J13" s="33"/>
+      <c r="K13" s="34"/>
+      <c r="L13" s="34"/>
+      <c r="M13" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="N13" s="35"/>
-      <c r="O13" s="36"/>
-      <c r="P13" s="36"/>
-      <c r="Q13" s="37"/>
-      <c r="R13" s="38" t="s">
+      <c r="N13" s="36"/>
+      <c r="O13" s="37"/>
+      <c r="P13" s="37"/>
+      <c r="Q13" s="38"/>
+      <c r="R13" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="S13" s="39"/>
+      <c r="S13" s="40"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="29" t="s">
+      <c r="A14" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="24"/>
-      <c r="C14" s="30"/>
-      <c r="D14" s="30"/>
-      <c r="E14" s="30"/>
-      <c r="F14" s="30"/>
-      <c r="G14" s="31" t="s">
+      <c r="B14" s="25"/>
+      <c r="C14" s="31"/>
+      <c r="D14" s="31"/>
+      <c r="E14" s="31"/>
+      <c r="F14" s="31"/>
+      <c r="G14" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="H14" s="31"/>
-      <c r="I14" s="31"/>
-      <c r="J14" s="32"/>
-      <c r="K14" s="33"/>
-      <c r="L14" s="33"/>
-      <c r="M14" s="34" t="s">
+      <c r="H14" s="32"/>
+      <c r="I14" s="32"/>
+      <c r="J14" s="33"/>
+      <c r="K14" s="34"/>
+      <c r="L14" s="34"/>
+      <c r="M14" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="N14" s="35"/>
-      <c r="O14" s="40"/>
-      <c r="P14" s="40"/>
-      <c r="Q14" s="41"/>
-      <c r="R14" s="38" t="s">
+      <c r="N14" s="36"/>
+      <c r="O14" s="41"/>
+      <c r="P14" s="41"/>
+      <c r="Q14" s="42"/>
+      <c r="R14" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="S14" s="28"/>
+      <c r="S14" s="29"/>
     </row>
     <row r="15" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="42" t="s">
+      <c r="A15" s="43" t="s">
         <v>21</v>
       </c>
-      <c r="B15" s="42" t="s">
+      <c r="B15" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="C15" s="42" t="s">
+      <c r="C15" s="43" t="s">
         <v>23</v>
       </c>
-      <c r="D15" s="42" t="s">
+      <c r="D15" s="43" t="s">
         <v>24</v>
       </c>
-      <c r="E15" s="42" t="s">
+      <c r="E15" s="43" t="s">
         <v>25</v>
       </c>
-      <c r="F15" s="42" t="s">
+      <c r="F15" s="43" t="s">
         <v>26</v>
       </c>
-      <c r="G15" s="43" t="s">
+      <c r="G15" s="44" t="s">
         <v>27</v>
       </c>
-      <c r="H15" s="43" t="s">
+      <c r="H15" s="44" t="s">
         <v>28</v>
       </c>
-      <c r="I15" s="43" t="s">
+      <c r="I15" s="44" t="s">
         <v>29</v>
       </c>
-      <c r="J15" s="43" t="s">
+      <c r="J15" s="44" t="s">
         <v>30</v>
       </c>
-      <c r="K15" s="43" t="s">
+      <c r="K15" s="44" t="s">
         <v>31</v>
       </c>
-      <c r="L15" s="44" t="s">
+      <c r="L15" s="45" t="s">
         <v>32</v>
       </c>
-      <c r="M15" s="45" t="s">
+      <c r="M15" s="46" t="s">
         <v>33</v>
       </c>
-      <c r="N15" s="45" t="s">
+      <c r="N15" s="46" t="s">
         <v>34</v>
       </c>
-      <c r="O15" s="46" t="s">
+      <c r="O15" s="47" t="s">
         <v>35</v>
       </c>
-      <c r="P15" s="46" t="s">
+      <c r="P15" s="47" t="s">
         <v>36</v>
       </c>
-      <c r="Q15" s="46" t="s">
+      <c r="Q15" s="47" t="s">
         <v>37</v>
       </c>
-      <c r="R15" s="47" t="s">
+      <c r="R15" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="S15" s="48" t="s">
+      <c r="S15" s="49" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="49" t="n">
+      <c r="A16" s="50" t="n">
         <v>10</v>
       </c>
       <c r="B16" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="C16" s="49" t="n">
+      <c r="C16" s="50" t="n">
         <v>5</v>
       </c>
-      <c r="D16" s="50" t="s">
+      <c r="D16" s="51" t="s">
         <v>41</v>
       </c>
-      <c r="E16" s="51" t="s">
+      <c r="E16" s="52" t="s">
         <v>42</v>
       </c>
-      <c r="F16" s="51" t="n">
+      <c r="F16" s="52" t="n">
         <v>0</v>
       </c>
-      <c r="G16" s="52" t="s">
+      <c r="G16" s="53" t="s">
         <v>43</v>
       </c>
-      <c r="H16" s="51" t="s">
+      <c r="H16" s="52" t="s">
         <v>44</v>
       </c>
-      <c r="I16" s="51" t="s">
+      <c r="I16" s="52" t="s">
         <v>45</v>
       </c>
-      <c r="J16" s="53" t="n">
+      <c r="J16" s="54" t="n">
         <f aca="false">+VLOOKUP(B16,Parametros!A$1:D$121,3,)</f>
         <v>0</v>
       </c>
-      <c r="K16" s="53" t="n">
+      <c r="K16" s="54" t="n">
         <v>100</v>
       </c>
-      <c r="L16" s="53" t="s">
+      <c r="L16" s="54" t="s">
         <v>46</v>
       </c>
-      <c r="M16" s="54"/>
-      <c r="N16" s="54"/>
-      <c r="O16" s="54"/>
-      <c r="P16" s="54"/>
-      <c r="Q16" s="54"/>
-      <c r="R16" s="54"/>
-      <c r="S16" s="54"/>
+      <c r="M16" s="55"/>
+      <c r="N16" s="55"/>
+      <c r="O16" s="55"/>
+      <c r="P16" s="55"/>
+      <c r="Q16" s="55"/>
+      <c r="R16" s="55"/>
+      <c r="S16" s="55"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="49" t="n">
+      <c r="A17" s="50" t="n">
         <v>11</v>
       </c>
-      <c r="B17" s="54" t="s">
+      <c r="B17" s="55" t="s">
         <v>47</v>
       </c>
-      <c r="C17" s="49" t="n">
+      <c r="C17" s="50" t="n">
         <v>5</v>
       </c>
-      <c r="D17" s="50" t="s">
+      <c r="D17" s="51" t="s">
         <v>48</v>
       </c>
-      <c r="E17" s="51" t="s">
+      <c r="E17" s="52" t="s">
         <v>42</v>
       </c>
-      <c r="F17" s="51"/>
-      <c r="G17" s="55" t="s">
+      <c r="F17" s="52"/>
+      <c r="G17" s="56" t="s">
         <v>49</v>
       </c>
-      <c r="H17" s="51"/>
-      <c r="I17" s="51" t="s">
+      <c r="H17" s="52"/>
+      <c r="I17" s="52" t="s">
         <v>50</v>
       </c>
-      <c r="J17" s="53" t="n">
+      <c r="J17" s="54" t="n">
         <f aca="false">+VLOOKUP(B17,Parametros!A$1:D$121,3,)</f>
         <v>0</v>
       </c>
-      <c r="K17" s="53" t="n">
+      <c r="K17" s="54" t="n">
         <v>101</v>
       </c>
-      <c r="L17" s="53" t="s">
+      <c r="L17" s="54" t="s">
         <v>51</v>
       </c>
-      <c r="M17" s="54"/>
-      <c r="N17" s="54"/>
-      <c r="O17" s="54"/>
-      <c r="P17" s="54"/>
-      <c r="Q17" s="54"/>
-      <c r="R17" s="54"/>
-      <c r="S17" s="54"/>
+      <c r="M17" s="55"/>
+      <c r="N17" s="55"/>
+      <c r="O17" s="55"/>
+      <c r="P17" s="55"/>
+      <c r="Q17" s="55"/>
+      <c r="R17" s="55"/>
+      <c r="S17" s="55"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="49" t="n">
+      <c r="A18" s="50" t="n">
         <v>12</v>
       </c>
-      <c r="B18" s="54" t="s">
+      <c r="B18" s="55" t="s">
         <v>52</v>
       </c>
-      <c r="C18" s="49" t="n">
+      <c r="C18" s="50" t="n">
         <v>3</v>
       </c>
-      <c r="D18" s="50" t="s">
+      <c r="D18" s="51" t="s">
         <v>41</v>
       </c>
-      <c r="E18" s="51" t="s">
+      <c r="E18" s="52" t="s">
         <v>42</v>
       </c>
-      <c r="F18" s="51"/>
-      <c r="G18" s="55" t="s">
+      <c r="F18" s="52"/>
+      <c r="G18" s="56" t="s">
         <v>53</v>
       </c>
-      <c r="H18" s="51"/>
-      <c r="I18" s="51" t="s">
+      <c r="H18" s="52"/>
+      <c r="I18" s="52" t="s">
         <v>54</v>
       </c>
-      <c r="J18" s="53" t="n">
+      <c r="J18" s="54" t="n">
         <f aca="false">+VLOOKUP(B18,Parametros!A$1:D$121,3,)</f>
         <v>0</v>
       </c>
-      <c r="K18" s="53" t="n">
+      <c r="K18" s="54" t="n">
         <v>102</v>
       </c>
-      <c r="L18" s="53" t="s">
+      <c r="L18" s="54" t="s">
         <v>55</v>
       </c>
-      <c r="M18" s="54"/>
-      <c r="N18" s="54"/>
-      <c r="O18" s="54"/>
-      <c r="P18" s="54"/>
-      <c r="Q18" s="54"/>
-      <c r="R18" s="54"/>
-      <c r="S18" s="54"/>
+      <c r="M18" s="55"/>
+      <c r="N18" s="55"/>
+      <c r="O18" s="55"/>
+      <c r="P18" s="55"/>
+      <c r="Q18" s="55"/>
+      <c r="R18" s="55"/>
+      <c r="S18" s="55"/>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="49" t="n">
+      <c r="A19" s="50" t="n">
         <v>13</v>
       </c>
-      <c r="B19" s="54" t="s">
+      <c r="B19" s="55" t="s">
         <v>40</v>
       </c>
-      <c r="C19" s="49" t="n">
+      <c r="C19" s="50" t="n">
         <v>4</v>
       </c>
-      <c r="D19" s="50" t="s">
+      <c r="D19" s="51" t="s">
         <v>41</v>
       </c>
-      <c r="E19" s="51" t="s">
+      <c r="E19" s="52" t="s">
         <v>42</v>
       </c>
-      <c r="F19" s="51"/>
-      <c r="G19" s="52" t="s">
+      <c r="F19" s="52"/>
+      <c r="G19" s="53" t="s">
         <v>43</v>
       </c>
-      <c r="H19" s="51"/>
-      <c r="I19" s="51" t="s">
+      <c r="H19" s="52"/>
+      <c r="I19" s="52" t="s">
         <v>56</v>
       </c>
-      <c r="J19" s="53" t="n">
+      <c r="J19" s="54" t="n">
         <f aca="false">+VLOOKUP(B19,Parametros!A$1:D$121,3,)</f>
         <v>0</v>
       </c>
-      <c r="K19" s="53" t="n">
+      <c r="K19" s="54" t="n">
         <v>103</v>
       </c>
-      <c r="L19" s="53" t="s">
+      <c r="L19" s="54" t="s">
         <v>55</v>
       </c>
-      <c r="M19" s="54"/>
-      <c r="N19" s="54"/>
-      <c r="O19" s="54"/>
-      <c r="P19" s="54"/>
-      <c r="Q19" s="54"/>
-      <c r="R19" s="54"/>
-      <c r="S19" s="54"/>
+      <c r="M19" s="55"/>
+      <c r="N19" s="55"/>
+      <c r="O19" s="55"/>
+      <c r="P19" s="55"/>
+      <c r="Q19" s="55"/>
+      <c r="R19" s="55"/>
+      <c r="S19" s="55"/>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="49" t="n">
+      <c r="A20" s="50" t="n">
         <v>14</v>
       </c>
-      <c r="B20" s="54" t="s">
+      <c r="B20" s="55" t="s">
         <v>57</v>
       </c>
-      <c r="C20" s="49" t="n">
+      <c r="C20" s="50" t="n">
         <v>5</v>
       </c>
-      <c r="D20" s="50" t="s">
+      <c r="D20" s="51" t="s">
         <v>41</v>
       </c>
-      <c r="E20" s="51" t="s">
+      <c r="E20" s="52" t="s">
         <v>42</v>
       </c>
-      <c r="F20" s="51"/>
-      <c r="G20" s="52" t="s">
+      <c r="F20" s="52"/>
+      <c r="G20" s="53" t="s">
         <v>43</v>
       </c>
-      <c r="H20" s="51"/>
-      <c r="I20" s="51" t="s">
+      <c r="H20" s="52"/>
+      <c r="I20" s="52" t="s">
         <v>58</v>
       </c>
-      <c r="J20" s="53" t="n">
+      <c r="J20" s="54" t="n">
         <f aca="false">+VLOOKUP(B20,Parametros!A$1:D$121,3,)</f>
         <v>0</v>
       </c>
-      <c r="K20" s="53" t="n">
+      <c r="K20" s="54" t="n">
         <v>104</v>
       </c>
-      <c r="L20" s="53" t="s">
+      <c r="L20" s="54" t="s">
         <v>55</v>
       </c>
-      <c r="M20" s="54"/>
-      <c r="N20" s="54"/>
-      <c r="O20" s="54"/>
-      <c r="P20" s="54"/>
-      <c r="Q20" s="54"/>
-      <c r="R20" s="54"/>
-      <c r="S20" s="54"/>
+      <c r="M20" s="55"/>
+      <c r="N20" s="55"/>
+      <c r="O20" s="55"/>
+      <c r="P20" s="55"/>
+      <c r="Q20" s="55"/>
+      <c r="R20" s="55"/>
+      <c r="S20" s="55"/>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="49" t="n">
+      <c r="A21" s="50" t="n">
         <v>15</v>
       </c>
-      <c r="B21" s="54" t="s">
+      <c r="B21" s="55" t="s">
         <v>59</v>
       </c>
-      <c r="C21" s="49" t="n">
+      <c r="C21" s="50" t="n">
         <v>6</v>
       </c>
-      <c r="D21" s="50" t="s">
+      <c r="D21" s="51" t="s">
         <v>41</v>
       </c>
-      <c r="E21" s="51" t="s">
+      <c r="E21" s="52" t="s">
         <v>42</v>
       </c>
-      <c r="F21" s="51"/>
-      <c r="G21" s="52" t="s">
+      <c r="F21" s="52"/>
+      <c r="G21" s="53" t="s">
         <v>43</v>
       </c>
-      <c r="H21" s="51"/>
-      <c r="I21" s="51" t="s">
+      <c r="H21" s="52"/>
+      <c r="I21" s="52" t="s">
         <v>60</v>
       </c>
-      <c r="J21" s="53" t="n">
+      <c r="J21" s="54" t="n">
         <f aca="false">+VLOOKUP(B21,Parametros!A$1:D$121,3,)</f>
         <v>0</v>
       </c>
-      <c r="K21" s="53" t="n">
+      <c r="K21" s="54" t="n">
         <v>105</v>
       </c>
-      <c r="L21" s="53" t="s">
+      <c r="L21" s="54" t="s">
         <v>55</v>
       </c>
-      <c r="M21" s="54"/>
-      <c r="N21" s="54"/>
-      <c r="O21" s="54"/>
-      <c r="P21" s="54"/>
-      <c r="Q21" s="54"/>
-      <c r="R21" s="54"/>
-      <c r="S21" s="54"/>
+      <c r="M21" s="55"/>
+      <c r="N21" s="55"/>
+      <c r="O21" s="55"/>
+      <c r="P21" s="55"/>
+      <c r="Q21" s="55"/>
+      <c r="R21" s="55"/>
+      <c r="S21" s="55"/>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="49" t="n">
+      <c r="A22" s="50" t="n">
         <v>16</v>
       </c>
-      <c r="B22" s="54" t="s">
+      <c r="B22" s="55" t="s">
         <v>61</v>
       </c>
-      <c r="C22" s="49" t="n">
+      <c r="C22" s="50" t="n">
         <v>7</v>
       </c>
-      <c r="D22" s="50" t="s">
+      <c r="D22" s="51" t="s">
         <v>48</v>
       </c>
-      <c r="E22" s="51" t="s">
+      <c r="E22" s="52" t="s">
         <v>42</v>
       </c>
-      <c r="F22" s="51"/>
-      <c r="G22" s="52" t="s">
+      <c r="F22" s="52"/>
+      <c r="G22" s="53" t="s">
         <v>43</v>
       </c>
-      <c r="H22" s="51"/>
-      <c r="I22" s="51" t="s">
+      <c r="H22" s="52"/>
+      <c r="I22" s="52" t="s">
         <v>62</v>
       </c>
-      <c r="J22" s="53" t="n">
+      <c r="J22" s="54" t="n">
         <f aca="false">+VLOOKUP(B22,Parametros!A$1:D$121,3,)</f>
         <v>0</v>
       </c>
-      <c r="K22" s="53" t="n">
+      <c r="K22" s="54" t="n">
         <v>106</v>
       </c>
-      <c r="L22" s="53" t="s">
+      <c r="L22" s="54" t="s">
         <v>55</v>
       </c>
-      <c r="M22" s="54"/>
-      <c r="N22" s="54"/>
-      <c r="O22" s="54"/>
-      <c r="P22" s="54"/>
-      <c r="Q22" s="54"/>
-      <c r="R22" s="54"/>
-      <c r="S22" s="54"/>
+      <c r="M22" s="55"/>
+      <c r="N22" s="55"/>
+      <c r="O22" s="55"/>
+      <c r="P22" s="55"/>
+      <c r="Q22" s="55"/>
+      <c r="R22" s="55"/>
+      <c r="S22" s="55"/>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="49" t="n">
+      <c r="A23" s="50" t="n">
         <v>17</v>
       </c>
-      <c r="B23" s="54" t="s">
+      <c r="B23" s="55" t="s">
         <v>63</v>
       </c>
-      <c r="C23" s="49" t="n">
+      <c r="C23" s="50" t="n">
         <v>8</v>
       </c>
-      <c r="D23" s="50" t="s">
+      <c r="D23" s="51" t="s">
         <v>41</v>
       </c>
-      <c r="E23" s="51" t="s">
+      <c r="E23" s="52" t="s">
         <v>42</v>
       </c>
-      <c r="F23" s="51"/>
-      <c r="G23" s="52" t="s">
+      <c r="F23" s="52"/>
+      <c r="G23" s="53" t="s">
         <v>43</v>
       </c>
-      <c r="H23" s="54"/>
-      <c r="I23" s="51" t="s">
+      <c r="H23" s="55"/>
+      <c r="I23" s="52" t="s">
         <v>64</v>
       </c>
-      <c r="J23" s="53" t="n">
+      <c r="J23" s="54" t="n">
         <f aca="false">+VLOOKUP(B23,Parametros!A$1:D$121,3,)</f>
         <v>0</v>
       </c>
-      <c r="K23" s="53" t="n">
+      <c r="K23" s="54" t="n">
         <v>107</v>
       </c>
-      <c r="L23" s="53" t="s">
+      <c r="L23" s="54" t="s">
         <v>55</v>
       </c>
-      <c r="M23" s="54"/>
-      <c r="N23" s="54"/>
-      <c r="O23" s="54"/>
-      <c r="P23" s="54"/>
-      <c r="Q23" s="54"/>
-      <c r="R23" s="54"/>
-      <c r="S23" s="54"/>
+      <c r="M23" s="55"/>
+      <c r="N23" s="55"/>
+      <c r="O23" s="55"/>
+      <c r="P23" s="55"/>
+      <c r="Q23" s="55"/>
+      <c r="R23" s="55"/>
+      <c r="S23" s="55"/>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="49" t="n">
+      <c r="A24" s="50" t="n">
         <v>18</v>
       </c>
-      <c r="B24" s="54" t="s">
+      <c r="B24" s="55" t="s">
         <v>65</v>
       </c>
-      <c r="C24" s="49" t="n">
+      <c r="C24" s="50" t="n">
         <v>9</v>
       </c>
-      <c r="D24" s="50" t="s">
+      <c r="D24" s="51" t="s">
         <v>48</v>
       </c>
-      <c r="E24" s="51" t="s">
+      <c r="E24" s="52" t="s">
         <v>42</v>
       </c>
-      <c r="F24" s="54"/>
-      <c r="G24" s="52" t="s">
+      <c r="F24" s="55"/>
+      <c r="G24" s="53" t="s">
         <v>43</v>
       </c>
-      <c r="H24" s="51"/>
-      <c r="I24" s="51" t="s">
+      <c r="H24" s="52"/>
+      <c r="I24" s="52" t="s">
         <v>66</v>
       </c>
-      <c r="J24" s="53" t="n">
+      <c r="J24" s="54" t="n">
         <f aca="false">+VLOOKUP(B24,Parametros!A$1:D$121,3,)</f>
         <v>0</v>
       </c>
-      <c r="K24" s="53" t="n">
+      <c r="K24" s="54" t="n">
         <v>108</v>
       </c>
-      <c r="L24" s="53" t="s">
+      <c r="L24" s="54" t="s">
         <v>55</v>
       </c>
-      <c r="M24" s="54"/>
-      <c r="N24" s="54"/>
-      <c r="O24" s="54"/>
-      <c r="P24" s="54"/>
-      <c r="Q24" s="54"/>
-      <c r="R24" s="54"/>
-      <c r="S24" s="54"/>
+      <c r="M24" s="55"/>
+      <c r="N24" s="55"/>
+      <c r="O24" s="55"/>
+      <c r="P24" s="55"/>
+      <c r="Q24" s="55"/>
+      <c r="R24" s="55"/>
+      <c r="S24" s="55"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="26" customFormat="false" ht="17.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="56" t="s">
+      <c r="A26" s="57" t="s">
         <v>67</v>
       </c>
-      <c r="B26" s="57" t="s">
+      <c r="B26" s="58" t="s">
         <v>68</v>
       </c>
-      <c r="C26" s="57"/>
-      <c r="D26" s="57"/>
-      <c r="E26" s="57"/>
-      <c r="F26" s="57"/>
-      <c r="G26" s="57"/>
-      <c r="H26" s="57"/>
-      <c r="I26" s="57"/>
+      <c r="C26" s="58"/>
+      <c r="D26" s="58"/>
+      <c r="E26" s="58"/>
+      <c r="F26" s="58"/>
+      <c r="G26" s="58"/>
+      <c r="H26" s="58"/>
+      <c r="I26" s="58"/>
     </row>
     <row r="27" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="56"/>
-      <c r="B27" s="57" t="s">
+      <c r="A27" s="57"/>
+      <c r="B27" s="58" t="s">
         <v>69</v>
       </c>
-      <c r="C27" s="57"/>
-      <c r="D27" s="57"/>
-      <c r="E27" s="57"/>
-      <c r="F27" s="57"/>
-      <c r="G27" s="57"/>
-      <c r="H27" s="57"/>
-      <c r="I27" s="57"/>
-    </row>
-    <row r="28" s="60" customFormat="true" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="58"/>
-      <c r="B28" s="59"/>
-      <c r="C28" s="59"/>
-      <c r="D28" s="59"/>
-      <c r="E28" s="59"/>
-      <c r="F28" s="59"/>
-      <c r="G28" s="59"/>
+      <c r="C27" s="58"/>
+      <c r="D27" s="58"/>
+      <c r="E27" s="58"/>
+      <c r="F27" s="58"/>
+      <c r="G27" s="58"/>
+      <c r="H27" s="58"/>
+      <c r="I27" s="58"/>
+    </row>
+    <row r="28" s="61" customFormat="true" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="59"/>
+      <c r="B28" s="60"/>
+      <c r="C28" s="60"/>
+      <c r="D28" s="60"/>
+      <c r="E28" s="60"/>
+      <c r="F28" s="60"/>
+      <c r="G28" s="60"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="61" t="s">
+      <c r="A29" s="62" t="s">
         <v>70</v>
       </c>
-      <c r="B29" s="62" t="s">
+      <c r="B29" s="63" t="s">
         <v>41</v>
       </c>
-      <c r="C29" s="62" t="s">
+      <c r="C29" s="63" t="s">
         <v>48</v>
       </c>
-      <c r="D29" s="62" t="s">
+      <c r="D29" s="63" t="s">
         <v>71</v>
       </c>
-      <c r="E29" s="62" t="s">
+      <c r="E29" s="63" t="s">
         <v>72</v>
       </c>
-      <c r="F29" s="62" t="s">
+      <c r="F29" s="63" t="s">
         <v>73</v>
       </c>
-      <c r="G29" s="62" t="s">
+      <c r="G29" s="63" t="s">
         <v>74</v>
       </c>
-      <c r="H29" s="62" t="s">
+      <c r="H29" s="63" t="s">
         <v>75</v>
       </c>
-      <c r="I29" s="62" t="s">
+      <c r="I29" s="63" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="63" t="s">
+      <c r="A30" s="64" t="s">
         <v>77</v>
       </c>
-      <c r="B30" s="64" t="n">
+      <c r="B30" s="65" t="n">
         <v>1</v>
       </c>
-      <c r="C30" s="64" t="n">
+      <c r="C30" s="65" t="n">
         <v>1</v>
       </c>
-      <c r="D30" s="64"/>
-      <c r="E30" s="64"/>
-      <c r="F30" s="64"/>
-      <c r="G30" s="64"/>
-      <c r="H30" s="64"/>
-      <c r="I30" s="64"/>
-      <c r="L30" s="8"/>
-      <c r="M30" s="8"/>
-      <c r="N30" s="8"/>
-      <c r="O30" s="8"/>
-      <c r="P30" s="8"/>
-      <c r="Q30" s="8"/>
-      <c r="R30" s="8"/>
-      <c r="S30" s="8"/>
+      <c r="D30" s="65"/>
+      <c r="E30" s="65"/>
+      <c r="F30" s="65"/>
+      <c r="G30" s="65"/>
+      <c r="H30" s="65"/>
+      <c r="I30" s="65"/>
+      <c r="L30" s="9"/>
+      <c r="M30" s="9"/>
+      <c r="N30" s="9"/>
+      <c r="O30" s="9"/>
+      <c r="P30" s="9"/>
+      <c r="Q30" s="9"/>
+      <c r="R30" s="9"/>
+      <c r="S30" s="9"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="63" t="s">
+      <c r="A31" s="64" t="s">
         <v>78</v>
       </c>
-      <c r="B31" s="64" t="n">
+      <c r="B31" s="65" t="n">
         <v>1</v>
       </c>
-      <c r="C31" s="64" t="n">
+      <c r="C31" s="65" t="n">
         <v>1</v>
       </c>
-      <c r="D31" s="64"/>
-      <c r="E31" s="64"/>
-      <c r="F31" s="64"/>
-      <c r="G31" s="64"/>
-      <c r="H31" s="64"/>
-      <c r="I31" s="64"/>
-      <c r="L31" s="8"/>
-      <c r="M31" s="8"/>
-      <c r="N31" s="8"/>
-      <c r="O31" s="8"/>
-      <c r="P31" s="8"/>
-      <c r="Q31" s="8"/>
-      <c r="R31" s="8"/>
-      <c r="S31" s="8"/>
+      <c r="D31" s="65"/>
+      <c r="E31" s="65"/>
+      <c r="F31" s="65"/>
+      <c r="G31" s="65"/>
+      <c r="H31" s="65"/>
+      <c r="I31" s="65"/>
+      <c r="L31" s="9"/>
+      <c r="M31" s="9"/>
+      <c r="N31" s="9"/>
+      <c r="O31" s="9"/>
+      <c r="P31" s="9"/>
+      <c r="Q31" s="9"/>
+      <c r="R31" s="9"/>
+      <c r="S31" s="9"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="63" t="s">
+      <c r="A32" s="64" t="s">
         <v>79</v>
       </c>
-      <c r="B32" s="64" t="n">
+      <c r="B32" s="65" t="n">
         <v>1</v>
       </c>
-      <c r="C32" s="64"/>
-      <c r="D32" s="64"/>
-      <c r="E32" s="64"/>
-      <c r="F32" s="64"/>
-      <c r="G32" s="64"/>
-      <c r="H32" s="64"/>
-      <c r="I32" s="64"/>
-      <c r="L32" s="8"/>
-      <c r="M32" s="8"/>
-      <c r="N32" s="8"/>
-      <c r="O32" s="8"/>
-      <c r="P32" s="8"/>
-      <c r="Q32" s="8"/>
-      <c r="R32" s="8"/>
-      <c r="S32" s="8"/>
+      <c r="C32" s="65"/>
+      <c r="D32" s="65"/>
+      <c r="E32" s="65"/>
+      <c r="F32" s="65"/>
+      <c r="G32" s="65"/>
+      <c r="H32" s="65"/>
+      <c r="I32" s="65"/>
+      <c r="L32" s="9"/>
+      <c r="M32" s="9"/>
+      <c r="N32" s="9"/>
+      <c r="O32" s="9"/>
+      <c r="P32" s="9"/>
+      <c r="Q32" s="9"/>
+      <c r="R32" s="9"/>
+      <c r="S32" s="9"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="63" t="s">
+      <c r="A33" s="64" t="s">
         <v>80</v>
       </c>
-      <c r="B33" s="64" t="n">
+      <c r="B33" s="65" t="n">
         <v>1</v>
       </c>
-      <c r="C33" s="64"/>
-      <c r="D33" s="64"/>
-      <c r="E33" s="64"/>
-      <c r="F33" s="64"/>
-      <c r="G33" s="64"/>
-      <c r="H33" s="64"/>
-      <c r="I33" s="64"/>
-      <c r="L33" s="8"/>
-      <c r="M33" s="8"/>
-      <c r="N33" s="8"/>
-      <c r="O33" s="8"/>
-      <c r="P33" s="8"/>
-      <c r="Q33" s="8"/>
-      <c r="R33" s="8"/>
-      <c r="S33" s="8"/>
+      <c r="C33" s="65"/>
+      <c r="D33" s="65"/>
+      <c r="E33" s="65"/>
+      <c r="F33" s="65"/>
+      <c r="G33" s="65"/>
+      <c r="H33" s="65"/>
+      <c r="I33" s="65"/>
+      <c r="L33" s="9"/>
+      <c r="M33" s="9"/>
+      <c r="N33" s="9"/>
+      <c r="O33" s="9"/>
+      <c r="P33" s="9"/>
+      <c r="Q33" s="9"/>
+      <c r="R33" s="9"/>
+      <c r="S33" s="9"/>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="63" t="s">
+      <c r="A34" s="64" t="s">
         <v>81</v>
       </c>
-      <c r="B34" s="64" t="n">
+      <c r="B34" s="65" t="n">
         <v>1</v>
       </c>
-      <c r="C34" s="64" t="n">
+      <c r="C34" s="65" t="n">
         <v>1</v>
       </c>
-      <c r="D34" s="64"/>
-      <c r="E34" s="64"/>
-      <c r="F34" s="64"/>
-      <c r="G34" s="64"/>
-      <c r="H34" s="64"/>
-      <c r="I34" s="64"/>
-      <c r="L34" s="8"/>
-      <c r="M34" s="8"/>
-      <c r="N34" s="8"/>
-      <c r="O34" s="8"/>
-      <c r="P34" s="8"/>
-      <c r="Q34" s="8"/>
-      <c r="R34" s="8"/>
-      <c r="S34" s="8"/>
+      <c r="D34" s="65"/>
+      <c r="E34" s="65"/>
+      <c r="F34" s="65"/>
+      <c r="G34" s="65"/>
+      <c r="H34" s="65"/>
+      <c r="I34" s="65"/>
+      <c r="L34" s="9"/>
+      <c r="M34" s="9"/>
+      <c r="N34" s="9"/>
+      <c r="O34" s="9"/>
+      <c r="P34" s="9"/>
+      <c r="Q34" s="9"/>
+      <c r="R34" s="9"/>
+      <c r="S34" s="9"/>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="63" t="s">
+      <c r="A35" s="64" t="s">
         <v>82</v>
       </c>
-      <c r="B35" s="64" t="n">
+      <c r="B35" s="65" t="n">
         <v>1</v>
       </c>
-      <c r="C35" s="64"/>
-      <c r="D35" s="64"/>
-      <c r="E35" s="64"/>
-      <c r="F35" s="64"/>
-      <c r="G35" s="64"/>
-      <c r="H35" s="64"/>
-      <c r="I35" s="64"/>
-      <c r="L35" s="8"/>
-      <c r="M35" s="8"/>
-      <c r="N35" s="8"/>
-      <c r="O35" s="8"/>
-      <c r="P35" s="8"/>
-      <c r="Q35" s="8"/>
-      <c r="R35" s="8"/>
-      <c r="S35" s="8"/>
+      <c r="C35" s="65"/>
+      <c r="D35" s="65"/>
+      <c r="E35" s="65"/>
+      <c r="F35" s="65"/>
+      <c r="G35" s="65"/>
+      <c r="H35" s="65"/>
+      <c r="I35" s="65"/>
+      <c r="L35" s="9"/>
+      <c r="M35" s="9"/>
+      <c r="N35" s="9"/>
+      <c r="O35" s="9"/>
+      <c r="P35" s="9"/>
+      <c r="Q35" s="9"/>
+      <c r="R35" s="9"/>
+      <c r="S35" s="9"/>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="63" t="s">
+      <c r="A36" s="64" t="s">
         <v>83</v>
       </c>
-      <c r="B36" s="64" t="n">
+      <c r="B36" s="65" t="n">
         <v>1</v>
       </c>
-      <c r="C36" s="64"/>
-      <c r="D36" s="64"/>
-      <c r="E36" s="64"/>
-      <c r="F36" s="64"/>
-      <c r="G36" s="64"/>
-      <c r="H36" s="64"/>
-      <c r="I36" s="64"/>
-      <c r="L36" s="8"/>
-      <c r="M36" s="8"/>
-      <c r="N36" s="8"/>
-      <c r="O36" s="8"/>
-      <c r="P36" s="8"/>
-      <c r="Q36" s="8"/>
-      <c r="R36" s="8"/>
-      <c r="S36" s="8"/>
+      <c r="C36" s="65"/>
+      <c r="D36" s="65"/>
+      <c r="E36" s="65"/>
+      <c r="F36" s="65"/>
+      <c r="G36" s="65"/>
+      <c r="H36" s="65"/>
+      <c r="I36" s="65"/>
+      <c r="L36" s="9"/>
+      <c r="M36" s="9"/>
+      <c r="N36" s="9"/>
+      <c r="O36" s="9"/>
+      <c r="P36" s="9"/>
+      <c r="Q36" s="9"/>
+      <c r="R36" s="9"/>
+      <c r="S36" s="9"/>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="63" t="s">
+      <c r="A37" s="64" t="s">
         <v>84</v>
       </c>
-      <c r="B37" s="64" t="n">
+      <c r="B37" s="65" t="n">
         <v>1</v>
       </c>
-      <c r="C37" s="64" t="n">
+      <c r="C37" s="65" t="n">
         <v>1</v>
       </c>
-      <c r="D37" s="64"/>
-      <c r="E37" s="64"/>
-      <c r="F37" s="64"/>
-      <c r="G37" s="64"/>
-      <c r="H37" s="64"/>
-      <c r="I37" s="64"/>
-      <c r="L37" s="8"/>
-      <c r="M37" s="8"/>
-      <c r="N37" s="8"/>
-      <c r="O37" s="8"/>
-      <c r="P37" s="8"/>
-      <c r="Q37" s="8"/>
-      <c r="R37" s="8"/>
-      <c r="S37" s="8"/>
+      <c r="D37" s="65"/>
+      <c r="E37" s="65"/>
+      <c r="F37" s="65"/>
+      <c r="G37" s="65"/>
+      <c r="H37" s="65"/>
+      <c r="I37" s="65"/>
+      <c r="L37" s="9"/>
+      <c r="M37" s="9"/>
+      <c r="N37" s="9"/>
+      <c r="O37" s="9"/>
+      <c r="P37" s="9"/>
+      <c r="Q37" s="9"/>
+      <c r="R37" s="9"/>
+      <c r="S37" s="9"/>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="63" t="s">
+      <c r="A38" s="64" t="s">
         <v>85</v>
       </c>
-      <c r="B38" s="64" t="n">
+      <c r="B38" s="65" t="n">
         <v>1</v>
       </c>
-      <c r="C38" s="64"/>
-      <c r="D38" s="64"/>
-      <c r="E38" s="64"/>
-      <c r="F38" s="64"/>
-      <c r="G38" s="64"/>
-      <c r="H38" s="64"/>
-      <c r="I38" s="64"/>
-      <c r="L38" s="8"/>
-      <c r="M38" s="8"/>
-      <c r="N38" s="8"/>
-      <c r="O38" s="8"/>
-      <c r="P38" s="8"/>
-      <c r="Q38" s="8"/>
-      <c r="R38" s="8"/>
-      <c r="S38" s="8"/>
+      <c r="C38" s="65"/>
+      <c r="D38" s="65"/>
+      <c r="E38" s="65"/>
+      <c r="F38" s="65"/>
+      <c r="G38" s="65"/>
+      <c r="H38" s="65"/>
+      <c r="I38" s="65"/>
+      <c r="L38" s="9"/>
+      <c r="M38" s="9"/>
+      <c r="N38" s="9"/>
+      <c r="O38" s="9"/>
+      <c r="P38" s="9"/>
+      <c r="Q38" s="9"/>
+      <c r="R38" s="9"/>
+      <c r="S38" s="9"/>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="63" t="s">
+      <c r="A39" s="64" t="s">
         <v>86</v>
       </c>
-      <c r="B39" s="64" t="n">
+      <c r="B39" s="65" t="n">
         <v>1</v>
       </c>
-      <c r="C39" s="64" t="n">
+      <c r="C39" s="65" t="n">
         <v>1</v>
       </c>
-      <c r="D39" s="64"/>
-      <c r="E39" s="64"/>
-      <c r="F39" s="64"/>
-      <c r="G39" s="64"/>
-      <c r="H39" s="64"/>
-      <c r="I39" s="64"/>
-      <c r="L39" s="8"/>
-      <c r="M39" s="8"/>
-      <c r="N39" s="8"/>
-      <c r="O39" s="8"/>
-      <c r="P39" s="8"/>
-      <c r="Q39" s="8"/>
-      <c r="R39" s="8"/>
-      <c r="S39" s="8"/>
+      <c r="D39" s="65"/>
+      <c r="E39" s="65"/>
+      <c r="F39" s="65"/>
+      <c r="G39" s="65"/>
+      <c r="H39" s="65"/>
+      <c r="I39" s="65"/>
+      <c r="L39" s="9"/>
+      <c r="M39" s="9"/>
+      <c r="N39" s="9"/>
+      <c r="O39" s="9"/>
+      <c r="P39" s="9"/>
+      <c r="Q39" s="9"/>
+      <c r="R39" s="9"/>
+      <c r="S39" s="9"/>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="L40" s="8"/>
-      <c r="M40" s="8"/>
-      <c r="N40" s="8"/>
-      <c r="O40" s="8"/>
-      <c r="P40" s="8"/>
-      <c r="Q40" s="8"/>
-      <c r="R40" s="8"/>
-      <c r="S40" s="8"/>
+      <c r="L40" s="9"/>
+      <c r="M40" s="9"/>
+      <c r="N40" s="9"/>
+      <c r="O40" s="9"/>
+      <c r="P40" s="9"/>
+      <c r="Q40" s="9"/>
+      <c r="R40" s="9"/>
+      <c r="S40" s="9"/>
     </row>
     <row r="41" customFormat="false" ht="17.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A41" s="56" t="s">
+      <c r="A41" s="57" t="s">
         <v>87</v>
       </c>
-      <c r="B41" s="57" t="s">
+      <c r="B41" s="58" t="s">
         <v>88</v>
       </c>
-      <c r="C41" s="57"/>
-      <c r="D41" s="57"/>
-      <c r="E41" s="57"/>
-      <c r="F41" s="65"/>
-      <c r="G41" s="65"/>
-      <c r="L41" s="8"/>
-      <c r="M41" s="8"/>
-      <c r="N41" s="8"/>
-      <c r="O41" s="8"/>
-      <c r="P41" s="8"/>
-      <c r="Q41" s="8"/>
-      <c r="R41" s="8"/>
-      <c r="S41" s="8"/>
+      <c r="C41" s="58"/>
+      <c r="D41" s="58"/>
+      <c r="E41" s="58"/>
+      <c r="F41" s="66"/>
+      <c r="G41" s="66"/>
+      <c r="L41" s="9"/>
+      <c r="M41" s="9"/>
+      <c r="N41" s="9"/>
+      <c r="O41" s="9"/>
+      <c r="P41" s="9"/>
+      <c r="Q41" s="9"/>
+      <c r="R41" s="9"/>
+      <c r="S41" s="9"/>
     </row>
     <row r="42" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="56"/>
-      <c r="B42" s="57" t="s">
+      <c r="A42" s="57"/>
+      <c r="B42" s="58" t="s">
         <v>69</v>
       </c>
-      <c r="C42" s="57"/>
-      <c r="D42" s="57"/>
-      <c r="E42" s="57"/>
-      <c r="F42" s="65"/>
-      <c r="G42" s="65"/>
-      <c r="L42" s="8"/>
-      <c r="M42" s="8"/>
-      <c r="N42" s="8"/>
-      <c r="O42" s="8"/>
-      <c r="P42" s="8"/>
-      <c r="Q42" s="8"/>
-      <c r="R42" s="8"/>
-      <c r="S42" s="8"/>
+      <c r="C42" s="58"/>
+      <c r="D42" s="58"/>
+      <c r="E42" s="58"/>
+      <c r="F42" s="66"/>
+      <c r="G42" s="66"/>
+      <c r="L42" s="9"/>
+      <c r="M42" s="9"/>
+      <c r="N42" s="9"/>
+      <c r="O42" s="9"/>
+      <c r="P42" s="9"/>
+      <c r="Q42" s="9"/>
+      <c r="R42" s="9"/>
+      <c r="S42" s="9"/>
     </row>
     <row r="43" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="66"/>
-      <c r="B43" s="65"/>
-      <c r="C43" s="65"/>
-      <c r="D43" s="65"/>
-      <c r="E43" s="65"/>
-      <c r="F43" s="65"/>
-      <c r="G43" s="65"/>
-      <c r="L43" s="8"/>
-      <c r="M43" s="8"/>
-      <c r="N43" s="8"/>
-      <c r="O43" s="8"/>
-      <c r="P43" s="8"/>
-      <c r="Q43" s="8"/>
-      <c r="R43" s="8"/>
-      <c r="S43" s="8"/>
+      <c r="A43" s="67"/>
+      <c r="B43" s="66"/>
+      <c r="C43" s="66"/>
+      <c r="D43" s="66"/>
+      <c r="E43" s="66"/>
+      <c r="F43" s="66"/>
+      <c r="G43" s="66"/>
+      <c r="L43" s="9"/>
+      <c r="M43" s="9"/>
+      <c r="N43" s="9"/>
+      <c r="O43" s="9"/>
+      <c r="P43" s="9"/>
+      <c r="Q43" s="9"/>
+      <c r="R43" s="9"/>
+      <c r="S43" s="9"/>
     </row>
     <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="67" t="s">
+      <c r="A44" s="68" t="s">
         <v>89</v>
       </c>
-      <c r="B44" s="67" t="s">
+      <c r="B44" s="68" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="68" t="n">
+      <c r="A45" s="69" t="n">
         <v>1</v>
       </c>
-      <c r="B45" s="69" t="s">
+      <c r="B45" s="70" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="68" t="n">
+      <c r="A46" s="69" t="n">
         <v>3</v>
       </c>
-      <c r="B46" s="69" t="s">
+      <c r="B46" s="70" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="68" t="n">
+      <c r="A47" s="69" t="n">
         <v>2</v>
       </c>
-      <c r="B47" s="69" t="s">
+      <c r="B47" s="70" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="68" t="n">
+      <c r="A48" s="69" t="n">
         <v>1</v>
       </c>
-      <c r="B48" s="69" t="s">
+      <c r="B48" s="70" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="68" t="n">
+      <c r="A49" s="69" t="n">
         <v>2</v>
       </c>
-      <c r="B49" s="69" t="s">
+      <c r="B49" s="70" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="13"/>
-      <c r="B50" s="70"/>
+      <c r="A50" s="14"/>
+      <c r="B50" s="71"/>
     </row>
     <row r="51" customFormat="false" ht="17.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A51" s="56" t="s">
+      <c r="A51" s="57" t="s">
         <v>96</v>
       </c>
-      <c r="B51" s="57" t="s">
+      <c r="B51" s="58" t="s">
         <v>97</v>
       </c>
-      <c r="C51" s="57"/>
-      <c r="D51" s="57"/>
-      <c r="E51" s="57"/>
-      <c r="F51" s="57"/>
-      <c r="G51" s="57"/>
-      <c r="H51" s="57"/>
-      <c r="I51" s="57"/>
+      <c r="C51" s="58"/>
+      <c r="D51" s="58"/>
+      <c r="E51" s="58"/>
+      <c r="F51" s="58"/>
+      <c r="G51" s="58"/>
+      <c r="H51" s="58"/>
+      <c r="I51" s="58"/>
     </row>
     <row r="52" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="56"/>
-      <c r="B52" s="57" t="s">
+      <c r="A52" s="57"/>
+      <c r="B52" s="58" t="s">
         <v>69</v>
       </c>
-      <c r="C52" s="57"/>
-      <c r="D52" s="57"/>
-      <c r="E52" s="57"/>
-      <c r="F52" s="57"/>
-      <c r="G52" s="57"/>
-      <c r="H52" s="57"/>
-      <c r="I52" s="57"/>
+      <c r="C52" s="58"/>
+      <c r="D52" s="58"/>
+      <c r="E52" s="58"/>
+      <c r="F52" s="58"/>
+      <c r="G52" s="58"/>
+      <c r="H52" s="58"/>
+      <c r="I52" s="58"/>
     </row>
     <row r="53" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="66"/>
-      <c r="B53" s="65"/>
-      <c r="C53" s="65"/>
-      <c r="D53" s="65"/>
-      <c r="E53" s="65"/>
-      <c r="F53" s="65"/>
-      <c r="G53" s="65"/>
-      <c r="H53" s="71"/>
-      <c r="I53" s="71"/>
+      <c r="A53" s="67"/>
+      <c r="B53" s="66"/>
+      <c r="C53" s="66"/>
+      <c r="D53" s="66"/>
+      <c r="E53" s="66"/>
+      <c r="F53" s="66"/>
+      <c r="G53" s="66"/>
+      <c r="H53" s="72"/>
+      <c r="I53" s="72"/>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="61" t="s">
+      <c r="A54" s="62" t="s">
         <v>98</v>
       </c>
-      <c r="B54" s="72" t="s">
+      <c r="B54" s="73" t="s">
         <v>27</v>
       </c>
-      <c r="C54" s="62" t="s">
+      <c r="C54" s="63" t="s">
         <v>41</v>
       </c>
-      <c r="D54" s="62" t="s">
+      <c r="D54" s="63" t="s">
         <v>48</v>
       </c>
-      <c r="E54" s="62" t="s">
+      <c r="E54" s="63" t="s">
         <v>71</v>
       </c>
-      <c r="F54" s="62" t="s">
+      <c r="F54" s="63" t="s">
         <v>72</v>
       </c>
-      <c r="G54" s="62" t="s">
+      <c r="G54" s="63" t="s">
         <v>73</v>
       </c>
-      <c r="H54" s="62" t="s">
+      <c r="H54" s="63" t="s">
         <v>74</v>
       </c>
-      <c r="I54" s="62" t="s">
+      <c r="I54" s="63" t="s">
         <v>75</v>
       </c>
-      <c r="J54" s="62" t="s">
+      <c r="J54" s="63" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="46.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="73" t="s">
+      <c r="A55" s="74" t="s">
         <v>99</v>
       </c>
-      <c r="B55" s="74" t="s">
+      <c r="B55" s="75" t="s">
         <v>43</v>
       </c>
-      <c r="C55" s="75" t="s">
+      <c r="C55" s="76" t="s">
         <v>100</v>
       </c>
-      <c r="D55" s="76"/>
-      <c r="E55" s="76"/>
-      <c r="F55" s="76"/>
-      <c r="G55" s="76"/>
-      <c r="H55" s="76"/>
-      <c r="I55" s="76"/>
-      <c r="J55" s="76"/>
+      <c r="D55" s="77"/>
+      <c r="E55" s="77"/>
+      <c r="F55" s="77"/>
+      <c r="G55" s="77"/>
+      <c r="H55" s="77"/>
+      <c r="I55" s="77"/>
+      <c r="J55" s="77"/>
     </row>
     <row r="56" customFormat="false" ht="23.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A56" s="77" t="s">
+      <c r="A56" s="78" t="s">
         <v>101</v>
       </c>
-      <c r="B56" s="78" t="s">
+      <c r="B56" s="79" t="s">
         <v>102</v>
       </c>
-      <c r="C56" s="64"/>
-      <c r="D56" s="79" t="s">
+      <c r="C56" s="65"/>
+      <c r="D56" s="80" t="s">
         <v>103</v>
       </c>
-      <c r="E56" s="64"/>
-      <c r="F56" s="64"/>
-      <c r="G56" s="64"/>
-      <c r="H56" s="64"/>
-      <c r="I56" s="64"/>
-      <c r="J56" s="64"/>
+      <c r="E56" s="65"/>
+      <c r="F56" s="65"/>
+      <c r="G56" s="65"/>
+      <c r="H56" s="65"/>
+      <c r="I56" s="65"/>
+      <c r="J56" s="65"/>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="77" t="s">
+      <c r="A57" s="78" t="s">
         <v>101</v>
       </c>
-      <c r="B57" s="78" t="s">
+      <c r="B57" s="79" t="s">
         <v>104</v>
       </c>
-      <c r="C57" s="64"/>
-      <c r="D57" s="79" t="s">
+      <c r="C57" s="65"/>
+      <c r="D57" s="80" t="s">
         <v>103</v>
       </c>
-      <c r="E57" s="64"/>
-      <c r="F57" s="64"/>
-      <c r="G57" s="64"/>
-      <c r="H57" s="64"/>
-      <c r="I57" s="64"/>
-      <c r="J57" s="64"/>
+      <c r="E57" s="65"/>
+      <c r="F57" s="65"/>
+      <c r="G57" s="65"/>
+      <c r="H57" s="65"/>
+      <c r="I57" s="65"/>
+      <c r="J57" s="65"/>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="77" t="s">
+      <c r="A58" s="78" t="s">
         <v>101</v>
       </c>
-      <c r="B58" s="80" t="s">
+      <c r="B58" s="81" t="s">
         <v>105</v>
       </c>
-      <c r="C58" s="64"/>
-      <c r="D58" s="79" t="s">
+      <c r="C58" s="65"/>
+      <c r="D58" s="80" t="s">
         <v>103</v>
       </c>
-      <c r="E58" s="64"/>
-      <c r="F58" s="64"/>
-      <c r="G58" s="64"/>
-      <c r="H58" s="64"/>
-      <c r="I58" s="64"/>
-      <c r="J58" s="64"/>
+      <c r="E58" s="65"/>
+      <c r="F58" s="65"/>
+      <c r="G58" s="65"/>
+      <c r="H58" s="65"/>
+      <c r="I58" s="65"/>
+      <c r="J58" s="65"/>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="77" t="s">
+      <c r="A59" s="78" t="s">
         <v>101</v>
       </c>
-      <c r="B59" s="80" t="s">
+      <c r="B59" s="81" t="s">
         <v>49</v>
       </c>
-      <c r="C59" s="64"/>
-      <c r="D59" s="79" t="s">
+      <c r="C59" s="65"/>
+      <c r="D59" s="80" t="s">
         <v>103</v>
       </c>
-      <c r="E59" s="64"/>
-      <c r="F59" s="64"/>
-      <c r="G59" s="64"/>
-      <c r="H59" s="64"/>
-      <c r="I59" s="64"/>
-      <c r="J59" s="64"/>
+      <c r="E59" s="65"/>
+      <c r="F59" s="65"/>
+      <c r="G59" s="65"/>
+      <c r="H59" s="65"/>
+      <c r="I59" s="65"/>
+      <c r="J59" s="65"/>
     </row>
     <row r="61" customFormat="false" ht="17.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A61" s="56" t="s">
+      <c r="A61" s="57" t="s">
         <v>106</v>
       </c>
-      <c r="B61" s="57" t="s">
+      <c r="B61" s="58" t="s">
         <v>107</v>
       </c>
-      <c r="C61" s="57"/>
-      <c r="D61" s="57"/>
-      <c r="E61" s="57"/>
-      <c r="F61" s="57"/>
-      <c r="G61" s="57"/>
+      <c r="C61" s="58"/>
+      <c r="D61" s="58"/>
+      <c r="E61" s="58"/>
+      <c r="F61" s="58"/>
+      <c r="G61" s="58"/>
     </row>
     <row r="62" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="56"/>
-      <c r="B62" s="57" t="s">
+      <c r="A62" s="57"/>
+      <c r="B62" s="58" t="s">
         <v>69</v>
       </c>
-      <c r="C62" s="57"/>
-      <c r="D62" s="57"/>
-      <c r="E62" s="57"/>
-      <c r="F62" s="57"/>
-      <c r="G62" s="57"/>
+      <c r="C62" s="58"/>
+      <c r="D62" s="58"/>
+      <c r="E62" s="58"/>
+      <c r="F62" s="58"/>
+      <c r="G62" s="58"/>
     </row>
     <row r="63" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="66"/>
-      <c r="B63" s="65"/>
-      <c r="C63" s="65"/>
-      <c r="D63" s="65"/>
-      <c r="E63" s="65"/>
-      <c r="F63" s="65"/>
-      <c r="G63" s="65"/>
+      <c r="A63" s="67"/>
+      <c r="B63" s="66"/>
+      <c r="C63" s="66"/>
+      <c r="D63" s="66"/>
+      <c r="E63" s="66"/>
+      <c r="F63" s="66"/>
+      <c r="G63" s="66"/>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="72" t="s">
+      <c r="A64" s="73" t="s">
         <v>27</v>
       </c>
-      <c r="B64" s="62" t="s">
-        <v>41</v>
-      </c>
-      <c r="C64" s="62" t="s">
-        <v>48</v>
-      </c>
-      <c r="D64" s="62" t="s">
-        <v>71</v>
-      </c>
-      <c r="E64" s="62" t="s">
-        <v>72</v>
-      </c>
-      <c r="F64" s="62" t="s">
-        <v>73</v>
-      </c>
-      <c r="G64" s="62" t="s">
-        <v>74</v>
-      </c>
-      <c r="H64" s="62" t="s">
-        <v>75</v>
-      </c>
-      <c r="I64" s="62" t="s">
-        <v>76</v>
-      </c>
+      <c r="B64" s="63" t="s">
+        <v>108</v>
+      </c>
+      <c r="C64" s="82"/>
+      <c r="D64" s="82"/>
+      <c r="E64" s="82"/>
+      <c r="F64" s="82"/>
+      <c r="G64" s="82"/>
+      <c r="H64" s="82"/>
+      <c r="I64" s="82"/>
+      <c r="J64" s="83"/>
+      <c r="K64" s="83"/>
+      <c r="L64" s="83"/>
+      <c r="M64" s="83"/>
+      <c r="N64" s="83"/>
+      <c r="O64" s="83"/>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="80" t="s">
+      <c r="A65" s="81" t="s">
         <v>43</v>
       </c>
-      <c r="B65" s="64" t="s">
-        <v>108</v>
-      </c>
-      <c r="C65" s="64" t="s">
-        <v>108</v>
-      </c>
-      <c r="D65" s="64"/>
-      <c r="E65" s="64"/>
-      <c r="F65" s="64"/>
-      <c r="G65" s="64"/>
-      <c r="H65" s="64"/>
-      <c r="I65" s="64"/>
+      <c r="B65" s="65" t="s">
+        <v>109</v>
+      </c>
+      <c r="C65" s="84"/>
+      <c r="D65" s="84"/>
+      <c r="E65" s="84"/>
+      <c r="F65" s="84"/>
+      <c r="G65" s="84"/>
+      <c r="H65" s="84"/>
+      <c r="I65" s="84"/>
+      <c r="J65" s="83"/>
+      <c r="K65" s="83"/>
+      <c r="L65" s="83"/>
+      <c r="M65" s="83"/>
+      <c r="N65" s="83"/>
+      <c r="O65" s="83"/>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="81" t="s">
+      <c r="A66" s="85" t="s">
         <v>102</v>
       </c>
-      <c r="B66" s="64"/>
-      <c r="C66" s="64"/>
-      <c r="D66" s="64"/>
-      <c r="E66" s="64"/>
-      <c r="F66" s="64"/>
-      <c r="G66" s="64"/>
-      <c r="H66" s="64"/>
-      <c r="I66" s="64"/>
+      <c r="B66" s="65"/>
+      <c r="C66" s="84"/>
+      <c r="D66" s="84"/>
+      <c r="E66" s="84"/>
+      <c r="F66" s="84"/>
+      <c r="G66" s="84"/>
+      <c r="H66" s="84"/>
+      <c r="I66" s="84"/>
+      <c r="J66" s="83"/>
+      <c r="K66" s="83"/>
+      <c r="L66" s="83"/>
+      <c r="M66" s="83"/>
+      <c r="N66" s="83"/>
+      <c r="O66" s="83"/>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="81" t="s">
+      <c r="A67" s="85" t="s">
         <v>104</v>
       </c>
-      <c r="B67" s="64" t="s">
-        <v>108</v>
-      </c>
-      <c r="C67" s="64" t="s">
-        <v>108</v>
-      </c>
-      <c r="D67" s="64"/>
-      <c r="E67" s="64"/>
-      <c r="F67" s="64"/>
-      <c r="G67" s="64"/>
-      <c r="H67" s="64"/>
-      <c r="I67" s="64"/>
+      <c r="B67" s="65" t="s">
+        <v>109</v>
+      </c>
+      <c r="C67" s="84"/>
+      <c r="D67" s="84"/>
+      <c r="E67" s="84"/>
+      <c r="F67" s="84"/>
+      <c r="G67" s="84"/>
+      <c r="H67" s="84"/>
+      <c r="I67" s="84"/>
+      <c r="J67" s="83"/>
+      <c r="K67" s="83"/>
+      <c r="L67" s="83"/>
+      <c r="M67" s="83"/>
+      <c r="N67" s="83"/>
+      <c r="O67" s="83"/>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="80" t="s">
+      <c r="A68" s="81" t="s">
         <v>105</v>
       </c>
-      <c r="B68" s="64"/>
-      <c r="C68" s="64"/>
-      <c r="D68" s="64"/>
-      <c r="E68" s="64"/>
-      <c r="F68" s="64"/>
-      <c r="G68" s="64"/>
-      <c r="H68" s="64"/>
-      <c r="I68" s="64"/>
+      <c r="B68" s="65"/>
+      <c r="C68" s="84"/>
+      <c r="D68" s="84"/>
+      <c r="E68" s="84"/>
+      <c r="F68" s="84"/>
+      <c r="G68" s="84"/>
+      <c r="H68" s="84"/>
+      <c r="I68" s="84"/>
+      <c r="J68" s="83"/>
+      <c r="K68" s="83"/>
+      <c r="L68" s="83"/>
+      <c r="M68" s="83"/>
+      <c r="N68" s="83"/>
+      <c r="O68" s="83"/>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="80" t="s">
+      <c r="A69" s="81" t="s">
         <v>49</v>
       </c>
-      <c r="B69" s="64"/>
-      <c r="C69" s="64" t="s">
-        <v>108</v>
-      </c>
-      <c r="D69" s="64"/>
-      <c r="E69" s="64"/>
-      <c r="F69" s="64"/>
-      <c r="G69" s="64"/>
-      <c r="H69" s="64"/>
-      <c r="I69" s="64"/>
+      <c r="B69" s="65"/>
+      <c r="C69" s="84"/>
+      <c r="D69" s="84"/>
+      <c r="E69" s="84"/>
+      <c r="F69" s="84"/>
+      <c r="G69" s="84"/>
+      <c r="H69" s="84"/>
+      <c r="I69" s="84"/>
+      <c r="J69" s="83"/>
+      <c r="K69" s="83"/>
+      <c r="L69" s="83"/>
+      <c r="M69" s="83"/>
+      <c r="N69" s="83"/>
+      <c r="O69" s="83"/>
     </row>
   </sheetData>
   <mergeCells count="19">
@@ -3213,207 +3256,207 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="82" t="s">
-        <v>109</v>
-      </c>
-      <c r="B1" s="82" t="s">
+      <c r="A1" s="86" t="s">
         <v>110</v>
       </c>
-      <c r="C1" s="82" t="s">
+      <c r="B1" s="86" t="s">
         <v>111</v>
       </c>
-      <c r="D1" s="82" t="s">
+      <c r="C1" s="86" t="s">
         <v>112</v>
       </c>
-      <c r="E1" s="82" t="s">
+      <c r="D1" s="86" t="s">
         <v>113</v>
       </c>
+      <c r="E1" s="86" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="52" t="s">
+      <c r="A2" s="53" t="s">
         <v>43</v>
       </c>
-      <c r="B2" s="82"/>
-      <c r="C2" s="82"/>
-      <c r="D2" s="82"/>
-      <c r="E2" s="82"/>
+      <c r="B2" s="86"/>
+      <c r="C2" s="86"/>
+      <c r="D2" s="86"/>
+      <c r="E2" s="86"/>
     </row>
     <row r="3" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="55" t="s">
+      <c r="A3" s="56" t="s">
         <v>49</v>
       </c>
-      <c r="B3" s="55" t="s">
-        <v>114</v>
-      </c>
-      <c r="C3" s="83" t="s">
+      <c r="B3" s="56" t="s">
         <v>115</v>
       </c>
-      <c r="D3" s="83"/>
-      <c r="E3" s="55" t="s">
+      <c r="C3" s="87" t="s">
         <v>116</v>
       </c>
+      <c r="D3" s="87"/>
+      <c r="E3" s="56" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="55" t="s">
+      <c r="A4" s="56" t="s">
         <v>53</v>
       </c>
-      <c r="B4" s="55" t="s">
-        <v>117</v>
-      </c>
-      <c r="C4" s="55"/>
-      <c r="D4" s="55"/>
-      <c r="E4" s="83" t="s">
+      <c r="B4" s="56" t="s">
         <v>118</v>
       </c>
+      <c r="C4" s="56"/>
+      <c r="D4" s="56"/>
+      <c r="E4" s="87" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="55" t="s">
+      <c r="A5" s="56" t="s">
         <v>102</v>
       </c>
-      <c r="B5" s="55" t="s">
-        <v>119</v>
-      </c>
-      <c r="C5" s="55" t="s">
+      <c r="B5" s="56" t="s">
         <v>120</v>
       </c>
-      <c r="D5" s="55"/>
-      <c r="E5" s="55" t="s">
+      <c r="C5" s="56" t="s">
         <v>121</v>
       </c>
+      <c r="D5" s="56"/>
+      <c r="E5" s="56" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="55" t="s">
-        <v>122</v>
-      </c>
-      <c r="B6" s="55" t="s">
+      <c r="A6" s="56" t="s">
         <v>123</v>
       </c>
-      <c r="C6" s="55" t="s">
+      <c r="B6" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="D6" s="55"/>
-      <c r="E6" s="55" t="s">
+      <c r="C6" s="56" t="s">
         <v>125</v>
       </c>
+      <c r="D6" s="56"/>
+      <c r="E6" s="56" t="s">
+        <v>126</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="55" t="s">
+      <c r="A7" s="56" t="s">
         <v>104</v>
       </c>
-      <c r="B7" s="55" t="s">
-        <v>126</v>
-      </c>
-      <c r="C7" s="55" t="s">
+      <c r="B7" s="56" t="s">
         <v>127</v>
       </c>
-      <c r="D7" s="55" t="s">
+      <c r="C7" s="56" t="s">
         <v>128</v>
       </c>
-      <c r="E7" s="83" t="s">
+      <c r="D7" s="56" t="s">
         <v>129</v>
       </c>
+      <c r="E7" s="87" t="s">
+        <v>130</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="55" t="s">
-        <v>130</v>
-      </c>
-      <c r="B8" s="55" t="s">
+      <c r="A8" s="56" t="s">
         <v>131</v>
       </c>
-      <c r="C8" s="83" t="s">
+      <c r="B8" s="56" t="s">
         <v>132</v>
       </c>
-      <c r="D8" s="83"/>
-      <c r="E8" s="55" t="s">
+      <c r="C8" s="87" t="s">
         <v>133</v>
       </c>
+      <c r="D8" s="87"/>
+      <c r="E8" s="56" t="s">
+        <v>134</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="55" t="s">
-        <v>134</v>
-      </c>
-      <c r="B9" s="55" t="s">
+      <c r="A9" s="56" t="s">
         <v>135</v>
       </c>
-      <c r="C9" s="83"/>
-      <c r="D9" s="83" t="s">
+      <c r="B9" s="56" t="s">
         <v>136</v>
       </c>
-      <c r="E9" s="55" t="s">
-        <v>134</v>
+      <c r="C9" s="87"/>
+      <c r="D9" s="87" t="s">
+        <v>137</v>
+      </c>
+      <c r="E9" s="56" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="55" t="s">
-        <v>137</v>
-      </c>
-      <c r="B10" s="55" t="s">
+      <c r="A10" s="56" t="s">
         <v>138</v>
       </c>
-      <c r="C10" s="55"/>
-      <c r="D10" s="55"/>
-      <c r="E10" s="55" t="s">
+      <c r="B10" s="56" t="s">
         <v>139</v>
       </c>
+      <c r="C10" s="56"/>
+      <c r="D10" s="56"/>
+      <c r="E10" s="56" t="s">
+        <v>140</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="55" t="s">
-        <v>140</v>
-      </c>
-      <c r="B11" s="55" t="s">
+      <c r="A11" s="56" t="s">
         <v>141</v>
       </c>
-      <c r="C11" s="55" t="s">
+      <c r="B11" s="56" t="s">
         <v>142</v>
       </c>
-      <c r="D11" s="55"/>
-      <c r="E11" s="83" t="s">
+      <c r="C11" s="56" t="s">
         <v>143</v>
       </c>
+      <c r="D11" s="56"/>
+      <c r="E11" s="87" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="55" t="s">
-        <v>144</v>
-      </c>
-      <c r="B12" s="55" t="s">
+      <c r="A12" s="56" t="s">
         <v>145</v>
       </c>
-      <c r="C12" s="55" t="s">
+      <c r="B12" s="56" t="s">
         <v>146</v>
       </c>
-      <c r="D12" s="55"/>
-      <c r="E12" s="83" t="s">
+      <c r="C12" s="56" t="s">
         <v>147</v>
       </c>
+      <c r="D12" s="56"/>
+      <c r="E12" s="87" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="55" t="s">
+      <c r="A13" s="56" t="s">
         <v>105</v>
       </c>
-      <c r="B13" s="55" t="s">
-        <v>148</v>
-      </c>
-      <c r="C13" s="55" t="s">
+      <c r="B13" s="56" t="s">
         <v>149</v>
       </c>
-      <c r="D13" s="55"/>
-      <c r="E13" s="83" t="s">
+      <c r="C13" s="56" t="s">
         <v>150</v>
       </c>
+      <c r="D13" s="56"/>
+      <c r="E13" s="87" t="s">
+        <v>151</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="55" t="s">
-        <v>151</v>
-      </c>
-      <c r="B14" s="83" t="s">
+      <c r="A14" s="56" t="s">
         <v>152</v>
       </c>
-      <c r="C14" s="55" t="s">
+      <c r="B14" s="87" t="s">
         <v>153</v>
       </c>
-      <c r="D14" s="55"/>
-      <c r="E14" s="83" t="s">
+      <c r="C14" s="56" t="s">
         <v>154</v>
+      </c>
+      <c r="D14" s="56"/>
+      <c r="E14" s="87" t="s">
+        <v>155</v>
       </c>
     </row>
   </sheetData>
@@ -3450,28 +3493,28 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="84" t="s">
-        <v>155</v>
-      </c>
-      <c r="B1" s="84" t="s">
+      <c r="A1" s="88" t="s">
         <v>156</v>
       </c>
-      <c r="C1" s="84" t="s">
+      <c r="B1" s="88" t="s">
         <v>157</v>
       </c>
-      <c r="D1" s="84" t="s">
+      <c r="C1" s="88" t="s">
         <v>158</v>
       </c>
-      <c r="E1" s="84" t="s">
+      <c r="D1" s="88" t="s">
         <v>159</v>
       </c>
-      <c r="F1" s="84" t="s">
+      <c r="E1" s="88" t="s">
         <v>160</v>
+      </c>
+      <c r="F1" s="88" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>43</v>
@@ -3479,7 +3522,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>43</v>
@@ -3495,7 +3538,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B5" s="0" t="s">
         <v>43</v>
@@ -3503,7 +3546,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B6" s="0" t="s">
         <v>43</v>
@@ -3519,7 +3562,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B8" s="0" t="s">
         <v>43</v>
@@ -3543,7 +3586,7 @@
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B11" s="0" t="s">
         <v>43</v>
@@ -3551,7 +3594,7 @@
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B12" s="0" t="s">
         <v>43</v>
@@ -3559,7 +3602,7 @@
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B13" s="0" t="s">
         <v>43</v>
@@ -3567,7 +3610,7 @@
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B14" s="0" t="s">
         <v>43</v>
@@ -3575,7 +3618,7 @@
     </row>
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B15" s="0" t="s">
         <v>43</v>
@@ -3583,7 +3626,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B16" s="0" t="s">
         <v>43</v>
@@ -3591,7 +3634,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B17" s="0" t="s">
         <v>43</v>
@@ -3599,7 +3642,7 @@
     </row>
     <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B18" s="0" t="s">
         <v>43</v>
@@ -3607,7 +3650,7 @@
     </row>
     <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B19" s="0" t="s">
         <v>43</v>
@@ -3615,7 +3658,7 @@
     </row>
     <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B20" s="0" t="s">
         <v>43</v>
@@ -3631,7 +3674,7 @@
     </row>
     <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B22" s="0" t="s">
         <v>43</v>
@@ -3639,7 +3682,7 @@
     </row>
     <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B23" s="0" t="s">
         <v>43</v>
@@ -3647,7 +3690,7 @@
     </row>
     <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B24" s="0" t="s">
         <v>43</v>
@@ -3655,7 +3698,7 @@
     </row>
     <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B25" s="0" t="s">
         <v>43</v>
@@ -3663,7 +3706,7 @@
     </row>
     <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B26" s="0" t="s">
         <v>105</v>
@@ -3671,7 +3714,7 @@
     </row>
     <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B27" s="0" t="s">
         <v>105</v>
@@ -3682,31 +3725,31 @@
         <v>65</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3714,20 +3757,20 @@
         <v>61</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B34" s="0" t="s">
         <v>102</v>
@@ -3735,7 +3778,7 @@
     </row>
     <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B35" s="0" t="s">
         <v>102</v>
@@ -3743,7 +3786,7 @@
     </row>
     <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B36" s="0" t="s">
         <v>49</v>
@@ -3751,7 +3794,7 @@
     </row>
     <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B37" s="0" t="s">
         <v>49</v>
@@ -3767,7 +3810,7 @@
     </row>
     <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B39" s="0" t="s">
         <v>49</v>
@@ -3775,7 +3818,7 @@
     </row>
     <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B40" s="0" t="s">
         <v>49</v>
@@ -3783,7 +3826,7 @@
     </row>
     <row r="41" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B41" s="0" t="s">
         <v>49</v>
@@ -3791,7 +3834,7 @@
     </row>
     <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B42" s="0" t="s">
         <v>49</v>
@@ -3799,7 +3842,7 @@
     </row>
     <row r="43" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B43" s="0" t="s">
         <v>49</v>
@@ -3807,7 +3850,7 @@
     </row>
     <row r="44" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B44" s="0" t="s">
         <v>49</v>
@@ -3815,7 +3858,7 @@
     </row>
     <row r="45" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B45" s="0" t="s">
         <v>49</v>
@@ -3823,7 +3866,7 @@
     </row>
     <row r="46" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B46" s="0" t="s">
         <v>102</v>
@@ -3831,7 +3874,7 @@
     </row>
     <row r="47" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B47" s="0" t="s">
         <v>102</v>
@@ -3839,7 +3882,7 @@
     </row>
     <row r="48" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B48" s="0" t="s">
         <v>102</v>
@@ -3847,7 +3890,7 @@
     </row>
     <row r="49" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B49" s="0" t="s">
         <v>102</v>
@@ -3855,7 +3898,7 @@
     </row>
     <row r="50" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B50" s="0" t="s">
         <v>102</v>
@@ -3863,7 +3906,7 @@
     </row>
     <row r="51" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B51" s="0" t="s">
         <v>102</v>
@@ -3871,7 +3914,7 @@
     </row>
     <row r="52" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B52" s="0" t="s">
         <v>102</v>
@@ -3879,13 +3922,13 @@
     </row>
     <row r="53" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B53" s="0" t="s">
         <v>102</v>
       </c>
       <c r="D53" s="0" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="E53" s="0" t="str">
         <f aca="false">+VLOOKUP(D53,A1:B121,1)</f>
@@ -3894,7 +3937,7 @@
     </row>
     <row r="54" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B54" s="0" t="s">
         <v>102</v>
@@ -3902,7 +3945,7 @@
     </row>
     <row r="55" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B55" s="0" t="s">
         <v>102</v>
@@ -3910,7 +3953,7 @@
     </row>
     <row r="56" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B56" s="0" t="s">
         <v>102</v>
@@ -3918,7 +3961,7 @@
     </row>
     <row r="57" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B57" s="0" t="s">
         <v>102</v>
@@ -3926,7 +3969,7 @@
     </row>
     <row r="58" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B58" s="0" t="s">
         <v>102</v>
@@ -3934,7 +3977,7 @@
     </row>
     <row r="59" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B59" s="0" t="s">
         <v>102</v>
@@ -3942,7 +3985,7 @@
     </row>
     <row r="60" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B60" s="0" t="s">
         <v>102</v>
@@ -3950,7 +3993,7 @@
     </row>
     <row r="61" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B61" s="0" t="s">
         <v>102</v>
@@ -3958,7 +4001,7 @@
     </row>
     <row r="62" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B62" s="0" t="s">
         <v>102</v>
@@ -3966,7 +4009,7 @@
     </row>
     <row r="63" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B63" s="0" t="s">
         <v>102</v>
@@ -3974,33 +4017,33 @@
     </row>
     <row r="64" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>205</v>
-      </c>
-      <c r="B64" s="85" t="s">
+        <v>206</v>
+      </c>
+      <c r="B64" s="89" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>206</v>
-      </c>
-      <c r="B65" s="85" t="s">
+        <v>207</v>
+      </c>
+      <c r="B65" s="89" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>207</v>
-      </c>
-      <c r="B66" s="85" t="s">
+        <v>208</v>
+      </c>
+      <c r="B66" s="89" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>208</v>
-      </c>
-      <c r="B67" s="85" t="s">
+        <v>209</v>
+      </c>
+      <c r="B67" s="89" t="s">
         <v>53</v>
       </c>
     </row>
@@ -4008,421 +4051,421 @@
       <c r="A68" s="0" t="s">
         <v>65</v>
       </c>
-      <c r="B68" s="85" t="s">
+      <c r="B68" s="89" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>182</v>
-      </c>
-      <c r="B69" s="85" t="s">
+        <v>183</v>
+      </c>
+      <c r="B69" s="89" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>209</v>
-      </c>
-      <c r="B70" s="85" t="s">
+        <v>210</v>
+      </c>
+      <c r="B70" s="89" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>210</v>
-      </c>
-      <c r="B71" s="85" t="s">
+        <v>211</v>
+      </c>
+      <c r="B71" s="89" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>211</v>
-      </c>
-      <c r="B72" s="85" t="s">
+        <v>212</v>
+      </c>
+      <c r="B72" s="89" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
-        <v>212</v>
-      </c>
-      <c r="B73" s="85" t="s">
+        <v>213</v>
+      </c>
+      <c r="B73" s="89" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
-        <v>213</v>
-      </c>
-      <c r="B74" s="85" t="s">
+        <v>214</v>
+      </c>
+      <c r="B74" s="89" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
-        <v>214</v>
-      </c>
-      <c r="B75" s="85" t="s">
+        <v>215</v>
+      </c>
+      <c r="B75" s="89" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
-        <v>215</v>
-      </c>
-      <c r="B76" s="85" t="s">
+        <v>216</v>
+      </c>
+      <c r="B76" s="89" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
-        <v>216</v>
-      </c>
-      <c r="B77" s="85" t="s">
+        <v>217</v>
+      </c>
+      <c r="B77" s="89" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
-        <v>217</v>
-      </c>
-      <c r="B78" s="85" t="s">
+        <v>218</v>
+      </c>
+      <c r="B78" s="89" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
-        <v>218</v>
-      </c>
-      <c r="B79" s="85" t="s">
+        <v>219</v>
+      </c>
+      <c r="B79" s="89" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
-        <v>219</v>
-      </c>
-      <c r="B80" s="85" t="s">
+        <v>220</v>
+      </c>
+      <c r="B80" s="89" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
-        <v>220</v>
-      </c>
-      <c r="B81" s="85" t="s">
+        <v>221</v>
+      </c>
+      <c r="B81" s="89" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
-        <v>221</v>
-      </c>
-      <c r="B82" s="85" t="s">
+        <v>222</v>
+      </c>
+      <c r="B82" s="89" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
-        <v>222</v>
-      </c>
-      <c r="B83" s="85" t="s">
+        <v>223</v>
+      </c>
+      <c r="B83" s="89" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
-        <v>223</v>
-      </c>
-      <c r="B84" s="85" t="s">
+        <v>224</v>
+      </c>
+      <c r="B84" s="89" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="s">
-        <v>224</v>
-      </c>
-      <c r="B85" s="85" t="s">
+        <v>225</v>
+      </c>
+      <c r="B85" s="89" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
-        <v>225</v>
-      </c>
-      <c r="B86" s="85" t="s">
+        <v>226</v>
+      </c>
+      <c r="B86" s="89" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
-        <v>226</v>
-      </c>
-      <c r="B87" s="85" t="s">
+        <v>227</v>
+      </c>
+      <c r="B87" s="89" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
-        <v>227</v>
-      </c>
-      <c r="B88" s="85" t="s">
+        <v>228</v>
+      </c>
+      <c r="B88" s="89" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
-        <v>228</v>
-      </c>
-      <c r="B89" s="85" t="s">
+        <v>229</v>
+      </c>
+      <c r="B89" s="89" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B90" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B91" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="B92" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="B93" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="B94" s="0" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="s">
+        <v>234</v>
+      </c>
+      <c r="B95" s="0" t="s">
         <v>233</v>
-      </c>
-      <c r="B95" s="0" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="0" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="B96" s="0" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="0" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="B97" s="0" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="0" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="B98" s="0" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="0" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="B99" s="0" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="0" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="B100" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="0" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="B101" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="0" t="s">
-        <v>240</v>
-      </c>
-      <c r="B102" s="85" t="s">
+        <v>241</v>
+      </c>
+      <c r="B102" s="89" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="0" t="s">
-        <v>241</v>
-      </c>
-      <c r="B103" s="85" t="s">
+        <v>242</v>
+      </c>
+      <c r="B103" s="89" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="0" t="s">
-        <v>242</v>
-      </c>
-      <c r="B104" s="85" t="s">
+        <v>243</v>
+      </c>
+      <c r="B104" s="89" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="0" t="s">
-        <v>243</v>
-      </c>
-      <c r="B105" s="85" t="s">
+        <v>244</v>
+      </c>
+      <c r="B105" s="89" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="0" t="s">
-        <v>244</v>
-      </c>
-      <c r="B106" s="85" t="s">
+        <v>245</v>
+      </c>
+      <c r="B106" s="89" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="0" t="s">
-        <v>245</v>
-      </c>
-      <c r="B107" s="85" t="s">
+        <v>246</v>
+      </c>
+      <c r="B107" s="89" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="0" t="s">
-        <v>246</v>
-      </c>
-      <c r="B108" s="85" t="s">
+        <v>247</v>
+      </c>
+      <c r="B108" s="89" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="0" t="s">
-        <v>247</v>
-      </c>
-      <c r="B109" s="85" t="s">
+        <v>248</v>
+      </c>
+      <c r="B109" s="89" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="0" t="s">
-        <v>248</v>
-      </c>
-      <c r="B110" s="85" t="s">
+        <v>249</v>
+      </c>
+      <c r="B110" s="89" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="0" t="s">
-        <v>249</v>
-      </c>
-      <c r="B111" s="85" t="s">
+        <v>250</v>
+      </c>
+      <c r="B111" s="89" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="0" t="s">
-        <v>250</v>
-      </c>
-      <c r="B112" s="85" t="s">
+        <v>251</v>
+      </c>
+      <c r="B112" s="89" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="0" t="s">
-        <v>251</v>
-      </c>
-      <c r="B113" s="85" t="s">
+        <v>252</v>
+      </c>
+      <c r="B113" s="89" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="0" t="s">
-        <v>252</v>
-      </c>
-      <c r="B114" s="85" t="s">
+        <v>253</v>
+      </c>
+      <c r="B114" s="89" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="0" t="s">
-        <v>253</v>
-      </c>
-      <c r="B115" s="85" t="s">
+        <v>254</v>
+      </c>
+      <c r="B115" s="89" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="0" t="s">
-        <v>254</v>
-      </c>
-      <c r="B116" s="85" t="s">
+        <v>255</v>
+      </c>
+      <c r="B116" s="89" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="0" t="s">
-        <v>255</v>
-      </c>
-      <c r="B117" s="85" t="s">
+        <v>256</v>
+      </c>
+      <c r="B117" s="89" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="0" t="s">
-        <v>256</v>
-      </c>
-      <c r="B118" s="85" t="s">
+        <v>257</v>
+      </c>
+      <c r="B118" s="89" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="0" t="s">
-        <v>257</v>
-      </c>
-      <c r="B119" s="85" t="s">
+        <v>258</v>
+      </c>
+      <c r="B119" s="89" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="0" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="B120" s="0" t="s">
         <v>102</v>
@@ -4430,7 +4473,7 @@
     </row>
     <row r="121" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="0" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="B121" s="0" t="s">
         <v>102</v>
@@ -4469,63 +4512,63 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="86" t="s">
-        <v>260</v>
-      </c>
-      <c r="B1" s="87" t="s">
+      <c r="A1" s="90" t="s">
+        <v>261</v>
+      </c>
+      <c r="B1" s="91" t="s">
         <v>48</v>
       </c>
-      <c r="C1" s="87" t="s">
+      <c r="C1" s="91" t="s">
         <v>72</v>
       </c>
-      <c r="D1" s="87" t="s">
+      <c r="D1" s="91" t="s">
         <v>74</v>
       </c>
-      <c r="E1" s="87" t="s">
+      <c r="E1" s="91" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="88" t="s">
+      <c r="A2" s="92" t="s">
         <v>41</v>
       </c>
-      <c r="B2" s="64" t="n">
+      <c r="B2" s="65" t="n">
         <v>1</v>
       </c>
-      <c r="C2" s="64"/>
-      <c r="D2" s="64"/>
-      <c r="E2" s="64"/>
+      <c r="C2" s="65"/>
+      <c r="D2" s="65"/>
+      <c r="E2" s="65"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="88" t="s">
+      <c r="A3" s="92" t="s">
         <v>71</v>
       </c>
-      <c r="B3" s="64"/>
-      <c r="C3" s="64" t="n">
+      <c r="B3" s="65"/>
+      <c r="C3" s="65" t="n">
         <v>1</v>
       </c>
-      <c r="D3" s="64"/>
-      <c r="E3" s="64"/>
+      <c r="D3" s="65"/>
+      <c r="E3" s="65"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="88" t="s">
+      <c r="A4" s="92" t="s">
         <v>73</v>
       </c>
-      <c r="B4" s="64"/>
-      <c r="C4" s="64"/>
-      <c r="D4" s="64" t="n">
+      <c r="B4" s="65"/>
+      <c r="C4" s="65"/>
+      <c r="D4" s="65" t="n">
         <v>1</v>
       </c>
-      <c r="E4" s="64"/>
+      <c r="E4" s="65"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="88" t="s">
+      <c r="A5" s="92" t="s">
         <v>75</v>
       </c>
-      <c r="B5" s="64"/>
-      <c r="C5" s="64"/>
-      <c r="D5" s="64"/>
-      <c r="E5" s="64" t="n">
+      <c r="B5" s="65"/>
+      <c r="C5" s="65"/>
+      <c r="D5" s="65"/>
+      <c r="E5" s="65" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>